<commit_message>
Added jrpacman driver (small artifacts left side of screen)
</commit_message>
<xml_diff>
--- a/compatibility_list.xlsx
+++ b/compatibility_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9330" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="working" sheetId="9" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19120" uniqueCount="6957">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19121" uniqueCount="6958">
   <si>
     <t>pacman</t>
   </si>
@@ -20946,6 +20946,9 @@
   </si>
   <si>
     <t>screen doesn't clear blue color in left and right of screen</t>
+  </si>
+  <si>
+    <t>small artifacts left side of screen</t>
   </si>
 </sst>
 </file>
@@ -21261,7 +21264,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -21271,7 +21274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
@@ -22473,10 +22476,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22603,6 +22606,29 @@
         <v>6956</v>
       </c>
     </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>74</v>
+      </c>
+      <c r="R5" t="s">
+        <v>6957</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22612,8 +22638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R3103"/>
   <sheetViews>
-    <sheetView topLeftCell="A2507" workbookViewId="0">
-      <selection activeCell="A2525" sqref="A2525:XFD2526"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22693,23 +22719,6 @@
         <v>5014</v>
       </c>
     </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>74</v>
-      </c>
-    </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
Added support for triviaes game (from mame 0.104u7) in balsente driver
</commit_message>
<xml_diff>
--- a/compatibility_list.xlsx
+++ b/compatibility_list.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19137" uniqueCount="6958">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19143" uniqueCount="6960">
   <si>
     <t>pacman</t>
   </si>
@@ -20955,6 +20955,12 @@
   </si>
   <si>
     <t>small artifacts left side of screen</t>
+  </si>
+  <si>
+    <t>triviaes</t>
+  </si>
+  <si>
+    <t>Trivial Pursuit (Spanish Edition)</t>
   </si>
 </sst>
 </file>
@@ -21290,8 +21296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q156"/>
   <sheetViews>
-    <sheetView topLeftCell="G46" workbookViewId="0">
-      <selection activeCell="Q57" sqref="Q57"/>
+    <sheetView topLeftCell="J126" workbookViewId="0">
+      <selection activeCell="B141" sqref="B141:Q141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -82532,10 +82538,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Q342"/>
+  <dimension ref="B1:Q344"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A322" workbookViewId="0">
-      <selection activeCell="F339" sqref="F339"/>
+    <sheetView tabSelected="1" topLeftCell="A331" workbookViewId="0">
+      <selection activeCell="Q344" sqref="Q344"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -89627,6 +89633,29 @@
         <v>3761</v>
       </c>
     </row>
+    <row r="343" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B343" s="1" t="s">
+        <v>6958</v>
+      </c>
+      <c r="C343" t="s">
+        <v>865</v>
+      </c>
+      <c r="D343" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="E343" t="s">
+        <v>2426</v>
+      </c>
+      <c r="L343" t="s">
+        <v>3894</v>
+      </c>
+      <c r="Q343" t="s">
+        <v>6959</v>
+      </c>
+    </row>
+    <row r="344" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q344" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
added working speedbal driver
</commit_message>
<xml_diff>
--- a/compatibility_list.xlsx
+++ b/compatibility_list.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NetBeansProjects\arcadeflex056\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9330" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9330" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="working" sheetId="9" r:id="rId1"/>
@@ -21,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="DETAILS" localSheetId="4">WIP!#REF!</definedName>
-    <definedName name="DETAILS_1" localSheetId="4">WIP!$B$1:$Q$2636</definedName>
+    <definedName name="DETAILS_1" localSheetId="4">WIP!$B$1:$Q$2635</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -21014,7 +21009,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -21288,7 +21283,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -21296,13 +21291,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q156"/>
+  <dimension ref="A1:Q157"/>
   <sheetViews>
-    <sheetView topLeftCell="J126" workbookViewId="0">
-      <selection activeCell="B141" sqref="B141:Q141"/>
+    <sheetView topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="G153" sqref="G153"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -24743,6 +24738,29 @@
       </c>
       <c r="Q156" t="s">
         <v>4828</v>
+      </c>
+    </row>
+    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>156</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>3454</v>
+      </c>
+      <c r="C157" t="s">
+        <v>3455</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E157" t="s">
+        <v>2</v>
+      </c>
+      <c r="L157" t="s">
+        <v>5071</v>
+      </c>
+      <c r="Q157" t="s">
+        <v>3456</v>
       </c>
     </row>
   </sheetData>
@@ -24758,7 +24776,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
@@ -24873,7 +24891,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
   </cols>
@@ -24961,7 +24979,7 @@
       <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -25116,13 +25134,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R2636"/>
+  <dimension ref="B1:R2635"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A511" workbookViewId="0">
-      <selection activeCell="B517" sqref="B517"/>
+    <sheetView tabSelected="1" topLeftCell="A2406" workbookViewId="0">
+      <selection activeCell="H2415" sqref="H2415"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
@@ -77934,27 +77952,21 @@
     </row>
     <row r="2421" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2421" s="1" t="s">
-        <v>3454</v>
+        <v>6808</v>
       </c>
       <c r="C2421" t="s">
-        <v>3455</v>
-      </c>
-      <c r="D2421" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2421" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2421" t="s">
-        <v>5071</v>
+        <v>6809</v>
+      </c>
+      <c r="D2421" s="1">
+        <v>68000</v>
       </c>
       <c r="Q2421" t="s">
-        <v>3456</v>
+        <v>6810</v>
       </c>
     </row>
     <row r="2422" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2422" s="1" t="s">
-        <v>6808</v>
+        <v>6811</v>
       </c>
       <c r="C2422" t="s">
         <v>6809</v>
@@ -77963,12 +77975,12 @@
         <v>68000</v>
       </c>
       <c r="Q2422" t="s">
-        <v>6810</v>
+        <v>6812</v>
       </c>
     </row>
     <row r="2423" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2423" s="1" t="s">
-        <v>6811</v>
+        <v>6813</v>
       </c>
       <c r="C2423" t="s">
         <v>6809</v>
@@ -77977,12 +77989,12 @@
         <v>68000</v>
       </c>
       <c r="Q2423" t="s">
-        <v>6812</v>
+        <v>6814</v>
       </c>
     </row>
     <row r="2424" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2424" s="1" t="s">
-        <v>6813</v>
+        <v>6815</v>
       </c>
       <c r="C2424" t="s">
         <v>6809</v>
@@ -77991,12 +78003,12 @@
         <v>68000</v>
       </c>
       <c r="Q2424" t="s">
-        <v>6814</v>
+        <v>6816</v>
       </c>
     </row>
     <row r="2425" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2425" s="1" t="s">
-        <v>6815</v>
+        <v>6817</v>
       </c>
       <c r="C2425" t="s">
         <v>6809</v>
@@ -78005,12 +78017,12 @@
         <v>68000</v>
       </c>
       <c r="Q2425" t="s">
-        <v>6816</v>
+        <v>6818</v>
       </c>
     </row>
     <row r="2426" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2426" s="1" t="s">
-        <v>6817</v>
+        <v>6819</v>
       </c>
       <c r="C2426" t="s">
         <v>6809</v>
@@ -78019,12 +78031,12 @@
         <v>68000</v>
       </c>
       <c r="Q2426" t="s">
-        <v>6818</v>
+        <v>6820</v>
       </c>
     </row>
     <row r="2427" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2427" s="1" t="s">
-        <v>6819</v>
+        <v>6821</v>
       </c>
       <c r="C2427" t="s">
         <v>6809</v>
@@ -78033,12 +78045,12 @@
         <v>68000</v>
       </c>
       <c r="Q2427" t="s">
-        <v>6820</v>
+        <v>6822</v>
       </c>
     </row>
     <row r="2428" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2428" s="1" t="s">
-        <v>6821</v>
+        <v>6823</v>
       </c>
       <c r="C2428" t="s">
         <v>6809</v>
@@ -78047,12 +78059,12 @@
         <v>68000</v>
       </c>
       <c r="Q2428" t="s">
-        <v>6822</v>
+        <v>6824</v>
       </c>
     </row>
     <row r="2429" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2429" s="1" t="s">
-        <v>6823</v>
+        <v>6825</v>
       </c>
       <c r="C2429" t="s">
         <v>6809</v>
@@ -78061,12 +78073,12 @@
         <v>68000</v>
       </c>
       <c r="Q2429" t="s">
-        <v>6824</v>
+        <v>6826</v>
       </c>
     </row>
     <row r="2430" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2430" s="1" t="s">
-        <v>6825</v>
+        <v>6827</v>
       </c>
       <c r="C2430" t="s">
         <v>6809</v>
@@ -78075,12 +78087,12 @@
         <v>68000</v>
       </c>
       <c r="Q2430" t="s">
-        <v>6826</v>
+        <v>6828</v>
       </c>
     </row>
     <row r="2431" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2431" s="1" t="s">
-        <v>6827</v>
+        <v>6829</v>
       </c>
       <c r="C2431" t="s">
         <v>6809</v>
@@ -78089,12 +78101,12 @@
         <v>68000</v>
       </c>
       <c r="Q2431" t="s">
-        <v>6828</v>
+        <v>6830</v>
       </c>
     </row>
     <row r="2432" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2432" s="1" t="s">
-        <v>6829</v>
+        <v>6831</v>
       </c>
       <c r="C2432" t="s">
         <v>6809</v>
@@ -78103,12 +78115,12 @@
         <v>68000</v>
       </c>
       <c r="Q2432" t="s">
-        <v>6830</v>
+        <v>6832</v>
       </c>
     </row>
     <row r="2433" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2433" s="1" t="s">
-        <v>6831</v>
+        <v>6833</v>
       </c>
       <c r="C2433" t="s">
         <v>6809</v>
@@ -78116,13 +78128,19 @@
       <c r="D2433" s="1">
         <v>68000</v>
       </c>
+      <c r="L2433" t="s">
+        <v>1687</v>
+      </c>
+      <c r="M2433" t="s">
+        <v>6093</v>
+      </c>
       <c r="Q2433" t="s">
-        <v>6832</v>
+        <v>6834</v>
       </c>
     </row>
     <row r="2434" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2434" s="1" t="s">
-        <v>6833</v>
+        <v>6835</v>
       </c>
       <c r="C2434" t="s">
         <v>6809</v>
@@ -78137,12 +78155,12 @@
         <v>6093</v>
       </c>
       <c r="Q2434" t="s">
-        <v>6834</v>
+        <v>6836</v>
       </c>
     </row>
     <row r="2435" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2435" s="1" t="s">
-        <v>6835</v>
+        <v>6837</v>
       </c>
       <c r="C2435" t="s">
         <v>6809</v>
@@ -78150,19 +78168,13 @@
       <c r="D2435" s="1">
         <v>68000</v>
       </c>
-      <c r="L2435" t="s">
-        <v>1687</v>
-      </c>
-      <c r="M2435" t="s">
-        <v>6093</v>
-      </c>
       <c r="Q2435" t="s">
-        <v>6836</v>
+        <v>6838</v>
       </c>
     </row>
     <row r="2436" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2436" s="1" t="s">
-        <v>6837</v>
+        <v>6839</v>
       </c>
       <c r="C2436" t="s">
         <v>6809</v>
@@ -78171,12 +78183,12 @@
         <v>68000</v>
       </c>
       <c r="Q2436" t="s">
-        <v>6838</v>
+        <v>6840</v>
       </c>
     </row>
     <row r="2437" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2437" s="1" t="s">
-        <v>6839</v>
+        <v>6841</v>
       </c>
       <c r="C2437" t="s">
         <v>6809</v>
@@ -78185,12 +78197,12 @@
         <v>68000</v>
       </c>
       <c r="Q2437" t="s">
-        <v>6840</v>
+        <v>6842</v>
       </c>
     </row>
     <row r="2438" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2438" s="1" t="s">
-        <v>6841</v>
+        <v>6843</v>
       </c>
       <c r="C2438" t="s">
         <v>6809</v>
@@ -78198,13 +78210,19 @@
       <c r="D2438" s="1">
         <v>68000</v>
       </c>
+      <c r="L2438" t="s">
+        <v>1687</v>
+      </c>
+      <c r="M2438" t="s">
+        <v>6093</v>
+      </c>
       <c r="Q2438" t="s">
-        <v>6842</v>
+        <v>6844</v>
       </c>
     </row>
     <row r="2439" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2439" s="1" t="s">
-        <v>6843</v>
+        <v>6845</v>
       </c>
       <c r="C2439" t="s">
         <v>6809</v>
@@ -78212,19 +78230,13 @@
       <c r="D2439" s="1">
         <v>68000</v>
       </c>
-      <c r="L2439" t="s">
-        <v>1687</v>
-      </c>
-      <c r="M2439" t="s">
-        <v>6093</v>
-      </c>
       <c r="Q2439" t="s">
-        <v>6844</v>
+        <v>6846</v>
       </c>
     </row>
     <row r="2440" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2440" s="1" t="s">
-        <v>6845</v>
+        <v>6847</v>
       </c>
       <c r="C2440" t="s">
         <v>6809</v>
@@ -78232,13 +78244,19 @@
       <c r="D2440" s="1">
         <v>68000</v>
       </c>
+      <c r="L2440" t="s">
+        <v>1687</v>
+      </c>
+      <c r="M2440" t="s">
+        <v>6093</v>
+      </c>
       <c r="Q2440" t="s">
-        <v>6846</v>
+        <v>6848</v>
       </c>
     </row>
     <row r="2441" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2441" s="1" t="s">
-        <v>6847</v>
+        <v>6849</v>
       </c>
       <c r="C2441" t="s">
         <v>6809</v>
@@ -78253,12 +78271,12 @@
         <v>6093</v>
       </c>
       <c r="Q2441" t="s">
-        <v>6848</v>
+        <v>6850</v>
       </c>
     </row>
     <row r="2442" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2442" s="1" t="s">
-        <v>6849</v>
+        <v>6851</v>
       </c>
       <c r="C2442" t="s">
         <v>6809</v>
@@ -78266,33 +78284,33 @@
       <c r="D2442" s="1">
         <v>68000</v>
       </c>
-      <c r="L2442" t="s">
-        <v>1687</v>
-      </c>
-      <c r="M2442" t="s">
-        <v>6093</v>
-      </c>
       <c r="Q2442" t="s">
-        <v>6850</v>
+        <v>6852</v>
       </c>
     </row>
     <row r="2443" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2443" s="1" t="s">
-        <v>6851</v>
+        <v>6853</v>
       </c>
       <c r="C2443" t="s">
-        <v>6809</v>
-      </c>
-      <c r="D2443" s="1">
-        <v>68000</v>
+        <v>6854</v>
+      </c>
+      <c r="D2443" s="1" t="s">
+        <v>3469</v>
+      </c>
+      <c r="E2443" t="s">
+        <v>3794</v>
+      </c>
+      <c r="L2443" t="s">
+        <v>1900</v>
       </c>
       <c r="Q2443" t="s">
-        <v>6852</v>
+        <v>6855</v>
       </c>
     </row>
     <row r="2444" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2444" s="1" t="s">
-        <v>6853</v>
+        <v>6856</v>
       </c>
       <c r="C2444" t="s">
         <v>6854</v>
@@ -78307,12 +78325,12 @@
         <v>1900</v>
       </c>
       <c r="Q2444" t="s">
-        <v>6855</v>
+        <v>6857</v>
       </c>
     </row>
     <row r="2445" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2445" s="1" t="s">
-        <v>6856</v>
+        <v>3468</v>
       </c>
       <c r="C2445" t="s">
         <v>6854</v>
@@ -78327,32 +78345,44 @@
         <v>1900</v>
       </c>
       <c r="Q2445" t="s">
-        <v>6857</v>
+        <v>3470</v>
       </c>
     </row>
     <row r="2446" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2446" s="1" t="s">
-        <v>3468</v>
+        <v>6858</v>
       </c>
       <c r="C2446" t="s">
-        <v>6854</v>
+        <v>6859</v>
       </c>
       <c r="D2446" s="1" t="s">
-        <v>3469</v>
+        <v>6860</v>
       </c>
       <c r="E2446" t="s">
-        <v>3794</v>
+        <v>6861</v>
+      </c>
+      <c r="F2446" t="s">
+        <v>6862</v>
       </c>
       <c r="L2446" t="s">
-        <v>1900</v>
+        <v>6863</v>
+      </c>
+      <c r="M2446" t="s">
+        <v>6864</v>
+      </c>
+      <c r="N2446" t="s">
+        <v>6865</v>
+      </c>
+      <c r="O2446" t="s">
+        <v>6866</v>
       </c>
       <c r="Q2446" t="s">
-        <v>3470</v>
+        <v>6867</v>
       </c>
     </row>
     <row r="2447" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2447" s="1" t="s">
-        <v>6858</v>
+        <v>6868</v>
       </c>
       <c r="C2447" t="s">
         <v>6859</v>
@@ -78379,12 +78409,12 @@
         <v>6866</v>
       </c>
       <c r="Q2447" t="s">
-        <v>6867</v>
+        <v>6869</v>
       </c>
     </row>
     <row r="2448" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2448" s="1" t="s">
-        <v>6868</v>
+        <v>6870</v>
       </c>
       <c r="C2448" t="s">
         <v>6859</v>
@@ -78411,44 +78441,35 @@
         <v>6866</v>
       </c>
       <c r="Q2448" t="s">
-        <v>6869</v>
+        <v>6871</v>
       </c>
     </row>
     <row r="2449" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2449" s="1" t="s">
-        <v>6870</v>
+        <v>6872</v>
       </c>
       <c r="C2449" t="s">
-        <v>6859</v>
+        <v>6873</v>
       </c>
       <c r="D2449" s="1" t="s">
-        <v>6860</v>
+        <v>2</v>
       </c>
       <c r="E2449" t="s">
-        <v>6861</v>
-      </c>
-      <c r="F2449" t="s">
-        <v>6862</v>
+        <v>2426</v>
       </c>
       <c r="L2449" t="s">
-        <v>6863</v>
+        <v>5071</v>
       </c>
       <c r="M2449" t="s">
-        <v>6864</v>
-      </c>
-      <c r="N2449" t="s">
-        <v>6865</v>
-      </c>
-      <c r="O2449" t="s">
-        <v>6866</v>
+        <v>3974</v>
       </c>
       <c r="Q2449" t="s">
-        <v>6871</v>
+        <v>6874</v>
       </c>
     </row>
     <row r="2450" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2450" s="1" t="s">
-        <v>6872</v>
+        <v>3490</v>
       </c>
       <c r="C2450" t="s">
         <v>6873</v>
@@ -78466,18 +78487,18 @@
         <v>3974</v>
       </c>
       <c r="Q2450" t="s">
-        <v>6874</v>
+        <v>6875</v>
       </c>
     </row>
     <row r="2451" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2451" s="1" t="s">
-        <v>3490</v>
+        <v>6876</v>
       </c>
       <c r="C2451" t="s">
-        <v>6873</v>
-      </c>
-      <c r="D2451" s="1" t="s">
-        <v>2</v>
+        <v>6877</v>
+      </c>
+      <c r="D2451" s="1">
+        <v>68000</v>
       </c>
       <c r="E2451" t="s">
         <v>2426</v>
@@ -78486,15 +78507,15 @@
         <v>5071</v>
       </c>
       <c r="M2451" t="s">
-        <v>3974</v>
+        <v>1687</v>
       </c>
       <c r="Q2451" t="s">
-        <v>6875</v>
+        <v>6878</v>
       </c>
     </row>
     <row r="2452" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2452" s="1" t="s">
-        <v>6876</v>
+        <v>6879</v>
       </c>
       <c r="C2452" t="s">
         <v>6877</v>
@@ -78502,39 +78523,42 @@
       <c r="D2452" s="1">
         <v>68000</v>
       </c>
-      <c r="E2452" t="s">
-        <v>2426</v>
-      </c>
       <c r="L2452" t="s">
-        <v>5071</v>
-      </c>
-      <c r="M2452" t="s">
         <v>1687</v>
       </c>
       <c r="Q2452" t="s">
-        <v>6878</v>
+        <v>6880</v>
       </c>
     </row>
     <row r="2453" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2453" s="1" t="s">
-        <v>6879</v>
+        <v>6881</v>
       </c>
       <c r="C2453" t="s">
-        <v>6877</v>
+        <v>6882</v>
       </c>
       <c r="D2453" s="1">
         <v>68000</v>
       </c>
+      <c r="E2453" t="s">
+        <v>2426</v>
+      </c>
       <c r="L2453" t="s">
+        <v>5070</v>
+      </c>
+      <c r="M2453" t="s">
+        <v>5071</v>
+      </c>
+      <c r="N2453" t="s">
         <v>1687</v>
       </c>
       <c r="Q2453" t="s">
-        <v>6880</v>
+        <v>6883</v>
       </c>
     </row>
     <row r="2454" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2454" s="1" t="s">
-        <v>6881</v>
+        <v>6884</v>
       </c>
       <c r="C2454" t="s">
         <v>6882</v>
@@ -78555,12 +78579,12 @@
         <v>1687</v>
       </c>
       <c r="Q2454" t="s">
-        <v>6883</v>
+        <v>6885</v>
       </c>
     </row>
     <row r="2455" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2455" s="1" t="s">
-        <v>6884</v>
+        <v>6886</v>
       </c>
       <c r="C2455" t="s">
         <v>6882</v>
@@ -78581,38 +78605,32 @@
         <v>1687</v>
       </c>
       <c r="Q2455" t="s">
-        <v>6885</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="2456" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2456" s="1" t="s">
-        <v>6886</v>
+        <v>6888</v>
       </c>
       <c r="C2456" t="s">
-        <v>6882</v>
+        <v>6889</v>
       </c>
       <c r="D2456" s="1">
         <v>68000</v>
       </c>
-      <c r="E2456" t="s">
-        <v>2426</v>
-      </c>
       <c r="L2456" t="s">
-        <v>5070</v>
+        <v>5071</v>
       </c>
       <c r="M2456" t="s">
-        <v>5071</v>
-      </c>
-      <c r="N2456" t="s">
         <v>1687</v>
       </c>
       <c r="Q2456" t="s">
-        <v>6887</v>
+        <v>6890</v>
       </c>
     </row>
     <row r="2457" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2457" s="1" t="s">
-        <v>6888</v>
+        <v>6891</v>
       </c>
       <c r="C2457" t="s">
         <v>6889</v>
@@ -78627,32 +78645,35 @@
         <v>1687</v>
       </c>
       <c r="Q2457" t="s">
-        <v>6890</v>
+        <v>6892</v>
       </c>
     </row>
     <row r="2458" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2458" s="1" t="s">
-        <v>6891</v>
+        <v>6893</v>
       </c>
       <c r="C2458" t="s">
-        <v>6889</v>
+        <v>6894</v>
       </c>
       <c r="D2458" s="1">
         <v>68000</v>
       </c>
+      <c r="E2458" t="s">
+        <v>2426</v>
+      </c>
       <c r="L2458" t="s">
-        <v>5071</v>
+        <v>5238</v>
       </c>
       <c r="M2458" t="s">
         <v>1687</v>
       </c>
       <c r="Q2458" t="s">
-        <v>6892</v>
+        <v>6895</v>
       </c>
     </row>
     <row r="2459" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2459" s="1" t="s">
-        <v>6893</v>
+        <v>6896</v>
       </c>
       <c r="C2459" t="s">
         <v>6894</v>
@@ -78670,15 +78691,15 @@
         <v>1687</v>
       </c>
       <c r="Q2459" t="s">
-        <v>6895</v>
+        <v>6897</v>
       </c>
     </row>
     <row r="2460" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2460" s="1" t="s">
-        <v>6896</v>
+        <v>6898</v>
       </c>
       <c r="C2460" t="s">
-        <v>6894</v>
+        <v>6899</v>
       </c>
       <c r="D2460" s="1">
         <v>68000</v>
@@ -78687,58 +78708,61 @@
         <v>2426</v>
       </c>
       <c r="L2460" t="s">
-        <v>5238</v>
+        <v>5071</v>
       </c>
       <c r="M2460" t="s">
         <v>1687</v>
       </c>
       <c r="Q2460" t="s">
-        <v>6897</v>
+        <v>6900</v>
       </c>
     </row>
     <row r="2461" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2461" s="1" t="s">
-        <v>6898</v>
+        <v>6901</v>
       </c>
       <c r="C2461" t="s">
-        <v>6899</v>
-      </c>
-      <c r="D2461" s="1">
-        <v>68000</v>
-      </c>
-      <c r="E2461" t="s">
-        <v>2426</v>
+        <v>6902</v>
+      </c>
+      <c r="D2461" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="L2461" t="s">
-        <v>5071</v>
-      </c>
-      <c r="M2461" t="s">
-        <v>1687</v>
+        <v>5070</v>
       </c>
       <c r="Q2461" t="s">
-        <v>6900</v>
+        <v>6903</v>
       </c>
     </row>
     <row r="2462" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2462" s="1" t="s">
-        <v>6901</v>
+        <v>6904</v>
       </c>
       <c r="C2462" t="s">
-        <v>6902</v>
+        <v>6905</v>
       </c>
       <c r="D2462" s="1" t="s">
-        <v>2</v>
+        <v>404</v>
+      </c>
+      <c r="E2462" t="s">
+        <v>6906</v>
+      </c>
+      <c r="F2462" t="s">
+        <v>6906</v>
       </c>
       <c r="L2462" t="s">
-        <v>5070</v>
+        <v>3714</v>
+      </c>
+      <c r="M2462" t="s">
+        <v>2605</v>
       </c>
       <c r="Q2462" t="s">
-        <v>6903</v>
+        <v>6907</v>
       </c>
     </row>
     <row r="2463" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2463" s="1" t="s">
-        <v>6904</v>
+        <v>6908</v>
       </c>
       <c r="C2463" t="s">
         <v>6905</v>
@@ -78759,12 +78783,12 @@
         <v>2605</v>
       </c>
       <c r="Q2463" t="s">
-        <v>6907</v>
+        <v>6909</v>
       </c>
     </row>
     <row r="2464" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2464" s="1" t="s">
-        <v>6908</v>
+        <v>6910</v>
       </c>
       <c r="C2464" t="s">
         <v>6905</v>
@@ -78785,38 +78809,29 @@
         <v>2605</v>
       </c>
       <c r="Q2464" t="s">
-        <v>6909</v>
+        <v>6911</v>
       </c>
     </row>
     <row r="2465" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2465" s="1" t="s">
-        <v>6910</v>
+        <v>3439</v>
       </c>
       <c r="C2465" t="s">
-        <v>6905</v>
+        <v>3440</v>
       </c>
       <c r="D2465" s="1" t="s">
         <v>404</v>
       </c>
       <c r="E2465" t="s">
-        <v>6906</v>
-      </c>
-      <c r="F2465" t="s">
-        <v>6906</v>
-      </c>
-      <c r="L2465" t="s">
-        <v>3714</v>
-      </c>
-      <c r="M2465" t="s">
-        <v>2605</v>
+        <v>3888</v>
       </c>
       <c r="Q2465" t="s">
-        <v>6911</v>
+        <v>3441</v>
       </c>
     </row>
     <row r="2466" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2466" s="1" t="s">
-        <v>3439</v>
+        <v>3442</v>
       </c>
       <c r="C2466" t="s">
         <v>3440</v>
@@ -78828,29 +78843,32 @@
         <v>3888</v>
       </c>
       <c r="Q2466" t="s">
-        <v>3441</v>
+        <v>3443</v>
       </c>
     </row>
     <row r="2467" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2467" s="1" t="s">
-        <v>3442</v>
+        <v>3402</v>
       </c>
       <c r="C2467" t="s">
-        <v>3440</v>
+        <v>3403</v>
       </c>
       <c r="D2467" s="1" t="s">
-        <v>404</v>
+        <v>2</v>
       </c>
       <c r="E2467" t="s">
-        <v>3888</v>
+        <v>3794</v>
+      </c>
+      <c r="L2467" t="s">
+        <v>542</v>
       </c>
       <c r="Q2467" t="s">
-        <v>3443</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="2468" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2468" s="1" t="s">
-        <v>3402</v>
+        <v>3404</v>
       </c>
       <c r="C2468" t="s">
         <v>3403</v>
@@ -78865,12 +78883,12 @@
         <v>542</v>
       </c>
       <c r="Q2468" t="s">
-        <v>4580</v>
+        <v>3405</v>
       </c>
     </row>
     <row r="2469" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2469" s="1" t="s">
-        <v>3404</v>
+        <v>3406</v>
       </c>
       <c r="C2469" t="s">
         <v>3403</v>
@@ -78885,12 +78903,12 @@
         <v>542</v>
       </c>
       <c r="Q2469" t="s">
-        <v>3405</v>
+        <v>3407</v>
       </c>
     </row>
     <row r="2470" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2470" s="1" t="s">
-        <v>3406</v>
+        <v>3408</v>
       </c>
       <c r="C2470" t="s">
         <v>3403</v>
@@ -78905,12 +78923,12 @@
         <v>542</v>
       </c>
       <c r="Q2470" t="s">
-        <v>3407</v>
+        <v>3409</v>
       </c>
     </row>
     <row r="2471" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2471" s="1" t="s">
-        <v>3408</v>
+        <v>3410</v>
       </c>
       <c r="C2471" t="s">
         <v>3403</v>
@@ -78925,52 +78943,49 @@
         <v>542</v>
       </c>
       <c r="Q2471" t="s">
-        <v>3409</v>
+        <v>3411</v>
       </c>
     </row>
     <row r="2472" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2472" s="1" t="s">
-        <v>3410</v>
+        <v>3419</v>
       </c>
       <c r="C2472" t="s">
-        <v>3403</v>
+        <v>3420</v>
       </c>
       <c r="D2472" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E2472" t="s">
-        <v>3794</v>
+        <v>2426</v>
       </c>
       <c r="L2472" t="s">
-        <v>542</v>
+        <v>1155</v>
       </c>
       <c r="Q2472" t="s">
-        <v>3411</v>
+        <v>3421</v>
       </c>
     </row>
     <row r="2473" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2473" s="1" t="s">
-        <v>3419</v>
+        <v>3422</v>
       </c>
       <c r="C2473" t="s">
-        <v>3420</v>
+        <v>3423</v>
       </c>
       <c r="D2473" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="E2473" t="s">
-        <v>2426</v>
       </c>
       <c r="L2473" t="s">
         <v>1155</v>
       </c>
       <c r="Q2473" t="s">
-        <v>3421</v>
+        <v>3424</v>
       </c>
     </row>
     <row r="2474" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2474" s="1" t="s">
-        <v>3422</v>
+        <v>3425</v>
       </c>
       <c r="C2474" t="s">
         <v>3423</v>
@@ -78982,180 +78997,180 @@
         <v>1155</v>
       </c>
       <c r="Q2474" t="s">
-        <v>3424</v>
+        <v>3426</v>
       </c>
     </row>
     <row r="2475" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2475" s="1" t="s">
-        <v>3425</v>
+        <v>3432</v>
       </c>
       <c r="C2475" t="s">
-        <v>3423</v>
+        <v>3433</v>
       </c>
       <c r="D2475" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L2475" t="s">
-        <v>1155</v>
+        <v>55</v>
       </c>
       <c r="Q2475" t="s">
-        <v>3426</v>
+        <v>3434</v>
       </c>
     </row>
     <row r="2476" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2476" s="1" t="s">
-        <v>3432</v>
+        <v>3444</v>
       </c>
       <c r="C2476" t="s">
-        <v>3433</v>
-      </c>
-      <c r="D2476" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2476" t="s">
-        <v>55</v>
+        <v>3445</v>
+      </c>
+      <c r="D2476" s="1">
+        <v>8080</v>
       </c>
       <c r="Q2476" t="s">
-        <v>3434</v>
+        <v>3446</v>
       </c>
     </row>
     <row r="2477" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2477" s="1" t="s">
-        <v>3444</v>
+        <v>3447</v>
       </c>
       <c r="C2477" t="s">
-        <v>3445</v>
-      </c>
-      <c r="D2477" s="1">
-        <v>8080</v>
+        <v>3448</v>
+      </c>
+      <c r="D2477" s="1" t="s">
+        <v>3006</v>
+      </c>
+      <c r="E2477" t="s">
+        <v>3006</v>
+      </c>
+      <c r="F2477" t="s">
+        <v>3899</v>
+      </c>
+      <c r="G2477" t="s">
+        <v>3899</v>
+      </c>
+      <c r="L2477" t="s">
+        <v>2605</v>
+      </c>
+      <c r="M2477" t="s">
+        <v>5238</v>
       </c>
       <c r="Q2477" t="s">
-        <v>3446</v>
+        <v>4581</v>
       </c>
     </row>
     <row r="2478" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2478" s="1" t="s">
-        <v>3447</v>
+        <v>3460</v>
       </c>
       <c r="C2478" t="s">
-        <v>3448</v>
+        <v>3461</v>
       </c>
       <c r="D2478" s="1" t="s">
-        <v>3006</v>
-      </c>
-      <c r="E2478" t="s">
-        <v>3006</v>
-      </c>
-      <c r="F2478" t="s">
-        <v>3899</v>
-      </c>
-      <c r="G2478" t="s">
-        <v>3899</v>
+        <v>2</v>
       </c>
       <c r="L2478" t="s">
-        <v>2605</v>
-      </c>
-      <c r="M2478" t="s">
-        <v>5238</v>
+        <v>1155</v>
       </c>
       <c r="Q2478" t="s">
-        <v>4581</v>
+        <v>3462</v>
       </c>
     </row>
     <row r="2479" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2479" s="1" t="s">
-        <v>3460</v>
+        <v>3463</v>
       </c>
       <c r="C2479" t="s">
-        <v>3461</v>
-      </c>
-      <c r="D2479" s="1" t="s">
-        <v>2</v>
+        <v>3464</v>
+      </c>
+      <c r="D2479" s="1">
+        <v>8080</v>
       </c>
       <c r="L2479" t="s">
-        <v>1155</v>
+        <v>352</v>
       </c>
       <c r="Q2479" t="s">
-        <v>3462</v>
+        <v>3465</v>
       </c>
     </row>
     <row r="2480" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2480" s="1" t="s">
-        <v>3463</v>
+        <v>3466</v>
       </c>
       <c r="C2480" t="s">
-        <v>3464</v>
-      </c>
-      <c r="D2480" s="1">
-        <v>8080</v>
+        <v>3356</v>
+      </c>
+      <c r="D2480" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2480" t="s">
+        <v>2426</v>
       </c>
       <c r="L2480" t="s">
-        <v>352</v>
+        <v>5070</v>
       </c>
       <c r="Q2480" t="s">
-        <v>3465</v>
+        <v>3467</v>
       </c>
     </row>
     <row r="2481" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2481" s="1" t="s">
-        <v>3466</v>
+        <v>3471</v>
       </c>
       <c r="C2481" t="s">
-        <v>3356</v>
-      </c>
-      <c r="D2481" s="1" t="s">
-        <v>2</v>
+        <v>3472</v>
+      </c>
+      <c r="D2481" s="1">
+        <v>68000</v>
       </c>
       <c r="E2481" t="s">
         <v>2426</v>
       </c>
       <c r="L2481" t="s">
-        <v>5070</v>
+        <v>3954</v>
       </c>
       <c r="Q2481" t="s">
-        <v>3467</v>
+        <v>3473</v>
       </c>
     </row>
     <row r="2482" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2482" s="1" t="s">
-        <v>3471</v>
+        <v>3474</v>
       </c>
       <c r="C2482" t="s">
-        <v>3472</v>
-      </c>
-      <c r="D2482" s="1">
-        <v>68000</v>
-      </c>
-      <c r="E2482" t="s">
-        <v>2426</v>
+        <v>3475</v>
+      </c>
+      <c r="D2482" s="1" t="s">
+        <v>351</v>
       </c>
       <c r="L2482" t="s">
-        <v>3954</v>
+        <v>55</v>
       </c>
       <c r="Q2482" t="s">
-        <v>3473</v>
+        <v>3476</v>
       </c>
     </row>
     <row r="2483" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2483" s="1" t="s">
-        <v>3474</v>
+        <v>6912</v>
       </c>
       <c r="C2483" t="s">
-        <v>3475</v>
+        <v>3478</v>
       </c>
       <c r="D2483" s="1" t="s">
-        <v>351</v>
+        <v>2</v>
       </c>
       <c r="L2483" t="s">
-        <v>55</v>
+        <v>352</v>
       </c>
       <c r="Q2483" t="s">
-        <v>3476</v>
+        <v>6913</v>
       </c>
     </row>
     <row r="2484" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2484" s="1" t="s">
-        <v>6912</v>
+        <v>3477</v>
       </c>
       <c r="C2484" t="s">
         <v>3478</v>
@@ -79167,29 +79182,29 @@
         <v>352</v>
       </c>
       <c r="Q2484" t="s">
-        <v>6913</v>
+        <v>4586</v>
       </c>
     </row>
     <row r="2485" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2485" s="1" t="s">
-        <v>3477</v>
+        <v>3479</v>
       </c>
       <c r="C2485" t="s">
-        <v>3478</v>
+        <v>3480</v>
       </c>
       <c r="D2485" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L2485" t="s">
-        <v>352</v>
+        <v>58</v>
       </c>
       <c r="Q2485" t="s">
-        <v>4586</v>
+        <v>3481</v>
       </c>
     </row>
     <row r="2486" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2486" s="1" t="s">
-        <v>3479</v>
+        <v>3482</v>
       </c>
       <c r="C2486" t="s">
         <v>3480</v>
@@ -79201,80 +79216,83 @@
         <v>58</v>
       </c>
       <c r="Q2486" t="s">
-        <v>3481</v>
+        <v>3483</v>
       </c>
     </row>
     <row r="2487" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2487" s="1" t="s">
-        <v>3482</v>
+        <v>3484</v>
       </c>
       <c r="C2487" t="s">
-        <v>3480</v>
+        <v>3485</v>
       </c>
       <c r="D2487" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L2487" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="Q2487" t="s">
-        <v>3483</v>
+        <v>3486</v>
       </c>
     </row>
     <row r="2488" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2488" s="1" t="s">
-        <v>3484</v>
+        <v>3487</v>
       </c>
       <c r="C2488" t="s">
-        <v>3485</v>
+        <v>3488</v>
       </c>
       <c r="D2488" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L2488" t="s">
-        <v>77</v>
+        <v>1155</v>
       </c>
       <c r="Q2488" t="s">
-        <v>3486</v>
+        <v>3489</v>
       </c>
     </row>
     <row r="2489" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2489" s="1" t="s">
-        <v>3487</v>
+        <v>3491</v>
       </c>
       <c r="C2489" t="s">
-        <v>3488</v>
+        <v>3492</v>
       </c>
       <c r="D2489" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L2489" t="s">
-        <v>1155</v>
+        <v>55</v>
       </c>
       <c r="Q2489" t="s">
-        <v>3489</v>
+        <v>3493</v>
       </c>
     </row>
     <row r="2490" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2490" s="1" t="s">
-        <v>3491</v>
+        <v>6914</v>
       </c>
       <c r="C2490" t="s">
-        <v>3492</v>
+        <v>6915</v>
       </c>
       <c r="D2490" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E2490" t="s">
+        <v>2</v>
+      </c>
       <c r="L2490" t="s">
-        <v>55</v>
+        <v>5238</v>
       </c>
       <c r="Q2490" t="s">
-        <v>3493</v>
+        <v>6916</v>
       </c>
     </row>
     <row r="2491" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2491" s="1" t="s">
-        <v>6914</v>
+        <v>6917</v>
       </c>
       <c r="C2491" t="s">
         <v>6915</v>
@@ -79289,32 +79307,29 @@
         <v>5238</v>
       </c>
       <c r="Q2491" t="s">
-        <v>6916</v>
+        <v>6918</v>
       </c>
     </row>
     <row r="2492" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2492" s="1" t="s">
-        <v>6917</v>
+        <v>6919</v>
       </c>
       <c r="C2492" t="s">
-        <v>6915</v>
+        <v>6920</v>
       </c>
       <c r="D2492" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2492" t="s">
-        <v>2</v>
-      </c>
       <c r="L2492" t="s">
-        <v>5238</v>
+        <v>55</v>
       </c>
       <c r="Q2492" t="s">
-        <v>6918</v>
+        <v>6921</v>
       </c>
     </row>
     <row r="2493" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2493" s="1" t="s">
-        <v>6919</v>
+        <v>6922</v>
       </c>
       <c r="C2493" t="s">
         <v>6920</v>
@@ -79322,16 +79337,25 @@
       <c r="D2493" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E2493" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2493" t="s">
+        <v>2426</v>
+      </c>
       <c r="L2493" t="s">
+        <v>542</v>
+      </c>
+      <c r="M2493" t="s">
         <v>55</v>
       </c>
       <c r="Q2493" t="s">
-        <v>6921</v>
+        <v>6923</v>
       </c>
     </row>
     <row r="2494" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2494" s="1" t="s">
-        <v>6922</v>
+        <v>6924</v>
       </c>
       <c r="C2494" t="s">
         <v>6920</v>
@@ -79352,55 +79376,49 @@
         <v>55</v>
       </c>
       <c r="Q2494" t="s">
-        <v>6923</v>
+        <v>6925</v>
       </c>
     </row>
     <row r="2495" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2495" s="1" t="s">
-        <v>6924</v>
+        <v>6926</v>
       </c>
       <c r="C2495" t="s">
-        <v>6920</v>
-      </c>
-      <c r="D2495" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2495" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2495" t="s">
-        <v>2426</v>
+        <v>6927</v>
+      </c>
+      <c r="D2495" s="1">
+        <v>68000</v>
       </c>
       <c r="L2495" t="s">
-        <v>542</v>
-      </c>
-      <c r="M2495" t="s">
-        <v>55</v>
+        <v>1687</v>
       </c>
       <c r="Q2495" t="s">
-        <v>6925</v>
+        <v>6928</v>
       </c>
     </row>
     <row r="2496" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2496" s="1" t="s">
-        <v>6926</v>
+        <v>3494</v>
       </c>
       <c r="C2496" t="s">
-        <v>6927</v>
+        <v>3495</v>
       </c>
       <c r="D2496" s="1">
         <v>68000</v>
       </c>
+      <c r="E2496" t="s">
+        <v>2426</v>
+      </c>
       <c r="L2496" t="s">
-        <v>1687</v>
+        <v>5549</v>
       </c>
       <c r="Q2496" t="s">
-        <v>6928</v>
+        <v>3496</v>
       </c>
     </row>
     <row r="2497" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2497" s="1" t="s">
-        <v>3494</v>
+        <v>3497</v>
       </c>
       <c r="C2497" t="s">
         <v>3495</v>
@@ -79415,12 +79433,12 @@
         <v>5549</v>
       </c>
       <c r="Q2497" t="s">
-        <v>3496</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="2498" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2498" s="1" t="s">
-        <v>3497</v>
+        <v>3498</v>
       </c>
       <c r="C2498" t="s">
         <v>3495</v>
@@ -79435,12 +79453,12 @@
         <v>5549</v>
       </c>
       <c r="Q2498" t="s">
-        <v>4587</v>
+        <v>3499</v>
       </c>
     </row>
     <row r="2499" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2499" s="1" t="s">
-        <v>3498</v>
+        <v>3500</v>
       </c>
       <c r="C2499" t="s">
         <v>3495</v>
@@ -79455,12 +79473,12 @@
         <v>5549</v>
       </c>
       <c r="Q2499" t="s">
-        <v>3499</v>
+        <v>3501</v>
       </c>
     </row>
     <row r="2500" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2500" s="1" t="s">
-        <v>3500</v>
+        <v>3502</v>
       </c>
       <c r="C2500" t="s">
         <v>3495</v>
@@ -79475,12 +79493,12 @@
         <v>5549</v>
       </c>
       <c r="Q2500" t="s">
-        <v>3501</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="2501" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2501" s="1" t="s">
-        <v>3502</v>
+        <v>3504</v>
       </c>
       <c r="C2501" t="s">
         <v>3495</v>
@@ -79495,12 +79513,12 @@
         <v>5549</v>
       </c>
       <c r="Q2501" t="s">
-        <v>3503</v>
+        <v>3505</v>
       </c>
     </row>
     <row r="2502" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2502" s="1" t="s">
-        <v>3504</v>
+        <v>3506</v>
       </c>
       <c r="C2502" t="s">
         <v>3495</v>
@@ -79515,12 +79533,12 @@
         <v>5549</v>
       </c>
       <c r="Q2502" t="s">
-        <v>3505</v>
+        <v>6929</v>
       </c>
     </row>
     <row r="2503" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2503" s="1" t="s">
-        <v>3506</v>
+        <v>6930</v>
       </c>
       <c r="C2503" t="s">
         <v>3495</v>
@@ -79535,12 +79553,12 @@
         <v>5549</v>
       </c>
       <c r="Q2503" t="s">
-        <v>6929</v>
+        <v>6931</v>
       </c>
     </row>
     <row r="2504" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2504" s="1" t="s">
-        <v>6930</v>
+        <v>3507</v>
       </c>
       <c r="C2504" t="s">
         <v>3495</v>
@@ -79555,12 +79573,12 @@
         <v>5549</v>
       </c>
       <c r="Q2504" t="s">
-        <v>6931</v>
+        <v>4952</v>
       </c>
     </row>
     <row r="2505" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2505" s="1" t="s">
-        <v>3507</v>
+        <v>3508</v>
       </c>
       <c r="C2505" t="s">
         <v>3495</v>
@@ -79575,12 +79593,12 @@
         <v>5549</v>
       </c>
       <c r="Q2505" t="s">
-        <v>4952</v>
+        <v>3509</v>
       </c>
     </row>
     <row r="2506" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2506" s="1" t="s">
-        <v>3508</v>
+        <v>3510</v>
       </c>
       <c r="C2506" t="s">
         <v>3495</v>
@@ -79595,12 +79613,12 @@
         <v>5549</v>
       </c>
       <c r="Q2506" t="s">
-        <v>3509</v>
+        <v>3511</v>
       </c>
     </row>
     <row r="2507" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2507" s="1" t="s">
-        <v>3510</v>
+        <v>3512</v>
       </c>
       <c r="C2507" t="s">
         <v>3495</v>
@@ -79615,12 +79633,12 @@
         <v>5549</v>
       </c>
       <c r="Q2507" t="s">
-        <v>3511</v>
+        <v>3513</v>
       </c>
     </row>
     <row r="2508" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2508" s="1" t="s">
-        <v>3512</v>
+        <v>3514</v>
       </c>
       <c r="C2508" t="s">
         <v>3495</v>
@@ -79635,12 +79653,12 @@
         <v>5549</v>
       </c>
       <c r="Q2508" t="s">
-        <v>3513</v>
+        <v>3515</v>
       </c>
     </row>
     <row r="2509" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2509" s="1" t="s">
-        <v>3514</v>
+        <v>3516</v>
       </c>
       <c r="C2509" t="s">
         <v>3495</v>
@@ -79655,12 +79673,12 @@
         <v>5549</v>
       </c>
       <c r="Q2509" t="s">
-        <v>3515</v>
+        <v>3517</v>
       </c>
     </row>
     <row r="2510" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2510" s="1" t="s">
-        <v>3516</v>
+        <v>3518</v>
       </c>
       <c r="C2510" t="s">
         <v>3495</v>
@@ -79675,12 +79693,12 @@
         <v>5549</v>
       </c>
       <c r="Q2510" t="s">
-        <v>3517</v>
+        <v>4953</v>
       </c>
     </row>
     <row r="2511" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2511" s="1" t="s">
-        <v>3518</v>
+        <v>3519</v>
       </c>
       <c r="C2511" t="s">
         <v>3495</v>
@@ -79695,12 +79713,12 @@
         <v>5549</v>
       </c>
       <c r="Q2511" t="s">
-        <v>4953</v>
+        <v>4954</v>
       </c>
     </row>
     <row r="2512" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2512" s="1" t="s">
-        <v>3519</v>
+        <v>3520</v>
       </c>
       <c r="C2512" t="s">
         <v>3495</v>
@@ -79715,12 +79733,12 @@
         <v>5549</v>
       </c>
       <c r="Q2512" t="s">
-        <v>4954</v>
+        <v>3521</v>
       </c>
     </row>
     <row r="2513" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2513" s="1" t="s">
-        <v>3520</v>
+        <v>3522</v>
       </c>
       <c r="C2513" t="s">
         <v>3495</v>
@@ -79735,12 +79753,12 @@
         <v>5549</v>
       </c>
       <c r="Q2513" t="s">
-        <v>3521</v>
+        <v>3523</v>
       </c>
     </row>
     <row r="2514" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2514" s="1" t="s">
-        <v>3522</v>
+        <v>3524</v>
       </c>
       <c r="C2514" t="s">
         <v>3495</v>
@@ -79755,12 +79773,12 @@
         <v>5549</v>
       </c>
       <c r="Q2514" t="s">
-        <v>3523</v>
+        <v>3525</v>
       </c>
     </row>
     <row r="2515" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2515" s="1" t="s">
-        <v>3524</v>
+        <v>3526</v>
       </c>
       <c r="C2515" t="s">
         <v>3495</v>
@@ -79775,12 +79793,12 @@
         <v>5549</v>
       </c>
       <c r="Q2515" t="s">
-        <v>3525</v>
+        <v>3527</v>
       </c>
     </row>
     <row r="2516" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2516" s="1" t="s">
-        <v>3526</v>
+        <v>3528</v>
       </c>
       <c r="C2516" t="s">
         <v>3495</v>
@@ -79795,12 +79813,12 @@
         <v>5549</v>
       </c>
       <c r="Q2516" t="s">
-        <v>3527</v>
+        <v>3529</v>
       </c>
     </row>
     <row r="2517" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2517" s="1" t="s">
-        <v>3528</v>
+        <v>3530</v>
       </c>
       <c r="C2517" t="s">
         <v>3495</v>
@@ -79815,12 +79833,12 @@
         <v>5549</v>
       </c>
       <c r="Q2517" t="s">
-        <v>3529</v>
+        <v>3531</v>
       </c>
     </row>
     <row r="2518" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2518" s="1" t="s">
-        <v>3530</v>
+        <v>3532</v>
       </c>
       <c r="C2518" t="s">
         <v>3495</v>
@@ -79835,12 +79853,12 @@
         <v>5549</v>
       </c>
       <c r="Q2518" t="s">
-        <v>3531</v>
+        <v>4955</v>
       </c>
     </row>
     <row r="2519" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2519" s="1" t="s">
-        <v>3532</v>
+        <v>3533</v>
       </c>
       <c r="C2519" t="s">
         <v>3495</v>
@@ -79855,12 +79873,12 @@
         <v>5549</v>
       </c>
       <c r="Q2519" t="s">
-        <v>4955</v>
+        <v>3534</v>
       </c>
     </row>
     <row r="2520" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2520" s="1" t="s">
-        <v>3533</v>
+        <v>3535</v>
       </c>
       <c r="C2520" t="s">
         <v>3495</v>
@@ -79875,12 +79893,12 @@
         <v>5549</v>
       </c>
       <c r="Q2520" t="s">
-        <v>3534</v>
+        <v>3536</v>
       </c>
     </row>
     <row r="2521" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2521" s="1" t="s">
-        <v>3535</v>
+        <v>3537</v>
       </c>
       <c r="C2521" t="s">
         <v>3495</v>
@@ -79895,12 +79913,12 @@
         <v>5549</v>
       </c>
       <c r="Q2521" t="s">
-        <v>3536</v>
+        <v>3538</v>
       </c>
     </row>
     <row r="2522" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2522" s="1" t="s">
-        <v>3537</v>
+        <v>3539</v>
       </c>
       <c r="C2522" t="s">
         <v>3495</v>
@@ -79915,12 +79933,12 @@
         <v>5549</v>
       </c>
       <c r="Q2522" t="s">
-        <v>3538</v>
+        <v>4956</v>
       </c>
     </row>
     <row r="2523" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2523" s="1" t="s">
-        <v>3539</v>
+        <v>3540</v>
       </c>
       <c r="C2523" t="s">
         <v>3495</v>
@@ -79935,12 +79953,12 @@
         <v>5549</v>
       </c>
       <c r="Q2523" t="s">
-        <v>4956</v>
+        <v>4588</v>
       </c>
     </row>
     <row r="2524" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2524" s="1" t="s">
-        <v>3540</v>
+        <v>3541</v>
       </c>
       <c r="C2524" t="s">
         <v>3495</v>
@@ -79955,12 +79973,12 @@
         <v>5549</v>
       </c>
       <c r="Q2524" t="s">
-        <v>4588</v>
+        <v>4589</v>
       </c>
     </row>
     <row r="2525" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2525" s="1" t="s">
-        <v>3541</v>
+        <v>3542</v>
       </c>
       <c r="C2525" t="s">
         <v>3495</v>
@@ -79975,12 +79993,12 @@
         <v>5549</v>
       </c>
       <c r="Q2525" t="s">
-        <v>4589</v>
+        <v>3543</v>
       </c>
     </row>
     <row r="2526" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2526" s="1" t="s">
-        <v>3542</v>
+        <v>3544</v>
       </c>
       <c r="C2526" t="s">
         <v>3495</v>
@@ -79995,12 +80013,12 @@
         <v>5549</v>
       </c>
       <c r="Q2526" t="s">
-        <v>3543</v>
+        <v>3545</v>
       </c>
     </row>
     <row r="2527" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2527" s="1" t="s">
-        <v>3544</v>
+        <v>3546</v>
       </c>
       <c r="C2527" t="s">
         <v>3495</v>
@@ -80015,12 +80033,12 @@
         <v>5549</v>
       </c>
       <c r="Q2527" t="s">
-        <v>3545</v>
+        <v>4957</v>
       </c>
     </row>
     <row r="2528" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2528" s="1" t="s">
-        <v>3546</v>
+        <v>3547</v>
       </c>
       <c r="C2528" t="s">
         <v>3495</v>
@@ -80035,12 +80053,12 @@
         <v>5549</v>
       </c>
       <c r="Q2528" t="s">
-        <v>4957</v>
+        <v>3548</v>
       </c>
     </row>
     <row r="2529" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2529" s="1" t="s">
-        <v>3547</v>
+        <v>3549</v>
       </c>
       <c r="C2529" t="s">
         <v>3495</v>
@@ -80055,12 +80073,12 @@
         <v>5549</v>
       </c>
       <c r="Q2529" t="s">
-        <v>3548</v>
+        <v>4590</v>
       </c>
     </row>
     <row r="2530" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2530" s="1" t="s">
-        <v>3549</v>
+        <v>3550</v>
       </c>
       <c r="C2530" t="s">
         <v>3495</v>
@@ -80075,12 +80093,12 @@
         <v>5549</v>
       </c>
       <c r="Q2530" t="s">
-        <v>4590</v>
+        <v>3551</v>
       </c>
     </row>
     <row r="2531" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2531" s="1" t="s">
-        <v>3550</v>
+        <v>3552</v>
       </c>
       <c r="C2531" t="s">
         <v>3495</v>
@@ -80095,12 +80113,12 @@
         <v>5549</v>
       </c>
       <c r="Q2531" t="s">
-        <v>3551</v>
+        <v>3553</v>
       </c>
     </row>
     <row r="2532" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2532" s="1" t="s">
-        <v>3552</v>
+        <v>3554</v>
       </c>
       <c r="C2532" t="s">
         <v>3495</v>
@@ -80115,12 +80133,12 @@
         <v>5549</v>
       </c>
       <c r="Q2532" t="s">
-        <v>3553</v>
+        <v>4958</v>
       </c>
     </row>
     <row r="2533" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2533" s="1" t="s">
-        <v>3554</v>
+        <v>3555</v>
       </c>
       <c r="C2533" t="s">
         <v>3495</v>
@@ -80135,12 +80153,12 @@
         <v>5549</v>
       </c>
       <c r="Q2533" t="s">
-        <v>4958</v>
+        <v>4591</v>
       </c>
     </row>
     <row r="2534" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2534" s="1" t="s">
-        <v>3555</v>
+        <v>3556</v>
       </c>
       <c r="C2534" t="s">
         <v>3495</v>
@@ -80155,12 +80173,12 @@
         <v>5549</v>
       </c>
       <c r="Q2534" t="s">
-        <v>4591</v>
+        <v>3557</v>
       </c>
     </row>
     <row r="2535" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2535" s="1" t="s">
-        <v>3556</v>
+        <v>3558</v>
       </c>
       <c r="C2535" t="s">
         <v>3495</v>
@@ -80175,12 +80193,12 @@
         <v>5549</v>
       </c>
       <c r="Q2535" t="s">
-        <v>3557</v>
+        <v>4959</v>
       </c>
     </row>
     <row r="2536" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2536" s="1" t="s">
-        <v>3558</v>
+        <v>3559</v>
       </c>
       <c r="C2536" t="s">
         <v>3495</v>
@@ -80195,12 +80213,12 @@
         <v>5549</v>
       </c>
       <c r="Q2536" t="s">
-        <v>4959</v>
+        <v>4592</v>
       </c>
     </row>
     <row r="2537" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2537" s="1" t="s">
-        <v>3559</v>
+        <v>3560</v>
       </c>
       <c r="C2537" t="s">
         <v>3495</v>
@@ -80215,12 +80233,12 @@
         <v>5549</v>
       </c>
       <c r="Q2537" t="s">
-        <v>4592</v>
+        <v>4593</v>
       </c>
     </row>
     <row r="2538" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2538" s="1" t="s">
-        <v>3560</v>
+        <v>3561</v>
       </c>
       <c r="C2538" t="s">
         <v>3495</v>
@@ -80235,12 +80253,12 @@
         <v>5549</v>
       </c>
       <c r="Q2538" t="s">
-        <v>4593</v>
+        <v>4960</v>
       </c>
     </row>
     <row r="2539" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2539" s="1" t="s">
-        <v>3561</v>
+        <v>3562</v>
       </c>
       <c r="C2539" t="s">
         <v>3495</v>
@@ -80255,12 +80273,12 @@
         <v>5549</v>
       </c>
       <c r="Q2539" t="s">
-        <v>4960</v>
+        <v>4594</v>
       </c>
     </row>
     <row r="2540" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2540" s="1" t="s">
-        <v>3562</v>
+        <v>3563</v>
       </c>
       <c r="C2540" t="s">
         <v>3495</v>
@@ -80275,12 +80293,12 @@
         <v>5549</v>
       </c>
       <c r="Q2540" t="s">
-        <v>4594</v>
+        <v>4961</v>
       </c>
     </row>
     <row r="2541" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2541" s="1" t="s">
-        <v>3563</v>
+        <v>3564</v>
       </c>
       <c r="C2541" t="s">
         <v>3495</v>
@@ -80295,12 +80313,12 @@
         <v>5549</v>
       </c>
       <c r="Q2541" t="s">
-        <v>4961</v>
+        <v>4962</v>
       </c>
     </row>
     <row r="2542" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2542" s="1" t="s">
-        <v>3564</v>
+        <v>3565</v>
       </c>
       <c r="C2542" t="s">
         <v>3495</v>
@@ -80315,12 +80333,12 @@
         <v>5549</v>
       </c>
       <c r="Q2542" t="s">
-        <v>4962</v>
+        <v>3566</v>
       </c>
     </row>
     <row r="2543" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2543" s="1" t="s">
-        <v>3565</v>
+        <v>3567</v>
       </c>
       <c r="C2543" t="s">
         <v>3495</v>
@@ -80335,12 +80353,12 @@
         <v>5549</v>
       </c>
       <c r="Q2543" t="s">
-        <v>3566</v>
+        <v>3568</v>
       </c>
     </row>
     <row r="2544" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2544" s="1" t="s">
-        <v>3567</v>
+        <v>3569</v>
       </c>
       <c r="C2544" t="s">
         <v>3495</v>
@@ -80355,12 +80373,12 @@
         <v>5549</v>
       </c>
       <c r="Q2544" t="s">
-        <v>3568</v>
+        <v>3570</v>
       </c>
     </row>
     <row r="2545" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2545" s="1" t="s">
-        <v>3569</v>
+        <v>3571</v>
       </c>
       <c r="C2545" t="s">
         <v>3495</v>
@@ -80375,12 +80393,12 @@
         <v>5549</v>
       </c>
       <c r="Q2545" t="s">
-        <v>3570</v>
+        <v>4595</v>
       </c>
     </row>
     <row r="2546" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2546" s="1" t="s">
-        <v>3571</v>
+        <v>3572</v>
       </c>
       <c r="C2546" t="s">
         <v>3495</v>
@@ -80395,12 +80413,12 @@
         <v>5549</v>
       </c>
       <c r="Q2546" t="s">
-        <v>4595</v>
+        <v>3573</v>
       </c>
     </row>
     <row r="2547" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2547" s="1" t="s">
-        <v>3572</v>
+        <v>3574</v>
       </c>
       <c r="C2547" t="s">
         <v>3495</v>
@@ -80415,12 +80433,12 @@
         <v>5549</v>
       </c>
       <c r="Q2547" t="s">
-        <v>3573</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="2548" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2548" s="1" t="s">
-        <v>3574</v>
+        <v>3576</v>
       </c>
       <c r="C2548" t="s">
         <v>3495</v>
@@ -80435,12 +80453,12 @@
         <v>5549</v>
       </c>
       <c r="Q2548" t="s">
-        <v>3575</v>
+        <v>4963</v>
       </c>
     </row>
     <row r="2549" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2549" s="1" t="s">
-        <v>3576</v>
+        <v>3577</v>
       </c>
       <c r="C2549" t="s">
         <v>3495</v>
@@ -80455,12 +80473,12 @@
         <v>5549</v>
       </c>
       <c r="Q2549" t="s">
-        <v>4963</v>
+        <v>3578</v>
       </c>
     </row>
     <row r="2550" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2550" s="1" t="s">
-        <v>3577</v>
+        <v>3579</v>
       </c>
       <c r="C2550" t="s">
         <v>3495</v>
@@ -80475,12 +80493,12 @@
         <v>5549</v>
       </c>
       <c r="Q2550" t="s">
-        <v>3578</v>
+        <v>4964</v>
       </c>
     </row>
     <row r="2551" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2551" s="1" t="s">
-        <v>3579</v>
+        <v>3580</v>
       </c>
       <c r="C2551" t="s">
         <v>3495</v>
@@ -80495,12 +80513,12 @@
         <v>5549</v>
       </c>
       <c r="Q2551" t="s">
-        <v>4964</v>
+        <v>4965</v>
       </c>
     </row>
     <row r="2552" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2552" s="1" t="s">
-        <v>3580</v>
+        <v>3581</v>
       </c>
       <c r="C2552" t="s">
         <v>3495</v>
@@ -80515,12 +80533,12 @@
         <v>5549</v>
       </c>
       <c r="Q2552" t="s">
-        <v>4965</v>
+        <v>4596</v>
       </c>
     </row>
     <row r="2553" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2553" s="1" t="s">
-        <v>3581</v>
+        <v>3582</v>
       </c>
       <c r="C2553" t="s">
         <v>3495</v>
@@ -80535,12 +80553,12 @@
         <v>5549</v>
       </c>
       <c r="Q2553" t="s">
-        <v>4596</v>
+        <v>4966</v>
       </c>
     </row>
     <row r="2554" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2554" s="1" t="s">
-        <v>3582</v>
+        <v>3583</v>
       </c>
       <c r="C2554" t="s">
         <v>3495</v>
@@ -80555,12 +80573,12 @@
         <v>5549</v>
       </c>
       <c r="Q2554" t="s">
-        <v>4966</v>
+        <v>4597</v>
       </c>
     </row>
     <row r="2555" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2555" s="1" t="s">
-        <v>3583</v>
+        <v>3584</v>
       </c>
       <c r="C2555" t="s">
         <v>3495</v>
@@ -80575,12 +80593,12 @@
         <v>5549</v>
       </c>
       <c r="Q2555" t="s">
-        <v>4597</v>
+        <v>4967</v>
       </c>
     </row>
     <row r="2556" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2556" s="1" t="s">
-        <v>3584</v>
+        <v>3585</v>
       </c>
       <c r="C2556" t="s">
         <v>3495</v>
@@ -80595,12 +80613,12 @@
         <v>5549</v>
       </c>
       <c r="Q2556" t="s">
-        <v>4967</v>
+        <v>3586</v>
       </c>
     </row>
     <row r="2557" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2557" s="1" t="s">
-        <v>3585</v>
+        <v>3587</v>
       </c>
       <c r="C2557" t="s">
         <v>3495</v>
@@ -80615,12 +80633,12 @@
         <v>5549</v>
       </c>
       <c r="Q2557" t="s">
-        <v>3586</v>
+        <v>4598</v>
       </c>
     </row>
     <row r="2558" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2558" s="1" t="s">
-        <v>3587</v>
+        <v>3588</v>
       </c>
       <c r="C2558" t="s">
         <v>3495</v>
@@ -80635,12 +80653,12 @@
         <v>5549</v>
       </c>
       <c r="Q2558" t="s">
-        <v>4598</v>
+        <v>4968</v>
       </c>
     </row>
     <row r="2559" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2559" s="1" t="s">
-        <v>3588</v>
+        <v>3589</v>
       </c>
       <c r="C2559" t="s">
         <v>3495</v>
@@ -80655,12 +80673,12 @@
         <v>5549</v>
       </c>
       <c r="Q2559" t="s">
-        <v>4968</v>
+        <v>3590</v>
       </c>
     </row>
     <row r="2560" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2560" s="1" t="s">
-        <v>3589</v>
+        <v>3591</v>
       </c>
       <c r="C2560" t="s">
         <v>3495</v>
@@ -80675,12 +80693,12 @@
         <v>5549</v>
       </c>
       <c r="Q2560" t="s">
-        <v>3590</v>
+        <v>3592</v>
       </c>
     </row>
     <row r="2561" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2561" s="1" t="s">
-        <v>3591</v>
+        <v>3593</v>
       </c>
       <c r="C2561" t="s">
         <v>3495</v>
@@ -80695,12 +80713,12 @@
         <v>5549</v>
       </c>
       <c r="Q2561" t="s">
-        <v>3592</v>
+        <v>4969</v>
       </c>
     </row>
     <row r="2562" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2562" s="1" t="s">
-        <v>3593</v>
+        <v>3594</v>
       </c>
       <c r="C2562" t="s">
         <v>3495</v>
@@ -80715,12 +80733,12 @@
         <v>5549</v>
       </c>
       <c r="Q2562" t="s">
-        <v>4969</v>
+        <v>3595</v>
       </c>
     </row>
     <row r="2563" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2563" s="1" t="s">
-        <v>3594</v>
+        <v>3596</v>
       </c>
       <c r="C2563" t="s">
         <v>3495</v>
@@ -80735,12 +80753,12 @@
         <v>5549</v>
       </c>
       <c r="Q2563" t="s">
-        <v>3595</v>
+        <v>4970</v>
       </c>
     </row>
     <row r="2564" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2564" s="1" t="s">
-        <v>3596</v>
+        <v>3597</v>
       </c>
       <c r="C2564" t="s">
         <v>3495</v>
@@ -80755,12 +80773,12 @@
         <v>5549</v>
       </c>
       <c r="Q2564" t="s">
-        <v>4970</v>
+        <v>4599</v>
       </c>
     </row>
     <row r="2565" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2565" s="1" t="s">
-        <v>3597</v>
+        <v>3598</v>
       </c>
       <c r="C2565" t="s">
         <v>3495</v>
@@ -80775,12 +80793,12 @@
         <v>5549</v>
       </c>
       <c r="Q2565" t="s">
-        <v>4599</v>
+        <v>4600</v>
       </c>
     </row>
     <row r="2566" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2566" s="1" t="s">
-        <v>3598</v>
+        <v>3599</v>
       </c>
       <c r="C2566" t="s">
         <v>3495</v>
@@ -80795,12 +80813,12 @@
         <v>5549</v>
       </c>
       <c r="Q2566" t="s">
-        <v>4600</v>
+        <v>4971</v>
       </c>
     </row>
     <row r="2567" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2567" s="1" t="s">
-        <v>3599</v>
+        <v>3600</v>
       </c>
       <c r="C2567" t="s">
         <v>3495</v>
@@ -80815,12 +80833,12 @@
         <v>5549</v>
       </c>
       <c r="Q2567" t="s">
-        <v>4971</v>
+        <v>4972</v>
       </c>
     </row>
     <row r="2568" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2568" s="1" t="s">
-        <v>3600</v>
+        <v>3601</v>
       </c>
       <c r="C2568" t="s">
         <v>3495</v>
@@ -80835,12 +80853,12 @@
         <v>5549</v>
       </c>
       <c r="Q2568" t="s">
-        <v>4972</v>
+        <v>3602</v>
       </c>
     </row>
     <row r="2569" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2569" s="1" t="s">
-        <v>3601</v>
+        <v>3603</v>
       </c>
       <c r="C2569" t="s">
         <v>3495</v>
@@ -80855,12 +80873,12 @@
         <v>5549</v>
       </c>
       <c r="Q2569" t="s">
-        <v>3602</v>
+        <v>4973</v>
       </c>
     </row>
     <row r="2570" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2570" s="1" t="s">
-        <v>3603</v>
+        <v>3604</v>
       </c>
       <c r="C2570" t="s">
         <v>3495</v>
@@ -80875,12 +80893,12 @@
         <v>5549</v>
       </c>
       <c r="Q2570" t="s">
-        <v>4973</v>
+        <v>3605</v>
       </c>
     </row>
     <row r="2571" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2571" s="1" t="s">
-        <v>3604</v>
+        <v>6932</v>
       </c>
       <c r="C2571" t="s">
         <v>3495</v>
@@ -80895,12 +80913,12 @@
         <v>5549</v>
       </c>
       <c r="Q2571" t="s">
-        <v>3605</v>
+        <v>4974</v>
       </c>
     </row>
     <row r="2572" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2572" s="1" t="s">
-        <v>6932</v>
+        <v>3607</v>
       </c>
       <c r="C2572" t="s">
         <v>3495</v>
@@ -80915,12 +80933,12 @@
         <v>5549</v>
       </c>
       <c r="Q2572" t="s">
-        <v>4974</v>
+        <v>3608</v>
       </c>
     </row>
     <row r="2573" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2573" s="1" t="s">
-        <v>3607</v>
+        <v>3609</v>
       </c>
       <c r="C2573" t="s">
         <v>3495</v>
@@ -80935,12 +80953,12 @@
         <v>5549</v>
       </c>
       <c r="Q2573" t="s">
-        <v>3608</v>
+        <v>3610</v>
       </c>
     </row>
     <row r="2574" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2574" s="1" t="s">
-        <v>3609</v>
+        <v>3611</v>
       </c>
       <c r="C2574" t="s">
         <v>3495</v>
@@ -80955,12 +80973,12 @@
         <v>5549</v>
       </c>
       <c r="Q2574" t="s">
-        <v>3610</v>
+        <v>4975</v>
       </c>
     </row>
     <row r="2575" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2575" s="1" t="s">
-        <v>3611</v>
+        <v>3612</v>
       </c>
       <c r="C2575" t="s">
         <v>3495</v>
@@ -80975,12 +80993,12 @@
         <v>5549</v>
       </c>
       <c r="Q2575" t="s">
-        <v>4975</v>
+        <v>4976</v>
       </c>
     </row>
     <row r="2576" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2576" s="1" t="s">
-        <v>3612</v>
+        <v>3613</v>
       </c>
       <c r="C2576" t="s">
         <v>3495</v>
@@ -80995,12 +81013,12 @@
         <v>5549</v>
       </c>
       <c r="Q2576" t="s">
-        <v>4976</v>
+        <v>3614</v>
       </c>
     </row>
     <row r="2577" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2577" s="1" t="s">
-        <v>3613</v>
+        <v>3615</v>
       </c>
       <c r="C2577" t="s">
         <v>3495</v>
@@ -81015,12 +81033,12 @@
         <v>5549</v>
       </c>
       <c r="Q2577" t="s">
-        <v>3614</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="2578" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2578" s="1" t="s">
-        <v>3615</v>
+        <v>3617</v>
       </c>
       <c r="C2578" t="s">
         <v>3495</v>
@@ -81035,12 +81053,12 @@
         <v>5549</v>
       </c>
       <c r="Q2578" t="s">
-        <v>3616</v>
+        <v>4977</v>
       </c>
     </row>
     <row r="2579" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2579" s="1" t="s">
-        <v>3617</v>
+        <v>3618</v>
       </c>
       <c r="C2579" t="s">
         <v>3495</v>
@@ -81055,12 +81073,12 @@
         <v>5549</v>
       </c>
       <c r="Q2579" t="s">
-        <v>4977</v>
+        <v>3619</v>
       </c>
     </row>
     <row r="2580" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2580" s="1" t="s">
-        <v>3618</v>
+        <v>3620</v>
       </c>
       <c r="C2580" t="s">
         <v>3495</v>
@@ -81075,12 +81093,12 @@
         <v>5549</v>
       </c>
       <c r="Q2580" t="s">
-        <v>3619</v>
+        <v>4978</v>
       </c>
     </row>
     <row r="2581" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2581" s="1" t="s">
-        <v>3620</v>
+        <v>3621</v>
       </c>
       <c r="C2581" t="s">
         <v>3495</v>
@@ -81095,12 +81113,12 @@
         <v>5549</v>
       </c>
       <c r="Q2581" t="s">
-        <v>4978</v>
+        <v>4979</v>
       </c>
     </row>
     <row r="2582" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2582" s="1" t="s">
-        <v>3621</v>
+        <v>3622</v>
       </c>
       <c r="C2582" t="s">
         <v>3495</v>
@@ -81115,12 +81133,12 @@
         <v>5549</v>
       </c>
       <c r="Q2582" t="s">
-        <v>4979</v>
+        <v>4980</v>
       </c>
     </row>
     <row r="2583" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2583" s="1" t="s">
-        <v>3622</v>
+        <v>3623</v>
       </c>
       <c r="C2583" t="s">
         <v>3495</v>
@@ -81135,12 +81153,12 @@
         <v>5549</v>
       </c>
       <c r="Q2583" t="s">
-        <v>4980</v>
+        <v>4601</v>
       </c>
     </row>
     <row r="2584" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2584" s="1" t="s">
-        <v>3623</v>
+        <v>3624</v>
       </c>
       <c r="C2584" t="s">
         <v>3495</v>
@@ -81155,12 +81173,12 @@
         <v>5549</v>
       </c>
       <c r="Q2584" t="s">
-        <v>4601</v>
+        <v>4981</v>
       </c>
     </row>
     <row r="2585" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2585" s="1" t="s">
-        <v>3624</v>
+        <v>3625</v>
       </c>
       <c r="C2585" t="s">
         <v>3495</v>
@@ -81175,12 +81193,12 @@
         <v>5549</v>
       </c>
       <c r="Q2585" t="s">
-        <v>4981</v>
+        <v>4602</v>
       </c>
     </row>
     <row r="2586" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2586" s="1" t="s">
-        <v>3625</v>
+        <v>3626</v>
       </c>
       <c r="C2586" t="s">
         <v>3495</v>
@@ -81195,12 +81213,12 @@
         <v>5549</v>
       </c>
       <c r="Q2586" t="s">
-        <v>4602</v>
+        <v>3627</v>
       </c>
     </row>
     <row r="2587" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2587" s="1" t="s">
-        <v>3626</v>
+        <v>3628</v>
       </c>
       <c r="C2587" t="s">
         <v>3495</v>
@@ -81215,12 +81233,12 @@
         <v>5549</v>
       </c>
       <c r="Q2587" t="s">
-        <v>3627</v>
+        <v>4982</v>
       </c>
     </row>
     <row r="2588" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2588" s="1" t="s">
-        <v>3628</v>
+        <v>3629</v>
       </c>
       <c r="C2588" t="s">
         <v>3495</v>
@@ -81235,12 +81253,12 @@
         <v>5549</v>
       </c>
       <c r="Q2588" t="s">
-        <v>4982</v>
+        <v>4603</v>
       </c>
     </row>
     <row r="2589" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2589" s="1" t="s">
-        <v>3629</v>
+        <v>3630</v>
       </c>
       <c r="C2589" t="s">
         <v>3495</v>
@@ -81255,12 +81273,12 @@
         <v>5549</v>
       </c>
       <c r="Q2589" t="s">
-        <v>4603</v>
+        <v>3631</v>
       </c>
     </row>
     <row r="2590" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2590" s="1" t="s">
-        <v>3630</v>
+        <v>3632</v>
       </c>
       <c r="C2590" t="s">
         <v>3495</v>
@@ -81275,12 +81293,12 @@
         <v>5549</v>
       </c>
       <c r="Q2590" t="s">
-        <v>3631</v>
+        <v>4983</v>
       </c>
     </row>
     <row r="2591" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2591" s="1" t="s">
-        <v>3632</v>
+        <v>3633</v>
       </c>
       <c r="C2591" t="s">
         <v>3495</v>
@@ -81295,12 +81313,12 @@
         <v>5549</v>
       </c>
       <c r="Q2591" t="s">
-        <v>4983</v>
+        <v>3634</v>
       </c>
     </row>
     <row r="2592" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2592" s="1" t="s">
-        <v>3633</v>
+        <v>3635</v>
       </c>
       <c r="C2592" t="s">
         <v>3495</v>
@@ -81315,12 +81333,12 @@
         <v>5549</v>
       </c>
       <c r="Q2592" t="s">
-        <v>3634</v>
+        <v>3636</v>
       </c>
     </row>
     <row r="2593" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2593" s="1" t="s">
-        <v>3635</v>
+        <v>3637</v>
       </c>
       <c r="C2593" t="s">
         <v>3495</v>
@@ -81335,12 +81353,12 @@
         <v>5549</v>
       </c>
       <c r="Q2593" t="s">
-        <v>3636</v>
+        <v>4604</v>
       </c>
     </row>
     <row r="2594" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2594" s="1" t="s">
-        <v>3637</v>
+        <v>3638</v>
       </c>
       <c r="C2594" t="s">
         <v>3495</v>
@@ -81355,12 +81373,12 @@
         <v>5549</v>
       </c>
       <c r="Q2594" t="s">
-        <v>4604</v>
+        <v>3639</v>
       </c>
     </row>
     <row r="2595" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2595" s="1" t="s">
-        <v>3638</v>
+        <v>3640</v>
       </c>
       <c r="C2595" t="s">
         <v>3495</v>
@@ -81375,12 +81393,12 @@
         <v>5549</v>
       </c>
       <c r="Q2595" t="s">
-        <v>3639</v>
+        <v>4984</v>
       </c>
     </row>
     <row r="2596" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2596" s="1" t="s">
-        <v>3640</v>
+        <v>3641</v>
       </c>
       <c r="C2596" t="s">
         <v>3495</v>
@@ -81395,12 +81413,12 @@
         <v>5549</v>
       </c>
       <c r="Q2596" t="s">
-        <v>4984</v>
+        <v>4985</v>
       </c>
     </row>
     <row r="2597" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2597" s="1" t="s">
-        <v>3641</v>
+        <v>3642</v>
       </c>
       <c r="C2597" t="s">
         <v>3495</v>
@@ -81415,12 +81433,12 @@
         <v>5549</v>
       </c>
       <c r="Q2597" t="s">
-        <v>4985</v>
+        <v>4605</v>
       </c>
     </row>
     <row r="2598" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2598" s="1" t="s">
-        <v>3642</v>
+        <v>3643</v>
       </c>
       <c r="C2598" t="s">
         <v>3495</v>
@@ -81435,12 +81453,12 @@
         <v>5549</v>
       </c>
       <c r="Q2598" t="s">
-        <v>4605</v>
+        <v>4986</v>
       </c>
     </row>
     <row r="2599" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2599" s="1" t="s">
-        <v>3643</v>
+        <v>3644</v>
       </c>
       <c r="C2599" t="s">
         <v>3495</v>
@@ -81455,12 +81473,12 @@
         <v>5549</v>
       </c>
       <c r="Q2599" t="s">
-        <v>4986</v>
+        <v>4987</v>
       </c>
     </row>
     <row r="2600" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2600" s="1" t="s">
-        <v>3644</v>
+        <v>3645</v>
       </c>
       <c r="C2600" t="s">
         <v>3495</v>
@@ -81475,12 +81493,12 @@
         <v>5549</v>
       </c>
       <c r="Q2600" t="s">
-        <v>4987</v>
+        <v>3646</v>
       </c>
     </row>
     <row r="2601" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2601" s="1" t="s">
-        <v>3645</v>
+        <v>3647</v>
       </c>
       <c r="C2601" t="s">
         <v>3495</v>
@@ -81495,12 +81513,12 @@
         <v>5549</v>
       </c>
       <c r="Q2601" t="s">
-        <v>3646</v>
+        <v>4988</v>
       </c>
     </row>
     <row r="2602" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2602" s="1" t="s">
-        <v>3647</v>
+        <v>3648</v>
       </c>
       <c r="C2602" t="s">
         <v>3495</v>
@@ -81515,12 +81533,12 @@
         <v>5549</v>
       </c>
       <c r="Q2602" t="s">
-        <v>4988</v>
+        <v>4989</v>
       </c>
     </row>
     <row r="2603" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2603" s="1" t="s">
-        <v>3648</v>
+        <v>3649</v>
       </c>
       <c r="C2603" t="s">
         <v>3495</v>
@@ -81535,12 +81553,12 @@
         <v>5549</v>
       </c>
       <c r="Q2603" t="s">
-        <v>4989</v>
+        <v>3650</v>
       </c>
     </row>
     <row r="2604" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2604" s="1" t="s">
-        <v>3649</v>
+        <v>3651</v>
       </c>
       <c r="C2604" t="s">
         <v>3495</v>
@@ -81555,12 +81573,12 @@
         <v>5549</v>
       </c>
       <c r="Q2604" t="s">
-        <v>3650</v>
+        <v>3652</v>
       </c>
     </row>
     <row r="2605" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2605" s="1" t="s">
-        <v>3651</v>
+        <v>3653</v>
       </c>
       <c r="C2605" t="s">
         <v>3495</v>
@@ -81575,12 +81593,12 @@
         <v>5549</v>
       </c>
       <c r="Q2605" t="s">
-        <v>3652</v>
+        <v>3654</v>
       </c>
     </row>
     <row r="2606" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2606" s="1" t="s">
-        <v>3653</v>
+        <v>3655</v>
       </c>
       <c r="C2606" t="s">
         <v>3495</v>
@@ -81595,12 +81613,12 @@
         <v>5549</v>
       </c>
       <c r="Q2606" t="s">
-        <v>3654</v>
+        <v>3656</v>
       </c>
     </row>
     <row r="2607" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2607" s="1" t="s">
-        <v>3655</v>
+        <v>3657</v>
       </c>
       <c r="C2607" t="s">
         <v>3495</v>
@@ -81615,12 +81633,12 @@
         <v>5549</v>
       </c>
       <c r="Q2607" t="s">
-        <v>3656</v>
+        <v>4990</v>
       </c>
     </row>
     <row r="2608" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2608" s="1" t="s">
-        <v>3657</v>
+        <v>3658</v>
       </c>
       <c r="C2608" t="s">
         <v>3495</v>
@@ -81635,12 +81653,12 @@
         <v>5549</v>
       </c>
       <c r="Q2608" t="s">
-        <v>4990</v>
+        <v>3659</v>
       </c>
     </row>
     <row r="2609" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2609" s="1" t="s">
-        <v>3658</v>
+        <v>3660</v>
       </c>
       <c r="C2609" t="s">
         <v>3495</v>
@@ -81655,12 +81673,12 @@
         <v>5549</v>
       </c>
       <c r="Q2609" t="s">
-        <v>3659</v>
+        <v>3661</v>
       </c>
     </row>
     <row r="2610" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2610" s="1" t="s">
-        <v>3660</v>
+        <v>3662</v>
       </c>
       <c r="C2610" t="s">
         <v>3495</v>
@@ -81675,12 +81693,12 @@
         <v>5549</v>
       </c>
       <c r="Q2610" t="s">
-        <v>3661</v>
+        <v>4991</v>
       </c>
     </row>
     <row r="2611" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2611" s="1" t="s">
-        <v>3662</v>
+        <v>3663</v>
       </c>
       <c r="C2611" t="s">
         <v>3495</v>
@@ -81695,12 +81713,12 @@
         <v>5549</v>
       </c>
       <c r="Q2611" t="s">
-        <v>4991</v>
+        <v>3664</v>
       </c>
     </row>
     <row r="2612" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2612" s="1" t="s">
-        <v>3663</v>
+        <v>3665</v>
       </c>
       <c r="C2612" t="s">
         <v>3495</v>
@@ -81715,12 +81733,12 @@
         <v>5549</v>
       </c>
       <c r="Q2612" t="s">
-        <v>3664</v>
+        <v>4992</v>
       </c>
     </row>
     <row r="2613" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2613" s="1" t="s">
-        <v>3665</v>
+        <v>3666</v>
       </c>
       <c r="C2613" t="s">
         <v>3495</v>
@@ -81735,12 +81753,12 @@
         <v>5549</v>
       </c>
       <c r="Q2613" t="s">
-        <v>4992</v>
+        <v>3667</v>
       </c>
     </row>
     <row r="2614" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2614" s="1" t="s">
-        <v>3666</v>
+        <v>3668</v>
       </c>
       <c r="C2614" t="s">
         <v>3495</v>
@@ -81755,12 +81773,12 @@
         <v>5549</v>
       </c>
       <c r="Q2614" t="s">
-        <v>3667</v>
+        <v>3669</v>
       </c>
     </row>
     <row r="2615" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2615" s="1" t="s">
-        <v>3668</v>
+        <v>3670</v>
       </c>
       <c r="C2615" t="s">
         <v>3495</v>
@@ -81775,12 +81793,12 @@
         <v>5549</v>
       </c>
       <c r="Q2615" t="s">
-        <v>3669</v>
+        <v>3671</v>
       </c>
     </row>
     <row r="2616" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2616" s="1" t="s">
-        <v>3670</v>
+        <v>3672</v>
       </c>
       <c r="C2616" t="s">
         <v>3495</v>
@@ -81795,12 +81813,12 @@
         <v>5549</v>
       </c>
       <c r="Q2616" t="s">
-        <v>3671</v>
+        <v>3673</v>
       </c>
     </row>
     <row r="2617" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2617" s="1" t="s">
-        <v>3672</v>
+        <v>3674</v>
       </c>
       <c r="C2617" t="s">
         <v>3495</v>
@@ -81815,12 +81833,12 @@
         <v>5549</v>
       </c>
       <c r="Q2617" t="s">
-        <v>3673</v>
+        <v>4993</v>
       </c>
     </row>
     <row r="2618" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2618" s="1" t="s">
-        <v>3674</v>
+        <v>3675</v>
       </c>
       <c r="C2618" t="s">
         <v>3495</v>
@@ -81835,12 +81853,12 @@
         <v>5549</v>
       </c>
       <c r="Q2618" t="s">
-        <v>4993</v>
+        <v>4994</v>
       </c>
     </row>
     <row r="2619" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2619" s="1" t="s">
-        <v>3675</v>
+        <v>3676</v>
       </c>
       <c r="C2619" t="s">
         <v>3495</v>
@@ -81855,12 +81873,12 @@
         <v>5549</v>
       </c>
       <c r="Q2619" t="s">
-        <v>4994</v>
+        <v>4995</v>
       </c>
     </row>
     <row r="2620" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2620" s="1" t="s">
-        <v>3676</v>
+        <v>3677</v>
       </c>
       <c r="C2620" t="s">
         <v>3495</v>
@@ -81875,12 +81893,12 @@
         <v>5549</v>
       </c>
       <c r="Q2620" t="s">
-        <v>4995</v>
+        <v>4996</v>
       </c>
     </row>
     <row r="2621" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2621" s="1" t="s">
-        <v>3677</v>
+        <v>3678</v>
       </c>
       <c r="C2621" t="s">
         <v>3495</v>
@@ -81895,12 +81913,12 @@
         <v>5549</v>
       </c>
       <c r="Q2621" t="s">
-        <v>4996</v>
+        <v>4997</v>
       </c>
     </row>
     <row r="2622" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2622" s="1" t="s">
-        <v>3678</v>
+        <v>3679</v>
       </c>
       <c r="C2622" t="s">
         <v>3495</v>
@@ -81915,12 +81933,12 @@
         <v>5549</v>
       </c>
       <c r="Q2622" t="s">
-        <v>4997</v>
+        <v>3680</v>
       </c>
     </row>
     <row r="2623" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2623" s="1" t="s">
-        <v>3679</v>
+        <v>3681</v>
       </c>
       <c r="C2623" t="s">
         <v>3495</v>
@@ -81935,12 +81953,12 @@
         <v>5549</v>
       </c>
       <c r="Q2623" t="s">
-        <v>3680</v>
+        <v>4606</v>
       </c>
     </row>
     <row r="2624" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2624" s="1" t="s">
-        <v>3681</v>
+        <v>3682</v>
       </c>
       <c r="C2624" t="s">
         <v>3495</v>
@@ -81955,12 +81973,12 @@
         <v>5549</v>
       </c>
       <c r="Q2624" t="s">
-        <v>4606</v>
+        <v>3683</v>
       </c>
     </row>
     <row r="2625" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2625" s="1" t="s">
-        <v>3682</v>
+        <v>6933</v>
       </c>
       <c r="C2625" t="s">
         <v>3495</v>
@@ -81975,12 +81993,12 @@
         <v>5549</v>
       </c>
       <c r="Q2625" t="s">
-        <v>3683</v>
+        <v>6934</v>
       </c>
     </row>
     <row r="2626" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2626" s="1" t="s">
-        <v>6933</v>
+        <v>6935</v>
       </c>
       <c r="C2626" t="s">
         <v>3495</v>
@@ -81995,12 +82013,12 @@
         <v>5549</v>
       </c>
       <c r="Q2626" t="s">
-        <v>6934</v>
+        <v>6936</v>
       </c>
     </row>
     <row r="2627" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2627" s="1" t="s">
-        <v>6935</v>
+        <v>6937</v>
       </c>
       <c r="C2627" t="s">
         <v>3495</v>
@@ -82015,12 +82033,12 @@
         <v>5549</v>
       </c>
       <c r="Q2627" t="s">
-        <v>6936</v>
+        <v>6938</v>
       </c>
     </row>
     <row r="2628" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2628" s="1" t="s">
-        <v>6937</v>
+        <v>6939</v>
       </c>
       <c r="C2628" t="s">
         <v>3495</v>
@@ -82035,12 +82053,12 @@
         <v>5549</v>
       </c>
       <c r="Q2628" t="s">
-        <v>6938</v>
+        <v>6940</v>
       </c>
     </row>
     <row r="2629" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2629" s="1" t="s">
-        <v>6939</v>
+        <v>6941</v>
       </c>
       <c r="C2629" t="s">
         <v>3495</v>
@@ -82055,12 +82073,12 @@
         <v>5549</v>
       </c>
       <c r="Q2629" t="s">
-        <v>6940</v>
+        <v>6942</v>
       </c>
     </row>
     <row r="2630" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2630" s="1" t="s">
-        <v>6941</v>
+        <v>6943</v>
       </c>
       <c r="C2630" t="s">
         <v>3495</v>
@@ -82075,12 +82093,12 @@
         <v>5549</v>
       </c>
       <c r="Q2630" t="s">
-        <v>6942</v>
+        <v>6944</v>
       </c>
     </row>
     <row r="2631" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2631" s="1" t="s">
-        <v>6943</v>
+        <v>6945</v>
       </c>
       <c r="C2631" t="s">
         <v>3495</v>
@@ -82095,12 +82113,12 @@
         <v>5549</v>
       </c>
       <c r="Q2631" t="s">
-        <v>6944</v>
+        <v>6946</v>
       </c>
     </row>
     <row r="2632" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2632" s="1" t="s">
-        <v>6945</v>
+        <v>6947</v>
       </c>
       <c r="C2632" t="s">
         <v>3495</v>
@@ -82115,12 +82133,12 @@
         <v>5549</v>
       </c>
       <c r="Q2632" t="s">
-        <v>6946</v>
+        <v>6948</v>
       </c>
     </row>
     <row r="2633" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2633" s="1" t="s">
-        <v>6947</v>
+        <v>6949</v>
       </c>
       <c r="C2633" t="s">
         <v>3495</v>
@@ -82135,12 +82153,12 @@
         <v>5549</v>
       </c>
       <c r="Q2633" t="s">
-        <v>6948</v>
+        <v>6950</v>
       </c>
     </row>
     <row r="2634" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2634" s="1" t="s">
-        <v>6949</v>
+        <v>6951</v>
       </c>
       <c r="C2634" t="s">
         <v>3495</v>
@@ -82155,12 +82173,12 @@
         <v>5549</v>
       </c>
       <c r="Q2634" t="s">
-        <v>6950</v>
+        <v>6952</v>
       </c>
     </row>
     <row r="2635" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2635" s="1" t="s">
-        <v>6951</v>
+        <v>6953</v>
       </c>
       <c r="C2635" t="s">
         <v>3495</v>
@@ -82175,26 +82193,6 @@
         <v>5549</v>
       </c>
       <c r="Q2635" t="s">
-        <v>6952</v>
-      </c>
-    </row>
-    <row r="2636" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2636" s="1" t="s">
-        <v>6953</v>
-      </c>
-      <c r="C2636" t="s">
-        <v>3495</v>
-      </c>
-      <c r="D2636" s="1">
-        <v>68000</v>
-      </c>
-      <c r="E2636" t="s">
-        <v>2426</v>
-      </c>
-      <c r="L2636" t="s">
-        <v>5549</v>
-      </c>
-      <c r="Q2636" t="s">
         <v>6954</v>
       </c>
     </row>
@@ -82212,7 +82210,7 @@
       <selection activeCell="A360" sqref="A360:XFD360"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">

</xml_diff>

<commit_message>
Added working polyplay driver
</commit_message>
<xml_diff>
--- a/compatibility_list.xlsx
+++ b/compatibility_list.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NetBeansProjects\arcadeflex056\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9330" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9330" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="working" sheetId="9" r:id="rId1"/>
@@ -21,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="DETAILS" localSheetId="4">WIP!#REF!</definedName>
-    <definedName name="DETAILS_1" localSheetId="4">WIP!$B$1:$Q$2626</definedName>
+    <definedName name="DETAILS_1" localSheetId="4">WIP!$B$1:$Q$2625</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -21014,7 +21009,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -21288,7 +21283,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -21296,13 +21291,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q157"/>
+  <dimension ref="A1:Q158"/>
   <sheetViews>
     <sheetView topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="B157" sqref="B157"/>
+      <selection activeCell="A159" sqref="A159"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -24766,6 +24761,26 @@
       </c>
       <c r="Q157" t="s">
         <v>3456</v>
+      </c>
+    </row>
+    <row r="158" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>157</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>3484</v>
+      </c>
+      <c r="C158" t="s">
+        <v>3485</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L158" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q158" t="s">
+        <v>3486</v>
       </c>
     </row>
   </sheetData>
@@ -24781,7 +24796,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
@@ -24896,7 +24911,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
   </cols>
@@ -24984,7 +24999,7 @@
       <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -25139,13 +25154,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R2626"/>
+  <dimension ref="B1:R2625"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="E112" sqref="E112"/>
+    <sheetView tabSelected="1" topLeftCell="A2463" workbookViewId="0">
+      <selection activeCell="A2478" sqref="A2478:XFD2478"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
@@ -79034,58 +79049,61 @@
     </row>
     <row r="2478" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2478" s="1" t="s">
-        <v>3484</v>
+        <v>3487</v>
       </c>
       <c r="C2478" t="s">
-        <v>3485</v>
+        <v>3488</v>
       </c>
       <c r="D2478" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L2478" t="s">
-        <v>77</v>
+        <v>1155</v>
       </c>
       <c r="Q2478" t="s">
-        <v>3486</v>
+        <v>3489</v>
       </c>
     </row>
     <row r="2479" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2479" s="1" t="s">
-        <v>3487</v>
+        <v>3491</v>
       </c>
       <c r="C2479" t="s">
-        <v>3488</v>
+        <v>3492</v>
       </c>
       <c r="D2479" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L2479" t="s">
-        <v>1155</v>
+        <v>55</v>
       </c>
       <c r="Q2479" t="s">
-        <v>3489</v>
+        <v>3493</v>
       </c>
     </row>
     <row r="2480" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2480" s="1" t="s">
-        <v>3491</v>
+        <v>6914</v>
       </c>
       <c r="C2480" t="s">
-        <v>3492</v>
+        <v>6915</v>
       </c>
       <c r="D2480" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E2480" t="s">
+        <v>2</v>
+      </c>
       <c r="L2480" t="s">
-        <v>55</v>
+        <v>5238</v>
       </c>
       <c r="Q2480" t="s">
-        <v>3493</v>
+        <v>6916</v>
       </c>
     </row>
     <row r="2481" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2481" s="1" t="s">
-        <v>6914</v>
+        <v>6917</v>
       </c>
       <c r="C2481" t="s">
         <v>6915</v>
@@ -79100,32 +79118,29 @@
         <v>5238</v>
       </c>
       <c r="Q2481" t="s">
-        <v>6916</v>
+        <v>6918</v>
       </c>
     </row>
     <row r="2482" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2482" s="1" t="s">
-        <v>6917</v>
+        <v>6919</v>
       </c>
       <c r="C2482" t="s">
-        <v>6915</v>
+        <v>6920</v>
       </c>
       <c r="D2482" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2482" t="s">
-        <v>2</v>
-      </c>
       <c r="L2482" t="s">
-        <v>5238</v>
+        <v>55</v>
       </c>
       <c r="Q2482" t="s">
-        <v>6918</v>
+        <v>6921</v>
       </c>
     </row>
     <row r="2483" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2483" s="1" t="s">
-        <v>6919</v>
+        <v>6922</v>
       </c>
       <c r="C2483" t="s">
         <v>6920</v>
@@ -79133,16 +79148,25 @@
       <c r="D2483" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E2483" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2483" t="s">
+        <v>2426</v>
+      </c>
       <c r="L2483" t="s">
+        <v>542</v>
+      </c>
+      <c r="M2483" t="s">
         <v>55</v>
       </c>
       <c r="Q2483" t="s">
-        <v>6921</v>
+        <v>6923</v>
       </c>
     </row>
     <row r="2484" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2484" s="1" t="s">
-        <v>6922</v>
+        <v>6924</v>
       </c>
       <c r="C2484" t="s">
         <v>6920</v>
@@ -79163,55 +79187,49 @@
         <v>55</v>
       </c>
       <c r="Q2484" t="s">
-        <v>6923</v>
+        <v>6925</v>
       </c>
     </row>
     <row r="2485" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2485" s="1" t="s">
-        <v>6924</v>
+        <v>6926</v>
       </c>
       <c r="C2485" t="s">
-        <v>6920</v>
-      </c>
-      <c r="D2485" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2485" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2485" t="s">
-        <v>2426</v>
+        <v>6927</v>
+      </c>
+      <c r="D2485" s="1">
+        <v>68000</v>
       </c>
       <c r="L2485" t="s">
-        <v>542</v>
-      </c>
-      <c r="M2485" t="s">
-        <v>55</v>
+        <v>1687</v>
       </c>
       <c r="Q2485" t="s">
-        <v>6925</v>
+        <v>6928</v>
       </c>
     </row>
     <row r="2486" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2486" s="1" t="s">
-        <v>6926</v>
+        <v>3494</v>
       </c>
       <c r="C2486" t="s">
-        <v>6927</v>
+        <v>3495</v>
       </c>
       <c r="D2486" s="1">
         <v>68000</v>
       </c>
+      <c r="E2486" t="s">
+        <v>2426</v>
+      </c>
       <c r="L2486" t="s">
-        <v>1687</v>
+        <v>5549</v>
       </c>
       <c r="Q2486" t="s">
-        <v>6928</v>
+        <v>3496</v>
       </c>
     </row>
     <row r="2487" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2487" s="1" t="s">
-        <v>3494</v>
+        <v>3497</v>
       </c>
       <c r="C2487" t="s">
         <v>3495</v>
@@ -79226,12 +79244,12 @@
         <v>5549</v>
       </c>
       <c r="Q2487" t="s">
-        <v>3496</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="2488" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2488" s="1" t="s">
-        <v>3497</v>
+        <v>3498</v>
       </c>
       <c r="C2488" t="s">
         <v>3495</v>
@@ -79246,12 +79264,12 @@
         <v>5549</v>
       </c>
       <c r="Q2488" t="s">
-        <v>4587</v>
+        <v>3499</v>
       </c>
     </row>
     <row r="2489" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2489" s="1" t="s">
-        <v>3498</v>
+        <v>3500</v>
       </c>
       <c r="C2489" t="s">
         <v>3495</v>
@@ -79266,12 +79284,12 @@
         <v>5549</v>
       </c>
       <c r="Q2489" t="s">
-        <v>3499</v>
+        <v>3501</v>
       </c>
     </row>
     <row r="2490" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2490" s="1" t="s">
-        <v>3500</v>
+        <v>3502</v>
       </c>
       <c r="C2490" t="s">
         <v>3495</v>
@@ -79286,12 +79304,12 @@
         <v>5549</v>
       </c>
       <c r="Q2490" t="s">
-        <v>3501</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="2491" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2491" s="1" t="s">
-        <v>3502</v>
+        <v>3504</v>
       </c>
       <c r="C2491" t="s">
         <v>3495</v>
@@ -79306,12 +79324,12 @@
         <v>5549</v>
       </c>
       <c r="Q2491" t="s">
-        <v>3503</v>
+        <v>3505</v>
       </c>
     </row>
     <row r="2492" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2492" s="1" t="s">
-        <v>3504</v>
+        <v>3506</v>
       </c>
       <c r="C2492" t="s">
         <v>3495</v>
@@ -79326,12 +79344,12 @@
         <v>5549</v>
       </c>
       <c r="Q2492" t="s">
-        <v>3505</v>
+        <v>6929</v>
       </c>
     </row>
     <row r="2493" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2493" s="1" t="s">
-        <v>3506</v>
+        <v>6930</v>
       </c>
       <c r="C2493" t="s">
         <v>3495</v>
@@ -79346,12 +79364,12 @@
         <v>5549</v>
       </c>
       <c r="Q2493" t="s">
-        <v>6929</v>
+        <v>6931</v>
       </c>
     </row>
     <row r="2494" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2494" s="1" t="s">
-        <v>6930</v>
+        <v>3507</v>
       </c>
       <c r="C2494" t="s">
         <v>3495</v>
@@ -79366,12 +79384,12 @@
         <v>5549</v>
       </c>
       <c r="Q2494" t="s">
-        <v>6931</v>
+        <v>4952</v>
       </c>
     </row>
     <row r="2495" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2495" s="1" t="s">
-        <v>3507</v>
+        <v>3508</v>
       </c>
       <c r="C2495" t="s">
         <v>3495</v>
@@ -79386,12 +79404,12 @@
         <v>5549</v>
       </c>
       <c r="Q2495" t="s">
-        <v>4952</v>
+        <v>3509</v>
       </c>
     </row>
     <row r="2496" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2496" s="1" t="s">
-        <v>3508</v>
+        <v>3510</v>
       </c>
       <c r="C2496" t="s">
         <v>3495</v>
@@ -79406,12 +79424,12 @@
         <v>5549</v>
       </c>
       <c r="Q2496" t="s">
-        <v>3509</v>
+        <v>3511</v>
       </c>
     </row>
     <row r="2497" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2497" s="1" t="s">
-        <v>3510</v>
+        <v>3512</v>
       </c>
       <c r="C2497" t="s">
         <v>3495</v>
@@ -79426,12 +79444,12 @@
         <v>5549</v>
       </c>
       <c r="Q2497" t="s">
-        <v>3511</v>
+        <v>3513</v>
       </c>
     </row>
     <row r="2498" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2498" s="1" t="s">
-        <v>3512</v>
+        <v>3514</v>
       </c>
       <c r="C2498" t="s">
         <v>3495</v>
@@ -79446,12 +79464,12 @@
         <v>5549</v>
       </c>
       <c r="Q2498" t="s">
-        <v>3513</v>
+        <v>3515</v>
       </c>
     </row>
     <row r="2499" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2499" s="1" t="s">
-        <v>3514</v>
+        <v>3516</v>
       </c>
       <c r="C2499" t="s">
         <v>3495</v>
@@ -79466,12 +79484,12 @@
         <v>5549</v>
       </c>
       <c r="Q2499" t="s">
-        <v>3515</v>
+        <v>3517</v>
       </c>
     </row>
     <row r="2500" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2500" s="1" t="s">
-        <v>3516</v>
+        <v>3518</v>
       </c>
       <c r="C2500" t="s">
         <v>3495</v>
@@ -79486,12 +79504,12 @@
         <v>5549</v>
       </c>
       <c r="Q2500" t="s">
-        <v>3517</v>
+        <v>4953</v>
       </c>
     </row>
     <row r="2501" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2501" s="1" t="s">
-        <v>3518</v>
+        <v>3519</v>
       </c>
       <c r="C2501" t="s">
         <v>3495</v>
@@ -79506,12 +79524,12 @@
         <v>5549</v>
       </c>
       <c r="Q2501" t="s">
-        <v>4953</v>
+        <v>4954</v>
       </c>
     </row>
     <row r="2502" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2502" s="1" t="s">
-        <v>3519</v>
+        <v>3520</v>
       </c>
       <c r="C2502" t="s">
         <v>3495</v>
@@ -79526,12 +79544,12 @@
         <v>5549</v>
       </c>
       <c r="Q2502" t="s">
-        <v>4954</v>
+        <v>3521</v>
       </c>
     </row>
     <row r="2503" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2503" s="1" t="s">
-        <v>3520</v>
+        <v>3522</v>
       </c>
       <c r="C2503" t="s">
         <v>3495</v>
@@ -79546,12 +79564,12 @@
         <v>5549</v>
       </c>
       <c r="Q2503" t="s">
-        <v>3521</v>
+        <v>3523</v>
       </c>
     </row>
     <row r="2504" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2504" s="1" t="s">
-        <v>3522</v>
+        <v>3524</v>
       </c>
       <c r="C2504" t="s">
         <v>3495</v>
@@ -79566,12 +79584,12 @@
         <v>5549</v>
       </c>
       <c r="Q2504" t="s">
-        <v>3523</v>
+        <v>3525</v>
       </c>
     </row>
     <row r="2505" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2505" s="1" t="s">
-        <v>3524</v>
+        <v>3526</v>
       </c>
       <c r="C2505" t="s">
         <v>3495</v>
@@ -79586,12 +79604,12 @@
         <v>5549</v>
       </c>
       <c r="Q2505" t="s">
-        <v>3525</v>
+        <v>3527</v>
       </c>
     </row>
     <row r="2506" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2506" s="1" t="s">
-        <v>3526</v>
+        <v>3528</v>
       </c>
       <c r="C2506" t="s">
         <v>3495</v>
@@ -79606,12 +79624,12 @@
         <v>5549</v>
       </c>
       <c r="Q2506" t="s">
-        <v>3527</v>
+        <v>3529</v>
       </c>
     </row>
     <row r="2507" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2507" s="1" t="s">
-        <v>3528</v>
+        <v>3530</v>
       </c>
       <c r="C2507" t="s">
         <v>3495</v>
@@ -79626,12 +79644,12 @@
         <v>5549</v>
       </c>
       <c r="Q2507" t="s">
-        <v>3529</v>
+        <v>3531</v>
       </c>
     </row>
     <row r="2508" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2508" s="1" t="s">
-        <v>3530</v>
+        <v>3532</v>
       </c>
       <c r="C2508" t="s">
         <v>3495</v>
@@ -79646,12 +79664,12 @@
         <v>5549</v>
       </c>
       <c r="Q2508" t="s">
-        <v>3531</v>
+        <v>4955</v>
       </c>
     </row>
     <row r="2509" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2509" s="1" t="s">
-        <v>3532</v>
+        <v>3533</v>
       </c>
       <c r="C2509" t="s">
         <v>3495</v>
@@ -79666,12 +79684,12 @@
         <v>5549</v>
       </c>
       <c r="Q2509" t="s">
-        <v>4955</v>
+        <v>3534</v>
       </c>
     </row>
     <row r="2510" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2510" s="1" t="s">
-        <v>3533</v>
+        <v>3535</v>
       </c>
       <c r="C2510" t="s">
         <v>3495</v>
@@ -79686,12 +79704,12 @@
         <v>5549</v>
       </c>
       <c r="Q2510" t="s">
-        <v>3534</v>
+        <v>3536</v>
       </c>
     </row>
     <row r="2511" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2511" s="1" t="s">
-        <v>3535</v>
+        <v>3537</v>
       </c>
       <c r="C2511" t="s">
         <v>3495</v>
@@ -79706,12 +79724,12 @@
         <v>5549</v>
       </c>
       <c r="Q2511" t="s">
-        <v>3536</v>
+        <v>3538</v>
       </c>
     </row>
     <row r="2512" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2512" s="1" t="s">
-        <v>3537</v>
+        <v>3539</v>
       </c>
       <c r="C2512" t="s">
         <v>3495</v>
@@ -79726,12 +79744,12 @@
         <v>5549</v>
       </c>
       <c r="Q2512" t="s">
-        <v>3538</v>
+        <v>4956</v>
       </c>
     </row>
     <row r="2513" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2513" s="1" t="s">
-        <v>3539</v>
+        <v>3540</v>
       </c>
       <c r="C2513" t="s">
         <v>3495</v>
@@ -79746,12 +79764,12 @@
         <v>5549</v>
       </c>
       <c r="Q2513" t="s">
-        <v>4956</v>
+        <v>4588</v>
       </c>
     </row>
     <row r="2514" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2514" s="1" t="s">
-        <v>3540</v>
+        <v>3541</v>
       </c>
       <c r="C2514" t="s">
         <v>3495</v>
@@ -79766,12 +79784,12 @@
         <v>5549</v>
       </c>
       <c r="Q2514" t="s">
-        <v>4588</v>
+        <v>4589</v>
       </c>
     </row>
     <row r="2515" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2515" s="1" t="s">
-        <v>3541</v>
+        <v>3542</v>
       </c>
       <c r="C2515" t="s">
         <v>3495</v>
@@ -79786,12 +79804,12 @@
         <v>5549</v>
       </c>
       <c r="Q2515" t="s">
-        <v>4589</v>
+        <v>3543</v>
       </c>
     </row>
     <row r="2516" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2516" s="1" t="s">
-        <v>3542</v>
+        <v>3544</v>
       </c>
       <c r="C2516" t="s">
         <v>3495</v>
@@ -79806,12 +79824,12 @@
         <v>5549</v>
       </c>
       <c r="Q2516" t="s">
-        <v>3543</v>
+        <v>3545</v>
       </c>
     </row>
     <row r="2517" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2517" s="1" t="s">
-        <v>3544</v>
+        <v>3546</v>
       </c>
       <c r="C2517" t="s">
         <v>3495</v>
@@ -79826,12 +79844,12 @@
         <v>5549</v>
       </c>
       <c r="Q2517" t="s">
-        <v>3545</v>
+        <v>4957</v>
       </c>
     </row>
     <row r="2518" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2518" s="1" t="s">
-        <v>3546</v>
+        <v>3547</v>
       </c>
       <c r="C2518" t="s">
         <v>3495</v>
@@ -79846,12 +79864,12 @@
         <v>5549</v>
       </c>
       <c r="Q2518" t="s">
-        <v>4957</v>
+        <v>3548</v>
       </c>
     </row>
     <row r="2519" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2519" s="1" t="s">
-        <v>3547</v>
+        <v>3549</v>
       </c>
       <c r="C2519" t="s">
         <v>3495</v>
@@ -79866,12 +79884,12 @@
         <v>5549</v>
       </c>
       <c r="Q2519" t="s">
-        <v>3548</v>
+        <v>4590</v>
       </c>
     </row>
     <row r="2520" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2520" s="1" t="s">
-        <v>3549</v>
+        <v>3550</v>
       </c>
       <c r="C2520" t="s">
         <v>3495</v>
@@ -79886,12 +79904,12 @@
         <v>5549</v>
       </c>
       <c r="Q2520" t="s">
-        <v>4590</v>
+        <v>3551</v>
       </c>
     </row>
     <row r="2521" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2521" s="1" t="s">
-        <v>3550</v>
+        <v>3552</v>
       </c>
       <c r="C2521" t="s">
         <v>3495</v>
@@ -79906,12 +79924,12 @@
         <v>5549</v>
       </c>
       <c r="Q2521" t="s">
-        <v>3551</v>
+        <v>3553</v>
       </c>
     </row>
     <row r="2522" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2522" s="1" t="s">
-        <v>3552</v>
+        <v>3554</v>
       </c>
       <c r="C2522" t="s">
         <v>3495</v>
@@ -79926,12 +79944,12 @@
         <v>5549</v>
       </c>
       <c r="Q2522" t="s">
-        <v>3553</v>
+        <v>4958</v>
       </c>
     </row>
     <row r="2523" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2523" s="1" t="s">
-        <v>3554</v>
+        <v>3555</v>
       </c>
       <c r="C2523" t="s">
         <v>3495</v>
@@ -79946,12 +79964,12 @@
         <v>5549</v>
       </c>
       <c r="Q2523" t="s">
-        <v>4958</v>
+        <v>4591</v>
       </c>
     </row>
     <row r="2524" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2524" s="1" t="s">
-        <v>3555</v>
+        <v>3556</v>
       </c>
       <c r="C2524" t="s">
         <v>3495</v>
@@ -79966,12 +79984,12 @@
         <v>5549</v>
       </c>
       <c r="Q2524" t="s">
-        <v>4591</v>
+        <v>3557</v>
       </c>
     </row>
     <row r="2525" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2525" s="1" t="s">
-        <v>3556</v>
+        <v>3558</v>
       </c>
       <c r="C2525" t="s">
         <v>3495</v>
@@ -79986,12 +80004,12 @@
         <v>5549</v>
       </c>
       <c r="Q2525" t="s">
-        <v>3557</v>
+        <v>4959</v>
       </c>
     </row>
     <row r="2526" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2526" s="1" t="s">
-        <v>3558</v>
+        <v>3559</v>
       </c>
       <c r="C2526" t="s">
         <v>3495</v>
@@ -80006,12 +80024,12 @@
         <v>5549</v>
       </c>
       <c r="Q2526" t="s">
-        <v>4959</v>
+        <v>4592</v>
       </c>
     </row>
     <row r="2527" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2527" s="1" t="s">
-        <v>3559</v>
+        <v>3560</v>
       </c>
       <c r="C2527" t="s">
         <v>3495</v>
@@ -80026,12 +80044,12 @@
         <v>5549</v>
       </c>
       <c r="Q2527" t="s">
-        <v>4592</v>
+        <v>4593</v>
       </c>
     </row>
     <row r="2528" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2528" s="1" t="s">
-        <v>3560</v>
+        <v>3561</v>
       </c>
       <c r="C2528" t="s">
         <v>3495</v>
@@ -80046,12 +80064,12 @@
         <v>5549</v>
       </c>
       <c r="Q2528" t="s">
-        <v>4593</v>
+        <v>4960</v>
       </c>
     </row>
     <row r="2529" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2529" s="1" t="s">
-        <v>3561</v>
+        <v>3562</v>
       </c>
       <c r="C2529" t="s">
         <v>3495</v>
@@ -80066,12 +80084,12 @@
         <v>5549</v>
       </c>
       <c r="Q2529" t="s">
-        <v>4960</v>
+        <v>4594</v>
       </c>
     </row>
     <row r="2530" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2530" s="1" t="s">
-        <v>3562</v>
+        <v>3563</v>
       </c>
       <c r="C2530" t="s">
         <v>3495</v>
@@ -80086,12 +80104,12 @@
         <v>5549</v>
       </c>
       <c r="Q2530" t="s">
-        <v>4594</v>
+        <v>4961</v>
       </c>
     </row>
     <row r="2531" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2531" s="1" t="s">
-        <v>3563</v>
+        <v>3564</v>
       </c>
       <c r="C2531" t="s">
         <v>3495</v>
@@ -80106,12 +80124,12 @@
         <v>5549</v>
       </c>
       <c r="Q2531" t="s">
-        <v>4961</v>
+        <v>4962</v>
       </c>
     </row>
     <row r="2532" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2532" s="1" t="s">
-        <v>3564</v>
+        <v>3565</v>
       </c>
       <c r="C2532" t="s">
         <v>3495</v>
@@ -80126,12 +80144,12 @@
         <v>5549</v>
       </c>
       <c r="Q2532" t="s">
-        <v>4962</v>
+        <v>3566</v>
       </c>
     </row>
     <row r="2533" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2533" s="1" t="s">
-        <v>3565</v>
+        <v>3567</v>
       </c>
       <c r="C2533" t="s">
         <v>3495</v>
@@ -80146,12 +80164,12 @@
         <v>5549</v>
       </c>
       <c r="Q2533" t="s">
-        <v>3566</v>
+        <v>3568</v>
       </c>
     </row>
     <row r="2534" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2534" s="1" t="s">
-        <v>3567</v>
+        <v>3569</v>
       </c>
       <c r="C2534" t="s">
         <v>3495</v>
@@ -80166,12 +80184,12 @@
         <v>5549</v>
       </c>
       <c r="Q2534" t="s">
-        <v>3568</v>
+        <v>3570</v>
       </c>
     </row>
     <row r="2535" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2535" s="1" t="s">
-        <v>3569</v>
+        <v>3571</v>
       </c>
       <c r="C2535" t="s">
         <v>3495</v>
@@ -80186,12 +80204,12 @@
         <v>5549</v>
       </c>
       <c r="Q2535" t="s">
-        <v>3570</v>
+        <v>4595</v>
       </c>
     </row>
     <row r="2536" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2536" s="1" t="s">
-        <v>3571</v>
+        <v>3572</v>
       </c>
       <c r="C2536" t="s">
         <v>3495</v>
@@ -80206,12 +80224,12 @@
         <v>5549</v>
       </c>
       <c r="Q2536" t="s">
-        <v>4595</v>
+        <v>3573</v>
       </c>
     </row>
     <row r="2537" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2537" s="1" t="s">
-        <v>3572</v>
+        <v>3574</v>
       </c>
       <c r="C2537" t="s">
         <v>3495</v>
@@ -80226,12 +80244,12 @@
         <v>5549</v>
       </c>
       <c r="Q2537" t="s">
-        <v>3573</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="2538" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2538" s="1" t="s">
-        <v>3574</v>
+        <v>3576</v>
       </c>
       <c r="C2538" t="s">
         <v>3495</v>
@@ -80246,12 +80264,12 @@
         <v>5549</v>
       </c>
       <c r="Q2538" t="s">
-        <v>3575</v>
+        <v>4963</v>
       </c>
     </row>
     <row r="2539" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2539" s="1" t="s">
-        <v>3576</v>
+        <v>3577</v>
       </c>
       <c r="C2539" t="s">
         <v>3495</v>
@@ -80266,12 +80284,12 @@
         <v>5549</v>
       </c>
       <c r="Q2539" t="s">
-        <v>4963</v>
+        <v>3578</v>
       </c>
     </row>
     <row r="2540" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2540" s="1" t="s">
-        <v>3577</v>
+        <v>3579</v>
       </c>
       <c r="C2540" t="s">
         <v>3495</v>
@@ -80286,12 +80304,12 @@
         <v>5549</v>
       </c>
       <c r="Q2540" t="s">
-        <v>3578</v>
+        <v>4964</v>
       </c>
     </row>
     <row r="2541" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2541" s="1" t="s">
-        <v>3579</v>
+        <v>3580</v>
       </c>
       <c r="C2541" t="s">
         <v>3495</v>
@@ -80306,12 +80324,12 @@
         <v>5549</v>
       </c>
       <c r="Q2541" t="s">
-        <v>4964</v>
+        <v>4965</v>
       </c>
     </row>
     <row r="2542" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2542" s="1" t="s">
-        <v>3580</v>
+        <v>3581</v>
       </c>
       <c r="C2542" t="s">
         <v>3495</v>
@@ -80326,12 +80344,12 @@
         <v>5549</v>
       </c>
       <c r="Q2542" t="s">
-        <v>4965</v>
+        <v>4596</v>
       </c>
     </row>
     <row r="2543" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2543" s="1" t="s">
-        <v>3581</v>
+        <v>3582</v>
       </c>
       <c r="C2543" t="s">
         <v>3495</v>
@@ -80346,12 +80364,12 @@
         <v>5549</v>
       </c>
       <c r="Q2543" t="s">
-        <v>4596</v>
+        <v>4966</v>
       </c>
     </row>
     <row r="2544" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2544" s="1" t="s">
-        <v>3582</v>
+        <v>3583</v>
       </c>
       <c r="C2544" t="s">
         <v>3495</v>
@@ -80366,12 +80384,12 @@
         <v>5549</v>
       </c>
       <c r="Q2544" t="s">
-        <v>4966</v>
+        <v>4597</v>
       </c>
     </row>
     <row r="2545" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2545" s="1" t="s">
-        <v>3583</v>
+        <v>3584</v>
       </c>
       <c r="C2545" t="s">
         <v>3495</v>
@@ -80386,12 +80404,12 @@
         <v>5549</v>
       </c>
       <c r="Q2545" t="s">
-        <v>4597</v>
+        <v>4967</v>
       </c>
     </row>
     <row r="2546" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2546" s="1" t="s">
-        <v>3584</v>
+        <v>3585</v>
       </c>
       <c r="C2546" t="s">
         <v>3495</v>
@@ -80406,12 +80424,12 @@
         <v>5549</v>
       </c>
       <c r="Q2546" t="s">
-        <v>4967</v>
+        <v>3586</v>
       </c>
     </row>
     <row r="2547" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2547" s="1" t="s">
-        <v>3585</v>
+        <v>3587</v>
       </c>
       <c r="C2547" t="s">
         <v>3495</v>
@@ -80426,12 +80444,12 @@
         <v>5549</v>
       </c>
       <c r="Q2547" t="s">
-        <v>3586</v>
+        <v>4598</v>
       </c>
     </row>
     <row r="2548" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2548" s="1" t="s">
-        <v>3587</v>
+        <v>3588</v>
       </c>
       <c r="C2548" t="s">
         <v>3495</v>
@@ -80446,12 +80464,12 @@
         <v>5549</v>
       </c>
       <c r="Q2548" t="s">
-        <v>4598</v>
+        <v>4968</v>
       </c>
     </row>
     <row r="2549" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2549" s="1" t="s">
-        <v>3588</v>
+        <v>3589</v>
       </c>
       <c r="C2549" t="s">
         <v>3495</v>
@@ -80466,12 +80484,12 @@
         <v>5549</v>
       </c>
       <c r="Q2549" t="s">
-        <v>4968</v>
+        <v>3590</v>
       </c>
     </row>
     <row r="2550" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2550" s="1" t="s">
-        <v>3589</v>
+        <v>3591</v>
       </c>
       <c r="C2550" t="s">
         <v>3495</v>
@@ -80486,12 +80504,12 @@
         <v>5549</v>
       </c>
       <c r="Q2550" t="s">
-        <v>3590</v>
+        <v>3592</v>
       </c>
     </row>
     <row r="2551" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2551" s="1" t="s">
-        <v>3591</v>
+        <v>3593</v>
       </c>
       <c r="C2551" t="s">
         <v>3495</v>
@@ -80506,12 +80524,12 @@
         <v>5549</v>
       </c>
       <c r="Q2551" t="s">
-        <v>3592</v>
+        <v>4969</v>
       </c>
     </row>
     <row r="2552" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2552" s="1" t="s">
-        <v>3593</v>
+        <v>3594</v>
       </c>
       <c r="C2552" t="s">
         <v>3495</v>
@@ -80526,12 +80544,12 @@
         <v>5549</v>
       </c>
       <c r="Q2552" t="s">
-        <v>4969</v>
+        <v>3595</v>
       </c>
     </row>
     <row r="2553" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2553" s="1" t="s">
-        <v>3594</v>
+        <v>3596</v>
       </c>
       <c r="C2553" t="s">
         <v>3495</v>
@@ -80546,12 +80564,12 @@
         <v>5549</v>
       </c>
       <c r="Q2553" t="s">
-        <v>3595</v>
+        <v>4970</v>
       </c>
     </row>
     <row r="2554" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2554" s="1" t="s">
-        <v>3596</v>
+        <v>3597</v>
       </c>
       <c r="C2554" t="s">
         <v>3495</v>
@@ -80566,12 +80584,12 @@
         <v>5549</v>
       </c>
       <c r="Q2554" t="s">
-        <v>4970</v>
+        <v>4599</v>
       </c>
     </row>
     <row r="2555" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2555" s="1" t="s">
-        <v>3597</v>
+        <v>3598</v>
       </c>
       <c r="C2555" t="s">
         <v>3495</v>
@@ -80586,12 +80604,12 @@
         <v>5549</v>
       </c>
       <c r="Q2555" t="s">
-        <v>4599</v>
+        <v>4600</v>
       </c>
     </row>
     <row r="2556" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2556" s="1" t="s">
-        <v>3598</v>
+        <v>3599</v>
       </c>
       <c r="C2556" t="s">
         <v>3495</v>
@@ -80606,12 +80624,12 @@
         <v>5549</v>
       </c>
       <c r="Q2556" t="s">
-        <v>4600</v>
+        <v>4971</v>
       </c>
     </row>
     <row r="2557" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2557" s="1" t="s">
-        <v>3599</v>
+        <v>3600</v>
       </c>
       <c r="C2557" t="s">
         <v>3495</v>
@@ -80626,12 +80644,12 @@
         <v>5549</v>
       </c>
       <c r="Q2557" t="s">
-        <v>4971</v>
+        <v>4972</v>
       </c>
     </row>
     <row r="2558" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2558" s="1" t="s">
-        <v>3600</v>
+        <v>3601</v>
       </c>
       <c r="C2558" t="s">
         <v>3495</v>
@@ -80646,12 +80664,12 @@
         <v>5549</v>
       </c>
       <c r="Q2558" t="s">
-        <v>4972</v>
+        <v>3602</v>
       </c>
     </row>
     <row r="2559" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2559" s="1" t="s">
-        <v>3601</v>
+        <v>3603</v>
       </c>
       <c r="C2559" t="s">
         <v>3495</v>
@@ -80666,12 +80684,12 @@
         <v>5549</v>
       </c>
       <c r="Q2559" t="s">
-        <v>3602</v>
+        <v>4973</v>
       </c>
     </row>
     <row r="2560" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2560" s="1" t="s">
-        <v>3603</v>
+        <v>3604</v>
       </c>
       <c r="C2560" t="s">
         <v>3495</v>
@@ -80686,12 +80704,12 @@
         <v>5549</v>
       </c>
       <c r="Q2560" t="s">
-        <v>4973</v>
+        <v>3605</v>
       </c>
     </row>
     <row r="2561" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2561" s="1" t="s">
-        <v>3604</v>
+        <v>6932</v>
       </c>
       <c r="C2561" t="s">
         <v>3495</v>
@@ -80706,12 +80724,12 @@
         <v>5549</v>
       </c>
       <c r="Q2561" t="s">
-        <v>3605</v>
+        <v>4974</v>
       </c>
     </row>
     <row r="2562" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2562" s="1" t="s">
-        <v>6932</v>
+        <v>3607</v>
       </c>
       <c r="C2562" t="s">
         <v>3495</v>
@@ -80726,12 +80744,12 @@
         <v>5549</v>
       </c>
       <c r="Q2562" t="s">
-        <v>4974</v>
+        <v>3608</v>
       </c>
     </row>
     <row r="2563" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2563" s="1" t="s">
-        <v>3607</v>
+        <v>3609</v>
       </c>
       <c r="C2563" t="s">
         <v>3495</v>
@@ -80746,12 +80764,12 @@
         <v>5549</v>
       </c>
       <c r="Q2563" t="s">
-        <v>3608</v>
+        <v>3610</v>
       </c>
     </row>
     <row r="2564" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2564" s="1" t="s">
-        <v>3609</v>
+        <v>3611</v>
       </c>
       <c r="C2564" t="s">
         <v>3495</v>
@@ -80766,12 +80784,12 @@
         <v>5549</v>
       </c>
       <c r="Q2564" t="s">
-        <v>3610</v>
+        <v>4975</v>
       </c>
     </row>
     <row r="2565" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2565" s="1" t="s">
-        <v>3611</v>
+        <v>3612</v>
       </c>
       <c r="C2565" t="s">
         <v>3495</v>
@@ -80786,12 +80804,12 @@
         <v>5549</v>
       </c>
       <c r="Q2565" t="s">
-        <v>4975</v>
+        <v>4976</v>
       </c>
     </row>
     <row r="2566" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2566" s="1" t="s">
-        <v>3612</v>
+        <v>3613</v>
       </c>
       <c r="C2566" t="s">
         <v>3495</v>
@@ -80806,12 +80824,12 @@
         <v>5549</v>
       </c>
       <c r="Q2566" t="s">
-        <v>4976</v>
+        <v>3614</v>
       </c>
     </row>
     <row r="2567" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2567" s="1" t="s">
-        <v>3613</v>
+        <v>3615</v>
       </c>
       <c r="C2567" t="s">
         <v>3495</v>
@@ -80826,12 +80844,12 @@
         <v>5549</v>
       </c>
       <c r="Q2567" t="s">
-        <v>3614</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="2568" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2568" s="1" t="s">
-        <v>3615</v>
+        <v>3617</v>
       </c>
       <c r="C2568" t="s">
         <v>3495</v>
@@ -80846,12 +80864,12 @@
         <v>5549</v>
       </c>
       <c r="Q2568" t="s">
-        <v>3616</v>
+        <v>4977</v>
       </c>
     </row>
     <row r="2569" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2569" s="1" t="s">
-        <v>3617</v>
+        <v>3618</v>
       </c>
       <c r="C2569" t="s">
         <v>3495</v>
@@ -80866,12 +80884,12 @@
         <v>5549</v>
       </c>
       <c r="Q2569" t="s">
-        <v>4977</v>
+        <v>3619</v>
       </c>
     </row>
     <row r="2570" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2570" s="1" t="s">
-        <v>3618</v>
+        <v>3620</v>
       </c>
       <c r="C2570" t="s">
         <v>3495</v>
@@ -80886,12 +80904,12 @@
         <v>5549</v>
       </c>
       <c r="Q2570" t="s">
-        <v>3619</v>
+        <v>4978</v>
       </c>
     </row>
     <row r="2571" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2571" s="1" t="s">
-        <v>3620</v>
+        <v>3621</v>
       </c>
       <c r="C2571" t="s">
         <v>3495</v>
@@ -80906,12 +80924,12 @@
         <v>5549</v>
       </c>
       <c r="Q2571" t="s">
-        <v>4978</v>
+        <v>4979</v>
       </c>
     </row>
     <row r="2572" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2572" s="1" t="s">
-        <v>3621</v>
+        <v>3622</v>
       </c>
       <c r="C2572" t="s">
         <v>3495</v>
@@ -80926,12 +80944,12 @@
         <v>5549</v>
       </c>
       <c r="Q2572" t="s">
-        <v>4979</v>
+        <v>4980</v>
       </c>
     </row>
     <row r="2573" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2573" s="1" t="s">
-        <v>3622</v>
+        <v>3623</v>
       </c>
       <c r="C2573" t="s">
         <v>3495</v>
@@ -80946,12 +80964,12 @@
         <v>5549</v>
       </c>
       <c r="Q2573" t="s">
-        <v>4980</v>
+        <v>4601</v>
       </c>
     </row>
     <row r="2574" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2574" s="1" t="s">
-        <v>3623</v>
+        <v>3624</v>
       </c>
       <c r="C2574" t="s">
         <v>3495</v>
@@ -80966,12 +80984,12 @@
         <v>5549</v>
       </c>
       <c r="Q2574" t="s">
-        <v>4601</v>
+        <v>4981</v>
       </c>
     </row>
     <row r="2575" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2575" s="1" t="s">
-        <v>3624</v>
+        <v>3625</v>
       </c>
       <c r="C2575" t="s">
         <v>3495</v>
@@ -80986,12 +81004,12 @@
         <v>5549</v>
       </c>
       <c r="Q2575" t="s">
-        <v>4981</v>
+        <v>4602</v>
       </c>
     </row>
     <row r="2576" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2576" s="1" t="s">
-        <v>3625</v>
+        <v>3626</v>
       </c>
       <c r="C2576" t="s">
         <v>3495</v>
@@ -81006,12 +81024,12 @@
         <v>5549</v>
       </c>
       <c r="Q2576" t="s">
-        <v>4602</v>
+        <v>3627</v>
       </c>
     </row>
     <row r="2577" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2577" s="1" t="s">
-        <v>3626</v>
+        <v>3628</v>
       </c>
       <c r="C2577" t="s">
         <v>3495</v>
@@ -81026,12 +81044,12 @@
         <v>5549</v>
       </c>
       <c r="Q2577" t="s">
-        <v>3627</v>
+        <v>4982</v>
       </c>
     </row>
     <row r="2578" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2578" s="1" t="s">
-        <v>3628</v>
+        <v>3629</v>
       </c>
       <c r="C2578" t="s">
         <v>3495</v>
@@ -81046,12 +81064,12 @@
         <v>5549</v>
       </c>
       <c r="Q2578" t="s">
-        <v>4982</v>
+        <v>4603</v>
       </c>
     </row>
     <row r="2579" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2579" s="1" t="s">
-        <v>3629</v>
+        <v>3630</v>
       </c>
       <c r="C2579" t="s">
         <v>3495</v>
@@ -81066,12 +81084,12 @@
         <v>5549</v>
       </c>
       <c r="Q2579" t="s">
-        <v>4603</v>
+        <v>3631</v>
       </c>
     </row>
     <row r="2580" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2580" s="1" t="s">
-        <v>3630</v>
+        <v>3632</v>
       </c>
       <c r="C2580" t="s">
         <v>3495</v>
@@ -81086,12 +81104,12 @@
         <v>5549</v>
       </c>
       <c r="Q2580" t="s">
-        <v>3631</v>
+        <v>4983</v>
       </c>
     </row>
     <row r="2581" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2581" s="1" t="s">
-        <v>3632</v>
+        <v>3633</v>
       </c>
       <c r="C2581" t="s">
         <v>3495</v>
@@ -81106,12 +81124,12 @@
         <v>5549</v>
       </c>
       <c r="Q2581" t="s">
-        <v>4983</v>
+        <v>3634</v>
       </c>
     </row>
     <row r="2582" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2582" s="1" t="s">
-        <v>3633</v>
+        <v>3635</v>
       </c>
       <c r="C2582" t="s">
         <v>3495</v>
@@ -81126,12 +81144,12 @@
         <v>5549</v>
       </c>
       <c r="Q2582" t="s">
-        <v>3634</v>
+        <v>3636</v>
       </c>
     </row>
     <row r="2583" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2583" s="1" t="s">
-        <v>3635</v>
+        <v>3637</v>
       </c>
       <c r="C2583" t="s">
         <v>3495</v>
@@ -81146,12 +81164,12 @@
         <v>5549</v>
       </c>
       <c r="Q2583" t="s">
-        <v>3636</v>
+        <v>4604</v>
       </c>
     </row>
     <row r="2584" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2584" s="1" t="s">
-        <v>3637</v>
+        <v>3638</v>
       </c>
       <c r="C2584" t="s">
         <v>3495</v>
@@ -81166,12 +81184,12 @@
         <v>5549</v>
       </c>
       <c r="Q2584" t="s">
-        <v>4604</v>
+        <v>3639</v>
       </c>
     </row>
     <row r="2585" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2585" s="1" t="s">
-        <v>3638</v>
+        <v>3640</v>
       </c>
       <c r="C2585" t="s">
         <v>3495</v>
@@ -81186,12 +81204,12 @@
         <v>5549</v>
       </c>
       <c r="Q2585" t="s">
-        <v>3639</v>
+        <v>4984</v>
       </c>
     </row>
     <row r="2586" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2586" s="1" t="s">
-        <v>3640</v>
+        <v>3641</v>
       </c>
       <c r="C2586" t="s">
         <v>3495</v>
@@ -81206,12 +81224,12 @@
         <v>5549</v>
       </c>
       <c r="Q2586" t="s">
-        <v>4984</v>
+        <v>4985</v>
       </c>
     </row>
     <row r="2587" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2587" s="1" t="s">
-        <v>3641</v>
+        <v>3642</v>
       </c>
       <c r="C2587" t="s">
         <v>3495</v>
@@ -81226,12 +81244,12 @@
         <v>5549</v>
       </c>
       <c r="Q2587" t="s">
-        <v>4985</v>
+        <v>4605</v>
       </c>
     </row>
     <row r="2588" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2588" s="1" t="s">
-        <v>3642</v>
+        <v>3643</v>
       </c>
       <c r="C2588" t="s">
         <v>3495</v>
@@ -81246,12 +81264,12 @@
         <v>5549</v>
       </c>
       <c r="Q2588" t="s">
-        <v>4605</v>
+        <v>4986</v>
       </c>
     </row>
     <row r="2589" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2589" s="1" t="s">
-        <v>3643</v>
+        <v>3644</v>
       </c>
       <c r="C2589" t="s">
         <v>3495</v>
@@ -81266,12 +81284,12 @@
         <v>5549</v>
       </c>
       <c r="Q2589" t="s">
-        <v>4986</v>
+        <v>4987</v>
       </c>
     </row>
     <row r="2590" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2590" s="1" t="s">
-        <v>3644</v>
+        <v>3645</v>
       </c>
       <c r="C2590" t="s">
         <v>3495</v>
@@ -81286,12 +81304,12 @@
         <v>5549</v>
       </c>
       <c r="Q2590" t="s">
-        <v>4987</v>
+        <v>3646</v>
       </c>
     </row>
     <row r="2591" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2591" s="1" t="s">
-        <v>3645</v>
+        <v>3647</v>
       </c>
       <c r="C2591" t="s">
         <v>3495</v>
@@ -81306,12 +81324,12 @@
         <v>5549</v>
       </c>
       <c r="Q2591" t="s">
-        <v>3646</v>
+        <v>4988</v>
       </c>
     </row>
     <row r="2592" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2592" s="1" t="s">
-        <v>3647</v>
+        <v>3648</v>
       </c>
       <c r="C2592" t="s">
         <v>3495</v>
@@ -81326,12 +81344,12 @@
         <v>5549</v>
       </c>
       <c r="Q2592" t="s">
-        <v>4988</v>
+        <v>4989</v>
       </c>
     </row>
     <row r="2593" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2593" s="1" t="s">
-        <v>3648</v>
+        <v>3649</v>
       </c>
       <c r="C2593" t="s">
         <v>3495</v>
@@ -81346,12 +81364,12 @@
         <v>5549</v>
       </c>
       <c r="Q2593" t="s">
-        <v>4989</v>
+        <v>3650</v>
       </c>
     </row>
     <row r="2594" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2594" s="1" t="s">
-        <v>3649</v>
+        <v>3651</v>
       </c>
       <c r="C2594" t="s">
         <v>3495</v>
@@ -81366,12 +81384,12 @@
         <v>5549</v>
       </c>
       <c r="Q2594" t="s">
-        <v>3650</v>
+        <v>3652</v>
       </c>
     </row>
     <row r="2595" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2595" s="1" t="s">
-        <v>3651</v>
+        <v>3653</v>
       </c>
       <c r="C2595" t="s">
         <v>3495</v>
@@ -81386,12 +81404,12 @@
         <v>5549</v>
       </c>
       <c r="Q2595" t="s">
-        <v>3652</v>
+        <v>3654</v>
       </c>
     </row>
     <row r="2596" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2596" s="1" t="s">
-        <v>3653</v>
+        <v>3655</v>
       </c>
       <c r="C2596" t="s">
         <v>3495</v>
@@ -81406,12 +81424,12 @@
         <v>5549</v>
       </c>
       <c r="Q2596" t="s">
-        <v>3654</v>
+        <v>3656</v>
       </c>
     </row>
     <row r="2597" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2597" s="1" t="s">
-        <v>3655</v>
+        <v>3657</v>
       </c>
       <c r="C2597" t="s">
         <v>3495</v>
@@ -81426,12 +81444,12 @@
         <v>5549</v>
       </c>
       <c r="Q2597" t="s">
-        <v>3656</v>
+        <v>4990</v>
       </c>
     </row>
     <row r="2598" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2598" s="1" t="s">
-        <v>3657</v>
+        <v>3658</v>
       </c>
       <c r="C2598" t="s">
         <v>3495</v>
@@ -81446,12 +81464,12 @@
         <v>5549</v>
       </c>
       <c r="Q2598" t="s">
-        <v>4990</v>
+        <v>3659</v>
       </c>
     </row>
     <row r="2599" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2599" s="1" t="s">
-        <v>3658</v>
+        <v>3660</v>
       </c>
       <c r="C2599" t="s">
         <v>3495</v>
@@ -81466,12 +81484,12 @@
         <v>5549</v>
       </c>
       <c r="Q2599" t="s">
-        <v>3659</v>
+        <v>3661</v>
       </c>
     </row>
     <row r="2600" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2600" s="1" t="s">
-        <v>3660</v>
+        <v>3662</v>
       </c>
       <c r="C2600" t="s">
         <v>3495</v>
@@ -81486,12 +81504,12 @@
         <v>5549</v>
       </c>
       <c r="Q2600" t="s">
-        <v>3661</v>
+        <v>4991</v>
       </c>
     </row>
     <row r="2601" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2601" s="1" t="s">
-        <v>3662</v>
+        <v>3663</v>
       </c>
       <c r="C2601" t="s">
         <v>3495</v>
@@ -81506,12 +81524,12 @@
         <v>5549</v>
       </c>
       <c r="Q2601" t="s">
-        <v>4991</v>
+        <v>3664</v>
       </c>
     </row>
     <row r="2602" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2602" s="1" t="s">
-        <v>3663</v>
+        <v>3665</v>
       </c>
       <c r="C2602" t="s">
         <v>3495</v>
@@ -81526,12 +81544,12 @@
         <v>5549</v>
       </c>
       <c r="Q2602" t="s">
-        <v>3664</v>
+        <v>4992</v>
       </c>
     </row>
     <row r="2603" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2603" s="1" t="s">
-        <v>3665</v>
+        <v>3666</v>
       </c>
       <c r="C2603" t="s">
         <v>3495</v>
@@ -81546,12 +81564,12 @@
         <v>5549</v>
       </c>
       <c r="Q2603" t="s">
-        <v>4992</v>
+        <v>3667</v>
       </c>
     </row>
     <row r="2604" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2604" s="1" t="s">
-        <v>3666</v>
+        <v>3668</v>
       </c>
       <c r="C2604" t="s">
         <v>3495</v>
@@ -81566,12 +81584,12 @@
         <v>5549</v>
       </c>
       <c r="Q2604" t="s">
-        <v>3667</v>
+        <v>3669</v>
       </c>
     </row>
     <row r="2605" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2605" s="1" t="s">
-        <v>3668</v>
+        <v>3670</v>
       </c>
       <c r="C2605" t="s">
         <v>3495</v>
@@ -81586,12 +81604,12 @@
         <v>5549</v>
       </c>
       <c r="Q2605" t="s">
-        <v>3669</v>
+        <v>3671</v>
       </c>
     </row>
     <row r="2606" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2606" s="1" t="s">
-        <v>3670</v>
+        <v>3672</v>
       </c>
       <c r="C2606" t="s">
         <v>3495</v>
@@ -81606,12 +81624,12 @@
         <v>5549</v>
       </c>
       <c r="Q2606" t="s">
-        <v>3671</v>
+        <v>3673</v>
       </c>
     </row>
     <row r="2607" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2607" s="1" t="s">
-        <v>3672</v>
+        <v>3674</v>
       </c>
       <c r="C2607" t="s">
         <v>3495</v>
@@ -81626,12 +81644,12 @@
         <v>5549</v>
       </c>
       <c r="Q2607" t="s">
-        <v>3673</v>
+        <v>4993</v>
       </c>
     </row>
     <row r="2608" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2608" s="1" t="s">
-        <v>3674</v>
+        <v>3675</v>
       </c>
       <c r="C2608" t="s">
         <v>3495</v>
@@ -81646,12 +81664,12 @@
         <v>5549</v>
       </c>
       <c r="Q2608" t="s">
-        <v>4993</v>
+        <v>4994</v>
       </c>
     </row>
     <row r="2609" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2609" s="1" t="s">
-        <v>3675</v>
+        <v>3676</v>
       </c>
       <c r="C2609" t="s">
         <v>3495</v>
@@ -81666,12 +81684,12 @@
         <v>5549</v>
       </c>
       <c r="Q2609" t="s">
-        <v>4994</v>
+        <v>4995</v>
       </c>
     </row>
     <row r="2610" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2610" s="1" t="s">
-        <v>3676</v>
+        <v>3677</v>
       </c>
       <c r="C2610" t="s">
         <v>3495</v>
@@ -81686,12 +81704,12 @@
         <v>5549</v>
       </c>
       <c r="Q2610" t="s">
-        <v>4995</v>
+        <v>4996</v>
       </c>
     </row>
     <row r="2611" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2611" s="1" t="s">
-        <v>3677</v>
+        <v>3678</v>
       </c>
       <c r="C2611" t="s">
         <v>3495</v>
@@ -81706,12 +81724,12 @@
         <v>5549</v>
       </c>
       <c r="Q2611" t="s">
-        <v>4996</v>
+        <v>4997</v>
       </c>
     </row>
     <row r="2612" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2612" s="1" t="s">
-        <v>3678</v>
+        <v>3679</v>
       </c>
       <c r="C2612" t="s">
         <v>3495</v>
@@ -81726,12 +81744,12 @@
         <v>5549</v>
       </c>
       <c r="Q2612" t="s">
-        <v>4997</v>
+        <v>3680</v>
       </c>
     </row>
     <row r="2613" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2613" s="1" t="s">
-        <v>3679</v>
+        <v>3681</v>
       </c>
       <c r="C2613" t="s">
         <v>3495</v>
@@ -81746,12 +81764,12 @@
         <v>5549</v>
       </c>
       <c r="Q2613" t="s">
-        <v>3680</v>
+        <v>4606</v>
       </c>
     </row>
     <row r="2614" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2614" s="1" t="s">
-        <v>3681</v>
+        <v>3682</v>
       </c>
       <c r="C2614" t="s">
         <v>3495</v>
@@ -81766,12 +81784,12 @@
         <v>5549</v>
       </c>
       <c r="Q2614" t="s">
-        <v>4606</v>
+        <v>3683</v>
       </c>
     </row>
     <row r="2615" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2615" s="1" t="s">
-        <v>3682</v>
+        <v>6933</v>
       </c>
       <c r="C2615" t="s">
         <v>3495</v>
@@ -81786,12 +81804,12 @@
         <v>5549</v>
       </c>
       <c r="Q2615" t="s">
-        <v>3683</v>
+        <v>6934</v>
       </c>
     </row>
     <row r="2616" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2616" s="1" t="s">
-        <v>6933</v>
+        <v>6935</v>
       </c>
       <c r="C2616" t="s">
         <v>3495</v>
@@ -81806,12 +81824,12 @@
         <v>5549</v>
       </c>
       <c r="Q2616" t="s">
-        <v>6934</v>
+        <v>6936</v>
       </c>
     </row>
     <row r="2617" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2617" s="1" t="s">
-        <v>6935</v>
+        <v>6937</v>
       </c>
       <c r="C2617" t="s">
         <v>3495</v>
@@ -81826,12 +81844,12 @@
         <v>5549</v>
       </c>
       <c r="Q2617" t="s">
-        <v>6936</v>
+        <v>6938</v>
       </c>
     </row>
     <row r="2618" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2618" s="1" t="s">
-        <v>6937</v>
+        <v>6939</v>
       </c>
       <c r="C2618" t="s">
         <v>3495</v>
@@ -81846,12 +81864,12 @@
         <v>5549</v>
       </c>
       <c r="Q2618" t="s">
-        <v>6938</v>
+        <v>6940</v>
       </c>
     </row>
     <row r="2619" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2619" s="1" t="s">
-        <v>6939</v>
+        <v>6941</v>
       </c>
       <c r="C2619" t="s">
         <v>3495</v>
@@ -81866,12 +81884,12 @@
         <v>5549</v>
       </c>
       <c r="Q2619" t="s">
-        <v>6940</v>
+        <v>6942</v>
       </c>
     </row>
     <row r="2620" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2620" s="1" t="s">
-        <v>6941</v>
+        <v>6943</v>
       </c>
       <c r="C2620" t="s">
         <v>3495</v>
@@ -81886,12 +81904,12 @@
         <v>5549</v>
       </c>
       <c r="Q2620" t="s">
-        <v>6942</v>
+        <v>6944</v>
       </c>
     </row>
     <row r="2621" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2621" s="1" t="s">
-        <v>6943</v>
+        <v>6945</v>
       </c>
       <c r="C2621" t="s">
         <v>3495</v>
@@ -81906,12 +81924,12 @@
         <v>5549</v>
       </c>
       <c r="Q2621" t="s">
-        <v>6944</v>
+        <v>6946</v>
       </c>
     </row>
     <row r="2622" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2622" s="1" t="s">
-        <v>6945</v>
+        <v>6947</v>
       </c>
       <c r="C2622" t="s">
         <v>3495</v>
@@ -81926,12 +81944,12 @@
         <v>5549</v>
       </c>
       <c r="Q2622" t="s">
-        <v>6946</v>
+        <v>6948</v>
       </c>
     </row>
     <row r="2623" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2623" s="1" t="s">
-        <v>6947</v>
+        <v>6949</v>
       </c>
       <c r="C2623" t="s">
         <v>3495</v>
@@ -81946,12 +81964,12 @@
         <v>5549</v>
       </c>
       <c r="Q2623" t="s">
-        <v>6948</v>
+        <v>6950</v>
       </c>
     </row>
     <row r="2624" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2624" s="1" t="s">
-        <v>6949</v>
+        <v>6951</v>
       </c>
       <c r="C2624" t="s">
         <v>3495</v>
@@ -81966,12 +81984,12 @@
         <v>5549</v>
       </c>
       <c r="Q2624" t="s">
-        <v>6950</v>
+        <v>6952</v>
       </c>
     </row>
     <row r="2625" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2625" s="1" t="s">
-        <v>6951</v>
+        <v>6953</v>
       </c>
       <c r="C2625" t="s">
         <v>3495</v>
@@ -81986,26 +82004,6 @@
         <v>5549</v>
       </c>
       <c r="Q2625" t="s">
-        <v>6952</v>
-      </c>
-    </row>
-    <row r="2626" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2626" s="1" t="s">
-        <v>6953</v>
-      </c>
-      <c r="C2626" t="s">
-        <v>3495</v>
-      </c>
-      <c r="D2626" s="1">
-        <v>68000</v>
-      </c>
-      <c r="E2626" t="s">
-        <v>2426</v>
-      </c>
-      <c r="L2626" t="s">
-        <v>5549</v>
-      </c>
-      <c r="Q2626" t="s">
         <v>6954</v>
       </c>
     </row>
@@ -82020,10 +82018,10 @@
   <dimension ref="B1:Q369"/>
   <sheetViews>
     <sheetView topLeftCell="A354" workbookViewId="0">
-      <selection activeCell="C364" sqref="C364"/>
+      <selection activeCell="G370" sqref="G370"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">

</xml_diff>

<commit_message>
added royalmah full working driver
</commit_message>
<xml_diff>
--- a/compatibility_list.xlsx
+++ b/compatibility_list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9330" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9330" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="working" sheetId="9" r:id="rId1"/>
@@ -21,9 +21,9 @@
     <sheet name="To Check" sheetId="13" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">WIP!$B$1:$R$1347</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">WIP!$B$1:$R$1346</definedName>
     <definedName name="DETAILS" localSheetId="4">WIP!#REF!</definedName>
-    <definedName name="DETAILS_1" localSheetId="4">WIP!$B$1:$Q$1347</definedName>
+    <definedName name="DETAILS_1" localSheetId="4">WIP!$B$1:$Q$1346</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25879,10 +25879,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Q1347"/>
+  <dimension ref="B1:Q1346"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
+    <sheetView topLeftCell="A1191" workbookViewId="0">
+      <selection activeCell="A1201" sqref="A1201:XFD1201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -52479,24 +52479,27 @@
     </row>
     <row r="1201" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1201" s="1" t="s">
-        <v>3491</v>
+        <v>6914</v>
       </c>
       <c r="C1201" t="s">
-        <v>3492</v>
+        <v>6915</v>
       </c>
       <c r="D1201" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1201" t="s">
+        <v>2</v>
+      </c>
       <c r="L1201" t="s">
-        <v>55</v>
+        <v>5238</v>
       </c>
       <c r="Q1201" t="s">
-        <v>3493</v>
+        <v>6916</v>
       </c>
     </row>
     <row r="1202" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1202" s="1" t="s">
-        <v>6914</v>
+        <v>6917</v>
       </c>
       <c r="C1202" t="s">
         <v>6915</v>
@@ -52511,32 +52514,29 @@
         <v>5238</v>
       </c>
       <c r="Q1202" t="s">
-        <v>6916</v>
+        <v>6918</v>
       </c>
     </row>
     <row r="1203" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1203" s="1" t="s">
-        <v>6917</v>
+        <v>6919</v>
       </c>
       <c r="C1203" t="s">
-        <v>6915</v>
+        <v>6920</v>
       </c>
       <c r="D1203" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1203" t="s">
-        <v>2</v>
-      </c>
       <c r="L1203" t="s">
-        <v>5238</v>
+        <v>55</v>
       </c>
       <c r="Q1203" t="s">
-        <v>6918</v>
+        <v>6921</v>
       </c>
     </row>
     <row r="1204" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1204" s="1" t="s">
-        <v>6919</v>
+        <v>6922</v>
       </c>
       <c r="C1204" t="s">
         <v>6920</v>
@@ -52544,16 +52544,25 @@
       <c r="D1204" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1204" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1204" t="s">
+        <v>2426</v>
+      </c>
       <c r="L1204" t="s">
+        <v>542</v>
+      </c>
+      <c r="M1204" t="s">
         <v>55</v>
       </c>
       <c r="Q1204" t="s">
-        <v>6921</v>
+        <v>6923</v>
       </c>
     </row>
     <row r="1205" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1205" s="1" t="s">
-        <v>6922</v>
+        <v>6924</v>
       </c>
       <c r="C1205" t="s">
         <v>6920</v>
@@ -52574,55 +52583,49 @@
         <v>55</v>
       </c>
       <c r="Q1205" t="s">
-        <v>6923</v>
+        <v>6925</v>
       </c>
     </row>
     <row r="1206" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1206" s="1" t="s">
-        <v>6924</v>
+        <v>6926</v>
       </c>
       <c r="C1206" t="s">
-        <v>6920</v>
-      </c>
-      <c r="D1206" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1206" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1206" t="s">
-        <v>2426</v>
+        <v>6927</v>
+      </c>
+      <c r="D1206" s="1">
+        <v>68000</v>
       </c>
       <c r="L1206" t="s">
-        <v>542</v>
-      </c>
-      <c r="M1206" t="s">
-        <v>55</v>
+        <v>1687</v>
       </c>
       <c r="Q1206" t="s">
-        <v>6925</v>
+        <v>6928</v>
       </c>
     </row>
     <row r="1207" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1207" s="1" t="s">
-        <v>6926</v>
+        <v>3494</v>
       </c>
       <c r="C1207" t="s">
-        <v>6927</v>
+        <v>3495</v>
       </c>
       <c r="D1207" s="1">
         <v>68000</v>
       </c>
+      <c r="E1207" t="s">
+        <v>2426</v>
+      </c>
       <c r="L1207" t="s">
-        <v>1687</v>
+        <v>5549</v>
       </c>
       <c r="Q1207" t="s">
-        <v>6928</v>
+        <v>3496</v>
       </c>
     </row>
     <row r="1208" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1208" s="1" t="s">
-        <v>3494</v>
+        <v>3497</v>
       </c>
       <c r="C1208" t="s">
         <v>3495</v>
@@ -52637,12 +52640,12 @@
         <v>5549</v>
       </c>
       <c r="Q1208" t="s">
-        <v>3496</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="1209" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1209" s="1" t="s">
-        <v>3497</v>
+        <v>3498</v>
       </c>
       <c r="C1209" t="s">
         <v>3495</v>
@@ -52657,12 +52660,12 @@
         <v>5549</v>
       </c>
       <c r="Q1209" t="s">
-        <v>4587</v>
+        <v>3499</v>
       </c>
     </row>
     <row r="1210" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1210" s="1" t="s">
-        <v>3498</v>
+        <v>3500</v>
       </c>
       <c r="C1210" t="s">
         <v>3495</v>
@@ -52677,12 +52680,12 @@
         <v>5549</v>
       </c>
       <c r="Q1210" t="s">
-        <v>3499</v>
+        <v>3501</v>
       </c>
     </row>
     <row r="1211" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1211" s="1" t="s">
-        <v>3500</v>
+        <v>3502</v>
       </c>
       <c r="C1211" t="s">
         <v>3495</v>
@@ -52697,12 +52700,12 @@
         <v>5549</v>
       </c>
       <c r="Q1211" t="s">
-        <v>3501</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="1212" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1212" s="1" t="s">
-        <v>3502</v>
+        <v>3504</v>
       </c>
       <c r="C1212" t="s">
         <v>3495</v>
@@ -52717,12 +52720,12 @@
         <v>5549</v>
       </c>
       <c r="Q1212" t="s">
-        <v>3503</v>
+        <v>3505</v>
       </c>
     </row>
     <row r="1213" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1213" s="1" t="s">
-        <v>3504</v>
+        <v>3506</v>
       </c>
       <c r="C1213" t="s">
         <v>3495</v>
@@ -52737,12 +52740,12 @@
         <v>5549</v>
       </c>
       <c r="Q1213" t="s">
-        <v>3505</v>
+        <v>6929</v>
       </c>
     </row>
     <row r="1214" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1214" s="1" t="s">
-        <v>3506</v>
+        <v>6930</v>
       </c>
       <c r="C1214" t="s">
         <v>3495</v>
@@ -52757,12 +52760,12 @@
         <v>5549</v>
       </c>
       <c r="Q1214" t="s">
-        <v>6929</v>
+        <v>6931</v>
       </c>
     </row>
     <row r="1215" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1215" s="1" t="s">
-        <v>6930</v>
+        <v>3507</v>
       </c>
       <c r="C1215" t="s">
         <v>3495</v>
@@ -52777,12 +52780,12 @@
         <v>5549</v>
       </c>
       <c r="Q1215" t="s">
-        <v>6931</v>
+        <v>4952</v>
       </c>
     </row>
     <row r="1216" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1216" s="1" t="s">
-        <v>3507</v>
+        <v>3508</v>
       </c>
       <c r="C1216" t="s">
         <v>3495</v>
@@ -52797,12 +52800,12 @@
         <v>5549</v>
       </c>
       <c r="Q1216" t="s">
-        <v>4952</v>
+        <v>3509</v>
       </c>
     </row>
     <row r="1217" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1217" s="1" t="s">
-        <v>3508</v>
+        <v>3510</v>
       </c>
       <c r="C1217" t="s">
         <v>3495</v>
@@ -52817,12 +52820,12 @@
         <v>5549</v>
       </c>
       <c r="Q1217" t="s">
-        <v>3509</v>
+        <v>3511</v>
       </c>
     </row>
     <row r="1218" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1218" s="1" t="s">
-        <v>3510</v>
+        <v>3512</v>
       </c>
       <c r="C1218" t="s">
         <v>3495</v>
@@ -52837,12 +52840,12 @@
         <v>5549</v>
       </c>
       <c r="Q1218" t="s">
-        <v>3511</v>
+        <v>3513</v>
       </c>
     </row>
     <row r="1219" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1219" s="1" t="s">
-        <v>3512</v>
+        <v>3514</v>
       </c>
       <c r="C1219" t="s">
         <v>3495</v>
@@ -52857,12 +52860,12 @@
         <v>5549</v>
       </c>
       <c r="Q1219" t="s">
-        <v>3513</v>
+        <v>3515</v>
       </c>
     </row>
     <row r="1220" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1220" s="1" t="s">
-        <v>3514</v>
+        <v>3516</v>
       </c>
       <c r="C1220" t="s">
         <v>3495</v>
@@ -52877,12 +52880,12 @@
         <v>5549</v>
       </c>
       <c r="Q1220" t="s">
-        <v>3515</v>
+        <v>3517</v>
       </c>
     </row>
     <row r="1221" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1221" s="1" t="s">
-        <v>3516</v>
+        <v>3518</v>
       </c>
       <c r="C1221" t="s">
         <v>3495</v>
@@ -52897,12 +52900,12 @@
         <v>5549</v>
       </c>
       <c r="Q1221" t="s">
-        <v>3517</v>
+        <v>4953</v>
       </c>
     </row>
     <row r="1222" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1222" s="1" t="s">
-        <v>3518</v>
+        <v>3519</v>
       </c>
       <c r="C1222" t="s">
         <v>3495</v>
@@ -52917,12 +52920,12 @@
         <v>5549</v>
       </c>
       <c r="Q1222" t="s">
-        <v>4953</v>
+        <v>4954</v>
       </c>
     </row>
     <row r="1223" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1223" s="1" t="s">
-        <v>3519</v>
+        <v>3520</v>
       </c>
       <c r="C1223" t="s">
         <v>3495</v>
@@ -52937,12 +52940,12 @@
         <v>5549</v>
       </c>
       <c r="Q1223" t="s">
-        <v>4954</v>
+        <v>3521</v>
       </c>
     </row>
     <row r="1224" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1224" s="1" t="s">
-        <v>3520</v>
+        <v>3522</v>
       </c>
       <c r="C1224" t="s">
         <v>3495</v>
@@ -52957,12 +52960,12 @@
         <v>5549</v>
       </c>
       <c r="Q1224" t="s">
-        <v>3521</v>
+        <v>3523</v>
       </c>
     </row>
     <row r="1225" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1225" s="1" t="s">
-        <v>3522</v>
+        <v>3524</v>
       </c>
       <c r="C1225" t="s">
         <v>3495</v>
@@ -52977,12 +52980,12 @@
         <v>5549</v>
       </c>
       <c r="Q1225" t="s">
-        <v>3523</v>
+        <v>3525</v>
       </c>
     </row>
     <row r="1226" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1226" s="1" t="s">
-        <v>3524</v>
+        <v>3526</v>
       </c>
       <c r="C1226" t="s">
         <v>3495</v>
@@ -52997,12 +53000,12 @@
         <v>5549</v>
       </c>
       <c r="Q1226" t="s">
-        <v>3525</v>
+        <v>3527</v>
       </c>
     </row>
     <row r="1227" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1227" s="1" t="s">
-        <v>3526</v>
+        <v>3528</v>
       </c>
       <c r="C1227" t="s">
         <v>3495</v>
@@ -53017,12 +53020,12 @@
         <v>5549</v>
       </c>
       <c r="Q1227" t="s">
-        <v>3527</v>
+        <v>3529</v>
       </c>
     </row>
     <row r="1228" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1228" s="1" t="s">
-        <v>3528</v>
+        <v>3530</v>
       </c>
       <c r="C1228" t="s">
         <v>3495</v>
@@ -53037,12 +53040,12 @@
         <v>5549</v>
       </c>
       <c r="Q1228" t="s">
-        <v>3529</v>
+        <v>3531</v>
       </c>
     </row>
     <row r="1229" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1229" s="1" t="s">
-        <v>3530</v>
+        <v>3532</v>
       </c>
       <c r="C1229" t="s">
         <v>3495</v>
@@ -53057,12 +53060,12 @@
         <v>5549</v>
       </c>
       <c r="Q1229" t="s">
-        <v>3531</v>
+        <v>4955</v>
       </c>
     </row>
     <row r="1230" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1230" s="1" t="s">
-        <v>3532</v>
+        <v>3533</v>
       </c>
       <c r="C1230" t="s">
         <v>3495</v>
@@ -53077,12 +53080,12 @@
         <v>5549</v>
       </c>
       <c r="Q1230" t="s">
-        <v>4955</v>
+        <v>3534</v>
       </c>
     </row>
     <row r="1231" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1231" s="1" t="s">
-        <v>3533</v>
+        <v>3535</v>
       </c>
       <c r="C1231" t="s">
         <v>3495</v>
@@ -53097,12 +53100,12 @@
         <v>5549</v>
       </c>
       <c r="Q1231" t="s">
-        <v>3534</v>
+        <v>3536</v>
       </c>
     </row>
     <row r="1232" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1232" s="1" t="s">
-        <v>3535</v>
+        <v>3537</v>
       </c>
       <c r="C1232" t="s">
         <v>3495</v>
@@ -53117,12 +53120,12 @@
         <v>5549</v>
       </c>
       <c r="Q1232" t="s">
-        <v>3536</v>
+        <v>3538</v>
       </c>
     </row>
     <row r="1233" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1233" s="1" t="s">
-        <v>3537</v>
+        <v>3539</v>
       </c>
       <c r="C1233" t="s">
         <v>3495</v>
@@ -53137,12 +53140,12 @@
         <v>5549</v>
       </c>
       <c r="Q1233" t="s">
-        <v>3538</v>
+        <v>4956</v>
       </c>
     </row>
     <row r="1234" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1234" s="1" t="s">
-        <v>3539</v>
+        <v>3540</v>
       </c>
       <c r="C1234" t="s">
         <v>3495</v>
@@ -53157,12 +53160,12 @@
         <v>5549</v>
       </c>
       <c r="Q1234" t="s">
-        <v>4956</v>
+        <v>4588</v>
       </c>
     </row>
     <row r="1235" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1235" s="1" t="s">
-        <v>3540</v>
+        <v>3541</v>
       </c>
       <c r="C1235" t="s">
         <v>3495</v>
@@ -53177,12 +53180,12 @@
         <v>5549</v>
       </c>
       <c r="Q1235" t="s">
-        <v>4588</v>
+        <v>4589</v>
       </c>
     </row>
     <row r="1236" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1236" s="1" t="s">
-        <v>3541</v>
+        <v>3542</v>
       </c>
       <c r="C1236" t="s">
         <v>3495</v>
@@ -53197,12 +53200,12 @@
         <v>5549</v>
       </c>
       <c r="Q1236" t="s">
-        <v>4589</v>
+        <v>3543</v>
       </c>
     </row>
     <row r="1237" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1237" s="1" t="s">
-        <v>3542</v>
+        <v>3544</v>
       </c>
       <c r="C1237" t="s">
         <v>3495</v>
@@ -53217,12 +53220,12 @@
         <v>5549</v>
       </c>
       <c r="Q1237" t="s">
-        <v>3543</v>
+        <v>3545</v>
       </c>
     </row>
     <row r="1238" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1238" s="1" t="s">
-        <v>3544</v>
+        <v>3546</v>
       </c>
       <c r="C1238" t="s">
         <v>3495</v>
@@ -53237,12 +53240,12 @@
         <v>5549</v>
       </c>
       <c r="Q1238" t="s">
-        <v>3545</v>
+        <v>4957</v>
       </c>
     </row>
     <row r="1239" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1239" s="1" t="s">
-        <v>3546</v>
+        <v>3547</v>
       </c>
       <c r="C1239" t="s">
         <v>3495</v>
@@ -53257,12 +53260,12 @@
         <v>5549</v>
       </c>
       <c r="Q1239" t="s">
-        <v>4957</v>
+        <v>3548</v>
       </c>
     </row>
     <row r="1240" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1240" s="1" t="s">
-        <v>3547</v>
+        <v>3549</v>
       </c>
       <c r="C1240" t="s">
         <v>3495</v>
@@ -53277,12 +53280,12 @@
         <v>5549</v>
       </c>
       <c r="Q1240" t="s">
-        <v>3548</v>
+        <v>4590</v>
       </c>
     </row>
     <row r="1241" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1241" s="1" t="s">
-        <v>3549</v>
+        <v>3550</v>
       </c>
       <c r="C1241" t="s">
         <v>3495</v>
@@ -53297,12 +53300,12 @@
         <v>5549</v>
       </c>
       <c r="Q1241" t="s">
-        <v>4590</v>
+        <v>3551</v>
       </c>
     </row>
     <row r="1242" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1242" s="1" t="s">
-        <v>3550</v>
+        <v>3552</v>
       </c>
       <c r="C1242" t="s">
         <v>3495</v>
@@ -53317,12 +53320,12 @@
         <v>5549</v>
       </c>
       <c r="Q1242" t="s">
-        <v>3551</v>
+        <v>3553</v>
       </c>
     </row>
     <row r="1243" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1243" s="1" t="s">
-        <v>3552</v>
+        <v>3554</v>
       </c>
       <c r="C1243" t="s">
         <v>3495</v>
@@ -53337,12 +53340,12 @@
         <v>5549</v>
       </c>
       <c r="Q1243" t="s">
-        <v>3553</v>
+        <v>4958</v>
       </c>
     </row>
     <row r="1244" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1244" s="1" t="s">
-        <v>3554</v>
+        <v>3555</v>
       </c>
       <c r="C1244" t="s">
         <v>3495</v>
@@ -53357,12 +53360,12 @@
         <v>5549</v>
       </c>
       <c r="Q1244" t="s">
-        <v>4958</v>
+        <v>4591</v>
       </c>
     </row>
     <row r="1245" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1245" s="1" t="s">
-        <v>3555</v>
+        <v>3556</v>
       </c>
       <c r="C1245" t="s">
         <v>3495</v>
@@ -53377,12 +53380,12 @@
         <v>5549</v>
       </c>
       <c r="Q1245" t="s">
-        <v>4591</v>
+        <v>3557</v>
       </c>
     </row>
     <row r="1246" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1246" s="1" t="s">
-        <v>3556</v>
+        <v>3558</v>
       </c>
       <c r="C1246" t="s">
         <v>3495</v>
@@ -53397,12 +53400,12 @@
         <v>5549</v>
       </c>
       <c r="Q1246" t="s">
-        <v>3557</v>
+        <v>4959</v>
       </c>
     </row>
     <row r="1247" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1247" s="1" t="s">
-        <v>3558</v>
+        <v>3559</v>
       </c>
       <c r="C1247" t="s">
         <v>3495</v>
@@ -53417,12 +53420,12 @@
         <v>5549</v>
       </c>
       <c r="Q1247" t="s">
-        <v>4959</v>
+        <v>4592</v>
       </c>
     </row>
     <row r="1248" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1248" s="1" t="s">
-        <v>3559</v>
+        <v>3560</v>
       </c>
       <c r="C1248" t="s">
         <v>3495</v>
@@ -53437,12 +53440,12 @@
         <v>5549</v>
       </c>
       <c r="Q1248" t="s">
-        <v>4592</v>
+        <v>4593</v>
       </c>
     </row>
     <row r="1249" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1249" s="1" t="s">
-        <v>3560</v>
+        <v>3561</v>
       </c>
       <c r="C1249" t="s">
         <v>3495</v>
@@ -53457,12 +53460,12 @@
         <v>5549</v>
       </c>
       <c r="Q1249" t="s">
-        <v>4593</v>
+        <v>4960</v>
       </c>
     </row>
     <row r="1250" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1250" s="1" t="s">
-        <v>3561</v>
+        <v>3562</v>
       </c>
       <c r="C1250" t="s">
         <v>3495</v>
@@ -53477,12 +53480,12 @@
         <v>5549</v>
       </c>
       <c r="Q1250" t="s">
-        <v>4960</v>
+        <v>4594</v>
       </c>
     </row>
     <row r="1251" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1251" s="1" t="s">
-        <v>3562</v>
+        <v>3563</v>
       </c>
       <c r="C1251" t="s">
         <v>3495</v>
@@ -53497,12 +53500,12 @@
         <v>5549</v>
       </c>
       <c r="Q1251" t="s">
-        <v>4594</v>
+        <v>4961</v>
       </c>
     </row>
     <row r="1252" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1252" s="1" t="s">
-        <v>3563</v>
+        <v>3564</v>
       </c>
       <c r="C1252" t="s">
         <v>3495</v>
@@ -53517,12 +53520,12 @@
         <v>5549</v>
       </c>
       <c r="Q1252" t="s">
-        <v>4961</v>
+        <v>4962</v>
       </c>
     </row>
     <row r="1253" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1253" s="1" t="s">
-        <v>3564</v>
+        <v>3565</v>
       </c>
       <c r="C1253" t="s">
         <v>3495</v>
@@ -53537,12 +53540,12 @@
         <v>5549</v>
       </c>
       <c r="Q1253" t="s">
-        <v>4962</v>
+        <v>3566</v>
       </c>
     </row>
     <row r="1254" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1254" s="1" t="s">
-        <v>3565</v>
+        <v>3567</v>
       </c>
       <c r="C1254" t="s">
         <v>3495</v>
@@ -53557,12 +53560,12 @@
         <v>5549</v>
       </c>
       <c r="Q1254" t="s">
-        <v>3566</v>
+        <v>3568</v>
       </c>
     </row>
     <row r="1255" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1255" s="1" t="s">
-        <v>3567</v>
+        <v>3569</v>
       </c>
       <c r="C1255" t="s">
         <v>3495</v>
@@ -53577,12 +53580,12 @@
         <v>5549</v>
       </c>
       <c r="Q1255" t="s">
-        <v>3568</v>
+        <v>3570</v>
       </c>
     </row>
     <row r="1256" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1256" s="1" t="s">
-        <v>3569</v>
+        <v>3571</v>
       </c>
       <c r="C1256" t="s">
         <v>3495</v>
@@ -53597,12 +53600,12 @@
         <v>5549</v>
       </c>
       <c r="Q1256" t="s">
-        <v>3570</v>
+        <v>4595</v>
       </c>
     </row>
     <row r="1257" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1257" s="1" t="s">
-        <v>3571</v>
+        <v>3572</v>
       </c>
       <c r="C1257" t="s">
         <v>3495</v>
@@ -53617,12 +53620,12 @@
         <v>5549</v>
       </c>
       <c r="Q1257" t="s">
-        <v>4595</v>
+        <v>3573</v>
       </c>
     </row>
     <row r="1258" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1258" s="1" t="s">
-        <v>3572</v>
+        <v>3574</v>
       </c>
       <c r="C1258" t="s">
         <v>3495</v>
@@ -53637,12 +53640,12 @@
         <v>5549</v>
       </c>
       <c r="Q1258" t="s">
-        <v>3573</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="1259" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1259" s="1" t="s">
-        <v>3574</v>
+        <v>3576</v>
       </c>
       <c r="C1259" t="s">
         <v>3495</v>
@@ -53657,12 +53660,12 @@
         <v>5549</v>
       </c>
       <c r="Q1259" t="s">
-        <v>3575</v>
+        <v>4963</v>
       </c>
     </row>
     <row r="1260" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1260" s="1" t="s">
-        <v>3576</v>
+        <v>3577</v>
       </c>
       <c r="C1260" t="s">
         <v>3495</v>
@@ -53677,12 +53680,12 @@
         <v>5549</v>
       </c>
       <c r="Q1260" t="s">
-        <v>4963</v>
+        <v>3578</v>
       </c>
     </row>
     <row r="1261" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1261" s="1" t="s">
-        <v>3577</v>
+        <v>3579</v>
       </c>
       <c r="C1261" t="s">
         <v>3495</v>
@@ -53697,12 +53700,12 @@
         <v>5549</v>
       </c>
       <c r="Q1261" t="s">
-        <v>3578</v>
+        <v>4964</v>
       </c>
     </row>
     <row r="1262" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1262" s="1" t="s">
-        <v>3579</v>
+        <v>3580</v>
       </c>
       <c r="C1262" t="s">
         <v>3495</v>
@@ -53717,12 +53720,12 @@
         <v>5549</v>
       </c>
       <c r="Q1262" t="s">
-        <v>4964</v>
+        <v>4965</v>
       </c>
     </row>
     <row r="1263" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1263" s="1" t="s">
-        <v>3580</v>
+        <v>3581</v>
       </c>
       <c r="C1263" t="s">
         <v>3495</v>
@@ -53737,12 +53740,12 @@
         <v>5549</v>
       </c>
       <c r="Q1263" t="s">
-        <v>4965</v>
+        <v>4596</v>
       </c>
     </row>
     <row r="1264" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1264" s="1" t="s">
-        <v>3581</v>
+        <v>3582</v>
       </c>
       <c r="C1264" t="s">
         <v>3495</v>
@@ -53757,12 +53760,12 @@
         <v>5549</v>
       </c>
       <c r="Q1264" t="s">
-        <v>4596</v>
+        <v>4966</v>
       </c>
     </row>
     <row r="1265" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1265" s="1" t="s">
-        <v>3582</v>
+        <v>3583</v>
       </c>
       <c r="C1265" t="s">
         <v>3495</v>
@@ -53777,12 +53780,12 @@
         <v>5549</v>
       </c>
       <c r="Q1265" t="s">
-        <v>4966</v>
+        <v>4597</v>
       </c>
     </row>
     <row r="1266" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1266" s="1" t="s">
-        <v>3583</v>
+        <v>3584</v>
       </c>
       <c r="C1266" t="s">
         <v>3495</v>
@@ -53797,12 +53800,12 @@
         <v>5549</v>
       </c>
       <c r="Q1266" t="s">
-        <v>4597</v>
+        <v>4967</v>
       </c>
     </row>
     <row r="1267" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1267" s="1" t="s">
-        <v>3584</v>
+        <v>3585</v>
       </c>
       <c r="C1267" t="s">
         <v>3495</v>
@@ -53817,12 +53820,12 @@
         <v>5549</v>
       </c>
       <c r="Q1267" t="s">
-        <v>4967</v>
+        <v>3586</v>
       </c>
     </row>
     <row r="1268" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1268" s="1" t="s">
-        <v>3585</v>
+        <v>3587</v>
       </c>
       <c r="C1268" t="s">
         <v>3495</v>
@@ -53837,12 +53840,12 @@
         <v>5549</v>
       </c>
       <c r="Q1268" t="s">
-        <v>3586</v>
+        <v>4598</v>
       </c>
     </row>
     <row r="1269" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1269" s="1" t="s">
-        <v>3587</v>
+        <v>3588</v>
       </c>
       <c r="C1269" t="s">
         <v>3495</v>
@@ -53857,12 +53860,12 @@
         <v>5549</v>
       </c>
       <c r="Q1269" t="s">
-        <v>4598</v>
+        <v>4968</v>
       </c>
     </row>
     <row r="1270" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1270" s="1" t="s">
-        <v>3588</v>
+        <v>3589</v>
       </c>
       <c r="C1270" t="s">
         <v>3495</v>
@@ -53877,12 +53880,12 @@
         <v>5549</v>
       </c>
       <c r="Q1270" t="s">
-        <v>4968</v>
+        <v>3590</v>
       </c>
     </row>
     <row r="1271" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1271" s="1" t="s">
-        <v>3589</v>
+        <v>3591</v>
       </c>
       <c r="C1271" t="s">
         <v>3495</v>
@@ -53897,12 +53900,12 @@
         <v>5549</v>
       </c>
       <c r="Q1271" t="s">
-        <v>3590</v>
+        <v>3592</v>
       </c>
     </row>
     <row r="1272" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1272" s="1" t="s">
-        <v>3591</v>
+        <v>3593</v>
       </c>
       <c r="C1272" t="s">
         <v>3495</v>
@@ -53917,12 +53920,12 @@
         <v>5549</v>
       </c>
       <c r="Q1272" t="s">
-        <v>3592</v>
+        <v>4969</v>
       </c>
     </row>
     <row r="1273" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1273" s="1" t="s">
-        <v>3593</v>
+        <v>3594</v>
       </c>
       <c r="C1273" t="s">
         <v>3495</v>
@@ -53937,12 +53940,12 @@
         <v>5549</v>
       </c>
       <c r="Q1273" t="s">
-        <v>4969</v>
+        <v>3595</v>
       </c>
     </row>
     <row r="1274" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1274" s="1" t="s">
-        <v>3594</v>
+        <v>3596</v>
       </c>
       <c r="C1274" t="s">
         <v>3495</v>
@@ -53957,12 +53960,12 @@
         <v>5549</v>
       </c>
       <c r="Q1274" t="s">
-        <v>3595</v>
+        <v>4970</v>
       </c>
     </row>
     <row r="1275" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1275" s="1" t="s">
-        <v>3596</v>
+        <v>3597</v>
       </c>
       <c r="C1275" t="s">
         <v>3495</v>
@@ -53977,12 +53980,12 @@
         <v>5549</v>
       </c>
       <c r="Q1275" t="s">
-        <v>4970</v>
+        <v>4599</v>
       </c>
     </row>
     <row r="1276" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1276" s="1" t="s">
-        <v>3597</v>
+        <v>3598</v>
       </c>
       <c r="C1276" t="s">
         <v>3495</v>
@@ -53997,12 +54000,12 @@
         <v>5549</v>
       </c>
       <c r="Q1276" t="s">
-        <v>4599</v>
+        <v>4600</v>
       </c>
     </row>
     <row r="1277" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1277" s="1" t="s">
-        <v>3598</v>
+        <v>3599</v>
       </c>
       <c r="C1277" t="s">
         <v>3495</v>
@@ -54017,12 +54020,12 @@
         <v>5549</v>
       </c>
       <c r="Q1277" t="s">
-        <v>4600</v>
+        <v>4971</v>
       </c>
     </row>
     <row r="1278" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1278" s="1" t="s">
-        <v>3599</v>
+        <v>3600</v>
       </c>
       <c r="C1278" t="s">
         <v>3495</v>
@@ -54037,12 +54040,12 @@
         <v>5549</v>
       </c>
       <c r="Q1278" t="s">
-        <v>4971</v>
+        <v>4972</v>
       </c>
     </row>
     <row r="1279" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1279" s="1" t="s">
-        <v>3600</v>
+        <v>3601</v>
       </c>
       <c r="C1279" t="s">
         <v>3495</v>
@@ -54057,12 +54060,12 @@
         <v>5549</v>
       </c>
       <c r="Q1279" t="s">
-        <v>4972</v>
+        <v>3602</v>
       </c>
     </row>
     <row r="1280" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1280" s="1" t="s">
-        <v>3601</v>
+        <v>3603</v>
       </c>
       <c r="C1280" t="s">
         <v>3495</v>
@@ -54077,12 +54080,12 @@
         <v>5549</v>
       </c>
       <c r="Q1280" t="s">
-        <v>3602</v>
+        <v>4973</v>
       </c>
     </row>
     <row r="1281" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1281" s="1" t="s">
-        <v>3603</v>
+        <v>3604</v>
       </c>
       <c r="C1281" t="s">
         <v>3495</v>
@@ -54097,12 +54100,12 @@
         <v>5549</v>
       </c>
       <c r="Q1281" t="s">
-        <v>4973</v>
+        <v>3605</v>
       </c>
     </row>
     <row r="1282" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1282" s="1" t="s">
-        <v>3604</v>
+        <v>6932</v>
       </c>
       <c r="C1282" t="s">
         <v>3495</v>
@@ -54117,12 +54120,12 @@
         <v>5549</v>
       </c>
       <c r="Q1282" t="s">
-        <v>3605</v>
+        <v>4974</v>
       </c>
     </row>
     <row r="1283" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1283" s="1" t="s">
-        <v>6932</v>
+        <v>3607</v>
       </c>
       <c r="C1283" t="s">
         <v>3495</v>
@@ -54137,12 +54140,12 @@
         <v>5549</v>
       </c>
       <c r="Q1283" t="s">
-        <v>4974</v>
+        <v>3608</v>
       </c>
     </row>
     <row r="1284" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1284" s="1" t="s">
-        <v>3607</v>
+        <v>3609</v>
       </c>
       <c r="C1284" t="s">
         <v>3495</v>
@@ -54157,12 +54160,12 @@
         <v>5549</v>
       </c>
       <c r="Q1284" t="s">
-        <v>3608</v>
+        <v>3610</v>
       </c>
     </row>
     <row r="1285" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1285" s="1" t="s">
-        <v>3609</v>
+        <v>3611</v>
       </c>
       <c r="C1285" t="s">
         <v>3495</v>
@@ -54177,12 +54180,12 @@
         <v>5549</v>
       </c>
       <c r="Q1285" t="s">
-        <v>3610</v>
+        <v>4975</v>
       </c>
     </row>
     <row r="1286" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1286" s="1" t="s">
-        <v>3611</v>
+        <v>3612</v>
       </c>
       <c r="C1286" t="s">
         <v>3495</v>
@@ -54197,12 +54200,12 @@
         <v>5549</v>
       </c>
       <c r="Q1286" t="s">
-        <v>4975</v>
+        <v>4976</v>
       </c>
     </row>
     <row r="1287" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1287" s="1" t="s">
-        <v>3612</v>
+        <v>3613</v>
       </c>
       <c r="C1287" t="s">
         <v>3495</v>
@@ -54217,12 +54220,12 @@
         <v>5549</v>
       </c>
       <c r="Q1287" t="s">
-        <v>4976</v>
+        <v>3614</v>
       </c>
     </row>
     <row r="1288" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1288" s="1" t="s">
-        <v>3613</v>
+        <v>3615</v>
       </c>
       <c r="C1288" t="s">
         <v>3495</v>
@@ -54237,12 +54240,12 @@
         <v>5549</v>
       </c>
       <c r="Q1288" t="s">
-        <v>3614</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="1289" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1289" s="1" t="s">
-        <v>3615</v>
+        <v>3617</v>
       </c>
       <c r="C1289" t="s">
         <v>3495</v>
@@ -54257,12 +54260,12 @@
         <v>5549</v>
       </c>
       <c r="Q1289" t="s">
-        <v>3616</v>
+        <v>4977</v>
       </c>
     </row>
     <row r="1290" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1290" s="1" t="s">
-        <v>3617</v>
+        <v>3618</v>
       </c>
       <c r="C1290" t="s">
         <v>3495</v>
@@ -54277,12 +54280,12 @@
         <v>5549</v>
       </c>
       <c r="Q1290" t="s">
-        <v>4977</v>
+        <v>3619</v>
       </c>
     </row>
     <row r="1291" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1291" s="1" t="s">
-        <v>3618</v>
+        <v>3620</v>
       </c>
       <c r="C1291" t="s">
         <v>3495</v>
@@ -54297,12 +54300,12 @@
         <v>5549</v>
       </c>
       <c r="Q1291" t="s">
-        <v>3619</v>
+        <v>4978</v>
       </c>
     </row>
     <row r="1292" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1292" s="1" t="s">
-        <v>3620</v>
+        <v>3621</v>
       </c>
       <c r="C1292" t="s">
         <v>3495</v>
@@ -54317,12 +54320,12 @@
         <v>5549</v>
       </c>
       <c r="Q1292" t="s">
-        <v>4978</v>
+        <v>4979</v>
       </c>
     </row>
     <row r="1293" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1293" s="1" t="s">
-        <v>3621</v>
+        <v>3622</v>
       </c>
       <c r="C1293" t="s">
         <v>3495</v>
@@ -54337,12 +54340,12 @@
         <v>5549</v>
       </c>
       <c r="Q1293" t="s">
-        <v>4979</v>
+        <v>4980</v>
       </c>
     </row>
     <row r="1294" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1294" s="1" t="s">
-        <v>3622</v>
+        <v>3623</v>
       </c>
       <c r="C1294" t="s">
         <v>3495</v>
@@ -54357,12 +54360,12 @@
         <v>5549</v>
       </c>
       <c r="Q1294" t="s">
-        <v>4980</v>
+        <v>4601</v>
       </c>
     </row>
     <row r="1295" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1295" s="1" t="s">
-        <v>3623</v>
+        <v>3624</v>
       </c>
       <c r="C1295" t="s">
         <v>3495</v>
@@ -54377,12 +54380,12 @@
         <v>5549</v>
       </c>
       <c r="Q1295" t="s">
-        <v>4601</v>
+        <v>4981</v>
       </c>
     </row>
     <row r="1296" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1296" s="1" t="s">
-        <v>3624</v>
+        <v>3625</v>
       </c>
       <c r="C1296" t="s">
         <v>3495</v>
@@ -54397,12 +54400,12 @@
         <v>5549</v>
       </c>
       <c r="Q1296" t="s">
-        <v>4981</v>
+        <v>4602</v>
       </c>
     </row>
     <row r="1297" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1297" s="1" t="s">
-        <v>3625</v>
+        <v>3626</v>
       </c>
       <c r="C1297" t="s">
         <v>3495</v>
@@ -54417,12 +54420,12 @@
         <v>5549</v>
       </c>
       <c r="Q1297" t="s">
-        <v>4602</v>
+        <v>3627</v>
       </c>
     </row>
     <row r="1298" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1298" s="1" t="s">
-        <v>3626</v>
+        <v>3628</v>
       </c>
       <c r="C1298" t="s">
         <v>3495</v>
@@ -54437,12 +54440,12 @@
         <v>5549</v>
       </c>
       <c r="Q1298" t="s">
-        <v>3627</v>
+        <v>4982</v>
       </c>
     </row>
     <row r="1299" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1299" s="1" t="s">
-        <v>3628</v>
+        <v>3629</v>
       </c>
       <c r="C1299" t="s">
         <v>3495</v>
@@ -54457,12 +54460,12 @@
         <v>5549</v>
       </c>
       <c r="Q1299" t="s">
-        <v>4982</v>
+        <v>4603</v>
       </c>
     </row>
     <row r="1300" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1300" s="1" t="s">
-        <v>3629</v>
+        <v>3630</v>
       </c>
       <c r="C1300" t="s">
         <v>3495</v>
@@ -54477,12 +54480,12 @@
         <v>5549</v>
       </c>
       <c r="Q1300" t="s">
-        <v>4603</v>
+        <v>3631</v>
       </c>
     </row>
     <row r="1301" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1301" s="1" t="s">
-        <v>3630</v>
+        <v>3632</v>
       </c>
       <c r="C1301" t="s">
         <v>3495</v>
@@ -54497,12 +54500,12 @@
         <v>5549</v>
       </c>
       <c r="Q1301" t="s">
-        <v>3631</v>
+        <v>4983</v>
       </c>
     </row>
     <row r="1302" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1302" s="1" t="s">
-        <v>3632</v>
+        <v>3633</v>
       </c>
       <c r="C1302" t="s">
         <v>3495</v>
@@ -54517,12 +54520,12 @@
         <v>5549</v>
       </c>
       <c r="Q1302" t="s">
-        <v>4983</v>
+        <v>3634</v>
       </c>
     </row>
     <row r="1303" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1303" s="1" t="s">
-        <v>3633</v>
+        <v>3635</v>
       </c>
       <c r="C1303" t="s">
         <v>3495</v>
@@ -54537,12 +54540,12 @@
         <v>5549</v>
       </c>
       <c r="Q1303" t="s">
-        <v>3634</v>
+        <v>3636</v>
       </c>
     </row>
     <row r="1304" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1304" s="1" t="s">
-        <v>3635</v>
+        <v>3637</v>
       </c>
       <c r="C1304" t="s">
         <v>3495</v>
@@ -54557,12 +54560,12 @@
         <v>5549</v>
       </c>
       <c r="Q1304" t="s">
-        <v>3636</v>
+        <v>4604</v>
       </c>
     </row>
     <row r="1305" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1305" s="1" t="s">
-        <v>3637</v>
+        <v>3638</v>
       </c>
       <c r="C1305" t="s">
         <v>3495</v>
@@ -54577,12 +54580,12 @@
         <v>5549</v>
       </c>
       <c r="Q1305" t="s">
-        <v>4604</v>
+        <v>3639</v>
       </c>
     </row>
     <row r="1306" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1306" s="1" t="s">
-        <v>3638</v>
+        <v>3640</v>
       </c>
       <c r="C1306" t="s">
         <v>3495</v>
@@ -54597,12 +54600,12 @@
         <v>5549</v>
       </c>
       <c r="Q1306" t="s">
-        <v>3639</v>
+        <v>4984</v>
       </c>
     </row>
     <row r="1307" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1307" s="1" t="s">
-        <v>3640</v>
+        <v>3641</v>
       </c>
       <c r="C1307" t="s">
         <v>3495</v>
@@ -54617,12 +54620,12 @@
         <v>5549</v>
       </c>
       <c r="Q1307" t="s">
-        <v>4984</v>
+        <v>4985</v>
       </c>
     </row>
     <row r="1308" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1308" s="1" t="s">
-        <v>3641</v>
+        <v>3642</v>
       </c>
       <c r="C1308" t="s">
         <v>3495</v>
@@ -54637,12 +54640,12 @@
         <v>5549</v>
       </c>
       <c r="Q1308" t="s">
-        <v>4985</v>
+        <v>4605</v>
       </c>
     </row>
     <row r="1309" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1309" s="1" t="s">
-        <v>3642</v>
+        <v>3643</v>
       </c>
       <c r="C1309" t="s">
         <v>3495</v>
@@ -54657,12 +54660,12 @@
         <v>5549</v>
       </c>
       <c r="Q1309" t="s">
-        <v>4605</v>
+        <v>4986</v>
       </c>
     </row>
     <row r="1310" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1310" s="1" t="s">
-        <v>3643</v>
+        <v>3644</v>
       </c>
       <c r="C1310" t="s">
         <v>3495</v>
@@ -54677,12 +54680,12 @@
         <v>5549</v>
       </c>
       <c r="Q1310" t="s">
-        <v>4986</v>
+        <v>4987</v>
       </c>
     </row>
     <row r="1311" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1311" s="1" t="s">
-        <v>3644</v>
+        <v>3645</v>
       </c>
       <c r="C1311" t="s">
         <v>3495</v>
@@ -54697,12 +54700,12 @@
         <v>5549</v>
       </c>
       <c r="Q1311" t="s">
-        <v>4987</v>
+        <v>3646</v>
       </c>
     </row>
     <row r="1312" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1312" s="1" t="s">
-        <v>3645</v>
+        <v>3647</v>
       </c>
       <c r="C1312" t="s">
         <v>3495</v>
@@ -54717,12 +54720,12 @@
         <v>5549</v>
       </c>
       <c r="Q1312" t="s">
-        <v>3646</v>
+        <v>4988</v>
       </c>
     </row>
     <row r="1313" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1313" s="1" t="s">
-        <v>3647</v>
+        <v>3648</v>
       </c>
       <c r="C1313" t="s">
         <v>3495</v>
@@ -54737,12 +54740,12 @@
         <v>5549</v>
       </c>
       <c r="Q1313" t="s">
-        <v>4988</v>
+        <v>4989</v>
       </c>
     </row>
     <row r="1314" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1314" s="1" t="s">
-        <v>3648</v>
+        <v>3649</v>
       </c>
       <c r="C1314" t="s">
         <v>3495</v>
@@ -54757,12 +54760,12 @@
         <v>5549</v>
       </c>
       <c r="Q1314" t="s">
-        <v>4989</v>
+        <v>3650</v>
       </c>
     </row>
     <row r="1315" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1315" s="1" t="s">
-        <v>3649</v>
+        <v>3651</v>
       </c>
       <c r="C1315" t="s">
         <v>3495</v>
@@ -54777,12 +54780,12 @@
         <v>5549</v>
       </c>
       <c r="Q1315" t="s">
-        <v>3650</v>
+        <v>3652</v>
       </c>
     </row>
     <row r="1316" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1316" s="1" t="s">
-        <v>3651</v>
+        <v>3653</v>
       </c>
       <c r="C1316" t="s">
         <v>3495</v>
@@ -54797,12 +54800,12 @@
         <v>5549</v>
       </c>
       <c r="Q1316" t="s">
-        <v>3652</v>
+        <v>3654</v>
       </c>
     </row>
     <row r="1317" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1317" s="1" t="s">
-        <v>3653</v>
+        <v>3655</v>
       </c>
       <c r="C1317" t="s">
         <v>3495</v>
@@ -54817,12 +54820,12 @@
         <v>5549</v>
       </c>
       <c r="Q1317" t="s">
-        <v>3654</v>
+        <v>3656</v>
       </c>
     </row>
     <row r="1318" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1318" s="1" t="s">
-        <v>3655</v>
+        <v>3657</v>
       </c>
       <c r="C1318" t="s">
         <v>3495</v>
@@ -54837,12 +54840,12 @@
         <v>5549</v>
       </c>
       <c r="Q1318" t="s">
-        <v>3656</v>
+        <v>4990</v>
       </c>
     </row>
     <row r="1319" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1319" s="1" t="s">
-        <v>3657</v>
+        <v>3658</v>
       </c>
       <c r="C1319" t="s">
         <v>3495</v>
@@ -54857,12 +54860,12 @@
         <v>5549</v>
       </c>
       <c r="Q1319" t="s">
-        <v>4990</v>
+        <v>3659</v>
       </c>
     </row>
     <row r="1320" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1320" s="1" t="s">
-        <v>3658</v>
+        <v>3660</v>
       </c>
       <c r="C1320" t="s">
         <v>3495</v>
@@ -54877,12 +54880,12 @@
         <v>5549</v>
       </c>
       <c r="Q1320" t="s">
-        <v>3659</v>
+        <v>3661</v>
       </c>
     </row>
     <row r="1321" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1321" s="1" t="s">
-        <v>3660</v>
+        <v>3662</v>
       </c>
       <c r="C1321" t="s">
         <v>3495</v>
@@ -54897,12 +54900,12 @@
         <v>5549</v>
       </c>
       <c r="Q1321" t="s">
-        <v>3661</v>
+        <v>4991</v>
       </c>
     </row>
     <row r="1322" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1322" s="1" t="s">
-        <v>3662</v>
+        <v>3663</v>
       </c>
       <c r="C1322" t="s">
         <v>3495</v>
@@ -54917,12 +54920,12 @@
         <v>5549</v>
       </c>
       <c r="Q1322" t="s">
-        <v>4991</v>
+        <v>3664</v>
       </c>
     </row>
     <row r="1323" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1323" s="1" t="s">
-        <v>3663</v>
+        <v>3665</v>
       </c>
       <c r="C1323" t="s">
         <v>3495</v>
@@ -54937,12 +54940,12 @@
         <v>5549</v>
       </c>
       <c r="Q1323" t="s">
-        <v>3664</v>
+        <v>4992</v>
       </c>
     </row>
     <row r="1324" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1324" s="1" t="s">
-        <v>3665</v>
+        <v>3666</v>
       </c>
       <c r="C1324" t="s">
         <v>3495</v>
@@ -54957,12 +54960,12 @@
         <v>5549</v>
       </c>
       <c r="Q1324" t="s">
-        <v>4992</v>
+        <v>3667</v>
       </c>
     </row>
     <row r="1325" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1325" s="1" t="s">
-        <v>3666</v>
+        <v>3668</v>
       </c>
       <c r="C1325" t="s">
         <v>3495</v>
@@ -54977,12 +54980,12 @@
         <v>5549</v>
       </c>
       <c r="Q1325" t="s">
-        <v>3667</v>
+        <v>3669</v>
       </c>
     </row>
     <row r="1326" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1326" s="1" t="s">
-        <v>3668</v>
+        <v>3670</v>
       </c>
       <c r="C1326" t="s">
         <v>3495</v>
@@ -54997,12 +55000,12 @@
         <v>5549</v>
       </c>
       <c r="Q1326" t="s">
-        <v>3669</v>
+        <v>3671</v>
       </c>
     </row>
     <row r="1327" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1327" s="1" t="s">
-        <v>3670</v>
+        <v>3672</v>
       </c>
       <c r="C1327" t="s">
         <v>3495</v>
@@ -55017,12 +55020,12 @@
         <v>5549</v>
       </c>
       <c r="Q1327" t="s">
-        <v>3671</v>
+        <v>3673</v>
       </c>
     </row>
     <row r="1328" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1328" s="1" t="s">
-        <v>3672</v>
+        <v>3674</v>
       </c>
       <c r="C1328" t="s">
         <v>3495</v>
@@ -55037,12 +55040,12 @@
         <v>5549</v>
       </c>
       <c r="Q1328" t="s">
-        <v>3673</v>
+        <v>4993</v>
       </c>
     </row>
     <row r="1329" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1329" s="1" t="s">
-        <v>3674</v>
+        <v>3675</v>
       </c>
       <c r="C1329" t="s">
         <v>3495</v>
@@ -55057,12 +55060,12 @@
         <v>5549</v>
       </c>
       <c r="Q1329" t="s">
-        <v>4993</v>
+        <v>4994</v>
       </c>
     </row>
     <row r="1330" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1330" s="1" t="s">
-        <v>3675</v>
+        <v>3676</v>
       </c>
       <c r="C1330" t="s">
         <v>3495</v>
@@ -55077,12 +55080,12 @@
         <v>5549</v>
       </c>
       <c r="Q1330" t="s">
-        <v>4994</v>
+        <v>4995</v>
       </c>
     </row>
     <row r="1331" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1331" s="1" t="s">
-        <v>3676</v>
+        <v>3677</v>
       </c>
       <c r="C1331" t="s">
         <v>3495</v>
@@ -55097,12 +55100,12 @@
         <v>5549</v>
       </c>
       <c r="Q1331" t="s">
-        <v>4995</v>
+        <v>4996</v>
       </c>
     </row>
     <row r="1332" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1332" s="1" t="s">
-        <v>3677</v>
+        <v>3678</v>
       </c>
       <c r="C1332" t="s">
         <v>3495</v>
@@ -55117,12 +55120,12 @@
         <v>5549</v>
       </c>
       <c r="Q1332" t="s">
-        <v>4996</v>
+        <v>4997</v>
       </c>
     </row>
     <row r="1333" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1333" s="1" t="s">
-        <v>3678</v>
+        <v>3679</v>
       </c>
       <c r="C1333" t="s">
         <v>3495</v>
@@ -55137,12 +55140,12 @@
         <v>5549</v>
       </c>
       <c r="Q1333" t="s">
-        <v>4997</v>
+        <v>3680</v>
       </c>
     </row>
     <row r="1334" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1334" s="1" t="s">
-        <v>3679</v>
+        <v>3681</v>
       </c>
       <c r="C1334" t="s">
         <v>3495</v>
@@ -55157,12 +55160,12 @@
         <v>5549</v>
       </c>
       <c r="Q1334" t="s">
-        <v>3680</v>
+        <v>4606</v>
       </c>
     </row>
     <row r="1335" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1335" s="1" t="s">
-        <v>3681</v>
+        <v>3682</v>
       </c>
       <c r="C1335" t="s">
         <v>3495</v>
@@ -55177,12 +55180,12 @@
         <v>5549</v>
       </c>
       <c r="Q1335" t="s">
-        <v>4606</v>
+        <v>3683</v>
       </c>
     </row>
     <row r="1336" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1336" s="1" t="s">
-        <v>3682</v>
+        <v>6933</v>
       </c>
       <c r="C1336" t="s">
         <v>3495</v>
@@ -55197,12 +55200,12 @@
         <v>5549</v>
       </c>
       <c r="Q1336" t="s">
-        <v>3683</v>
+        <v>6934</v>
       </c>
     </row>
     <row r="1337" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1337" s="1" t="s">
-        <v>6933</v>
+        <v>6935</v>
       </c>
       <c r="C1337" t="s">
         <v>3495</v>
@@ -55217,12 +55220,12 @@
         <v>5549</v>
       </c>
       <c r="Q1337" t="s">
-        <v>6934</v>
+        <v>6936</v>
       </c>
     </row>
     <row r="1338" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1338" s="1" t="s">
-        <v>6935</v>
+        <v>6937</v>
       </c>
       <c r="C1338" t="s">
         <v>3495</v>
@@ -55237,12 +55240,12 @@
         <v>5549</v>
       </c>
       <c r="Q1338" t="s">
-        <v>6936</v>
+        <v>6938</v>
       </c>
     </row>
     <row r="1339" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1339" s="1" t="s">
-        <v>6937</v>
+        <v>6939</v>
       </c>
       <c r="C1339" t="s">
         <v>3495</v>
@@ -55257,12 +55260,12 @@
         <v>5549</v>
       </c>
       <c r="Q1339" t="s">
-        <v>6938</v>
+        <v>6940</v>
       </c>
     </row>
     <row r="1340" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1340" s="1" t="s">
-        <v>6939</v>
+        <v>6941</v>
       </c>
       <c r="C1340" t="s">
         <v>3495</v>
@@ -55277,12 +55280,12 @@
         <v>5549</v>
       </c>
       <c r="Q1340" t="s">
-        <v>6940</v>
+        <v>6942</v>
       </c>
     </row>
     <row r="1341" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1341" s="1" t="s">
-        <v>6941</v>
+        <v>6943</v>
       </c>
       <c r="C1341" t="s">
         <v>3495</v>
@@ -55297,12 +55300,12 @@
         <v>5549</v>
       </c>
       <c r="Q1341" t="s">
-        <v>6942</v>
+        <v>6944</v>
       </c>
     </row>
     <row r="1342" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1342" s="1" t="s">
-        <v>6943</v>
+        <v>6945</v>
       </c>
       <c r="C1342" t="s">
         <v>3495</v>
@@ -55317,12 +55320,12 @@
         <v>5549</v>
       </c>
       <c r="Q1342" t="s">
-        <v>6944</v>
+        <v>6946</v>
       </c>
     </row>
     <row r="1343" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1343" s="1" t="s">
-        <v>6945</v>
+        <v>6947</v>
       </c>
       <c r="C1343" t="s">
         <v>3495</v>
@@ -55337,12 +55340,12 @@
         <v>5549</v>
       </c>
       <c r="Q1343" t="s">
-        <v>6946</v>
+        <v>6948</v>
       </c>
     </row>
     <row r="1344" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1344" s="1" t="s">
-        <v>6947</v>
+        <v>6949</v>
       </c>
       <c r="C1344" t="s">
         <v>3495</v>
@@ -55357,12 +55360,12 @@
         <v>5549</v>
       </c>
       <c r="Q1344" t="s">
-        <v>6948</v>
+        <v>6950</v>
       </c>
     </row>
     <row r="1345" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1345" s="1" t="s">
-        <v>6949</v>
+        <v>6951</v>
       </c>
       <c r="C1345" t="s">
         <v>3495</v>
@@ -55377,12 +55380,12 @@
         <v>5549</v>
       </c>
       <c r="Q1345" t="s">
-        <v>6950</v>
+        <v>6952</v>
       </c>
     </row>
     <row r="1346" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1346" s="1" t="s">
-        <v>6951</v>
+        <v>6953</v>
       </c>
       <c r="C1346" t="s">
         <v>3495</v>
@@ -55397,31 +55400,11 @@
         <v>5549</v>
       </c>
       <c r="Q1346" t="s">
-        <v>6952</v>
-      </c>
-    </row>
-    <row r="1347" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B1347" s="1" t="s">
-        <v>6953</v>
-      </c>
-      <c r="C1347" t="s">
-        <v>3495</v>
-      </c>
-      <c r="D1347" s="1">
-        <v>68000</v>
-      </c>
-      <c r="E1347" t="s">
-        <v>2426</v>
-      </c>
-      <c r="L1347" t="s">
-        <v>5549</v>
-      </c>
-      <c r="Q1347" t="s">
         <v>6954</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:R1347"/>
+  <autoFilter ref="B1:R1346"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -55429,10 +55412,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Q433"/>
+  <dimension ref="B1:Q434"/>
   <sheetViews>
-    <sheetView topLeftCell="A421" workbookViewId="0">
-      <selection activeCell="A431" sqref="A431:XFD433"/>
+    <sheetView tabSelected="1" topLeftCell="A421" workbookViewId="0">
+      <selection activeCell="E433" sqref="E433"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -64398,6 +64381,23 @@
       </c>
       <c r="Q433" t="s">
         <v>6911</v>
+      </c>
+    </row>
+    <row r="434" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B434" s="1" t="s">
+        <v>3491</v>
+      </c>
+      <c r="C434" t="s">
+        <v>3492</v>
+      </c>
+      <c r="D434" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L434" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q434" t="s">
+        <v>3493</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added cloak(works) and cloud9(crashes) drivers
</commit_message>
<xml_diff>
--- a/compatibility_list.xlsx
+++ b/compatibility_list.xlsx
@@ -25879,10 +25879,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Q1358"/>
+  <dimension ref="B1:Q1356"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1114" workbookViewId="0">
-      <selection activeCell="B1123" sqref="B1123"/>
+    <sheetView tabSelected="1" topLeftCell="A1328" workbookViewId="0">
+      <selection activeCell="A1338" sqref="A1338:XFD1338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -55222,44 +55222,59 @@
     </row>
     <row r="1338" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1338" s="1" t="s">
-        <v>2680</v>
+        <v>2691</v>
       </c>
       <c r="C1338" t="s">
-        <v>2681</v>
-      </c>
-      <c r="D1338" s="1" t="s">
-        <v>351</v>
+        <v>2689</v>
+      </c>
+      <c r="D1338" s="1">
+        <v>68010</v>
       </c>
       <c r="E1338" t="s">
         <v>351</v>
       </c>
       <c r="L1338" t="s">
-        <v>2538</v>
+        <v>5238</v>
+      </c>
+      <c r="M1338" t="s">
+        <v>2534</v>
+      </c>
+      <c r="N1338" t="s">
+        <v>3889</v>
       </c>
       <c r="Q1338" t="s">
-        <v>2682</v>
+        <v>4870</v>
       </c>
     </row>
     <row r="1339" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1339" s="1" t="s">
-        <v>2683</v>
+        <v>2688</v>
       </c>
       <c r="C1339" t="s">
-        <v>2684</v>
-      </c>
-      <c r="D1339" s="1" t="s">
+        <v>2689</v>
+      </c>
+      <c r="D1339" s="1">
+        <v>68010</v>
+      </c>
+      <c r="E1339" t="s">
         <v>351</v>
       </c>
       <c r="L1339" t="s">
-        <v>2538</v>
+        <v>5238</v>
+      </c>
+      <c r="M1339" t="s">
+        <v>2534</v>
+      </c>
+      <c r="N1339" t="s">
+        <v>3889</v>
       </c>
       <c r="Q1339" t="s">
-        <v>2685</v>
+        <v>4867</v>
       </c>
     </row>
     <row r="1340" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1340" s="1" t="s">
-        <v>2691</v>
+        <v>2690</v>
       </c>
       <c r="C1340" t="s">
         <v>2689</v>
@@ -55280,12 +55295,12 @@
         <v>3889</v>
       </c>
       <c r="Q1340" t="s">
-        <v>4870</v>
+        <v>4868</v>
       </c>
     </row>
     <row r="1341" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1341" s="1" t="s">
-        <v>2688</v>
+        <v>6487</v>
       </c>
       <c r="C1341" t="s">
         <v>2689</v>
@@ -55306,12 +55321,12 @@
         <v>3889</v>
       </c>
       <c r="Q1341" t="s">
-        <v>4867</v>
+        <v>4869</v>
       </c>
     </row>
     <row r="1342" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1342" s="1" t="s">
-        <v>2690</v>
+        <v>6488</v>
       </c>
       <c r="C1342" t="s">
         <v>2689</v>
@@ -55332,12 +55347,12 @@
         <v>3889</v>
       </c>
       <c r="Q1342" t="s">
-        <v>4868</v>
+        <v>6489</v>
       </c>
     </row>
     <row r="1343" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1343" s="1" t="s">
-        <v>6487</v>
+        <v>2692</v>
       </c>
       <c r="C1343" t="s">
         <v>2689</v>
@@ -55358,12 +55373,12 @@
         <v>3889</v>
       </c>
       <c r="Q1343" t="s">
-        <v>4869</v>
+        <v>4871</v>
       </c>
     </row>
     <row r="1344" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1344" s="1" t="s">
-        <v>6488</v>
+        <v>2693</v>
       </c>
       <c r="C1344" t="s">
         <v>2689</v>
@@ -55384,12 +55399,12 @@
         <v>3889</v>
       </c>
       <c r="Q1344" t="s">
-        <v>6489</v>
+        <v>4872</v>
       </c>
     </row>
     <row r="1345" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1345" s="1" t="s">
-        <v>2692</v>
+        <v>2694</v>
       </c>
       <c r="C1345" t="s">
         <v>2689</v>
@@ -55410,12 +55425,12 @@
         <v>3889</v>
       </c>
       <c r="Q1345" t="s">
-        <v>4871</v>
+        <v>4873</v>
       </c>
     </row>
     <row r="1346" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1346" s="1" t="s">
-        <v>2693</v>
+        <v>2695</v>
       </c>
       <c r="C1346" t="s">
         <v>2689</v>
@@ -55436,12 +55451,12 @@
         <v>3889</v>
       </c>
       <c r="Q1346" t="s">
-        <v>4872</v>
+        <v>4874</v>
       </c>
     </row>
     <row r="1347" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1347" s="1" t="s">
-        <v>2694</v>
+        <v>6490</v>
       </c>
       <c r="C1347" t="s">
         <v>2689</v>
@@ -55462,12 +55477,12 @@
         <v>3889</v>
       </c>
       <c r="Q1347" t="s">
-        <v>4873</v>
+        <v>6491</v>
       </c>
     </row>
     <row r="1348" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1348" s="1" t="s">
-        <v>2695</v>
+        <v>2696</v>
       </c>
       <c r="C1348" t="s">
         <v>2689</v>
@@ -55488,12 +55503,12 @@
         <v>3889</v>
       </c>
       <c r="Q1348" t="s">
-        <v>4874</v>
+        <v>4875</v>
       </c>
     </row>
     <row r="1349" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1349" s="1" t="s">
-        <v>6490</v>
+        <v>2697</v>
       </c>
       <c r="C1349" t="s">
         <v>2689</v>
@@ -55514,18 +55529,18 @@
         <v>3889</v>
       </c>
       <c r="Q1349" t="s">
-        <v>6491</v>
+        <v>4876</v>
       </c>
     </row>
     <row r="1350" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1350" s="1" t="s">
-        <v>2696</v>
+        <v>2698</v>
       </c>
       <c r="C1350" t="s">
-        <v>2689</v>
-      </c>
-      <c r="D1350" s="1">
-        <v>68010</v>
+        <v>2699</v>
+      </c>
+      <c r="D1350" s="1" t="s">
+        <v>2700</v>
       </c>
       <c r="E1350" t="s">
         <v>351</v>
@@ -55534,24 +55549,24 @@
         <v>5238</v>
       </c>
       <c r="M1350" t="s">
-        <v>2534</v>
+        <v>2538</v>
       </c>
       <c r="N1350" t="s">
         <v>3889</v>
       </c>
       <c r="Q1350" t="s">
-        <v>4875</v>
+        <v>4877</v>
       </c>
     </row>
     <row r="1351" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1351" s="1" t="s">
-        <v>2697</v>
+        <v>2701</v>
       </c>
       <c r="C1351" t="s">
-        <v>2689</v>
-      </c>
-      <c r="D1351" s="1">
-        <v>68010</v>
+        <v>2699</v>
+      </c>
+      <c r="D1351" s="1" t="s">
+        <v>2700</v>
       </c>
       <c r="E1351" t="s">
         <v>351</v>
@@ -55560,18 +55575,15 @@
         <v>5238</v>
       </c>
       <c r="M1351" t="s">
-        <v>2534</v>
-      </c>
-      <c r="N1351" t="s">
-        <v>3889</v>
+        <v>2538</v>
       </c>
       <c r="Q1351" t="s">
-        <v>4876</v>
+        <v>4416</v>
       </c>
     </row>
     <row r="1352" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1352" s="1" t="s">
-        <v>2698</v>
+        <v>2702</v>
       </c>
       <c r="C1352" t="s">
         <v>2699</v>
@@ -55588,16 +55600,13 @@
       <c r="M1352" t="s">
         <v>2538</v>
       </c>
-      <c r="N1352" t="s">
-        <v>3889</v>
-      </c>
       <c r="Q1352" t="s">
-        <v>4877</v>
+        <v>4417</v>
       </c>
     </row>
     <row r="1353" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1353" s="1" t="s">
-        <v>2701</v>
+        <v>6492</v>
       </c>
       <c r="C1353" t="s">
         <v>2699</v>
@@ -55614,13 +55623,16 @@
       <c r="M1353" t="s">
         <v>2538</v>
       </c>
+      <c r="N1353" t="s">
+        <v>3889</v>
+      </c>
       <c r="Q1353" t="s">
-        <v>4416</v>
+        <v>4878</v>
       </c>
     </row>
     <row r="1354" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1354" s="1" t="s">
-        <v>2702</v>
+        <v>2703</v>
       </c>
       <c r="C1354" t="s">
         <v>2699</v>
@@ -55637,13 +55649,16 @@
       <c r="M1354" t="s">
         <v>2538</v>
       </c>
+      <c r="N1354" t="s">
+        <v>3889</v>
+      </c>
       <c r="Q1354" t="s">
-        <v>4417</v>
+        <v>4879</v>
       </c>
     </row>
     <row r="1355" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1355" s="1" t="s">
-        <v>6492</v>
+        <v>2704</v>
       </c>
       <c r="C1355" t="s">
         <v>2699</v>
@@ -55664,12 +55679,12 @@
         <v>3889</v>
       </c>
       <c r="Q1355" t="s">
-        <v>4878</v>
+        <v>4880</v>
       </c>
     </row>
     <row r="1356" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1356" s="1" t="s">
-        <v>2703</v>
+        <v>2705</v>
       </c>
       <c r="C1356" t="s">
         <v>2699</v>
@@ -55690,58 +55705,6 @@
         <v>3889</v>
       </c>
       <c r="Q1356" t="s">
-        <v>4879</v>
-      </c>
-    </row>
-    <row r="1357" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B1357" s="1" t="s">
-        <v>2704</v>
-      </c>
-      <c r="C1357" t="s">
-        <v>2699</v>
-      </c>
-      <c r="D1357" s="1" t="s">
-        <v>2700</v>
-      </c>
-      <c r="E1357" t="s">
-        <v>351</v>
-      </c>
-      <c r="L1357" t="s">
-        <v>5238</v>
-      </c>
-      <c r="M1357" t="s">
-        <v>2538</v>
-      </c>
-      <c r="N1357" t="s">
-        <v>3889</v>
-      </c>
-      <c r="Q1357" t="s">
-        <v>4880</v>
-      </c>
-    </row>
-    <row r="1358" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B1358" s="1" t="s">
-        <v>2705</v>
-      </c>
-      <c r="C1358" t="s">
-        <v>2699</v>
-      </c>
-      <c r="D1358" s="1" t="s">
-        <v>2700</v>
-      </c>
-      <c r="E1358" t="s">
-        <v>351</v>
-      </c>
-      <c r="L1358" t="s">
-        <v>5238</v>
-      </c>
-      <c r="M1358" t="s">
-        <v>2538</v>
-      </c>
-      <c r="N1358" t="s">
-        <v>3889</v>
-      </c>
-      <c r="Q1358" t="s">
         <v>4881</v>
       </c>
     </row>
@@ -64947,10 +64910,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R1161"/>
+  <dimension ref="B1:R1163"/>
   <sheetViews>
     <sheetView topLeftCell="A1131" workbookViewId="0">
-      <selection activeCell="A1154" sqref="A1154:XFD1154"/>
+      <selection activeCell="A1163" sqref="A1163:XFD1163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -89788,6 +89751,43 @@
         <v>4535</v>
       </c>
     </row>
+    <row r="1162" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B1162" s="1" t="s">
+        <v>2680</v>
+      </c>
+      <c r="C1162" t="s">
+        <v>2681</v>
+      </c>
+      <c r="D1162" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="E1162" t="s">
+        <v>351</v>
+      </c>
+      <c r="L1162" t="s">
+        <v>2538</v>
+      </c>
+      <c r="Q1162" t="s">
+        <v>2682</v>
+      </c>
+    </row>
+    <row r="1163" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B1163" s="1" t="s">
+        <v>2683</v>
+      </c>
+      <c r="C1163" t="s">
+        <v>2684</v>
+      </c>
+      <c r="D1163" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="L1163" t="s">
+        <v>2538</v>
+      </c>
+      <c r="Q1163" t="s">
+        <v>2685</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
added gotya full working driver
</commit_message>
<xml_diff>
--- a/compatibility_list.xlsx
+++ b/compatibility_list.xlsx
@@ -21,9 +21,9 @@
     <sheet name="To Check" sheetId="13" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">WIP!$B$1:$R$1318</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">WIP!$B$1:$R$1316</definedName>
     <definedName name="DETAILS" localSheetId="4">WIP!#REF!</definedName>
-    <definedName name="DETAILS_1" localSheetId="4">WIP!$B$1:$Q$1318</definedName>
+    <definedName name="DETAILS_1" localSheetId="4">WIP!$B$1:$Q$1316</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25879,10 +25879,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Q1339"/>
+  <dimension ref="B1:Q1337"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A951" workbookViewId="0">
-      <selection activeCell="C961" sqref="C961"/>
+    <sheetView tabSelected="1" topLeftCell="A1161" workbookViewId="0">
+      <selection activeCell="B1170" sqref="B1170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -51891,64 +51891,67 @@
     </row>
     <row r="1171" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1171" s="1" t="s">
-        <v>6912</v>
+        <v>6914</v>
       </c>
       <c r="C1171" t="s">
-        <v>3478</v>
+        <v>6915</v>
       </c>
       <c r="D1171" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1171" t="s">
+        <v>2</v>
+      </c>
       <c r="L1171" t="s">
-        <v>352</v>
+        <v>5238</v>
       </c>
       <c r="Q1171" t="s">
-        <v>6913</v>
+        <v>6916</v>
       </c>
     </row>
     <row r="1172" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1172" s="1" t="s">
-        <v>3477</v>
+        <v>6917</v>
       </c>
       <c r="C1172" t="s">
-        <v>3478</v>
+        <v>6915</v>
       </c>
       <c r="D1172" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1172" t="s">
+        <v>2</v>
+      </c>
       <c r="L1172" t="s">
-        <v>352</v>
+        <v>5238</v>
       </c>
       <c r="Q1172" t="s">
-        <v>4586</v>
+        <v>6918</v>
       </c>
     </row>
     <row r="1173" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1173" s="1" t="s">
-        <v>6914</v>
+        <v>6919</v>
       </c>
       <c r="C1173" t="s">
-        <v>6915</v>
+        <v>6920</v>
       </c>
       <c r="D1173" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1173" t="s">
-        <v>2</v>
-      </c>
       <c r="L1173" t="s">
-        <v>5238</v>
+        <v>55</v>
       </c>
       <c r="Q1173" t="s">
-        <v>6916</v>
+        <v>6921</v>
       </c>
     </row>
     <row r="1174" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1174" s="1" t="s">
-        <v>6917</v>
+        <v>6922</v>
       </c>
       <c r="C1174" t="s">
-        <v>6915</v>
+        <v>6920</v>
       </c>
       <c r="D1174" s="1" t="s">
         <v>2</v>
@@ -51956,16 +51959,22 @@
       <c r="E1174" t="s">
         <v>2</v>
       </c>
+      <c r="F1174" t="s">
+        <v>2426</v>
+      </c>
       <c r="L1174" t="s">
-        <v>5238</v>
+        <v>542</v>
+      </c>
+      <c r="M1174" t="s">
+        <v>55</v>
       </c>
       <c r="Q1174" t="s">
-        <v>6918</v>
+        <v>6923</v>
       </c>
     </row>
     <row r="1175" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1175" s="1" t="s">
-        <v>6919</v>
+        <v>6924</v>
       </c>
       <c r="C1175" t="s">
         <v>6920</v>
@@ -51973,85 +51982,82 @@
       <c r="D1175" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1175" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1175" t="s">
+        <v>2426</v>
+      </c>
       <c r="L1175" t="s">
+        <v>542</v>
+      </c>
+      <c r="M1175" t="s">
         <v>55</v>
       </c>
       <c r="Q1175" t="s">
-        <v>6921</v>
+        <v>6925</v>
       </c>
     </row>
     <row r="1176" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1176" s="1" t="s">
-        <v>6922</v>
+        <v>6926</v>
       </c>
       <c r="C1176" t="s">
-        <v>6920</v>
-      </c>
-      <c r="D1176" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1176" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1176" t="s">
-        <v>2426</v>
+        <v>6927</v>
+      </c>
+      <c r="D1176" s="1">
+        <v>68000</v>
       </c>
       <c r="L1176" t="s">
-        <v>542</v>
-      </c>
-      <c r="M1176" t="s">
-        <v>55</v>
+        <v>1687</v>
       </c>
       <c r="Q1176" t="s">
-        <v>6923</v>
+        <v>6928</v>
       </c>
     </row>
     <row r="1177" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1177" s="1" t="s">
-        <v>6924</v>
+        <v>3494</v>
       </c>
       <c r="C1177" t="s">
-        <v>6920</v>
-      </c>
-      <c r="D1177" s="1" t="s">
-        <v>2</v>
+        <v>3495</v>
+      </c>
+      <c r="D1177" s="1">
+        <v>68000</v>
       </c>
       <c r="E1177" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1177" t="s">
         <v>2426</v>
       </c>
       <c r="L1177" t="s">
-        <v>542</v>
-      </c>
-      <c r="M1177" t="s">
-        <v>55</v>
+        <v>5549</v>
       </c>
       <c r="Q1177" t="s">
-        <v>6925</v>
+        <v>3496</v>
       </c>
     </row>
     <row r="1178" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1178" s="1" t="s">
-        <v>6926</v>
+        <v>3497</v>
       </c>
       <c r="C1178" t="s">
-        <v>6927</v>
+        <v>3495</v>
       </c>
       <c r="D1178" s="1">
         <v>68000</v>
       </c>
+      <c r="E1178" t="s">
+        <v>2426</v>
+      </c>
       <c r="L1178" t="s">
-        <v>1687</v>
+        <v>5549</v>
       </c>
       <c r="Q1178" t="s">
-        <v>6928</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="1179" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1179" s="1" t="s">
-        <v>3494</v>
+        <v>3498</v>
       </c>
       <c r="C1179" t="s">
         <v>3495</v>
@@ -52066,12 +52072,12 @@
         <v>5549</v>
       </c>
       <c r="Q1179" t="s">
-        <v>3496</v>
+        <v>3499</v>
       </c>
     </row>
     <row r="1180" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1180" s="1" t="s">
-        <v>3497</v>
+        <v>3500</v>
       </c>
       <c r="C1180" t="s">
         <v>3495</v>
@@ -52086,12 +52092,12 @@
         <v>5549</v>
       </c>
       <c r="Q1180" t="s">
-        <v>4587</v>
+        <v>3501</v>
       </c>
     </row>
     <row r="1181" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1181" s="1" t="s">
-        <v>3498</v>
+        <v>3502</v>
       </c>
       <c r="C1181" t="s">
         <v>3495</v>
@@ -52106,12 +52112,12 @@
         <v>5549</v>
       </c>
       <c r="Q1181" t="s">
-        <v>3499</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="1182" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1182" s="1" t="s">
-        <v>3500</v>
+        <v>3504</v>
       </c>
       <c r="C1182" t="s">
         <v>3495</v>
@@ -52126,12 +52132,12 @@
         <v>5549</v>
       </c>
       <c r="Q1182" t="s">
-        <v>3501</v>
+        <v>3505</v>
       </c>
     </row>
     <row r="1183" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1183" s="1" t="s">
-        <v>3502</v>
+        <v>3506</v>
       </c>
       <c r="C1183" t="s">
         <v>3495</v>
@@ -52146,12 +52152,12 @@
         <v>5549</v>
       </c>
       <c r="Q1183" t="s">
-        <v>3503</v>
+        <v>6929</v>
       </c>
     </row>
     <row r="1184" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1184" s="1" t="s">
-        <v>3504</v>
+        <v>6930</v>
       </c>
       <c r="C1184" t="s">
         <v>3495</v>
@@ -52166,12 +52172,12 @@
         <v>5549</v>
       </c>
       <c r="Q1184" t="s">
-        <v>3505</v>
+        <v>6931</v>
       </c>
     </row>
     <row r="1185" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1185" s="1" t="s">
-        <v>3506</v>
+        <v>3507</v>
       </c>
       <c r="C1185" t="s">
         <v>3495</v>
@@ -52186,12 +52192,12 @@
         <v>5549</v>
       </c>
       <c r="Q1185" t="s">
-        <v>6929</v>
+        <v>4952</v>
       </c>
     </row>
     <row r="1186" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1186" s="1" t="s">
-        <v>6930</v>
+        <v>3508</v>
       </c>
       <c r="C1186" t="s">
         <v>3495</v>
@@ -52206,12 +52212,12 @@
         <v>5549</v>
       </c>
       <c r="Q1186" t="s">
-        <v>6931</v>
+        <v>3509</v>
       </c>
     </row>
     <row r="1187" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1187" s="1" t="s">
-        <v>3507</v>
+        <v>3510</v>
       </c>
       <c r="C1187" t="s">
         <v>3495</v>
@@ -52226,12 +52232,12 @@
         <v>5549</v>
       </c>
       <c r="Q1187" t="s">
-        <v>4952</v>
+        <v>3511</v>
       </c>
     </row>
     <row r="1188" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1188" s="1" t="s">
-        <v>3508</v>
+        <v>3512</v>
       </c>
       <c r="C1188" t="s">
         <v>3495</v>
@@ -52246,12 +52252,12 @@
         <v>5549</v>
       </c>
       <c r="Q1188" t="s">
-        <v>3509</v>
+        <v>3513</v>
       </c>
     </row>
     <row r="1189" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1189" s="1" t="s">
-        <v>3510</v>
+        <v>3514</v>
       </c>
       <c r="C1189" t="s">
         <v>3495</v>
@@ -52266,12 +52272,12 @@
         <v>5549</v>
       </c>
       <c r="Q1189" t="s">
-        <v>3511</v>
+        <v>3515</v>
       </c>
     </row>
     <row r="1190" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1190" s="1" t="s">
-        <v>3512</v>
+        <v>3516</v>
       </c>
       <c r="C1190" t="s">
         <v>3495</v>
@@ -52286,12 +52292,12 @@
         <v>5549</v>
       </c>
       <c r="Q1190" t="s">
-        <v>3513</v>
+        <v>3517</v>
       </c>
     </row>
     <row r="1191" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1191" s="1" t="s">
-        <v>3514</v>
+        <v>3518</v>
       </c>
       <c r="C1191" t="s">
         <v>3495</v>
@@ -52306,12 +52312,12 @@
         <v>5549</v>
       </c>
       <c r="Q1191" t="s">
-        <v>3515</v>
+        <v>4953</v>
       </c>
     </row>
     <row r="1192" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1192" s="1" t="s">
-        <v>3516</v>
+        <v>3519</v>
       </c>
       <c r="C1192" t="s">
         <v>3495</v>
@@ -52326,12 +52332,12 @@
         <v>5549</v>
       </c>
       <c r="Q1192" t="s">
-        <v>3517</v>
+        <v>4954</v>
       </c>
     </row>
     <row r="1193" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1193" s="1" t="s">
-        <v>3518</v>
+        <v>3520</v>
       </c>
       <c r="C1193" t="s">
         <v>3495</v>
@@ -52346,12 +52352,12 @@
         <v>5549</v>
       </c>
       <c r="Q1193" t="s">
-        <v>4953</v>
+        <v>3521</v>
       </c>
     </row>
     <row r="1194" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1194" s="1" t="s">
-        <v>3519</v>
+        <v>3522</v>
       </c>
       <c r="C1194" t="s">
         <v>3495</v>
@@ -52366,12 +52372,12 @@
         <v>5549</v>
       </c>
       <c r="Q1194" t="s">
-        <v>4954</v>
+        <v>3523</v>
       </c>
     </row>
     <row r="1195" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1195" s="1" t="s">
-        <v>3520</v>
+        <v>3524</v>
       </c>
       <c r="C1195" t="s">
         <v>3495</v>
@@ -52386,12 +52392,12 @@
         <v>5549</v>
       </c>
       <c r="Q1195" t="s">
-        <v>3521</v>
+        <v>3525</v>
       </c>
     </row>
     <row r="1196" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1196" s="1" t="s">
-        <v>3522</v>
+        <v>3526</v>
       </c>
       <c r="C1196" t="s">
         <v>3495</v>
@@ -52406,12 +52412,12 @@
         <v>5549</v>
       </c>
       <c r="Q1196" t="s">
-        <v>3523</v>
+        <v>3527</v>
       </c>
     </row>
     <row r="1197" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1197" s="1" t="s">
-        <v>3524</v>
+        <v>3528</v>
       </c>
       <c r="C1197" t="s">
         <v>3495</v>
@@ -52426,12 +52432,12 @@
         <v>5549</v>
       </c>
       <c r="Q1197" t="s">
-        <v>3525</v>
+        <v>3529</v>
       </c>
     </row>
     <row r="1198" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1198" s="1" t="s">
-        <v>3526</v>
+        <v>3530</v>
       </c>
       <c r="C1198" t="s">
         <v>3495</v>
@@ -52446,12 +52452,12 @@
         <v>5549</v>
       </c>
       <c r="Q1198" t="s">
-        <v>3527</v>
+        <v>3531</v>
       </c>
     </row>
     <row r="1199" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1199" s="1" t="s">
-        <v>3528</v>
+        <v>3532</v>
       </c>
       <c r="C1199" t="s">
         <v>3495</v>
@@ -52466,12 +52472,12 @@
         <v>5549</v>
       </c>
       <c r="Q1199" t="s">
-        <v>3529</v>
+        <v>4955</v>
       </c>
     </row>
     <row r="1200" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1200" s="1" t="s">
-        <v>3530</v>
+        <v>3533</v>
       </c>
       <c r="C1200" t="s">
         <v>3495</v>
@@ -52486,12 +52492,12 @@
         <v>5549</v>
       </c>
       <c r="Q1200" t="s">
-        <v>3531</v>
+        <v>3534</v>
       </c>
     </row>
     <row r="1201" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1201" s="1" t="s">
-        <v>3532</v>
+        <v>3535</v>
       </c>
       <c r="C1201" t="s">
         <v>3495</v>
@@ -52506,12 +52512,12 @@
         <v>5549</v>
       </c>
       <c r="Q1201" t="s">
-        <v>4955</v>
+        <v>3536</v>
       </c>
     </row>
     <row r="1202" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1202" s="1" t="s">
-        <v>3533</v>
+        <v>3537</v>
       </c>
       <c r="C1202" t="s">
         <v>3495</v>
@@ -52526,12 +52532,12 @@
         <v>5549</v>
       </c>
       <c r="Q1202" t="s">
-        <v>3534</v>
+        <v>3538</v>
       </c>
     </row>
     <row r="1203" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1203" s="1" t="s">
-        <v>3535</v>
+        <v>3539</v>
       </c>
       <c r="C1203" t="s">
         <v>3495</v>
@@ -52546,12 +52552,12 @@
         <v>5549</v>
       </c>
       <c r="Q1203" t="s">
-        <v>3536</v>
+        <v>4956</v>
       </c>
     </row>
     <row r="1204" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1204" s="1" t="s">
-        <v>3537</v>
+        <v>3540</v>
       </c>
       <c r="C1204" t="s">
         <v>3495</v>
@@ -52566,12 +52572,12 @@
         <v>5549</v>
       </c>
       <c r="Q1204" t="s">
-        <v>3538</v>
+        <v>4588</v>
       </c>
     </row>
     <row r="1205" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1205" s="1" t="s">
-        <v>3539</v>
+        <v>3541</v>
       </c>
       <c r="C1205" t="s">
         <v>3495</v>
@@ -52586,12 +52592,12 @@
         <v>5549</v>
       </c>
       <c r="Q1205" t="s">
-        <v>4956</v>
+        <v>4589</v>
       </c>
     </row>
     <row r="1206" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1206" s="1" t="s">
-        <v>3540</v>
+        <v>3542</v>
       </c>
       <c r="C1206" t="s">
         <v>3495</v>
@@ -52606,12 +52612,12 @@
         <v>5549</v>
       </c>
       <c r="Q1206" t="s">
-        <v>4588</v>
+        <v>3543</v>
       </c>
     </row>
     <row r="1207" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1207" s="1" t="s">
-        <v>3541</v>
+        <v>3544</v>
       </c>
       <c r="C1207" t="s">
         <v>3495</v>
@@ -52626,12 +52632,12 @@
         <v>5549</v>
       </c>
       <c r="Q1207" t="s">
-        <v>4589</v>
+        <v>3545</v>
       </c>
     </row>
     <row r="1208" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1208" s="1" t="s">
-        <v>3542</v>
+        <v>3546</v>
       </c>
       <c r="C1208" t="s">
         <v>3495</v>
@@ -52646,12 +52652,12 @@
         <v>5549</v>
       </c>
       <c r="Q1208" t="s">
-        <v>3543</v>
+        <v>4957</v>
       </c>
     </row>
     <row r="1209" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1209" s="1" t="s">
-        <v>3544</v>
+        <v>3547</v>
       </c>
       <c r="C1209" t="s">
         <v>3495</v>
@@ -52666,12 +52672,12 @@
         <v>5549</v>
       </c>
       <c r="Q1209" t="s">
-        <v>3545</v>
+        <v>3548</v>
       </c>
     </row>
     <row r="1210" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1210" s="1" t="s">
-        <v>3546</v>
+        <v>3549</v>
       </c>
       <c r="C1210" t="s">
         <v>3495</v>
@@ -52686,12 +52692,12 @@
         <v>5549</v>
       </c>
       <c r="Q1210" t="s">
-        <v>4957</v>
+        <v>4590</v>
       </c>
     </row>
     <row r="1211" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1211" s="1" t="s">
-        <v>3547</v>
+        <v>3550</v>
       </c>
       <c r="C1211" t="s">
         <v>3495</v>
@@ -52706,12 +52712,12 @@
         <v>5549</v>
       </c>
       <c r="Q1211" t="s">
-        <v>3548</v>
+        <v>3551</v>
       </c>
     </row>
     <row r="1212" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1212" s="1" t="s">
-        <v>3549</v>
+        <v>3552</v>
       </c>
       <c r="C1212" t="s">
         <v>3495</v>
@@ -52726,12 +52732,12 @@
         <v>5549</v>
       </c>
       <c r="Q1212" t="s">
-        <v>4590</v>
+        <v>3553</v>
       </c>
     </row>
     <row r="1213" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1213" s="1" t="s">
-        <v>3550</v>
+        <v>3554</v>
       </c>
       <c r="C1213" t="s">
         <v>3495</v>
@@ -52746,12 +52752,12 @@
         <v>5549</v>
       </c>
       <c r="Q1213" t="s">
-        <v>3551</v>
+        <v>4958</v>
       </c>
     </row>
     <row r="1214" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1214" s="1" t="s">
-        <v>3552</v>
+        <v>3555</v>
       </c>
       <c r="C1214" t="s">
         <v>3495</v>
@@ -52766,12 +52772,12 @@
         <v>5549</v>
       </c>
       <c r="Q1214" t="s">
-        <v>3553</v>
+        <v>4591</v>
       </c>
     </row>
     <row r="1215" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1215" s="1" t="s">
-        <v>3554</v>
+        <v>3556</v>
       </c>
       <c r="C1215" t="s">
         <v>3495</v>
@@ -52786,12 +52792,12 @@
         <v>5549</v>
       </c>
       <c r="Q1215" t="s">
-        <v>4958</v>
+        <v>3557</v>
       </c>
     </row>
     <row r="1216" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1216" s="1" t="s">
-        <v>3555</v>
+        <v>3558</v>
       </c>
       <c r="C1216" t="s">
         <v>3495</v>
@@ -52806,12 +52812,12 @@
         <v>5549</v>
       </c>
       <c r="Q1216" t="s">
-        <v>4591</v>
+        <v>4959</v>
       </c>
     </row>
     <row r="1217" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1217" s="1" t="s">
-        <v>3556</v>
+        <v>3559</v>
       </c>
       <c r="C1217" t="s">
         <v>3495</v>
@@ -52826,12 +52832,12 @@
         <v>5549</v>
       </c>
       <c r="Q1217" t="s">
-        <v>3557</v>
+        <v>4592</v>
       </c>
     </row>
     <row r="1218" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1218" s="1" t="s">
-        <v>3558</v>
+        <v>3560</v>
       </c>
       <c r="C1218" t="s">
         <v>3495</v>
@@ -52846,12 +52852,12 @@
         <v>5549</v>
       </c>
       <c r="Q1218" t="s">
-        <v>4959</v>
+        <v>4593</v>
       </c>
     </row>
     <row r="1219" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1219" s="1" t="s">
-        <v>3559</v>
+        <v>3561</v>
       </c>
       <c r="C1219" t="s">
         <v>3495</v>
@@ -52866,12 +52872,12 @@
         <v>5549</v>
       </c>
       <c r="Q1219" t="s">
-        <v>4592</v>
+        <v>4960</v>
       </c>
     </row>
     <row r="1220" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1220" s="1" t="s">
-        <v>3560</v>
+        <v>3562</v>
       </c>
       <c r="C1220" t="s">
         <v>3495</v>
@@ -52886,12 +52892,12 @@
         <v>5549</v>
       </c>
       <c r="Q1220" t="s">
-        <v>4593</v>
+        <v>4594</v>
       </c>
     </row>
     <row r="1221" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1221" s="1" t="s">
-        <v>3561</v>
+        <v>3563</v>
       </c>
       <c r="C1221" t="s">
         <v>3495</v>
@@ -52906,12 +52912,12 @@
         <v>5549</v>
       </c>
       <c r="Q1221" t="s">
-        <v>4960</v>
+        <v>4961</v>
       </c>
     </row>
     <row r="1222" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1222" s="1" t="s">
-        <v>3562</v>
+        <v>3564</v>
       </c>
       <c r="C1222" t="s">
         <v>3495</v>
@@ -52926,12 +52932,12 @@
         <v>5549</v>
       </c>
       <c r="Q1222" t="s">
-        <v>4594</v>
+        <v>4962</v>
       </c>
     </row>
     <row r="1223" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1223" s="1" t="s">
-        <v>3563</v>
+        <v>3565</v>
       </c>
       <c r="C1223" t="s">
         <v>3495</v>
@@ -52946,12 +52952,12 @@
         <v>5549</v>
       </c>
       <c r="Q1223" t="s">
-        <v>4961</v>
+        <v>3566</v>
       </c>
     </row>
     <row r="1224" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1224" s="1" t="s">
-        <v>3564</v>
+        <v>3567</v>
       </c>
       <c r="C1224" t="s">
         <v>3495</v>
@@ -52966,12 +52972,12 @@
         <v>5549</v>
       </c>
       <c r="Q1224" t="s">
-        <v>4962</v>
+        <v>3568</v>
       </c>
     </row>
     <row r="1225" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1225" s="1" t="s">
-        <v>3565</v>
+        <v>3569</v>
       </c>
       <c r="C1225" t="s">
         <v>3495</v>
@@ -52986,12 +52992,12 @@
         <v>5549</v>
       </c>
       <c r="Q1225" t="s">
-        <v>3566</v>
+        <v>3570</v>
       </c>
     </row>
     <row r="1226" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1226" s="1" t="s">
-        <v>3567</v>
+        <v>3571</v>
       </c>
       <c r="C1226" t="s">
         <v>3495</v>
@@ -53006,12 +53012,12 @@
         <v>5549</v>
       </c>
       <c r="Q1226" t="s">
-        <v>3568</v>
+        <v>4595</v>
       </c>
     </row>
     <row r="1227" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1227" s="1" t="s">
-        <v>3569</v>
+        <v>3572</v>
       </c>
       <c r="C1227" t="s">
         <v>3495</v>
@@ -53026,12 +53032,12 @@
         <v>5549</v>
       </c>
       <c r="Q1227" t="s">
-        <v>3570</v>
+        <v>3573</v>
       </c>
     </row>
     <row r="1228" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1228" s="1" t="s">
-        <v>3571</v>
+        <v>3574</v>
       </c>
       <c r="C1228" t="s">
         <v>3495</v>
@@ -53046,12 +53052,12 @@
         <v>5549</v>
       </c>
       <c r="Q1228" t="s">
-        <v>4595</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="1229" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1229" s="1" t="s">
-        <v>3572</v>
+        <v>3576</v>
       </c>
       <c r="C1229" t="s">
         <v>3495</v>
@@ -53066,12 +53072,12 @@
         <v>5549</v>
       </c>
       <c r="Q1229" t="s">
-        <v>3573</v>
+        <v>4963</v>
       </c>
     </row>
     <row r="1230" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1230" s="1" t="s">
-        <v>3574</v>
+        <v>3577</v>
       </c>
       <c r="C1230" t="s">
         <v>3495</v>
@@ -53086,12 +53092,12 @@
         <v>5549</v>
       </c>
       <c r="Q1230" t="s">
-        <v>3575</v>
+        <v>3578</v>
       </c>
     </row>
     <row r="1231" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1231" s="1" t="s">
-        <v>3576</v>
+        <v>3579</v>
       </c>
       <c r="C1231" t="s">
         <v>3495</v>
@@ -53106,12 +53112,12 @@
         <v>5549</v>
       </c>
       <c r="Q1231" t="s">
-        <v>4963</v>
+        <v>4964</v>
       </c>
     </row>
     <row r="1232" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1232" s="1" t="s">
-        <v>3577</v>
+        <v>3580</v>
       </c>
       <c r="C1232" t="s">
         <v>3495</v>
@@ -53126,12 +53132,12 @@
         <v>5549</v>
       </c>
       <c r="Q1232" t="s">
-        <v>3578</v>
+        <v>4965</v>
       </c>
     </row>
     <row r="1233" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1233" s="1" t="s">
-        <v>3579</v>
+        <v>3581</v>
       </c>
       <c r="C1233" t="s">
         <v>3495</v>
@@ -53146,12 +53152,12 @@
         <v>5549</v>
       </c>
       <c r="Q1233" t="s">
-        <v>4964</v>
+        <v>4596</v>
       </c>
     </row>
     <row r="1234" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1234" s="1" t="s">
-        <v>3580</v>
+        <v>3582</v>
       </c>
       <c r="C1234" t="s">
         <v>3495</v>
@@ -53166,12 +53172,12 @@
         <v>5549</v>
       </c>
       <c r="Q1234" t="s">
-        <v>4965</v>
+        <v>4966</v>
       </c>
     </row>
     <row r="1235" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1235" s="1" t="s">
-        <v>3581</v>
+        <v>3583</v>
       </c>
       <c r="C1235" t="s">
         <v>3495</v>
@@ -53186,12 +53192,12 @@
         <v>5549</v>
       </c>
       <c r="Q1235" t="s">
-        <v>4596</v>
+        <v>4597</v>
       </c>
     </row>
     <row r="1236" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1236" s="1" t="s">
-        <v>3582</v>
+        <v>3584</v>
       </c>
       <c r="C1236" t="s">
         <v>3495</v>
@@ -53206,12 +53212,12 @@
         <v>5549</v>
       </c>
       <c r="Q1236" t="s">
-        <v>4966</v>
+        <v>4967</v>
       </c>
     </row>
     <row r="1237" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1237" s="1" t="s">
-        <v>3583</v>
+        <v>3585</v>
       </c>
       <c r="C1237" t="s">
         <v>3495</v>
@@ -53226,12 +53232,12 @@
         <v>5549</v>
       </c>
       <c r="Q1237" t="s">
-        <v>4597</v>
+        <v>3586</v>
       </c>
     </row>
     <row r="1238" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1238" s="1" t="s">
-        <v>3584</v>
+        <v>3587</v>
       </c>
       <c r="C1238" t="s">
         <v>3495</v>
@@ -53246,12 +53252,12 @@
         <v>5549</v>
       </c>
       <c r="Q1238" t="s">
-        <v>4967</v>
+        <v>4598</v>
       </c>
     </row>
     <row r="1239" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1239" s="1" t="s">
-        <v>3585</v>
+        <v>3588</v>
       </c>
       <c r="C1239" t="s">
         <v>3495</v>
@@ -53266,12 +53272,12 @@
         <v>5549</v>
       </c>
       <c r="Q1239" t="s">
-        <v>3586</v>
+        <v>4968</v>
       </c>
     </row>
     <row r="1240" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1240" s="1" t="s">
-        <v>3587</v>
+        <v>3589</v>
       </c>
       <c r="C1240" t="s">
         <v>3495</v>
@@ -53286,12 +53292,12 @@
         <v>5549</v>
       </c>
       <c r="Q1240" t="s">
-        <v>4598</v>
+        <v>3590</v>
       </c>
     </row>
     <row r="1241" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1241" s="1" t="s">
-        <v>3588</v>
+        <v>3591</v>
       </c>
       <c r="C1241" t="s">
         <v>3495</v>
@@ -53306,12 +53312,12 @@
         <v>5549</v>
       </c>
       <c r="Q1241" t="s">
-        <v>4968</v>
+        <v>3592</v>
       </c>
     </row>
     <row r="1242" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1242" s="1" t="s">
-        <v>3589</v>
+        <v>3593</v>
       </c>
       <c r="C1242" t="s">
         <v>3495</v>
@@ -53326,12 +53332,12 @@
         <v>5549</v>
       </c>
       <c r="Q1242" t="s">
-        <v>3590</v>
+        <v>4969</v>
       </c>
     </row>
     <row r="1243" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1243" s="1" t="s">
-        <v>3591</v>
+        <v>3594</v>
       </c>
       <c r="C1243" t="s">
         <v>3495</v>
@@ -53346,12 +53352,12 @@
         <v>5549</v>
       </c>
       <c r="Q1243" t="s">
-        <v>3592</v>
+        <v>3595</v>
       </c>
     </row>
     <row r="1244" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1244" s="1" t="s">
-        <v>3593</v>
+        <v>3596</v>
       </c>
       <c r="C1244" t="s">
         <v>3495</v>
@@ -53366,12 +53372,12 @@
         <v>5549</v>
       </c>
       <c r="Q1244" t="s">
-        <v>4969</v>
+        <v>4970</v>
       </c>
     </row>
     <row r="1245" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1245" s="1" t="s">
-        <v>3594</v>
+        <v>3597</v>
       </c>
       <c r="C1245" t="s">
         <v>3495</v>
@@ -53386,12 +53392,12 @@
         <v>5549</v>
       </c>
       <c r="Q1245" t="s">
-        <v>3595</v>
+        <v>4599</v>
       </c>
     </row>
     <row r="1246" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1246" s="1" t="s">
-        <v>3596</v>
+        <v>3598</v>
       </c>
       <c r="C1246" t="s">
         <v>3495</v>
@@ -53406,12 +53412,12 @@
         <v>5549</v>
       </c>
       <c r="Q1246" t="s">
-        <v>4970</v>
+        <v>4600</v>
       </c>
     </row>
     <row r="1247" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1247" s="1" t="s">
-        <v>3597</v>
+        <v>3599</v>
       </c>
       <c r="C1247" t="s">
         <v>3495</v>
@@ -53426,12 +53432,12 @@
         <v>5549</v>
       </c>
       <c r="Q1247" t="s">
-        <v>4599</v>
+        <v>4971</v>
       </c>
     </row>
     <row r="1248" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1248" s="1" t="s">
-        <v>3598</v>
+        <v>3600</v>
       </c>
       <c r="C1248" t="s">
         <v>3495</v>
@@ -53446,12 +53452,12 @@
         <v>5549</v>
       </c>
       <c r="Q1248" t="s">
-        <v>4600</v>
+        <v>4972</v>
       </c>
     </row>
     <row r="1249" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1249" s="1" t="s">
-        <v>3599</v>
+        <v>3601</v>
       </c>
       <c r="C1249" t="s">
         <v>3495</v>
@@ -53466,12 +53472,12 @@
         <v>5549</v>
       </c>
       <c r="Q1249" t="s">
-        <v>4971</v>
+        <v>3602</v>
       </c>
     </row>
     <row r="1250" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1250" s="1" t="s">
-        <v>3600</v>
+        <v>3603</v>
       </c>
       <c r="C1250" t="s">
         <v>3495</v>
@@ -53486,12 +53492,12 @@
         <v>5549</v>
       </c>
       <c r="Q1250" t="s">
-        <v>4972</v>
+        <v>4973</v>
       </c>
     </row>
     <row r="1251" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1251" s="1" t="s">
-        <v>3601</v>
+        <v>3604</v>
       </c>
       <c r="C1251" t="s">
         <v>3495</v>
@@ -53506,12 +53512,12 @@
         <v>5549</v>
       </c>
       <c r="Q1251" t="s">
-        <v>3602</v>
+        <v>3605</v>
       </c>
     </row>
     <row r="1252" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1252" s="1" t="s">
-        <v>3603</v>
+        <v>6932</v>
       </c>
       <c r="C1252" t="s">
         <v>3495</v>
@@ -53526,12 +53532,12 @@
         <v>5549</v>
       </c>
       <c r="Q1252" t="s">
-        <v>4973</v>
+        <v>4974</v>
       </c>
     </row>
     <row r="1253" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1253" s="1" t="s">
-        <v>3604</v>
+        <v>3607</v>
       </c>
       <c r="C1253" t="s">
         <v>3495</v>
@@ -53546,12 +53552,12 @@
         <v>5549</v>
       </c>
       <c r="Q1253" t="s">
-        <v>3605</v>
+        <v>3608</v>
       </c>
     </row>
     <row r="1254" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1254" s="1" t="s">
-        <v>6932</v>
+        <v>3609</v>
       </c>
       <c r="C1254" t="s">
         <v>3495</v>
@@ -53566,12 +53572,12 @@
         <v>5549</v>
       </c>
       <c r="Q1254" t="s">
-        <v>4974</v>
+        <v>3610</v>
       </c>
     </row>
     <row r="1255" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1255" s="1" t="s">
-        <v>3607</v>
+        <v>3611</v>
       </c>
       <c r="C1255" t="s">
         <v>3495</v>
@@ -53586,12 +53592,12 @@
         <v>5549</v>
       </c>
       <c r="Q1255" t="s">
-        <v>3608</v>
+        <v>4975</v>
       </c>
     </row>
     <row r="1256" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1256" s="1" t="s">
-        <v>3609</v>
+        <v>3612</v>
       </c>
       <c r="C1256" t="s">
         <v>3495</v>
@@ -53606,12 +53612,12 @@
         <v>5549</v>
       </c>
       <c r="Q1256" t="s">
-        <v>3610</v>
+        <v>4976</v>
       </c>
     </row>
     <row r="1257" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1257" s="1" t="s">
-        <v>3611</v>
+        <v>3613</v>
       </c>
       <c r="C1257" t="s">
         <v>3495</v>
@@ -53626,12 +53632,12 @@
         <v>5549</v>
       </c>
       <c r="Q1257" t="s">
-        <v>4975</v>
+        <v>3614</v>
       </c>
     </row>
     <row r="1258" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1258" s="1" t="s">
-        <v>3612</v>
+        <v>3615</v>
       </c>
       <c r="C1258" t="s">
         <v>3495</v>
@@ -53646,12 +53652,12 @@
         <v>5549</v>
       </c>
       <c r="Q1258" t="s">
-        <v>4976</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="1259" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1259" s="1" t="s">
-        <v>3613</v>
+        <v>3617</v>
       </c>
       <c r="C1259" t="s">
         <v>3495</v>
@@ -53666,12 +53672,12 @@
         <v>5549</v>
       </c>
       <c r="Q1259" t="s">
-        <v>3614</v>
+        <v>4977</v>
       </c>
     </row>
     <row r="1260" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1260" s="1" t="s">
-        <v>3615</v>
+        <v>3618</v>
       </c>
       <c r="C1260" t="s">
         <v>3495</v>
@@ -53686,12 +53692,12 @@
         <v>5549</v>
       </c>
       <c r="Q1260" t="s">
-        <v>3616</v>
+        <v>3619</v>
       </c>
     </row>
     <row r="1261" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1261" s="1" t="s">
-        <v>3617</v>
+        <v>3620</v>
       </c>
       <c r="C1261" t="s">
         <v>3495</v>
@@ -53706,12 +53712,12 @@
         <v>5549</v>
       </c>
       <c r="Q1261" t="s">
-        <v>4977</v>
+        <v>4978</v>
       </c>
     </row>
     <row r="1262" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1262" s="1" t="s">
-        <v>3618</v>
+        <v>3621</v>
       </c>
       <c r="C1262" t="s">
         <v>3495</v>
@@ -53726,12 +53732,12 @@
         <v>5549</v>
       </c>
       <c r="Q1262" t="s">
-        <v>3619</v>
+        <v>4979</v>
       </c>
     </row>
     <row r="1263" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1263" s="1" t="s">
-        <v>3620</v>
+        <v>3622</v>
       </c>
       <c r="C1263" t="s">
         <v>3495</v>
@@ -53746,12 +53752,12 @@
         <v>5549</v>
       </c>
       <c r="Q1263" t="s">
-        <v>4978</v>
+        <v>4980</v>
       </c>
     </row>
     <row r="1264" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1264" s="1" t="s">
-        <v>3621</v>
+        <v>3623</v>
       </c>
       <c r="C1264" t="s">
         <v>3495</v>
@@ -53766,12 +53772,12 @@
         <v>5549</v>
       </c>
       <c r="Q1264" t="s">
-        <v>4979</v>
+        <v>4601</v>
       </c>
     </row>
     <row r="1265" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1265" s="1" t="s">
-        <v>3622</v>
+        <v>3624</v>
       </c>
       <c r="C1265" t="s">
         <v>3495</v>
@@ -53786,12 +53792,12 @@
         <v>5549</v>
       </c>
       <c r="Q1265" t="s">
-        <v>4980</v>
+        <v>4981</v>
       </c>
     </row>
     <row r="1266" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1266" s="1" t="s">
-        <v>3623</v>
+        <v>3625</v>
       </c>
       <c r="C1266" t="s">
         <v>3495</v>
@@ -53806,12 +53812,12 @@
         <v>5549</v>
       </c>
       <c r="Q1266" t="s">
-        <v>4601</v>
+        <v>4602</v>
       </c>
     </row>
     <row r="1267" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1267" s="1" t="s">
-        <v>3624</v>
+        <v>3626</v>
       </c>
       <c r="C1267" t="s">
         <v>3495</v>
@@ -53826,12 +53832,12 @@
         <v>5549</v>
       </c>
       <c r="Q1267" t="s">
-        <v>4981</v>
+        <v>3627</v>
       </c>
     </row>
     <row r="1268" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1268" s="1" t="s">
-        <v>3625</v>
+        <v>3628</v>
       </c>
       <c r="C1268" t="s">
         <v>3495</v>
@@ -53846,12 +53852,12 @@
         <v>5549</v>
       </c>
       <c r="Q1268" t="s">
-        <v>4602</v>
+        <v>4982</v>
       </c>
     </row>
     <row r="1269" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1269" s="1" t="s">
-        <v>3626</v>
+        <v>3629</v>
       </c>
       <c r="C1269" t="s">
         <v>3495</v>
@@ -53866,12 +53872,12 @@
         <v>5549</v>
       </c>
       <c r="Q1269" t="s">
-        <v>3627</v>
+        <v>4603</v>
       </c>
     </row>
     <row r="1270" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1270" s="1" t="s">
-        <v>3628</v>
+        <v>3630</v>
       </c>
       <c r="C1270" t="s">
         <v>3495</v>
@@ -53886,12 +53892,12 @@
         <v>5549</v>
       </c>
       <c r="Q1270" t="s">
-        <v>4982</v>
+        <v>3631</v>
       </c>
     </row>
     <row r="1271" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1271" s="1" t="s">
-        <v>3629</v>
+        <v>3632</v>
       </c>
       <c r="C1271" t="s">
         <v>3495</v>
@@ -53906,12 +53912,12 @@
         <v>5549</v>
       </c>
       <c r="Q1271" t="s">
-        <v>4603</v>
+        <v>4983</v>
       </c>
     </row>
     <row r="1272" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1272" s="1" t="s">
-        <v>3630</v>
+        <v>3633</v>
       </c>
       <c r="C1272" t="s">
         <v>3495</v>
@@ -53926,12 +53932,12 @@
         <v>5549</v>
       </c>
       <c r="Q1272" t="s">
-        <v>3631</v>
+        <v>3634</v>
       </c>
     </row>
     <row r="1273" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1273" s="1" t="s">
-        <v>3632</v>
+        <v>3635</v>
       </c>
       <c r="C1273" t="s">
         <v>3495</v>
@@ -53946,12 +53952,12 @@
         <v>5549</v>
       </c>
       <c r="Q1273" t="s">
-        <v>4983</v>
+        <v>3636</v>
       </c>
     </row>
     <row r="1274" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1274" s="1" t="s">
-        <v>3633</v>
+        <v>3637</v>
       </c>
       <c r="C1274" t="s">
         <v>3495</v>
@@ -53966,12 +53972,12 @@
         <v>5549</v>
       </c>
       <c r="Q1274" t="s">
-        <v>3634</v>
+        <v>4604</v>
       </c>
     </row>
     <row r="1275" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1275" s="1" t="s">
-        <v>3635</v>
+        <v>3638</v>
       </c>
       <c r="C1275" t="s">
         <v>3495</v>
@@ -53986,12 +53992,12 @@
         <v>5549</v>
       </c>
       <c r="Q1275" t="s">
-        <v>3636</v>
+        <v>3639</v>
       </c>
     </row>
     <row r="1276" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1276" s="1" t="s">
-        <v>3637</v>
+        <v>3640</v>
       </c>
       <c r="C1276" t="s">
         <v>3495</v>
@@ -54006,12 +54012,12 @@
         <v>5549</v>
       </c>
       <c r="Q1276" t="s">
-        <v>4604</v>
+        <v>4984</v>
       </c>
     </row>
     <row r="1277" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1277" s="1" t="s">
-        <v>3638</v>
+        <v>3641</v>
       </c>
       <c r="C1277" t="s">
         <v>3495</v>
@@ -54026,12 +54032,12 @@
         <v>5549</v>
       </c>
       <c r="Q1277" t="s">
-        <v>3639</v>
+        <v>4985</v>
       </c>
     </row>
     <row r="1278" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1278" s="1" t="s">
-        <v>3640</v>
+        <v>3642</v>
       </c>
       <c r="C1278" t="s">
         <v>3495</v>
@@ -54046,12 +54052,12 @@
         <v>5549</v>
       </c>
       <c r="Q1278" t="s">
-        <v>4984</v>
+        <v>4605</v>
       </c>
     </row>
     <row r="1279" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1279" s="1" t="s">
-        <v>3641</v>
+        <v>3643</v>
       </c>
       <c r="C1279" t="s">
         <v>3495</v>
@@ -54066,12 +54072,12 @@
         <v>5549</v>
       </c>
       <c r="Q1279" t="s">
-        <v>4985</v>
+        <v>4986</v>
       </c>
     </row>
     <row r="1280" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1280" s="1" t="s">
-        <v>3642</v>
+        <v>3644</v>
       </c>
       <c r="C1280" t="s">
         <v>3495</v>
@@ -54086,12 +54092,12 @@
         <v>5549</v>
       </c>
       <c r="Q1280" t="s">
-        <v>4605</v>
+        <v>4987</v>
       </c>
     </row>
     <row r="1281" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1281" s="1" t="s">
-        <v>3643</v>
+        <v>3645</v>
       </c>
       <c r="C1281" t="s">
         <v>3495</v>
@@ -54106,12 +54112,12 @@
         <v>5549</v>
       </c>
       <c r="Q1281" t="s">
-        <v>4986</v>
+        <v>3646</v>
       </c>
     </row>
     <row r="1282" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1282" s="1" t="s">
-        <v>3644</v>
+        <v>3647</v>
       </c>
       <c r="C1282" t="s">
         <v>3495</v>
@@ -54126,12 +54132,12 @@
         <v>5549</v>
       </c>
       <c r="Q1282" t="s">
-        <v>4987</v>
+        <v>4988</v>
       </c>
     </row>
     <row r="1283" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1283" s="1" t="s">
-        <v>3645</v>
+        <v>3648</v>
       </c>
       <c r="C1283" t="s">
         <v>3495</v>
@@ -54146,12 +54152,12 @@
         <v>5549</v>
       </c>
       <c r="Q1283" t="s">
-        <v>3646</v>
+        <v>4989</v>
       </c>
     </row>
     <row r="1284" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1284" s="1" t="s">
-        <v>3647</v>
+        <v>3649</v>
       </c>
       <c r="C1284" t="s">
         <v>3495</v>
@@ -54166,12 +54172,12 @@
         <v>5549</v>
       </c>
       <c r="Q1284" t="s">
-        <v>4988</v>
+        <v>3650</v>
       </c>
     </row>
     <row r="1285" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1285" s="1" t="s">
-        <v>3648</v>
+        <v>3651</v>
       </c>
       <c r="C1285" t="s">
         <v>3495</v>
@@ -54186,12 +54192,12 @@
         <v>5549</v>
       </c>
       <c r="Q1285" t="s">
-        <v>4989</v>
+        <v>3652</v>
       </c>
     </row>
     <row r="1286" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1286" s="1" t="s">
-        <v>3649</v>
+        <v>3653</v>
       </c>
       <c r="C1286" t="s">
         <v>3495</v>
@@ -54206,12 +54212,12 @@
         <v>5549</v>
       </c>
       <c r="Q1286" t="s">
-        <v>3650</v>
+        <v>3654</v>
       </c>
     </row>
     <row r="1287" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1287" s="1" t="s">
-        <v>3651</v>
+        <v>3655</v>
       </c>
       <c r="C1287" t="s">
         <v>3495</v>
@@ -54226,12 +54232,12 @@
         <v>5549</v>
       </c>
       <c r="Q1287" t="s">
-        <v>3652</v>
+        <v>3656</v>
       </c>
     </row>
     <row r="1288" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1288" s="1" t="s">
-        <v>3653</v>
+        <v>3657</v>
       </c>
       <c r="C1288" t="s">
         <v>3495</v>
@@ -54246,12 +54252,12 @@
         <v>5549</v>
       </c>
       <c r="Q1288" t="s">
-        <v>3654</v>
+        <v>4990</v>
       </c>
     </row>
     <row r="1289" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1289" s="1" t="s">
-        <v>3655</v>
+        <v>3658</v>
       </c>
       <c r="C1289" t="s">
         <v>3495</v>
@@ -54266,12 +54272,12 @@
         <v>5549</v>
       </c>
       <c r="Q1289" t="s">
-        <v>3656</v>
+        <v>3659</v>
       </c>
     </row>
     <row r="1290" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1290" s="1" t="s">
-        <v>3657</v>
+        <v>3660</v>
       </c>
       <c r="C1290" t="s">
         <v>3495</v>
@@ -54286,12 +54292,12 @@
         <v>5549</v>
       </c>
       <c r="Q1290" t="s">
-        <v>4990</v>
+        <v>3661</v>
       </c>
     </row>
     <row r="1291" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1291" s="1" t="s">
-        <v>3658</v>
+        <v>3662</v>
       </c>
       <c r="C1291" t="s">
         <v>3495</v>
@@ -54306,12 +54312,12 @@
         <v>5549</v>
       </c>
       <c r="Q1291" t="s">
-        <v>3659</v>
+        <v>4991</v>
       </c>
     </row>
     <row r="1292" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1292" s="1" t="s">
-        <v>3660</v>
+        <v>3663</v>
       </c>
       <c r="C1292" t="s">
         <v>3495</v>
@@ -54326,12 +54332,12 @@
         <v>5549</v>
       </c>
       <c r="Q1292" t="s">
-        <v>3661</v>
+        <v>3664</v>
       </c>
     </row>
     <row r="1293" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1293" s="1" t="s">
-        <v>3662</v>
+        <v>3665</v>
       </c>
       <c r="C1293" t="s">
         <v>3495</v>
@@ -54346,12 +54352,12 @@
         <v>5549</v>
       </c>
       <c r="Q1293" t="s">
-        <v>4991</v>
+        <v>4992</v>
       </c>
     </row>
     <row r="1294" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1294" s="1" t="s">
-        <v>3663</v>
+        <v>3666</v>
       </c>
       <c r="C1294" t="s">
         <v>3495</v>
@@ -54366,12 +54372,12 @@
         <v>5549</v>
       </c>
       <c r="Q1294" t="s">
-        <v>3664</v>
+        <v>3667</v>
       </c>
     </row>
     <row r="1295" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1295" s="1" t="s">
-        <v>3665</v>
+        <v>3668</v>
       </c>
       <c r="C1295" t="s">
         <v>3495</v>
@@ -54386,12 +54392,12 @@
         <v>5549</v>
       </c>
       <c r="Q1295" t="s">
-        <v>4992</v>
+        <v>3669</v>
       </c>
     </row>
     <row r="1296" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1296" s="1" t="s">
-        <v>3666</v>
+        <v>3670</v>
       </c>
       <c r="C1296" t="s">
         <v>3495</v>
@@ -54406,12 +54412,12 @@
         <v>5549</v>
       </c>
       <c r="Q1296" t="s">
-        <v>3667</v>
+        <v>3671</v>
       </c>
     </row>
     <row r="1297" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1297" s="1" t="s">
-        <v>3668</v>
+        <v>3672</v>
       </c>
       <c r="C1297" t="s">
         <v>3495</v>
@@ -54426,12 +54432,12 @@
         <v>5549</v>
       </c>
       <c r="Q1297" t="s">
-        <v>3669</v>
+        <v>3673</v>
       </c>
     </row>
     <row r="1298" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1298" s="1" t="s">
-        <v>3670</v>
+        <v>3674</v>
       </c>
       <c r="C1298" t="s">
         <v>3495</v>
@@ -54446,12 +54452,12 @@
         <v>5549</v>
       </c>
       <c r="Q1298" t="s">
-        <v>3671</v>
+        <v>4993</v>
       </c>
     </row>
     <row r="1299" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1299" s="1" t="s">
-        <v>3672</v>
+        <v>3675</v>
       </c>
       <c r="C1299" t="s">
         <v>3495</v>
@@ -54466,12 +54472,12 @@
         <v>5549</v>
       </c>
       <c r="Q1299" t="s">
-        <v>3673</v>
+        <v>4994</v>
       </c>
     </row>
     <row r="1300" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1300" s="1" t="s">
-        <v>3674</v>
+        <v>3676</v>
       </c>
       <c r="C1300" t="s">
         <v>3495</v>
@@ -54486,12 +54492,12 @@
         <v>5549</v>
       </c>
       <c r="Q1300" t="s">
-        <v>4993</v>
+        <v>4995</v>
       </c>
     </row>
     <row r="1301" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1301" s="1" t="s">
-        <v>3675</v>
+        <v>3677</v>
       </c>
       <c r="C1301" t="s">
         <v>3495</v>
@@ -54506,12 +54512,12 @@
         <v>5549</v>
       </c>
       <c r="Q1301" t="s">
-        <v>4994</v>
+        <v>4996</v>
       </c>
     </row>
     <row r="1302" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1302" s="1" t="s">
-        <v>3676</v>
+        <v>3678</v>
       </c>
       <c r="C1302" t="s">
         <v>3495</v>
@@ -54526,12 +54532,12 @@
         <v>5549</v>
       </c>
       <c r="Q1302" t="s">
-        <v>4995</v>
+        <v>4997</v>
       </c>
     </row>
     <row r="1303" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1303" s="1" t="s">
-        <v>3677</v>
+        <v>3679</v>
       </c>
       <c r="C1303" t="s">
         <v>3495</v>
@@ -54546,12 +54552,12 @@
         <v>5549</v>
       </c>
       <c r="Q1303" t="s">
-        <v>4996</v>
+        <v>3680</v>
       </c>
     </row>
     <row r="1304" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1304" s="1" t="s">
-        <v>3678</v>
+        <v>3681</v>
       </c>
       <c r="C1304" t="s">
         <v>3495</v>
@@ -54566,12 +54572,12 @@
         <v>5549</v>
       </c>
       <c r="Q1304" t="s">
-        <v>4997</v>
+        <v>4606</v>
       </c>
     </row>
     <row r="1305" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1305" s="1" t="s">
-        <v>3679</v>
+        <v>3682</v>
       </c>
       <c r="C1305" t="s">
         <v>3495</v>
@@ -54586,12 +54592,12 @@
         <v>5549</v>
       </c>
       <c r="Q1305" t="s">
-        <v>3680</v>
+        <v>3683</v>
       </c>
     </row>
     <row r="1306" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1306" s="1" t="s">
-        <v>3681</v>
+        <v>6933</v>
       </c>
       <c r="C1306" t="s">
         <v>3495</v>
@@ -54606,12 +54612,12 @@
         <v>5549</v>
       </c>
       <c r="Q1306" t="s">
-        <v>4606</v>
+        <v>6934</v>
       </c>
     </row>
     <row r="1307" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1307" s="1" t="s">
-        <v>3682</v>
+        <v>6935</v>
       </c>
       <c r="C1307" t="s">
         <v>3495</v>
@@ -54626,12 +54632,12 @@
         <v>5549</v>
       </c>
       <c r="Q1307" t="s">
-        <v>3683</v>
+        <v>6936</v>
       </c>
     </row>
     <row r="1308" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1308" s="1" t="s">
-        <v>6933</v>
+        <v>6937</v>
       </c>
       <c r="C1308" t="s">
         <v>3495</v>
@@ -54646,12 +54652,12 @@
         <v>5549</v>
       </c>
       <c r="Q1308" t="s">
-        <v>6934</v>
+        <v>6938</v>
       </c>
     </row>
     <row r="1309" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1309" s="1" t="s">
-        <v>6935</v>
+        <v>6939</v>
       </c>
       <c r="C1309" t="s">
         <v>3495</v>
@@ -54666,12 +54672,12 @@
         <v>5549</v>
       </c>
       <c r="Q1309" t="s">
-        <v>6936</v>
+        <v>6940</v>
       </c>
     </row>
     <row r="1310" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1310" s="1" t="s">
-        <v>6937</v>
+        <v>6941</v>
       </c>
       <c r="C1310" t="s">
         <v>3495</v>
@@ -54686,12 +54692,12 @@
         <v>5549</v>
       </c>
       <c r="Q1310" t="s">
-        <v>6938</v>
+        <v>6942</v>
       </c>
     </row>
     <row r="1311" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1311" s="1" t="s">
-        <v>6939</v>
+        <v>6943</v>
       </c>
       <c r="C1311" t="s">
         <v>3495</v>
@@ -54706,12 +54712,12 @@
         <v>5549</v>
       </c>
       <c r="Q1311" t="s">
-        <v>6940</v>
+        <v>6944</v>
       </c>
     </row>
     <row r="1312" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1312" s="1" t="s">
-        <v>6941</v>
+        <v>6945</v>
       </c>
       <c r="C1312" t="s">
         <v>3495</v>
@@ -54726,12 +54732,12 @@
         <v>5549</v>
       </c>
       <c r="Q1312" t="s">
-        <v>6942</v>
+        <v>6946</v>
       </c>
     </row>
     <row r="1313" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1313" s="1" t="s">
-        <v>6943</v>
+        <v>6947</v>
       </c>
       <c r="C1313" t="s">
         <v>3495</v>
@@ -54746,12 +54752,12 @@
         <v>5549</v>
       </c>
       <c r="Q1313" t="s">
-        <v>6944</v>
+        <v>6948</v>
       </c>
     </row>
     <row r="1314" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1314" s="1" t="s">
-        <v>6945</v>
+        <v>6949</v>
       </c>
       <c r="C1314" t="s">
         <v>3495</v>
@@ -54766,12 +54772,12 @@
         <v>5549</v>
       </c>
       <c r="Q1314" t="s">
-        <v>6946</v>
+        <v>6950</v>
       </c>
     </row>
     <row r="1315" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1315" s="1" t="s">
-        <v>6947</v>
+        <v>6951</v>
       </c>
       <c r="C1315" t="s">
         <v>3495</v>
@@ -54786,12 +54792,12 @@
         <v>5549</v>
       </c>
       <c r="Q1315" t="s">
-        <v>6948</v>
+        <v>6952</v>
       </c>
     </row>
     <row r="1316" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1316" s="1" t="s">
-        <v>6949</v>
+        <v>6953</v>
       </c>
       <c r="C1316" t="s">
         <v>3495</v>
@@ -54806,86 +54812,98 @@
         <v>5549</v>
       </c>
       <c r="Q1316" t="s">
-        <v>6950</v>
+        <v>6954</v>
       </c>
     </row>
     <row r="1317" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1317" s="1" t="s">
-        <v>6951</v>
+        <v>2668</v>
       </c>
       <c r="C1317" t="s">
-        <v>3495</v>
+        <v>2669</v>
       </c>
       <c r="D1317" s="1">
         <v>68000</v>
       </c>
-      <c r="E1317" t="s">
-        <v>2426</v>
-      </c>
       <c r="L1317" t="s">
-        <v>5549</v>
+        <v>2670</v>
       </c>
       <c r="Q1317" t="s">
-        <v>6952</v>
+        <v>2671</v>
       </c>
     </row>
     <row r="1318" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1318" s="1" t="s">
-        <v>6953</v>
+        <v>2672</v>
       </c>
       <c r="C1318" t="s">
-        <v>3495</v>
-      </c>
-      <c r="D1318" s="1">
-        <v>68000</v>
-      </c>
-      <c r="E1318" t="s">
-        <v>2426</v>
+        <v>2673</v>
+      </c>
+      <c r="D1318" s="1" t="s">
+        <v>351</v>
       </c>
       <c r="L1318" t="s">
-        <v>5549</v>
+        <v>2538</v>
       </c>
       <c r="Q1318" t="s">
-        <v>6954</v>
+        <v>2674</v>
       </c>
     </row>
     <row r="1319" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1319" s="1" t="s">
-        <v>2668</v>
+        <v>2691</v>
       </c>
       <c r="C1319" t="s">
-        <v>2669</v>
+        <v>2689</v>
       </c>
       <c r="D1319" s="1">
-        <v>68000</v>
+        <v>68010</v>
+      </c>
+      <c r="E1319" t="s">
+        <v>351</v>
       </c>
       <c r="L1319" t="s">
-        <v>2670</v>
+        <v>5238</v>
+      </c>
+      <c r="M1319" t="s">
+        <v>2534</v>
+      </c>
+      <c r="N1319" t="s">
+        <v>3889</v>
       </c>
       <c r="Q1319" t="s">
-        <v>2671</v>
+        <v>4870</v>
       </c>
     </row>
     <row r="1320" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1320" s="1" t="s">
-        <v>2672</v>
+        <v>2688</v>
       </c>
       <c r="C1320" t="s">
-        <v>2673</v>
-      </c>
-      <c r="D1320" s="1" t="s">
+        <v>2689</v>
+      </c>
+      <c r="D1320" s="1">
+        <v>68010</v>
+      </c>
+      <c r="E1320" t="s">
         <v>351</v>
       </c>
       <c r="L1320" t="s">
-        <v>2538</v>
+        <v>5238</v>
+      </c>
+      <c r="M1320" t="s">
+        <v>2534</v>
+      </c>
+      <c r="N1320" t="s">
+        <v>3889</v>
       </c>
       <c r="Q1320" t="s">
-        <v>2674</v>
+        <v>4867</v>
       </c>
     </row>
     <row r="1321" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1321" s="1" t="s">
-        <v>2691</v>
+        <v>2690</v>
       </c>
       <c r="C1321" t="s">
         <v>2689</v>
@@ -54906,12 +54924,12 @@
         <v>3889</v>
       </c>
       <c r="Q1321" t="s">
-        <v>4870</v>
+        <v>4868</v>
       </c>
     </row>
     <row r="1322" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1322" s="1" t="s">
-        <v>2688</v>
+        <v>6487</v>
       </c>
       <c r="C1322" t="s">
         <v>2689</v>
@@ -54932,12 +54950,12 @@
         <v>3889</v>
       </c>
       <c r="Q1322" t="s">
-        <v>4867</v>
+        <v>4869</v>
       </c>
     </row>
     <row r="1323" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1323" s="1" t="s">
-        <v>2690</v>
+        <v>6488</v>
       </c>
       <c r="C1323" t="s">
         <v>2689</v>
@@ -54958,12 +54976,12 @@
         <v>3889</v>
       </c>
       <c r="Q1323" t="s">
-        <v>4868</v>
+        <v>6489</v>
       </c>
     </row>
     <row r="1324" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1324" s="1" t="s">
-        <v>6487</v>
+        <v>2692</v>
       </c>
       <c r="C1324" t="s">
         <v>2689</v>
@@ -54984,12 +55002,12 @@
         <v>3889</v>
       </c>
       <c r="Q1324" t="s">
-        <v>4869</v>
+        <v>4871</v>
       </c>
     </row>
     <row r="1325" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1325" s="1" t="s">
-        <v>6488</v>
+        <v>2693</v>
       </c>
       <c r="C1325" t="s">
         <v>2689</v>
@@ -55010,12 +55028,12 @@
         <v>3889</v>
       </c>
       <c r="Q1325" t="s">
-        <v>6489</v>
+        <v>4872</v>
       </c>
     </row>
     <row r="1326" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1326" s="1" t="s">
-        <v>2692</v>
+        <v>2694</v>
       </c>
       <c r="C1326" t="s">
         <v>2689</v>
@@ -55036,12 +55054,12 @@
         <v>3889</v>
       </c>
       <c r="Q1326" t="s">
-        <v>4871</v>
+        <v>4873</v>
       </c>
     </row>
     <row r="1327" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1327" s="1" t="s">
-        <v>2693</v>
+        <v>2695</v>
       </c>
       <c r="C1327" t="s">
         <v>2689</v>
@@ -55062,12 +55080,12 @@
         <v>3889</v>
       </c>
       <c r="Q1327" t="s">
-        <v>4872</v>
+        <v>4874</v>
       </c>
     </row>
     <row r="1328" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1328" s="1" t="s">
-        <v>2694</v>
+        <v>6490</v>
       </c>
       <c r="C1328" t="s">
         <v>2689</v>
@@ -55088,12 +55106,12 @@
         <v>3889</v>
       </c>
       <c r="Q1328" t="s">
-        <v>4873</v>
+        <v>6491</v>
       </c>
     </row>
     <row r="1329" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1329" s="1" t="s">
-        <v>2695</v>
+        <v>2696</v>
       </c>
       <c r="C1329" t="s">
         <v>2689</v>
@@ -55114,12 +55132,12 @@
         <v>3889</v>
       </c>
       <c r="Q1329" t="s">
-        <v>4874</v>
+        <v>4875</v>
       </c>
     </row>
     <row r="1330" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1330" s="1" t="s">
-        <v>6490</v>
+        <v>2697</v>
       </c>
       <c r="C1330" t="s">
         <v>2689</v>
@@ -55140,18 +55158,18 @@
         <v>3889</v>
       </c>
       <c r="Q1330" t="s">
-        <v>6491</v>
+        <v>4876</v>
       </c>
     </row>
     <row r="1331" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1331" s="1" t="s">
-        <v>2696</v>
+        <v>2698</v>
       </c>
       <c r="C1331" t="s">
-        <v>2689</v>
-      </c>
-      <c r="D1331" s="1">
-        <v>68010</v>
+        <v>2699</v>
+      </c>
+      <c r="D1331" s="1" t="s">
+        <v>2700</v>
       </c>
       <c r="E1331" t="s">
         <v>351</v>
@@ -55160,24 +55178,24 @@
         <v>5238</v>
       </c>
       <c r="M1331" t="s">
-        <v>2534</v>
+        <v>2538</v>
       </c>
       <c r="N1331" t="s">
         <v>3889</v>
       </c>
       <c r="Q1331" t="s">
-        <v>4875</v>
+        <v>4877</v>
       </c>
     </row>
     <row r="1332" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1332" s="1" t="s">
-        <v>2697</v>
+        <v>2701</v>
       </c>
       <c r="C1332" t="s">
-        <v>2689</v>
-      </c>
-      <c r="D1332" s="1">
-        <v>68010</v>
+        <v>2699</v>
+      </c>
+      <c r="D1332" s="1" t="s">
+        <v>2700</v>
       </c>
       <c r="E1332" t="s">
         <v>351</v>
@@ -55186,18 +55204,15 @@
         <v>5238</v>
       </c>
       <c r="M1332" t="s">
-        <v>2534</v>
-      </c>
-      <c r="N1332" t="s">
-        <v>3889</v>
+        <v>2538</v>
       </c>
       <c r="Q1332" t="s">
-        <v>4876</v>
+        <v>4416</v>
       </c>
     </row>
     <row r="1333" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1333" s="1" t="s">
-        <v>2698</v>
+        <v>2702</v>
       </c>
       <c r="C1333" t="s">
         <v>2699</v>
@@ -55214,16 +55229,13 @@
       <c r="M1333" t="s">
         <v>2538</v>
       </c>
-      <c r="N1333" t="s">
-        <v>3889</v>
-      </c>
       <c r="Q1333" t="s">
-        <v>4877</v>
+        <v>4417</v>
       </c>
     </row>
     <row r="1334" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1334" s="1" t="s">
-        <v>2701</v>
+        <v>6492</v>
       </c>
       <c r="C1334" t="s">
         <v>2699</v>
@@ -55240,13 +55252,16 @@
       <c r="M1334" t="s">
         <v>2538</v>
       </c>
+      <c r="N1334" t="s">
+        <v>3889</v>
+      </c>
       <c r="Q1334" t="s">
-        <v>4416</v>
+        <v>4878</v>
       </c>
     </row>
     <row r="1335" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1335" s="1" t="s">
-        <v>2702</v>
+        <v>2703</v>
       </c>
       <c r="C1335" t="s">
         <v>2699</v>
@@ -55263,13 +55278,16 @@
       <c r="M1335" t="s">
         <v>2538</v>
       </c>
+      <c r="N1335" t="s">
+        <v>3889</v>
+      </c>
       <c r="Q1335" t="s">
-        <v>4417</v>
+        <v>4879</v>
       </c>
     </row>
     <row r="1336" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1336" s="1" t="s">
-        <v>6492</v>
+        <v>2704</v>
       </c>
       <c r="C1336" t="s">
         <v>2699</v>
@@ -55290,12 +55308,12 @@
         <v>3889</v>
       </c>
       <c r="Q1336" t="s">
-        <v>4878</v>
+        <v>4880</v>
       </c>
     </row>
     <row r="1337" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1337" s="1" t="s">
-        <v>2703</v>
+        <v>2705</v>
       </c>
       <c r="C1337" t="s">
         <v>2699</v>
@@ -55316,63 +55334,11 @@
         <v>3889</v>
       </c>
       <c r="Q1337" t="s">
-        <v>4879</v>
-      </c>
-    </row>
-    <row r="1338" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B1338" s="1" t="s">
-        <v>2704</v>
-      </c>
-      <c r="C1338" t="s">
-        <v>2699</v>
-      </c>
-      <c r="D1338" s="1" t="s">
-        <v>2700</v>
-      </c>
-      <c r="E1338" t="s">
-        <v>351</v>
-      </c>
-      <c r="L1338" t="s">
-        <v>5238</v>
-      </c>
-      <c r="M1338" t="s">
-        <v>2538</v>
-      </c>
-      <c r="N1338" t="s">
-        <v>3889</v>
-      </c>
-      <c r="Q1338" t="s">
-        <v>4880</v>
-      </c>
-    </row>
-    <row r="1339" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B1339" s="1" t="s">
-        <v>2705</v>
-      </c>
-      <c r="C1339" t="s">
-        <v>2699</v>
-      </c>
-      <c r="D1339" s="1" t="s">
-        <v>2700</v>
-      </c>
-      <c r="E1339" t="s">
-        <v>351</v>
-      </c>
-      <c r="L1339" t="s">
-        <v>5238</v>
-      </c>
-      <c r="M1339" t="s">
-        <v>2538</v>
-      </c>
-      <c r="N1339" t="s">
-        <v>3889</v>
-      </c>
-      <c r="Q1339" t="s">
         <v>4881</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:R1318"/>
+  <autoFilter ref="B1:R1316"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -55380,10 +55346,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Q457"/>
+  <dimension ref="B1:Q459"/>
   <sheetViews>
     <sheetView topLeftCell="A445" workbookViewId="0">
-      <selection activeCell="A456" sqref="A456:XFD457"/>
+      <selection activeCell="A458" sqref="A458:XFD459"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -64820,6 +64786,40 @@
       </c>
       <c r="Q457" t="s">
         <v>3182</v>
+      </c>
+    </row>
+    <row r="458" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B458" s="1" t="s">
+        <v>6912</v>
+      </c>
+      <c r="C458" t="s">
+        <v>3478</v>
+      </c>
+      <c r="D458" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L458" t="s">
+        <v>352</v>
+      </c>
+      <c r="Q458" t="s">
+        <v>6913</v>
+      </c>
+    </row>
+    <row r="459" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B459" s="1" t="s">
+        <v>3477</v>
+      </c>
+      <c r="C459" t="s">
+        <v>3478</v>
+      </c>
+      <c r="D459" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L459" t="s">
+        <v>352</v>
+      </c>
+      <c r="Q459" t="s">
+        <v>4586</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added liberatr non working driver
</commit_message>
<xml_diff>
--- a/compatibility_list.xlsx
+++ b/compatibility_list.xlsx
@@ -25879,10 +25879,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Q1337"/>
+  <dimension ref="B1:Q1336"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1161" workbookViewId="0">
-      <selection activeCell="B1170" sqref="B1170"/>
+    <sheetView tabSelected="1" topLeftCell="A1308" workbookViewId="0">
+      <selection activeCell="A1318" sqref="A1318:XFD1318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -54834,24 +54834,33 @@
     </row>
     <row r="1318" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1318" s="1" t="s">
-        <v>2672</v>
+        <v>2691</v>
       </c>
       <c r="C1318" t="s">
-        <v>2673</v>
-      </c>
-      <c r="D1318" s="1" t="s">
+        <v>2689</v>
+      </c>
+      <c r="D1318" s="1">
+        <v>68010</v>
+      </c>
+      <c r="E1318" t="s">
         <v>351</v>
       </c>
       <c r="L1318" t="s">
-        <v>2538</v>
+        <v>5238</v>
+      </c>
+      <c r="M1318" t="s">
+        <v>2534</v>
+      </c>
+      <c r="N1318" t="s">
+        <v>3889</v>
       </c>
       <c r="Q1318" t="s">
-        <v>2674</v>
+        <v>4870</v>
       </c>
     </row>
     <row r="1319" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1319" s="1" t="s">
-        <v>2691</v>
+        <v>2688</v>
       </c>
       <c r="C1319" t="s">
         <v>2689</v>
@@ -54872,12 +54881,12 @@
         <v>3889</v>
       </c>
       <c r="Q1319" t="s">
-        <v>4870</v>
+        <v>4867</v>
       </c>
     </row>
     <row r="1320" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1320" s="1" t="s">
-        <v>2688</v>
+        <v>2690</v>
       </c>
       <c r="C1320" t="s">
         <v>2689</v>
@@ -54898,12 +54907,12 @@
         <v>3889</v>
       </c>
       <c r="Q1320" t="s">
-        <v>4867</v>
+        <v>4868</v>
       </c>
     </row>
     <row r="1321" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1321" s="1" t="s">
-        <v>2690</v>
+        <v>6487</v>
       </c>
       <c r="C1321" t="s">
         <v>2689</v>
@@ -54924,12 +54933,12 @@
         <v>3889</v>
       </c>
       <c r="Q1321" t="s">
-        <v>4868</v>
+        <v>4869</v>
       </c>
     </row>
     <row r="1322" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1322" s="1" t="s">
-        <v>6487</v>
+        <v>6488</v>
       </c>
       <c r="C1322" t="s">
         <v>2689</v>
@@ -54950,12 +54959,12 @@
         <v>3889</v>
       </c>
       <c r="Q1322" t="s">
-        <v>4869</v>
+        <v>6489</v>
       </c>
     </row>
     <row r="1323" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1323" s="1" t="s">
-        <v>6488</v>
+        <v>2692</v>
       </c>
       <c r="C1323" t="s">
         <v>2689</v>
@@ -54976,12 +54985,12 @@
         <v>3889</v>
       </c>
       <c r="Q1323" t="s">
-        <v>6489</v>
+        <v>4871</v>
       </c>
     </row>
     <row r="1324" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1324" s="1" t="s">
-        <v>2692</v>
+        <v>2693</v>
       </c>
       <c r="C1324" t="s">
         <v>2689</v>
@@ -55002,12 +55011,12 @@
         <v>3889</v>
       </c>
       <c r="Q1324" t="s">
-        <v>4871</v>
+        <v>4872</v>
       </c>
     </row>
     <row r="1325" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1325" s="1" t="s">
-        <v>2693</v>
+        <v>2694</v>
       </c>
       <c r="C1325" t="s">
         <v>2689</v>
@@ -55028,12 +55037,12 @@
         <v>3889</v>
       </c>
       <c r="Q1325" t="s">
-        <v>4872</v>
+        <v>4873</v>
       </c>
     </row>
     <row r="1326" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1326" s="1" t="s">
-        <v>2694</v>
+        <v>2695</v>
       </c>
       <c r="C1326" t="s">
         <v>2689</v>
@@ -55054,12 +55063,12 @@
         <v>3889</v>
       </c>
       <c r="Q1326" t="s">
-        <v>4873</v>
+        <v>4874</v>
       </c>
     </row>
     <row r="1327" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1327" s="1" t="s">
-        <v>2695</v>
+        <v>6490</v>
       </c>
       <c r="C1327" t="s">
         <v>2689</v>
@@ -55080,12 +55089,12 @@
         <v>3889</v>
       </c>
       <c r="Q1327" t="s">
-        <v>4874</v>
+        <v>6491</v>
       </c>
     </row>
     <row r="1328" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1328" s="1" t="s">
-        <v>6490</v>
+        <v>2696</v>
       </c>
       <c r="C1328" t="s">
         <v>2689</v>
@@ -55106,12 +55115,12 @@
         <v>3889</v>
       </c>
       <c r="Q1328" t="s">
-        <v>6491</v>
+        <v>4875</v>
       </c>
     </row>
     <row r="1329" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1329" s="1" t="s">
-        <v>2696</v>
+        <v>2697</v>
       </c>
       <c r="C1329" t="s">
         <v>2689</v>
@@ -55132,18 +55141,18 @@
         <v>3889</v>
       </c>
       <c r="Q1329" t="s">
-        <v>4875</v>
+        <v>4876</v>
       </c>
     </row>
     <row r="1330" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1330" s="1" t="s">
-        <v>2697</v>
+        <v>2698</v>
       </c>
       <c r="C1330" t="s">
-        <v>2689</v>
-      </c>
-      <c r="D1330" s="1">
-        <v>68010</v>
+        <v>2699</v>
+      </c>
+      <c r="D1330" s="1" t="s">
+        <v>2700</v>
       </c>
       <c r="E1330" t="s">
         <v>351</v>
@@ -55152,18 +55161,18 @@
         <v>5238</v>
       </c>
       <c r="M1330" t="s">
-        <v>2534</v>
+        <v>2538</v>
       </c>
       <c r="N1330" t="s">
         <v>3889</v>
       </c>
       <c r="Q1330" t="s">
-        <v>4876</v>
+        <v>4877</v>
       </c>
     </row>
     <row r="1331" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1331" s="1" t="s">
-        <v>2698</v>
+        <v>2701</v>
       </c>
       <c r="C1331" t="s">
         <v>2699</v>
@@ -55180,16 +55189,13 @@
       <c r="M1331" t="s">
         <v>2538</v>
       </c>
-      <c r="N1331" t="s">
-        <v>3889</v>
-      </c>
       <c r="Q1331" t="s">
-        <v>4877</v>
+        <v>4416</v>
       </c>
     </row>
     <row r="1332" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1332" s="1" t="s">
-        <v>2701</v>
+        <v>2702</v>
       </c>
       <c r="C1332" t="s">
         <v>2699</v>
@@ -55207,12 +55213,12 @@
         <v>2538</v>
       </c>
       <c r="Q1332" t="s">
-        <v>4416</v>
+        <v>4417</v>
       </c>
     </row>
     <row r="1333" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1333" s="1" t="s">
-        <v>2702</v>
+        <v>6492</v>
       </c>
       <c r="C1333" t="s">
         <v>2699</v>
@@ -55229,13 +55235,16 @@
       <c r="M1333" t="s">
         <v>2538</v>
       </c>
+      <c r="N1333" t="s">
+        <v>3889</v>
+      </c>
       <c r="Q1333" t="s">
-        <v>4417</v>
+        <v>4878</v>
       </c>
     </row>
     <row r="1334" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1334" s="1" t="s">
-        <v>6492</v>
+        <v>2703</v>
       </c>
       <c r="C1334" t="s">
         <v>2699</v>
@@ -55256,12 +55265,12 @@
         <v>3889</v>
       </c>
       <c r="Q1334" t="s">
-        <v>4878</v>
+        <v>4879</v>
       </c>
     </row>
     <row r="1335" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1335" s="1" t="s">
-        <v>2703</v>
+        <v>2704</v>
       </c>
       <c r="C1335" t="s">
         <v>2699</v>
@@ -55282,12 +55291,12 @@
         <v>3889</v>
       </c>
       <c r="Q1335" t="s">
-        <v>4879</v>
+        <v>4880</v>
       </c>
     </row>
     <row r="1336" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1336" s="1" t="s">
-        <v>2704</v>
+        <v>2705</v>
       </c>
       <c r="C1336" t="s">
         <v>2699</v>
@@ -55308,32 +55317,6 @@
         <v>3889</v>
       </c>
       <c r="Q1336" t="s">
-        <v>4880</v>
-      </c>
-    </row>
-    <row r="1337" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B1337" s="1" t="s">
-        <v>2705</v>
-      </c>
-      <c r="C1337" t="s">
-        <v>2699</v>
-      </c>
-      <c r="D1337" s="1" t="s">
-        <v>2700</v>
-      </c>
-      <c r="E1337" t="s">
-        <v>351</v>
-      </c>
-      <c r="L1337" t="s">
-        <v>5238</v>
-      </c>
-      <c r="M1337" t="s">
-        <v>2538</v>
-      </c>
-      <c r="N1337" t="s">
-        <v>3889</v>
-      </c>
-      <c r="Q1337" t="s">
         <v>4881</v>
       </c>
     </row>
@@ -64830,10 +64813,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R1167"/>
+  <dimension ref="B1:R1168"/>
   <sheetViews>
     <sheetView topLeftCell="A1131" workbookViewId="0">
-      <selection activeCell="A1164" sqref="A1164:XFD1167"/>
+      <selection activeCell="A1168" sqref="A1168:XFD1168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -89788,6 +89771,23 @@
         <v>2958</v>
       </c>
     </row>
+    <row r="1168" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B1168" s="1" t="s">
+        <v>2672</v>
+      </c>
+      <c r="C1168" t="s">
+        <v>2673</v>
+      </c>
+      <c r="D1168" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="L1168" t="s">
+        <v>2538</v>
+      </c>
+      <c r="Q1168" t="s">
+        <v>2674</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
added spiders WIP driver
</commit_message>
<xml_diff>
--- a/compatibility_list.xlsx
+++ b/compatibility_list.xlsx
@@ -21,9 +21,9 @@
     <sheet name="To Check" sheetId="13" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">WIP!$B$1:$R$1290</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">WIP!$B$1:$R$1288</definedName>
     <definedName name="DETAILS" localSheetId="4">WIP!#REF!</definedName>
-    <definedName name="DETAILS_1" localSheetId="4">WIP!$B$1:$Q$1290</definedName>
+    <definedName name="DETAILS_1" localSheetId="4">WIP!$B$1:$Q$1288</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25879,10 +25879,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Q1310"/>
+  <dimension ref="B1:Q1308"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A316" workbookViewId="0">
-      <selection activeCell="D324" sqref="D324"/>
+    <sheetView tabSelected="1" topLeftCell="A1125" workbookViewId="0">
+      <selection activeCell="C1136" sqref="C1136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -51234,218 +51234,221 @@
     </row>
     <row r="1135" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1135" s="1" t="s">
-        <v>3439</v>
+        <v>3419</v>
       </c>
       <c r="C1135" t="s">
-        <v>3440</v>
+        <v>3420</v>
       </c>
       <c r="D1135" s="1" t="s">
-        <v>404</v>
+        <v>2</v>
       </c>
       <c r="E1135" t="s">
-        <v>3888</v>
+        <v>2426</v>
+      </c>
+      <c r="L1135" t="s">
+        <v>1155</v>
       </c>
       <c r="Q1135" t="s">
-        <v>3441</v>
+        <v>3421</v>
       </c>
     </row>
     <row r="1136" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1136" s="1" t="s">
-        <v>3442</v>
+        <v>3422</v>
       </c>
       <c r="C1136" t="s">
-        <v>3440</v>
+        <v>3423</v>
       </c>
       <c r="D1136" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="E1136" t="s">
-        <v>3888</v>
+        <v>2</v>
+      </c>
+      <c r="L1136" t="s">
+        <v>1155</v>
       </c>
       <c r="Q1136" t="s">
-        <v>3443</v>
+        <v>3424</v>
       </c>
     </row>
     <row r="1137" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1137" s="1" t="s">
-        <v>3419</v>
+        <v>3425</v>
       </c>
       <c r="C1137" t="s">
-        <v>3420</v>
+        <v>3423</v>
       </c>
       <c r="D1137" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="E1137" t="s">
-        <v>2426</v>
       </c>
       <c r="L1137" t="s">
         <v>1155</v>
       </c>
       <c r="Q1137" t="s">
-        <v>3421</v>
+        <v>3426</v>
       </c>
     </row>
     <row r="1138" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1138" s="1" t="s">
-        <v>3422</v>
+        <v>3444</v>
       </c>
       <c r="C1138" t="s">
-        <v>3423</v>
-      </c>
-      <c r="D1138" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1138" t="s">
-        <v>1155</v>
+        <v>3445</v>
+      </c>
+      <c r="D1138" s="1">
+        <v>8080</v>
       </c>
       <c r="Q1138" t="s">
-        <v>3424</v>
+        <v>3446</v>
       </c>
     </row>
     <row r="1139" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1139" s="1" t="s">
-        <v>3425</v>
+        <v>3447</v>
       </c>
       <c r="C1139" t="s">
-        <v>3423</v>
+        <v>3448</v>
       </c>
       <c r="D1139" s="1" t="s">
-        <v>2</v>
+        <v>3006</v>
+      </c>
+      <c r="E1139" t="s">
+        <v>3006</v>
+      </c>
+      <c r="F1139" t="s">
+        <v>3899</v>
+      </c>
+      <c r="G1139" t="s">
+        <v>3899</v>
       </c>
       <c r="L1139" t="s">
-        <v>1155</v>
+        <v>2605</v>
+      </c>
+      <c r="M1139" t="s">
+        <v>5238</v>
       </c>
       <c r="Q1139" t="s">
-        <v>3426</v>
+        <v>4581</v>
       </c>
     </row>
     <row r="1140" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1140" s="1" t="s">
-        <v>3444</v>
+        <v>3463</v>
       </c>
       <c r="C1140" t="s">
-        <v>3445</v>
+        <v>3464</v>
       </c>
       <c r="D1140" s="1">
         <v>8080</v>
       </c>
+      <c r="L1140" t="s">
+        <v>352</v>
+      </c>
       <c r="Q1140" t="s">
-        <v>3446</v>
+        <v>3465</v>
       </c>
     </row>
     <row r="1141" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1141" s="1" t="s">
-        <v>3447</v>
+        <v>3466</v>
       </c>
       <c r="C1141" t="s">
-        <v>3448</v>
+        <v>3356</v>
       </c>
       <c r="D1141" s="1" t="s">
-        <v>3006</v>
+        <v>2</v>
       </c>
       <c r="E1141" t="s">
-        <v>3006</v>
-      </c>
-      <c r="F1141" t="s">
-        <v>3899</v>
-      </c>
-      <c r="G1141" t="s">
-        <v>3899</v>
+        <v>2426</v>
       </c>
       <c r="L1141" t="s">
-        <v>2605</v>
-      </c>
-      <c r="M1141" t="s">
-        <v>5238</v>
+        <v>5070</v>
       </c>
       <c r="Q1141" t="s">
-        <v>4581</v>
+        <v>3467</v>
       </c>
     </row>
     <row r="1142" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1142" s="1" t="s">
-        <v>3463</v>
+        <v>3471</v>
       </c>
       <c r="C1142" t="s">
-        <v>3464</v>
+        <v>3472</v>
       </c>
       <c r="D1142" s="1">
-        <v>8080</v>
+        <v>68000</v>
+      </c>
+      <c r="E1142" t="s">
+        <v>2426</v>
       </c>
       <c r="L1142" t="s">
-        <v>352</v>
+        <v>3954</v>
       </c>
       <c r="Q1142" t="s">
-        <v>3465</v>
+        <v>3473</v>
       </c>
     </row>
     <row r="1143" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1143" s="1" t="s">
-        <v>3466</v>
+        <v>6914</v>
       </c>
       <c r="C1143" t="s">
-        <v>3356</v>
+        <v>6915</v>
       </c>
       <c r="D1143" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1143" t="s">
-        <v>2426</v>
+        <v>2</v>
       </c>
       <c r="L1143" t="s">
-        <v>5070</v>
+        <v>5238</v>
       </c>
       <c r="Q1143" t="s">
-        <v>3467</v>
+        <v>6916</v>
       </c>
     </row>
     <row r="1144" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1144" s="1" t="s">
-        <v>3471</v>
+        <v>6917</v>
       </c>
       <c r="C1144" t="s">
-        <v>3472</v>
-      </c>
-      <c r="D1144" s="1">
-        <v>68000</v>
+        <v>6915</v>
+      </c>
+      <c r="D1144" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="E1144" t="s">
-        <v>2426</v>
+        <v>2</v>
       </c>
       <c r="L1144" t="s">
-        <v>3954</v>
+        <v>5238</v>
       </c>
       <c r="Q1144" t="s">
-        <v>3473</v>
+        <v>6918</v>
       </c>
     </row>
     <row r="1145" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1145" s="1" t="s">
-        <v>6914</v>
+        <v>6919</v>
       </c>
       <c r="C1145" t="s">
-        <v>6915</v>
+        <v>6920</v>
       </c>
       <c r="D1145" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1145" t="s">
-        <v>2</v>
-      </c>
       <c r="L1145" t="s">
-        <v>5238</v>
+        <v>55</v>
       </c>
       <c r="Q1145" t="s">
-        <v>6916</v>
+        <v>6921</v>
       </c>
     </row>
     <row r="1146" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1146" s="1" t="s">
-        <v>6917</v>
+        <v>6922</v>
       </c>
       <c r="C1146" t="s">
-        <v>6915</v>
+        <v>6920</v>
       </c>
       <c r="D1146" s="1" t="s">
         <v>2</v>
@@ -51453,16 +51456,22 @@
       <c r="E1146" t="s">
         <v>2</v>
       </c>
+      <c r="F1146" t="s">
+        <v>2426</v>
+      </c>
       <c r="L1146" t="s">
-        <v>5238</v>
+        <v>542</v>
+      </c>
+      <c r="M1146" t="s">
+        <v>55</v>
       </c>
       <c r="Q1146" t="s">
-        <v>6918</v>
+        <v>6923</v>
       </c>
     </row>
     <row r="1147" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1147" s="1" t="s">
-        <v>6919</v>
+        <v>6924</v>
       </c>
       <c r="C1147" t="s">
         <v>6920</v>
@@ -51470,85 +51479,82 @@
       <c r="D1147" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1147" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1147" t="s">
+        <v>2426</v>
+      </c>
       <c r="L1147" t="s">
+        <v>542</v>
+      </c>
+      <c r="M1147" t="s">
         <v>55</v>
       </c>
       <c r="Q1147" t="s">
-        <v>6921</v>
+        <v>6925</v>
       </c>
     </row>
     <row r="1148" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1148" s="1" t="s">
-        <v>6922</v>
+        <v>6926</v>
       </c>
       <c r="C1148" t="s">
-        <v>6920</v>
-      </c>
-      <c r="D1148" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1148" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1148" t="s">
-        <v>2426</v>
+        <v>6927</v>
+      </c>
+      <c r="D1148" s="1">
+        <v>68000</v>
       </c>
       <c r="L1148" t="s">
-        <v>542</v>
-      </c>
-      <c r="M1148" t="s">
-        <v>55</v>
+        <v>1687</v>
       </c>
       <c r="Q1148" t="s">
-        <v>6923</v>
+        <v>6928</v>
       </c>
     </row>
     <row r="1149" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1149" s="1" t="s">
-        <v>6924</v>
+        <v>3494</v>
       </c>
       <c r="C1149" t="s">
-        <v>6920</v>
-      </c>
-      <c r="D1149" s="1" t="s">
-        <v>2</v>
+        <v>3495</v>
+      </c>
+      <c r="D1149" s="1">
+        <v>68000</v>
       </c>
       <c r="E1149" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1149" t="s">
         <v>2426</v>
       </c>
       <c r="L1149" t="s">
-        <v>542</v>
-      </c>
-      <c r="M1149" t="s">
-        <v>55</v>
+        <v>5549</v>
       </c>
       <c r="Q1149" t="s">
-        <v>6925</v>
+        <v>3496</v>
       </c>
     </row>
     <row r="1150" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1150" s="1" t="s">
-        <v>6926</v>
+        <v>3497</v>
       </c>
       <c r="C1150" t="s">
-        <v>6927</v>
+        <v>3495</v>
       </c>
       <c r="D1150" s="1">
         <v>68000</v>
       </c>
+      <c r="E1150" t="s">
+        <v>2426</v>
+      </c>
       <c r="L1150" t="s">
-        <v>1687</v>
+        <v>5549</v>
       </c>
       <c r="Q1150" t="s">
-        <v>6928</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="1151" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1151" s="1" t="s">
-        <v>3494</v>
+        <v>3498</v>
       </c>
       <c r="C1151" t="s">
         <v>3495</v>
@@ -51563,12 +51569,12 @@
         <v>5549</v>
       </c>
       <c r="Q1151" t="s">
-        <v>3496</v>
+        <v>3499</v>
       </c>
     </row>
     <row r="1152" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1152" s="1" t="s">
-        <v>3497</v>
+        <v>3500</v>
       </c>
       <c r="C1152" t="s">
         <v>3495</v>
@@ -51583,12 +51589,12 @@
         <v>5549</v>
       </c>
       <c r="Q1152" t="s">
-        <v>4587</v>
+        <v>3501</v>
       </c>
     </row>
     <row r="1153" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1153" s="1" t="s">
-        <v>3498</v>
+        <v>3502</v>
       </c>
       <c r="C1153" t="s">
         <v>3495</v>
@@ -51603,12 +51609,12 @@
         <v>5549</v>
       </c>
       <c r="Q1153" t="s">
-        <v>3499</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="1154" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1154" s="1" t="s">
-        <v>3500</v>
+        <v>3504</v>
       </c>
       <c r="C1154" t="s">
         <v>3495</v>
@@ -51623,12 +51629,12 @@
         <v>5549</v>
       </c>
       <c r="Q1154" t="s">
-        <v>3501</v>
+        <v>3505</v>
       </c>
     </row>
     <row r="1155" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1155" s="1" t="s">
-        <v>3502</v>
+        <v>3506</v>
       </c>
       <c r="C1155" t="s">
         <v>3495</v>
@@ -51643,12 +51649,12 @@
         <v>5549</v>
       </c>
       <c r="Q1155" t="s">
-        <v>3503</v>
+        <v>6929</v>
       </c>
     </row>
     <row r="1156" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1156" s="1" t="s">
-        <v>3504</v>
+        <v>6930</v>
       </c>
       <c r="C1156" t="s">
         <v>3495</v>
@@ -51663,12 +51669,12 @@
         <v>5549</v>
       </c>
       <c r="Q1156" t="s">
-        <v>3505</v>
+        <v>6931</v>
       </c>
     </row>
     <row r="1157" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1157" s="1" t="s">
-        <v>3506</v>
+        <v>3507</v>
       </c>
       <c r="C1157" t="s">
         <v>3495</v>
@@ -51683,12 +51689,12 @@
         <v>5549</v>
       </c>
       <c r="Q1157" t="s">
-        <v>6929</v>
+        <v>4952</v>
       </c>
     </row>
     <row r="1158" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1158" s="1" t="s">
-        <v>6930</v>
+        <v>3508</v>
       </c>
       <c r="C1158" t="s">
         <v>3495</v>
@@ -51703,12 +51709,12 @@
         <v>5549</v>
       </c>
       <c r="Q1158" t="s">
-        <v>6931</v>
+        <v>3509</v>
       </c>
     </row>
     <row r="1159" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1159" s="1" t="s">
-        <v>3507</v>
+        <v>3510</v>
       </c>
       <c r="C1159" t="s">
         <v>3495</v>
@@ -51723,12 +51729,12 @@
         <v>5549</v>
       </c>
       <c r="Q1159" t="s">
-        <v>4952</v>
+        <v>3511</v>
       </c>
     </row>
     <row r="1160" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1160" s="1" t="s">
-        <v>3508</v>
+        <v>3512</v>
       </c>
       <c r="C1160" t="s">
         <v>3495</v>
@@ -51743,12 +51749,12 @@
         <v>5549</v>
       </c>
       <c r="Q1160" t="s">
-        <v>3509</v>
+        <v>3513</v>
       </c>
     </row>
     <row r="1161" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1161" s="1" t="s">
-        <v>3510</v>
+        <v>3514</v>
       </c>
       <c r="C1161" t="s">
         <v>3495</v>
@@ -51763,12 +51769,12 @@
         <v>5549</v>
       </c>
       <c r="Q1161" t="s">
-        <v>3511</v>
+        <v>3515</v>
       </c>
     </row>
     <row r="1162" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1162" s="1" t="s">
-        <v>3512</v>
+        <v>3516</v>
       </c>
       <c r="C1162" t="s">
         <v>3495</v>
@@ -51783,12 +51789,12 @@
         <v>5549</v>
       </c>
       <c r="Q1162" t="s">
-        <v>3513</v>
+        <v>3517</v>
       </c>
     </row>
     <row r="1163" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1163" s="1" t="s">
-        <v>3514</v>
+        <v>3518</v>
       </c>
       <c r="C1163" t="s">
         <v>3495</v>
@@ -51803,12 +51809,12 @@
         <v>5549</v>
       </c>
       <c r="Q1163" t="s">
-        <v>3515</v>
+        <v>4953</v>
       </c>
     </row>
     <row r="1164" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1164" s="1" t="s">
-        <v>3516</v>
+        <v>3519</v>
       </c>
       <c r="C1164" t="s">
         <v>3495</v>
@@ -51823,12 +51829,12 @@
         <v>5549</v>
       </c>
       <c r="Q1164" t="s">
-        <v>3517</v>
+        <v>4954</v>
       </c>
     </row>
     <row r="1165" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1165" s="1" t="s">
-        <v>3518</v>
+        <v>3520</v>
       </c>
       <c r="C1165" t="s">
         <v>3495</v>
@@ -51843,12 +51849,12 @@
         <v>5549</v>
       </c>
       <c r="Q1165" t="s">
-        <v>4953</v>
+        <v>3521</v>
       </c>
     </row>
     <row r="1166" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1166" s="1" t="s">
-        <v>3519</v>
+        <v>3522</v>
       </c>
       <c r="C1166" t="s">
         <v>3495</v>
@@ -51863,12 +51869,12 @@
         <v>5549</v>
       </c>
       <c r="Q1166" t="s">
-        <v>4954</v>
+        <v>3523</v>
       </c>
     </row>
     <row r="1167" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1167" s="1" t="s">
-        <v>3520</v>
+        <v>3524</v>
       </c>
       <c r="C1167" t="s">
         <v>3495</v>
@@ -51883,12 +51889,12 @@
         <v>5549</v>
       </c>
       <c r="Q1167" t="s">
-        <v>3521</v>
+        <v>3525</v>
       </c>
     </row>
     <row r="1168" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1168" s="1" t="s">
-        <v>3522</v>
+        <v>3526</v>
       </c>
       <c r="C1168" t="s">
         <v>3495</v>
@@ -51903,12 +51909,12 @@
         <v>5549</v>
       </c>
       <c r="Q1168" t="s">
-        <v>3523</v>
+        <v>3527</v>
       </c>
     </row>
     <row r="1169" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1169" s="1" t="s">
-        <v>3524</v>
+        <v>3528</v>
       </c>
       <c r="C1169" t="s">
         <v>3495</v>
@@ -51923,12 +51929,12 @@
         <v>5549</v>
       </c>
       <c r="Q1169" t="s">
-        <v>3525</v>
+        <v>3529</v>
       </c>
     </row>
     <row r="1170" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1170" s="1" t="s">
-        <v>3526</v>
+        <v>3530</v>
       </c>
       <c r="C1170" t="s">
         <v>3495</v>
@@ -51943,12 +51949,12 @@
         <v>5549</v>
       </c>
       <c r="Q1170" t="s">
-        <v>3527</v>
+        <v>3531</v>
       </c>
     </row>
     <row r="1171" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1171" s="1" t="s">
-        <v>3528</v>
+        <v>3532</v>
       </c>
       <c r="C1171" t="s">
         <v>3495</v>
@@ -51963,12 +51969,12 @@
         <v>5549</v>
       </c>
       <c r="Q1171" t="s">
-        <v>3529</v>
+        <v>4955</v>
       </c>
     </row>
     <row r="1172" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1172" s="1" t="s">
-        <v>3530</v>
+        <v>3533</v>
       </c>
       <c r="C1172" t="s">
         <v>3495</v>
@@ -51983,12 +51989,12 @@
         <v>5549</v>
       </c>
       <c r="Q1172" t="s">
-        <v>3531</v>
+        <v>3534</v>
       </c>
     </row>
     <row r="1173" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1173" s="1" t="s">
-        <v>3532</v>
+        <v>3535</v>
       </c>
       <c r="C1173" t="s">
         <v>3495</v>
@@ -52003,12 +52009,12 @@
         <v>5549</v>
       </c>
       <c r="Q1173" t="s">
-        <v>4955</v>
+        <v>3536</v>
       </c>
     </row>
     <row r="1174" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1174" s="1" t="s">
-        <v>3533</v>
+        <v>3537</v>
       </c>
       <c r="C1174" t="s">
         <v>3495</v>
@@ -52023,12 +52029,12 @@
         <v>5549</v>
       </c>
       <c r="Q1174" t="s">
-        <v>3534</v>
+        <v>3538</v>
       </c>
     </row>
     <row r="1175" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1175" s="1" t="s">
-        <v>3535</v>
+        <v>3539</v>
       </c>
       <c r="C1175" t="s">
         <v>3495</v>
@@ -52043,12 +52049,12 @@
         <v>5549</v>
       </c>
       <c r="Q1175" t="s">
-        <v>3536</v>
+        <v>4956</v>
       </c>
     </row>
     <row r="1176" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1176" s="1" t="s">
-        <v>3537</v>
+        <v>3540</v>
       </c>
       <c r="C1176" t="s">
         <v>3495</v>
@@ -52063,12 +52069,12 @@
         <v>5549</v>
       </c>
       <c r="Q1176" t="s">
-        <v>3538</v>
+        <v>4588</v>
       </c>
     </row>
     <row r="1177" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1177" s="1" t="s">
-        <v>3539</v>
+        <v>3541</v>
       </c>
       <c r="C1177" t="s">
         <v>3495</v>
@@ -52083,12 +52089,12 @@
         <v>5549</v>
       </c>
       <c r="Q1177" t="s">
-        <v>4956</v>
+        <v>4589</v>
       </c>
     </row>
     <row r="1178" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1178" s="1" t="s">
-        <v>3540</v>
+        <v>3542</v>
       </c>
       <c r="C1178" t="s">
         <v>3495</v>
@@ -52103,12 +52109,12 @@
         <v>5549</v>
       </c>
       <c r="Q1178" t="s">
-        <v>4588</v>
+        <v>3543</v>
       </c>
     </row>
     <row r="1179" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1179" s="1" t="s">
-        <v>3541</v>
+        <v>3544</v>
       </c>
       <c r="C1179" t="s">
         <v>3495</v>
@@ -52123,12 +52129,12 @@
         <v>5549</v>
       </c>
       <c r="Q1179" t="s">
-        <v>4589</v>
+        <v>3545</v>
       </c>
     </row>
     <row r="1180" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1180" s="1" t="s">
-        <v>3542</v>
+        <v>3546</v>
       </c>
       <c r="C1180" t="s">
         <v>3495</v>
@@ -52143,12 +52149,12 @@
         <v>5549</v>
       </c>
       <c r="Q1180" t="s">
-        <v>3543</v>
+        <v>4957</v>
       </c>
     </row>
     <row r="1181" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1181" s="1" t="s">
-        <v>3544</v>
+        <v>3547</v>
       </c>
       <c r="C1181" t="s">
         <v>3495</v>
@@ -52163,12 +52169,12 @@
         <v>5549</v>
       </c>
       <c r="Q1181" t="s">
-        <v>3545</v>
+        <v>3548</v>
       </c>
     </row>
     <row r="1182" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1182" s="1" t="s">
-        <v>3546</v>
+        <v>3549</v>
       </c>
       <c r="C1182" t="s">
         <v>3495</v>
@@ -52183,12 +52189,12 @@
         <v>5549</v>
       </c>
       <c r="Q1182" t="s">
-        <v>4957</v>
+        <v>4590</v>
       </c>
     </row>
     <row r="1183" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1183" s="1" t="s">
-        <v>3547</v>
+        <v>3550</v>
       </c>
       <c r="C1183" t="s">
         <v>3495</v>
@@ -52203,12 +52209,12 @@
         <v>5549</v>
       </c>
       <c r="Q1183" t="s">
-        <v>3548</v>
+        <v>3551</v>
       </c>
     </row>
     <row r="1184" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1184" s="1" t="s">
-        <v>3549</v>
+        <v>3552</v>
       </c>
       <c r="C1184" t="s">
         <v>3495</v>
@@ -52223,12 +52229,12 @@
         <v>5549</v>
       </c>
       <c r="Q1184" t="s">
-        <v>4590</v>
+        <v>3553</v>
       </c>
     </row>
     <row r="1185" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1185" s="1" t="s">
-        <v>3550</v>
+        <v>3554</v>
       </c>
       <c r="C1185" t="s">
         <v>3495</v>
@@ -52243,12 +52249,12 @@
         <v>5549</v>
       </c>
       <c r="Q1185" t="s">
-        <v>3551</v>
+        <v>4958</v>
       </c>
     </row>
     <row r="1186" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1186" s="1" t="s">
-        <v>3552</v>
+        <v>3555</v>
       </c>
       <c r="C1186" t="s">
         <v>3495</v>
@@ -52263,12 +52269,12 @@
         <v>5549</v>
       </c>
       <c r="Q1186" t="s">
-        <v>3553</v>
+        <v>4591</v>
       </c>
     </row>
     <row r="1187" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1187" s="1" t="s">
-        <v>3554</v>
+        <v>3556</v>
       </c>
       <c r="C1187" t="s">
         <v>3495</v>
@@ -52283,12 +52289,12 @@
         <v>5549</v>
       </c>
       <c r="Q1187" t="s">
-        <v>4958</v>
+        <v>3557</v>
       </c>
     </row>
     <row r="1188" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1188" s="1" t="s">
-        <v>3555</v>
+        <v>3558</v>
       </c>
       <c r="C1188" t="s">
         <v>3495</v>
@@ -52303,12 +52309,12 @@
         <v>5549</v>
       </c>
       <c r="Q1188" t="s">
-        <v>4591</v>
+        <v>4959</v>
       </c>
     </row>
     <row r="1189" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1189" s="1" t="s">
-        <v>3556</v>
+        <v>3559</v>
       </c>
       <c r="C1189" t="s">
         <v>3495</v>
@@ -52323,12 +52329,12 @@
         <v>5549</v>
       </c>
       <c r="Q1189" t="s">
-        <v>3557</v>
+        <v>4592</v>
       </c>
     </row>
     <row r="1190" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1190" s="1" t="s">
-        <v>3558</v>
+        <v>3560</v>
       </c>
       <c r="C1190" t="s">
         <v>3495</v>
@@ -52343,12 +52349,12 @@
         <v>5549</v>
       </c>
       <c r="Q1190" t="s">
-        <v>4959</v>
+        <v>4593</v>
       </c>
     </row>
     <row r="1191" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1191" s="1" t="s">
-        <v>3559</v>
+        <v>3561</v>
       </c>
       <c r="C1191" t="s">
         <v>3495</v>
@@ -52363,12 +52369,12 @@
         <v>5549</v>
       </c>
       <c r="Q1191" t="s">
-        <v>4592</v>
+        <v>4960</v>
       </c>
     </row>
     <row r="1192" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1192" s="1" t="s">
-        <v>3560</v>
+        <v>3562</v>
       </c>
       <c r="C1192" t="s">
         <v>3495</v>
@@ -52383,12 +52389,12 @@
         <v>5549</v>
       </c>
       <c r="Q1192" t="s">
-        <v>4593</v>
+        <v>4594</v>
       </c>
     </row>
     <row r="1193" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1193" s="1" t="s">
-        <v>3561</v>
+        <v>3563</v>
       </c>
       <c r="C1193" t="s">
         <v>3495</v>
@@ -52403,12 +52409,12 @@
         <v>5549</v>
       </c>
       <c r="Q1193" t="s">
-        <v>4960</v>
+        <v>4961</v>
       </c>
     </row>
     <row r="1194" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1194" s="1" t="s">
-        <v>3562</v>
+        <v>3564</v>
       </c>
       <c r="C1194" t="s">
         <v>3495</v>
@@ -52423,12 +52429,12 @@
         <v>5549</v>
       </c>
       <c r="Q1194" t="s">
-        <v>4594</v>
+        <v>4962</v>
       </c>
     </row>
     <row r="1195" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1195" s="1" t="s">
-        <v>3563</v>
+        <v>3565</v>
       </c>
       <c r="C1195" t="s">
         <v>3495</v>
@@ -52443,12 +52449,12 @@
         <v>5549</v>
       </c>
       <c r="Q1195" t="s">
-        <v>4961</v>
+        <v>3566</v>
       </c>
     </row>
     <row r="1196" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1196" s="1" t="s">
-        <v>3564</v>
+        <v>3567</v>
       </c>
       <c r="C1196" t="s">
         <v>3495</v>
@@ -52463,12 +52469,12 @@
         <v>5549</v>
       </c>
       <c r="Q1196" t="s">
-        <v>4962</v>
+        <v>3568</v>
       </c>
     </row>
     <row r="1197" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1197" s="1" t="s">
-        <v>3565</v>
+        <v>3569</v>
       </c>
       <c r="C1197" t="s">
         <v>3495</v>
@@ -52483,12 +52489,12 @@
         <v>5549</v>
       </c>
       <c r="Q1197" t="s">
-        <v>3566</v>
+        <v>3570</v>
       </c>
     </row>
     <row r="1198" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1198" s="1" t="s">
-        <v>3567</v>
+        <v>3571</v>
       </c>
       <c r="C1198" t="s">
         <v>3495</v>
@@ -52503,12 +52509,12 @@
         <v>5549</v>
       </c>
       <c r="Q1198" t="s">
-        <v>3568</v>
+        <v>4595</v>
       </c>
     </row>
     <row r="1199" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1199" s="1" t="s">
-        <v>3569</v>
+        <v>3572</v>
       </c>
       <c r="C1199" t="s">
         <v>3495</v>
@@ -52523,12 +52529,12 @@
         <v>5549</v>
       </c>
       <c r="Q1199" t="s">
-        <v>3570</v>
+        <v>3573</v>
       </c>
     </row>
     <row r="1200" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1200" s="1" t="s">
-        <v>3571</v>
+        <v>3574</v>
       </c>
       <c r="C1200" t="s">
         <v>3495</v>
@@ -52543,12 +52549,12 @@
         <v>5549</v>
       </c>
       <c r="Q1200" t="s">
-        <v>4595</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="1201" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1201" s="1" t="s">
-        <v>3572</v>
+        <v>3576</v>
       </c>
       <c r="C1201" t="s">
         <v>3495</v>
@@ -52563,12 +52569,12 @@
         <v>5549</v>
       </c>
       <c r="Q1201" t="s">
-        <v>3573</v>
+        <v>4963</v>
       </c>
     </row>
     <row r="1202" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1202" s="1" t="s">
-        <v>3574</v>
+        <v>3577</v>
       </c>
       <c r="C1202" t="s">
         <v>3495</v>
@@ -52583,12 +52589,12 @@
         <v>5549</v>
       </c>
       <c r="Q1202" t="s">
-        <v>3575</v>
+        <v>3578</v>
       </c>
     </row>
     <row r="1203" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1203" s="1" t="s">
-        <v>3576</v>
+        <v>3579</v>
       </c>
       <c r="C1203" t="s">
         <v>3495</v>
@@ -52603,12 +52609,12 @@
         <v>5549</v>
       </c>
       <c r="Q1203" t="s">
-        <v>4963</v>
+        <v>4964</v>
       </c>
     </row>
     <row r="1204" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1204" s="1" t="s">
-        <v>3577</v>
+        <v>3580</v>
       </c>
       <c r="C1204" t="s">
         <v>3495</v>
@@ -52623,12 +52629,12 @@
         <v>5549</v>
       </c>
       <c r="Q1204" t="s">
-        <v>3578</v>
+        <v>4965</v>
       </c>
     </row>
     <row r="1205" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1205" s="1" t="s">
-        <v>3579</v>
+        <v>3581</v>
       </c>
       <c r="C1205" t="s">
         <v>3495</v>
@@ -52643,12 +52649,12 @@
         <v>5549</v>
       </c>
       <c r="Q1205" t="s">
-        <v>4964</v>
+        <v>4596</v>
       </c>
     </row>
     <row r="1206" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1206" s="1" t="s">
-        <v>3580</v>
+        <v>3582</v>
       </c>
       <c r="C1206" t="s">
         <v>3495</v>
@@ -52663,12 +52669,12 @@
         <v>5549</v>
       </c>
       <c r="Q1206" t="s">
-        <v>4965</v>
+        <v>4966</v>
       </c>
     </row>
     <row r="1207" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1207" s="1" t="s">
-        <v>3581</v>
+        <v>3583</v>
       </c>
       <c r="C1207" t="s">
         <v>3495</v>
@@ -52683,12 +52689,12 @@
         <v>5549</v>
       </c>
       <c r="Q1207" t="s">
-        <v>4596</v>
+        <v>4597</v>
       </c>
     </row>
     <row r="1208" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1208" s="1" t="s">
-        <v>3582</v>
+        <v>3584</v>
       </c>
       <c r="C1208" t="s">
         <v>3495</v>
@@ -52703,12 +52709,12 @@
         <v>5549</v>
       </c>
       <c r="Q1208" t="s">
-        <v>4966</v>
+        <v>4967</v>
       </c>
     </row>
     <row r="1209" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1209" s="1" t="s">
-        <v>3583</v>
+        <v>3585</v>
       </c>
       <c r="C1209" t="s">
         <v>3495</v>
@@ -52723,12 +52729,12 @@
         <v>5549</v>
       </c>
       <c r="Q1209" t="s">
-        <v>4597</v>
+        <v>3586</v>
       </c>
     </row>
     <row r="1210" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1210" s="1" t="s">
-        <v>3584</v>
+        <v>3587</v>
       </c>
       <c r="C1210" t="s">
         <v>3495</v>
@@ -52743,12 +52749,12 @@
         <v>5549</v>
       </c>
       <c r="Q1210" t="s">
-        <v>4967</v>
+        <v>4598</v>
       </c>
     </row>
     <row r="1211" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1211" s="1" t="s">
-        <v>3585</v>
+        <v>3588</v>
       </c>
       <c r="C1211" t="s">
         <v>3495</v>
@@ -52763,12 +52769,12 @@
         <v>5549</v>
       </c>
       <c r="Q1211" t="s">
-        <v>3586</v>
+        <v>4968</v>
       </c>
     </row>
     <row r="1212" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1212" s="1" t="s">
-        <v>3587</v>
+        <v>3589</v>
       </c>
       <c r="C1212" t="s">
         <v>3495</v>
@@ -52783,12 +52789,12 @@
         <v>5549</v>
       </c>
       <c r="Q1212" t="s">
-        <v>4598</v>
+        <v>3590</v>
       </c>
     </row>
     <row r="1213" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1213" s="1" t="s">
-        <v>3588</v>
+        <v>3591</v>
       </c>
       <c r="C1213" t="s">
         <v>3495</v>
@@ -52803,12 +52809,12 @@
         <v>5549</v>
       </c>
       <c r="Q1213" t="s">
-        <v>4968</v>
+        <v>3592</v>
       </c>
     </row>
     <row r="1214" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1214" s="1" t="s">
-        <v>3589</v>
+        <v>3593</v>
       </c>
       <c r="C1214" t="s">
         <v>3495</v>
@@ -52823,12 +52829,12 @@
         <v>5549</v>
       </c>
       <c r="Q1214" t="s">
-        <v>3590</v>
+        <v>4969</v>
       </c>
     </row>
     <row r="1215" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1215" s="1" t="s">
-        <v>3591</v>
+        <v>3594</v>
       </c>
       <c r="C1215" t="s">
         <v>3495</v>
@@ -52843,12 +52849,12 @@
         <v>5549</v>
       </c>
       <c r="Q1215" t="s">
-        <v>3592</v>
+        <v>3595</v>
       </c>
     </row>
     <row r="1216" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1216" s="1" t="s">
-        <v>3593</v>
+        <v>3596</v>
       </c>
       <c r="C1216" t="s">
         <v>3495</v>
@@ -52863,12 +52869,12 @@
         <v>5549</v>
       </c>
       <c r="Q1216" t="s">
-        <v>4969</v>
+        <v>4970</v>
       </c>
     </row>
     <row r="1217" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1217" s="1" t="s">
-        <v>3594</v>
+        <v>3597</v>
       </c>
       <c r="C1217" t="s">
         <v>3495</v>
@@ -52883,12 +52889,12 @@
         <v>5549</v>
       </c>
       <c r="Q1217" t="s">
-        <v>3595</v>
+        <v>4599</v>
       </c>
     </row>
     <row r="1218" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1218" s="1" t="s">
-        <v>3596</v>
+        <v>3598</v>
       </c>
       <c r="C1218" t="s">
         <v>3495</v>
@@ -52903,12 +52909,12 @@
         <v>5549</v>
       </c>
       <c r="Q1218" t="s">
-        <v>4970</v>
+        <v>4600</v>
       </c>
     </row>
     <row r="1219" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1219" s="1" t="s">
-        <v>3597</v>
+        <v>3599</v>
       </c>
       <c r="C1219" t="s">
         <v>3495</v>
@@ -52923,12 +52929,12 @@
         <v>5549</v>
       </c>
       <c r="Q1219" t="s">
-        <v>4599</v>
+        <v>4971</v>
       </c>
     </row>
     <row r="1220" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1220" s="1" t="s">
-        <v>3598</v>
+        <v>3600</v>
       </c>
       <c r="C1220" t="s">
         <v>3495</v>
@@ -52943,12 +52949,12 @@
         <v>5549</v>
       </c>
       <c r="Q1220" t="s">
-        <v>4600</v>
+        <v>4972</v>
       </c>
     </row>
     <row r="1221" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1221" s="1" t="s">
-        <v>3599</v>
+        <v>3601</v>
       </c>
       <c r="C1221" t="s">
         <v>3495</v>
@@ -52963,12 +52969,12 @@
         <v>5549</v>
       </c>
       <c r="Q1221" t="s">
-        <v>4971</v>
+        <v>3602</v>
       </c>
     </row>
     <row r="1222" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1222" s="1" t="s">
-        <v>3600</v>
+        <v>3603</v>
       </c>
       <c r="C1222" t="s">
         <v>3495</v>
@@ -52983,12 +52989,12 @@
         <v>5549</v>
       </c>
       <c r="Q1222" t="s">
-        <v>4972</v>
+        <v>4973</v>
       </c>
     </row>
     <row r="1223" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1223" s="1" t="s">
-        <v>3601</v>
+        <v>3604</v>
       </c>
       <c r="C1223" t="s">
         <v>3495</v>
@@ -53003,12 +53009,12 @@
         <v>5549</v>
       </c>
       <c r="Q1223" t="s">
-        <v>3602</v>
+        <v>3605</v>
       </c>
     </row>
     <row r="1224" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1224" s="1" t="s">
-        <v>3603</v>
+        <v>6932</v>
       </c>
       <c r="C1224" t="s">
         <v>3495</v>
@@ -53023,12 +53029,12 @@
         <v>5549</v>
       </c>
       <c r="Q1224" t="s">
-        <v>4973</v>
+        <v>4974</v>
       </c>
     </row>
     <row r="1225" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1225" s="1" t="s">
-        <v>3604</v>
+        <v>3607</v>
       </c>
       <c r="C1225" t="s">
         <v>3495</v>
@@ -53043,12 +53049,12 @@
         <v>5549</v>
       </c>
       <c r="Q1225" t="s">
-        <v>3605</v>
+        <v>3608</v>
       </c>
     </row>
     <row r="1226" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1226" s="1" t="s">
-        <v>6932</v>
+        <v>3609</v>
       </c>
       <c r="C1226" t="s">
         <v>3495</v>
@@ -53063,12 +53069,12 @@
         <v>5549</v>
       </c>
       <c r="Q1226" t="s">
-        <v>4974</v>
+        <v>3610</v>
       </c>
     </row>
     <row r="1227" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1227" s="1" t="s">
-        <v>3607</v>
+        <v>3611</v>
       </c>
       <c r="C1227" t="s">
         <v>3495</v>
@@ -53083,12 +53089,12 @@
         <v>5549</v>
       </c>
       <c r="Q1227" t="s">
-        <v>3608</v>
+        <v>4975</v>
       </c>
     </row>
     <row r="1228" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1228" s="1" t="s">
-        <v>3609</v>
+        <v>3612</v>
       </c>
       <c r="C1228" t="s">
         <v>3495</v>
@@ -53103,12 +53109,12 @@
         <v>5549</v>
       </c>
       <c r="Q1228" t="s">
-        <v>3610</v>
+        <v>4976</v>
       </c>
     </row>
     <row r="1229" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1229" s="1" t="s">
-        <v>3611</v>
+        <v>3613</v>
       </c>
       <c r="C1229" t="s">
         <v>3495</v>
@@ -53123,12 +53129,12 @@
         <v>5549</v>
       </c>
       <c r="Q1229" t="s">
-        <v>4975</v>
+        <v>3614</v>
       </c>
     </row>
     <row r="1230" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1230" s="1" t="s">
-        <v>3612</v>
+        <v>3615</v>
       </c>
       <c r="C1230" t="s">
         <v>3495</v>
@@ -53143,12 +53149,12 @@
         <v>5549</v>
       </c>
       <c r="Q1230" t="s">
-        <v>4976</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="1231" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1231" s="1" t="s">
-        <v>3613</v>
+        <v>3617</v>
       </c>
       <c r="C1231" t="s">
         <v>3495</v>
@@ -53163,12 +53169,12 @@
         <v>5549</v>
       </c>
       <c r="Q1231" t="s">
-        <v>3614</v>
+        <v>4977</v>
       </c>
     </row>
     <row r="1232" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1232" s="1" t="s">
-        <v>3615</v>
+        <v>3618</v>
       </c>
       <c r="C1232" t="s">
         <v>3495</v>
@@ -53183,12 +53189,12 @@
         <v>5549</v>
       </c>
       <c r="Q1232" t="s">
-        <v>3616</v>
+        <v>3619</v>
       </c>
     </row>
     <row r="1233" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1233" s="1" t="s">
-        <v>3617</v>
+        <v>3620</v>
       </c>
       <c r="C1233" t="s">
         <v>3495</v>
@@ -53203,12 +53209,12 @@
         <v>5549</v>
       </c>
       <c r="Q1233" t="s">
-        <v>4977</v>
+        <v>4978</v>
       </c>
     </row>
     <row r="1234" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1234" s="1" t="s">
-        <v>3618</v>
+        <v>3621</v>
       </c>
       <c r="C1234" t="s">
         <v>3495</v>
@@ -53223,12 +53229,12 @@
         <v>5549</v>
       </c>
       <c r="Q1234" t="s">
-        <v>3619</v>
+        <v>4979</v>
       </c>
     </row>
     <row r="1235" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1235" s="1" t="s">
-        <v>3620</v>
+        <v>3622</v>
       </c>
       <c r="C1235" t="s">
         <v>3495</v>
@@ -53243,12 +53249,12 @@
         <v>5549</v>
       </c>
       <c r="Q1235" t="s">
-        <v>4978</v>
+        <v>4980</v>
       </c>
     </row>
     <row r="1236" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1236" s="1" t="s">
-        <v>3621</v>
+        <v>3623</v>
       </c>
       <c r="C1236" t="s">
         <v>3495</v>
@@ -53263,12 +53269,12 @@
         <v>5549</v>
       </c>
       <c r="Q1236" t="s">
-        <v>4979</v>
+        <v>4601</v>
       </c>
     </row>
     <row r="1237" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1237" s="1" t="s">
-        <v>3622</v>
+        <v>3624</v>
       </c>
       <c r="C1237" t="s">
         <v>3495</v>
@@ -53283,12 +53289,12 @@
         <v>5549</v>
       </c>
       <c r="Q1237" t="s">
-        <v>4980</v>
+        <v>4981</v>
       </c>
     </row>
     <row r="1238" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1238" s="1" t="s">
-        <v>3623</v>
+        <v>3625</v>
       </c>
       <c r="C1238" t="s">
         <v>3495</v>
@@ -53303,12 +53309,12 @@
         <v>5549</v>
       </c>
       <c r="Q1238" t="s">
-        <v>4601</v>
+        <v>4602</v>
       </c>
     </row>
     <row r="1239" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1239" s="1" t="s">
-        <v>3624</v>
+        <v>3626</v>
       </c>
       <c r="C1239" t="s">
         <v>3495</v>
@@ -53323,12 +53329,12 @@
         <v>5549</v>
       </c>
       <c r="Q1239" t="s">
-        <v>4981</v>
+        <v>3627</v>
       </c>
     </row>
     <row r="1240" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1240" s="1" t="s">
-        <v>3625</v>
+        <v>3628</v>
       </c>
       <c r="C1240" t="s">
         <v>3495</v>
@@ -53343,12 +53349,12 @@
         <v>5549</v>
       </c>
       <c r="Q1240" t="s">
-        <v>4602</v>
+        <v>4982</v>
       </c>
     </row>
     <row r="1241" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1241" s="1" t="s">
-        <v>3626</v>
+        <v>3629</v>
       </c>
       <c r="C1241" t="s">
         <v>3495</v>
@@ -53363,12 +53369,12 @@
         <v>5549</v>
       </c>
       <c r="Q1241" t="s">
-        <v>3627</v>
+        <v>4603</v>
       </c>
     </row>
     <row r="1242" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1242" s="1" t="s">
-        <v>3628</v>
+        <v>3630</v>
       </c>
       <c r="C1242" t="s">
         <v>3495</v>
@@ -53383,12 +53389,12 @@
         <v>5549</v>
       </c>
       <c r="Q1242" t="s">
-        <v>4982</v>
+        <v>3631</v>
       </c>
     </row>
     <row r="1243" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1243" s="1" t="s">
-        <v>3629</v>
+        <v>3632</v>
       </c>
       <c r="C1243" t="s">
         <v>3495</v>
@@ -53403,12 +53409,12 @@
         <v>5549</v>
       </c>
       <c r="Q1243" t="s">
-        <v>4603</v>
+        <v>4983</v>
       </c>
     </row>
     <row r="1244" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1244" s="1" t="s">
-        <v>3630</v>
+        <v>3633</v>
       </c>
       <c r="C1244" t="s">
         <v>3495</v>
@@ -53423,12 +53429,12 @@
         <v>5549</v>
       </c>
       <c r="Q1244" t="s">
-        <v>3631</v>
+        <v>3634</v>
       </c>
     </row>
     <row r="1245" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1245" s="1" t="s">
-        <v>3632</v>
+        <v>3635</v>
       </c>
       <c r="C1245" t="s">
         <v>3495</v>
@@ -53443,12 +53449,12 @@
         <v>5549</v>
       </c>
       <c r="Q1245" t="s">
-        <v>4983</v>
+        <v>3636</v>
       </c>
     </row>
     <row r="1246" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1246" s="1" t="s">
-        <v>3633</v>
+        <v>3637</v>
       </c>
       <c r="C1246" t="s">
         <v>3495</v>
@@ -53463,12 +53469,12 @@
         <v>5549</v>
       </c>
       <c r="Q1246" t="s">
-        <v>3634</v>
+        <v>4604</v>
       </c>
     </row>
     <row r="1247" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1247" s="1" t="s">
-        <v>3635</v>
+        <v>3638</v>
       </c>
       <c r="C1247" t="s">
         <v>3495</v>
@@ -53483,12 +53489,12 @@
         <v>5549</v>
       </c>
       <c r="Q1247" t="s">
-        <v>3636</v>
+        <v>3639</v>
       </c>
     </row>
     <row r="1248" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1248" s="1" t="s">
-        <v>3637</v>
+        <v>3640</v>
       </c>
       <c r="C1248" t="s">
         <v>3495</v>
@@ -53503,12 +53509,12 @@
         <v>5549</v>
       </c>
       <c r="Q1248" t="s">
-        <v>4604</v>
+        <v>4984</v>
       </c>
     </row>
     <row r="1249" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1249" s="1" t="s">
-        <v>3638</v>
+        <v>3641</v>
       </c>
       <c r="C1249" t="s">
         <v>3495</v>
@@ -53523,12 +53529,12 @@
         <v>5549</v>
       </c>
       <c r="Q1249" t="s">
-        <v>3639</v>
+        <v>4985</v>
       </c>
     </row>
     <row r="1250" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1250" s="1" t="s">
-        <v>3640</v>
+        <v>3642</v>
       </c>
       <c r="C1250" t="s">
         <v>3495</v>
@@ -53543,12 +53549,12 @@
         <v>5549</v>
       </c>
       <c r="Q1250" t="s">
-        <v>4984</v>
+        <v>4605</v>
       </c>
     </row>
     <row r="1251" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1251" s="1" t="s">
-        <v>3641</v>
+        <v>3643</v>
       </c>
       <c r="C1251" t="s">
         <v>3495</v>
@@ -53563,12 +53569,12 @@
         <v>5549</v>
       </c>
       <c r="Q1251" t="s">
-        <v>4985</v>
+        <v>4986</v>
       </c>
     </row>
     <row r="1252" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1252" s="1" t="s">
-        <v>3642</v>
+        <v>3644</v>
       </c>
       <c r="C1252" t="s">
         <v>3495</v>
@@ -53583,12 +53589,12 @@
         <v>5549</v>
       </c>
       <c r="Q1252" t="s">
-        <v>4605</v>
+        <v>4987</v>
       </c>
     </row>
     <row r="1253" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1253" s="1" t="s">
-        <v>3643</v>
+        <v>3645</v>
       </c>
       <c r="C1253" t="s">
         <v>3495</v>
@@ -53603,12 +53609,12 @@
         <v>5549</v>
       </c>
       <c r="Q1253" t="s">
-        <v>4986</v>
+        <v>3646</v>
       </c>
     </row>
     <row r="1254" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1254" s="1" t="s">
-        <v>3644</v>
+        <v>3647</v>
       </c>
       <c r="C1254" t="s">
         <v>3495</v>
@@ -53623,12 +53629,12 @@
         <v>5549</v>
       </c>
       <c r="Q1254" t="s">
-        <v>4987</v>
+        <v>4988</v>
       </c>
     </row>
     <row r="1255" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1255" s="1" t="s">
-        <v>3645</v>
+        <v>3648</v>
       </c>
       <c r="C1255" t="s">
         <v>3495</v>
@@ -53643,12 +53649,12 @@
         <v>5549</v>
       </c>
       <c r="Q1255" t="s">
-        <v>3646</v>
+        <v>4989</v>
       </c>
     </row>
     <row r="1256" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1256" s="1" t="s">
-        <v>3647</v>
+        <v>3649</v>
       </c>
       <c r="C1256" t="s">
         <v>3495</v>
@@ -53663,12 +53669,12 @@
         <v>5549</v>
       </c>
       <c r="Q1256" t="s">
-        <v>4988</v>
+        <v>3650</v>
       </c>
     </row>
     <row r="1257" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1257" s="1" t="s">
-        <v>3648</v>
+        <v>3651</v>
       </c>
       <c r="C1257" t="s">
         <v>3495</v>
@@ -53683,12 +53689,12 @@
         <v>5549</v>
       </c>
       <c r="Q1257" t="s">
-        <v>4989</v>
+        <v>3652</v>
       </c>
     </row>
     <row r="1258" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1258" s="1" t="s">
-        <v>3649</v>
+        <v>3653</v>
       </c>
       <c r="C1258" t="s">
         <v>3495</v>
@@ -53703,12 +53709,12 @@
         <v>5549</v>
       </c>
       <c r="Q1258" t="s">
-        <v>3650</v>
+        <v>3654</v>
       </c>
     </row>
     <row r="1259" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1259" s="1" t="s">
-        <v>3651</v>
+        <v>3655</v>
       </c>
       <c r="C1259" t="s">
         <v>3495</v>
@@ -53723,12 +53729,12 @@
         <v>5549</v>
       </c>
       <c r="Q1259" t="s">
-        <v>3652</v>
+        <v>3656</v>
       </c>
     </row>
     <row r="1260" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1260" s="1" t="s">
-        <v>3653</v>
+        <v>3657</v>
       </c>
       <c r="C1260" t="s">
         <v>3495</v>
@@ -53743,12 +53749,12 @@
         <v>5549</v>
       </c>
       <c r="Q1260" t="s">
-        <v>3654</v>
+        <v>4990</v>
       </c>
     </row>
     <row r="1261" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1261" s="1" t="s">
-        <v>3655</v>
+        <v>3658</v>
       </c>
       <c r="C1261" t="s">
         <v>3495</v>
@@ -53763,12 +53769,12 @@
         <v>5549</v>
       </c>
       <c r="Q1261" t="s">
-        <v>3656</v>
+        <v>3659</v>
       </c>
     </row>
     <row r="1262" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1262" s="1" t="s">
-        <v>3657</v>
+        <v>3660</v>
       </c>
       <c r="C1262" t="s">
         <v>3495</v>
@@ -53783,12 +53789,12 @@
         <v>5549</v>
       </c>
       <c r="Q1262" t="s">
-        <v>4990</v>
+        <v>3661</v>
       </c>
     </row>
     <row r="1263" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1263" s="1" t="s">
-        <v>3658</v>
+        <v>3662</v>
       </c>
       <c r="C1263" t="s">
         <v>3495</v>
@@ -53803,12 +53809,12 @@
         <v>5549</v>
       </c>
       <c r="Q1263" t="s">
-        <v>3659</v>
+        <v>4991</v>
       </c>
     </row>
     <row r="1264" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1264" s="1" t="s">
-        <v>3660</v>
+        <v>3663</v>
       </c>
       <c r="C1264" t="s">
         <v>3495</v>
@@ -53823,12 +53829,12 @@
         <v>5549</v>
       </c>
       <c r="Q1264" t="s">
-        <v>3661</v>
+        <v>3664</v>
       </c>
     </row>
     <row r="1265" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1265" s="1" t="s">
-        <v>3662</v>
+        <v>3665</v>
       </c>
       <c r="C1265" t="s">
         <v>3495</v>
@@ -53843,12 +53849,12 @@
         <v>5549</v>
       </c>
       <c r="Q1265" t="s">
-        <v>4991</v>
+        <v>4992</v>
       </c>
     </row>
     <row r="1266" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1266" s="1" t="s">
-        <v>3663</v>
+        <v>3666</v>
       </c>
       <c r="C1266" t="s">
         <v>3495</v>
@@ -53863,12 +53869,12 @@
         <v>5549</v>
       </c>
       <c r="Q1266" t="s">
-        <v>3664</v>
+        <v>3667</v>
       </c>
     </row>
     <row r="1267" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1267" s="1" t="s">
-        <v>3665</v>
+        <v>3668</v>
       </c>
       <c r="C1267" t="s">
         <v>3495</v>
@@ -53883,12 +53889,12 @@
         <v>5549</v>
       </c>
       <c r="Q1267" t="s">
-        <v>4992</v>
+        <v>3669</v>
       </c>
     </row>
     <row r="1268" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1268" s="1" t="s">
-        <v>3666</v>
+        <v>3670</v>
       </c>
       <c r="C1268" t="s">
         <v>3495</v>
@@ -53903,12 +53909,12 @@
         <v>5549</v>
       </c>
       <c r="Q1268" t="s">
-        <v>3667</v>
+        <v>3671</v>
       </c>
     </row>
     <row r="1269" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1269" s="1" t="s">
-        <v>3668</v>
+        <v>3672</v>
       </c>
       <c r="C1269" t="s">
         <v>3495</v>
@@ -53923,12 +53929,12 @@
         <v>5549</v>
       </c>
       <c r="Q1269" t="s">
-        <v>3669</v>
+        <v>3673</v>
       </c>
     </row>
     <row r="1270" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1270" s="1" t="s">
-        <v>3670</v>
+        <v>3674</v>
       </c>
       <c r="C1270" t="s">
         <v>3495</v>
@@ -53943,12 +53949,12 @@
         <v>5549</v>
       </c>
       <c r="Q1270" t="s">
-        <v>3671</v>
+        <v>4993</v>
       </c>
     </row>
     <row r="1271" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1271" s="1" t="s">
-        <v>3672</v>
+        <v>3675</v>
       </c>
       <c r="C1271" t="s">
         <v>3495</v>
@@ -53963,12 +53969,12 @@
         <v>5549</v>
       </c>
       <c r="Q1271" t="s">
-        <v>3673</v>
+        <v>4994</v>
       </c>
     </row>
     <row r="1272" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1272" s="1" t="s">
-        <v>3674</v>
+        <v>3676</v>
       </c>
       <c r="C1272" t="s">
         <v>3495</v>
@@ -53983,12 +53989,12 @@
         <v>5549</v>
       </c>
       <c r="Q1272" t="s">
-        <v>4993</v>
+        <v>4995</v>
       </c>
     </row>
     <row r="1273" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1273" s="1" t="s">
-        <v>3675</v>
+        <v>3677</v>
       </c>
       <c r="C1273" t="s">
         <v>3495</v>
@@ -54003,12 +54009,12 @@
         <v>5549</v>
       </c>
       <c r="Q1273" t="s">
-        <v>4994</v>
+        <v>4996</v>
       </c>
     </row>
     <row r="1274" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1274" s="1" t="s">
-        <v>3676</v>
+        <v>3678</v>
       </c>
       <c r="C1274" t="s">
         <v>3495</v>
@@ -54023,12 +54029,12 @@
         <v>5549</v>
       </c>
       <c r="Q1274" t="s">
-        <v>4995</v>
+        <v>4997</v>
       </c>
     </row>
     <row r="1275" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1275" s="1" t="s">
-        <v>3677</v>
+        <v>3679</v>
       </c>
       <c r="C1275" t="s">
         <v>3495</v>
@@ -54043,12 +54049,12 @@
         <v>5549</v>
       </c>
       <c r="Q1275" t="s">
-        <v>4996</v>
+        <v>3680</v>
       </c>
     </row>
     <row r="1276" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1276" s="1" t="s">
-        <v>3678</v>
+        <v>3681</v>
       </c>
       <c r="C1276" t="s">
         <v>3495</v>
@@ -54063,12 +54069,12 @@
         <v>5549</v>
       </c>
       <c r="Q1276" t="s">
-        <v>4997</v>
+        <v>4606</v>
       </c>
     </row>
     <row r="1277" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1277" s="1" t="s">
-        <v>3679</v>
+        <v>3682</v>
       </c>
       <c r="C1277" t="s">
         <v>3495</v>
@@ -54083,12 +54089,12 @@
         <v>5549</v>
       </c>
       <c r="Q1277" t="s">
-        <v>3680</v>
+        <v>3683</v>
       </c>
     </row>
     <row r="1278" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1278" s="1" t="s">
-        <v>3681</v>
+        <v>6933</v>
       </c>
       <c r="C1278" t="s">
         <v>3495</v>
@@ -54103,12 +54109,12 @@
         <v>5549</v>
       </c>
       <c r="Q1278" t="s">
-        <v>4606</v>
+        <v>6934</v>
       </c>
     </row>
     <row r="1279" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1279" s="1" t="s">
-        <v>3682</v>
+        <v>6935</v>
       </c>
       <c r="C1279" t="s">
         <v>3495</v>
@@ -54123,12 +54129,12 @@
         <v>5549</v>
       </c>
       <c r="Q1279" t="s">
-        <v>3683</v>
+        <v>6936</v>
       </c>
     </row>
     <row r="1280" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1280" s="1" t="s">
-        <v>6933</v>
+        <v>6937</v>
       </c>
       <c r="C1280" t="s">
         <v>3495</v>
@@ -54143,12 +54149,12 @@
         <v>5549</v>
       </c>
       <c r="Q1280" t="s">
-        <v>6934</v>
+        <v>6938</v>
       </c>
     </row>
     <row r="1281" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1281" s="1" t="s">
-        <v>6935</v>
+        <v>6939</v>
       </c>
       <c r="C1281" t="s">
         <v>3495</v>
@@ -54163,12 +54169,12 @@
         <v>5549</v>
       </c>
       <c r="Q1281" t="s">
-        <v>6936</v>
+        <v>6940</v>
       </c>
     </row>
     <row r="1282" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1282" s="1" t="s">
-        <v>6937</v>
+        <v>6941</v>
       </c>
       <c r="C1282" t="s">
         <v>3495</v>
@@ -54183,12 +54189,12 @@
         <v>5549</v>
       </c>
       <c r="Q1282" t="s">
-        <v>6938</v>
+        <v>6942</v>
       </c>
     </row>
     <row r="1283" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1283" s="1" t="s">
-        <v>6939</v>
+        <v>6943</v>
       </c>
       <c r="C1283" t="s">
         <v>3495</v>
@@ -54203,12 +54209,12 @@
         <v>5549</v>
       </c>
       <c r="Q1283" t="s">
-        <v>6940</v>
+        <v>6944</v>
       </c>
     </row>
     <row r="1284" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1284" s="1" t="s">
-        <v>6941</v>
+        <v>6945</v>
       </c>
       <c r="C1284" t="s">
         <v>3495</v>
@@ -54223,12 +54229,12 @@
         <v>5549</v>
       </c>
       <c r="Q1284" t="s">
-        <v>6942</v>
+        <v>6946</v>
       </c>
     </row>
     <row r="1285" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1285" s="1" t="s">
-        <v>6943</v>
+        <v>6947</v>
       </c>
       <c r="C1285" t="s">
         <v>3495</v>
@@ -54243,12 +54249,12 @@
         <v>5549</v>
       </c>
       <c r="Q1285" t="s">
-        <v>6944</v>
+        <v>6948</v>
       </c>
     </row>
     <row r="1286" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1286" s="1" t="s">
-        <v>6945</v>
+        <v>6949</v>
       </c>
       <c r="C1286" t="s">
         <v>3495</v>
@@ -54263,12 +54269,12 @@
         <v>5549</v>
       </c>
       <c r="Q1286" t="s">
-        <v>6946</v>
+        <v>6950</v>
       </c>
     </row>
     <row r="1287" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1287" s="1" t="s">
-        <v>6947</v>
+        <v>6951</v>
       </c>
       <c r="C1287" t="s">
         <v>3495</v>
@@ -54283,12 +54289,12 @@
         <v>5549</v>
       </c>
       <c r="Q1287" t="s">
-        <v>6948</v>
+        <v>6952</v>
       </c>
     </row>
     <row r="1288" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1288" s="1" t="s">
-        <v>6949</v>
+        <v>6953</v>
       </c>
       <c r="C1288" t="s">
         <v>3495</v>
@@ -54303,69 +54309,81 @@
         <v>5549</v>
       </c>
       <c r="Q1288" t="s">
-        <v>6950</v>
+        <v>6954</v>
       </c>
     </row>
     <row r="1289" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1289" s="1" t="s">
-        <v>6951</v>
+        <v>2668</v>
       </c>
       <c r="C1289" t="s">
-        <v>3495</v>
+        <v>2669</v>
       </c>
       <c r="D1289" s="1">
         <v>68000</v>
       </c>
-      <c r="E1289" t="s">
-        <v>2426</v>
-      </c>
       <c r="L1289" t="s">
-        <v>5549</v>
+        <v>2670</v>
       </c>
       <c r="Q1289" t="s">
-        <v>6952</v>
+        <v>2671</v>
       </c>
     </row>
     <row r="1290" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1290" s="1" t="s">
-        <v>6953</v>
+        <v>2691</v>
       </c>
       <c r="C1290" t="s">
-        <v>3495</v>
+        <v>2689</v>
       </c>
       <c r="D1290" s="1">
-        <v>68000</v>
+        <v>68010</v>
       </c>
       <c r="E1290" t="s">
-        <v>2426</v>
+        <v>351</v>
       </c>
       <c r="L1290" t="s">
-        <v>5549</v>
+        <v>5238</v>
+      </c>
+      <c r="M1290" t="s">
+        <v>2534</v>
+      </c>
+      <c r="N1290" t="s">
+        <v>3889</v>
       </c>
       <c r="Q1290" t="s">
-        <v>6954</v>
+        <v>4870</v>
       </c>
     </row>
     <row r="1291" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1291" s="1" t="s">
-        <v>2668</v>
+        <v>2688</v>
       </c>
       <c r="C1291" t="s">
-        <v>2669</v>
+        <v>2689</v>
       </c>
       <c r="D1291" s="1">
-        <v>68000</v>
+        <v>68010</v>
+      </c>
+      <c r="E1291" t="s">
+        <v>351</v>
       </c>
       <c r="L1291" t="s">
-        <v>2670</v>
+        <v>5238</v>
+      </c>
+      <c r="M1291" t="s">
+        <v>2534</v>
+      </c>
+      <c r="N1291" t="s">
+        <v>3889</v>
       </c>
       <c r="Q1291" t="s">
-        <v>2671</v>
+        <v>4867</v>
       </c>
     </row>
     <row r="1292" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1292" s="1" t="s">
-        <v>2691</v>
+        <v>2690</v>
       </c>
       <c r="C1292" t="s">
         <v>2689</v>
@@ -54386,12 +54404,12 @@
         <v>3889</v>
       </c>
       <c r="Q1292" t="s">
-        <v>4870</v>
+        <v>4868</v>
       </c>
     </row>
     <row r="1293" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1293" s="1" t="s">
-        <v>2688</v>
+        <v>6487</v>
       </c>
       <c r="C1293" t="s">
         <v>2689</v>
@@ -54412,12 +54430,12 @@
         <v>3889</v>
       </c>
       <c r="Q1293" t="s">
-        <v>4867</v>
+        <v>4869</v>
       </c>
     </row>
     <row r="1294" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1294" s="1" t="s">
-        <v>2690</v>
+        <v>6488</v>
       </c>
       <c r="C1294" t="s">
         <v>2689</v>
@@ -54438,12 +54456,12 @@
         <v>3889</v>
       </c>
       <c r="Q1294" t="s">
-        <v>4868</v>
+        <v>6489</v>
       </c>
     </row>
     <row r="1295" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1295" s="1" t="s">
-        <v>6487</v>
+        <v>2692</v>
       </c>
       <c r="C1295" t="s">
         <v>2689</v>
@@ -54464,12 +54482,12 @@
         <v>3889</v>
       </c>
       <c r="Q1295" t="s">
-        <v>4869</v>
+        <v>4871</v>
       </c>
     </row>
     <row r="1296" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1296" s="1" t="s">
-        <v>6488</v>
+        <v>2693</v>
       </c>
       <c r="C1296" t="s">
         <v>2689</v>
@@ -54490,12 +54508,12 @@
         <v>3889</v>
       </c>
       <c r="Q1296" t="s">
-        <v>6489</v>
+        <v>4872</v>
       </c>
     </row>
     <row r="1297" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1297" s="1" t="s">
-        <v>2692</v>
+        <v>2694</v>
       </c>
       <c r="C1297" t="s">
         <v>2689</v>
@@ -54516,12 +54534,12 @@
         <v>3889</v>
       </c>
       <c r="Q1297" t="s">
-        <v>4871</v>
+        <v>4873</v>
       </c>
     </row>
     <row r="1298" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1298" s="1" t="s">
-        <v>2693</v>
+        <v>2695</v>
       </c>
       <c r="C1298" t="s">
         <v>2689</v>
@@ -54542,12 +54560,12 @@
         <v>3889</v>
       </c>
       <c r="Q1298" t="s">
-        <v>4872</v>
+        <v>4874</v>
       </c>
     </row>
     <row r="1299" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1299" s="1" t="s">
-        <v>2694</v>
+        <v>6490</v>
       </c>
       <c r="C1299" t="s">
         <v>2689</v>
@@ -54568,12 +54586,12 @@
         <v>3889</v>
       </c>
       <c r="Q1299" t="s">
-        <v>4873</v>
+        <v>6491</v>
       </c>
     </row>
     <row r="1300" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1300" s="1" t="s">
-        <v>2695</v>
+        <v>2696</v>
       </c>
       <c r="C1300" t="s">
         <v>2689</v>
@@ -54594,12 +54612,12 @@
         <v>3889</v>
       </c>
       <c r="Q1300" t="s">
-        <v>4874</v>
+        <v>4875</v>
       </c>
     </row>
     <row r="1301" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1301" s="1" t="s">
-        <v>6490</v>
+        <v>2697</v>
       </c>
       <c r="C1301" t="s">
         <v>2689</v>
@@ -54620,18 +54638,18 @@
         <v>3889</v>
       </c>
       <c r="Q1301" t="s">
-        <v>6491</v>
+        <v>4876</v>
       </c>
     </row>
     <row r="1302" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1302" s="1" t="s">
-        <v>2696</v>
+        <v>2698</v>
       </c>
       <c r="C1302" t="s">
-        <v>2689</v>
-      </c>
-      <c r="D1302" s="1">
-        <v>68010</v>
+        <v>2699</v>
+      </c>
+      <c r="D1302" s="1" t="s">
+        <v>2700</v>
       </c>
       <c r="E1302" t="s">
         <v>351</v>
@@ -54640,24 +54658,24 @@
         <v>5238</v>
       </c>
       <c r="M1302" t="s">
-        <v>2534</v>
+        <v>2538</v>
       </c>
       <c r="N1302" t="s">
         <v>3889</v>
       </c>
       <c r="Q1302" t="s">
-        <v>4875</v>
+        <v>4877</v>
       </c>
     </row>
     <row r="1303" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1303" s="1" t="s">
-        <v>2697</v>
+        <v>2701</v>
       </c>
       <c r="C1303" t="s">
-        <v>2689</v>
-      </c>
-      <c r="D1303" s="1">
-        <v>68010</v>
+        <v>2699</v>
+      </c>
+      <c r="D1303" s="1" t="s">
+        <v>2700</v>
       </c>
       <c r="E1303" t="s">
         <v>351</v>
@@ -54666,18 +54684,15 @@
         <v>5238</v>
       </c>
       <c r="M1303" t="s">
-        <v>2534</v>
-      </c>
-      <c r="N1303" t="s">
-        <v>3889</v>
+        <v>2538</v>
       </c>
       <c r="Q1303" t="s">
-        <v>4876</v>
+        <v>4416</v>
       </c>
     </row>
     <row r="1304" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1304" s="1" t="s">
-        <v>2698</v>
+        <v>2702</v>
       </c>
       <c r="C1304" t="s">
         <v>2699</v>
@@ -54694,16 +54709,13 @@
       <c r="M1304" t="s">
         <v>2538</v>
       </c>
-      <c r="N1304" t="s">
-        <v>3889</v>
-      </c>
       <c r="Q1304" t="s">
-        <v>4877</v>
+        <v>4417</v>
       </c>
     </row>
     <row r="1305" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1305" s="1" t="s">
-        <v>2701</v>
+        <v>6492</v>
       </c>
       <c r="C1305" t="s">
         <v>2699</v>
@@ -54720,13 +54732,16 @@
       <c r="M1305" t="s">
         <v>2538</v>
       </c>
+      <c r="N1305" t="s">
+        <v>3889</v>
+      </c>
       <c r="Q1305" t="s">
-        <v>4416</v>
+        <v>4878</v>
       </c>
     </row>
     <row r="1306" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1306" s="1" t="s">
-        <v>2702</v>
+        <v>2703</v>
       </c>
       <c r="C1306" t="s">
         <v>2699</v>
@@ -54743,13 +54758,16 @@
       <c r="M1306" t="s">
         <v>2538</v>
       </c>
+      <c r="N1306" t="s">
+        <v>3889</v>
+      </c>
       <c r="Q1306" t="s">
-        <v>4417</v>
+        <v>4879</v>
       </c>
     </row>
     <row r="1307" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1307" s="1" t="s">
-        <v>6492</v>
+        <v>2704</v>
       </c>
       <c r="C1307" t="s">
         <v>2699</v>
@@ -54770,12 +54788,12 @@
         <v>3889</v>
       </c>
       <c r="Q1307" t="s">
-        <v>4878</v>
+        <v>4880</v>
       </c>
     </row>
     <row r="1308" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1308" s="1" t="s">
-        <v>2703</v>
+        <v>2705</v>
       </c>
       <c r="C1308" t="s">
         <v>2699</v>
@@ -54796,63 +54814,11 @@
         <v>3889</v>
       </c>
       <c r="Q1308" t="s">
-        <v>4879</v>
-      </c>
-    </row>
-    <row r="1309" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B1309" s="1" t="s">
-        <v>2704</v>
-      </c>
-      <c r="C1309" t="s">
-        <v>2699</v>
-      </c>
-      <c r="D1309" s="1" t="s">
-        <v>2700</v>
-      </c>
-      <c r="E1309" t="s">
-        <v>351</v>
-      </c>
-      <c r="L1309" t="s">
-        <v>5238</v>
-      </c>
-      <c r="M1309" t="s">
-        <v>2538</v>
-      </c>
-      <c r="N1309" t="s">
-        <v>3889</v>
-      </c>
-      <c r="Q1309" t="s">
-        <v>4880</v>
-      </c>
-    </row>
-    <row r="1310" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B1310" s="1" t="s">
-        <v>2705</v>
-      </c>
-      <c r="C1310" t="s">
-        <v>2699</v>
-      </c>
-      <c r="D1310" s="1" t="s">
-        <v>2700</v>
-      </c>
-      <c r="E1310" t="s">
-        <v>351</v>
-      </c>
-      <c r="L1310" t="s">
-        <v>5238</v>
-      </c>
-      <c r="M1310" t="s">
-        <v>2538</v>
-      </c>
-      <c r="N1310" t="s">
-        <v>3889</v>
-      </c>
-      <c r="Q1310" t="s">
         <v>4881</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:R1290"/>
+  <autoFilter ref="B1:R1288"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -54863,7 +54829,7 @@
   <dimension ref="B1:Q468"/>
   <sheetViews>
     <sheetView topLeftCell="A454" workbookViewId="0">
-      <selection activeCell="D470" sqref="D470"/>
+      <selection activeCell="A469" sqref="A469:XFD470"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -64524,10 +64490,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R1185"/>
+  <dimension ref="B1:R1187"/>
   <sheetViews>
     <sheetView topLeftCell="A1171" workbookViewId="0">
-      <selection activeCell="A1181" sqref="A1181:XFD1185"/>
+      <selection activeCell="A1186" sqref="A1186:XFD1187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -89788,6 +89754,40 @@
         <v>6170</v>
       </c>
     </row>
+    <row r="1186" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B1186" s="1" t="s">
+        <v>3439</v>
+      </c>
+      <c r="C1186" t="s">
+        <v>3440</v>
+      </c>
+      <c r="D1186" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="E1186" t="s">
+        <v>3888</v>
+      </c>
+      <c r="Q1186" t="s">
+        <v>3441</v>
+      </c>
+    </row>
+    <row r="1187" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B1187" s="1" t="s">
+        <v>3442</v>
+      </c>
+      <c r="C1187" t="s">
+        <v>3440</v>
+      </c>
+      <c r="D1187" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="E1187" t="s">
+        <v>3888</v>
+      </c>
+      <c r="Q1187" t="s">
+        <v>3443</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
added spcforce NOT TESTED driver
</commit_message>
<xml_diff>
--- a/compatibility_list.xlsx
+++ b/compatibility_list.xlsx
@@ -21,9 +21,9 @@
     <sheet name="To Check" sheetId="13" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">WIP!$B$1:$R$1288</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">WIP!$B$1:$R$1285</definedName>
     <definedName name="DETAILS" localSheetId="4">WIP!#REF!</definedName>
-    <definedName name="DETAILS_1" localSheetId="4">WIP!$B$1:$Q$1288</definedName>
+    <definedName name="DETAILS_1" localSheetId="4">WIP!$B$1:$Q$1285</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25879,10 +25879,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Q1308"/>
+  <dimension ref="B1:Q1305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1125" workbookViewId="0">
-      <selection activeCell="C1136" sqref="C1136"/>
+    <sheetView tabSelected="1" topLeftCell="A1107" workbookViewId="0">
+      <selection activeCell="B1117" sqref="B1117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -50805,212 +50805,218 @@
     </row>
     <row r="1117" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1117" s="1" t="s">
-        <v>6853</v>
+        <v>6858</v>
       </c>
       <c r="C1117" t="s">
-        <v>6854</v>
+        <v>6859</v>
       </c>
       <c r="D1117" s="1" t="s">
-        <v>3469</v>
+        <v>6860</v>
       </c>
       <c r="E1117" t="s">
-        <v>3794</v>
+        <v>6861</v>
+      </c>
+      <c r="F1117" t="s">
+        <v>6862</v>
       </c>
       <c r="L1117" t="s">
-        <v>1900</v>
+        <v>6863</v>
+      </c>
+      <c r="M1117" t="s">
+        <v>6864</v>
+      </c>
+      <c r="N1117" t="s">
+        <v>6865</v>
+      </c>
+      <c r="O1117" t="s">
+        <v>6866</v>
       </c>
       <c r="Q1117" t="s">
-        <v>6855</v>
+        <v>6867</v>
       </c>
     </row>
     <row r="1118" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1118" s="1" t="s">
-        <v>6856</v>
+        <v>6868</v>
       </c>
       <c r="C1118" t="s">
-        <v>6854</v>
+        <v>6859</v>
       </c>
       <c r="D1118" s="1" t="s">
-        <v>3469</v>
+        <v>6860</v>
       </c>
       <c r="E1118" t="s">
-        <v>3794</v>
+        <v>6861</v>
+      </c>
+      <c r="F1118" t="s">
+        <v>6862</v>
       </c>
       <c r="L1118" t="s">
-        <v>1900</v>
+        <v>6863</v>
+      </c>
+      <c r="M1118" t="s">
+        <v>6864</v>
+      </c>
+      <c r="N1118" t="s">
+        <v>6865</v>
+      </c>
+      <c r="O1118" t="s">
+        <v>6866</v>
       </c>
       <c r="Q1118" t="s">
-        <v>6857</v>
+        <v>6869</v>
       </c>
     </row>
     <row r="1119" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1119" s="1" t="s">
-        <v>3468</v>
+        <v>6870</v>
       </c>
       <c r="C1119" t="s">
-        <v>6854</v>
+        <v>6859</v>
       </c>
       <c r="D1119" s="1" t="s">
-        <v>3469</v>
+        <v>6860</v>
       </c>
       <c r="E1119" t="s">
-        <v>3794</v>
+        <v>6861</v>
+      </c>
+      <c r="F1119" t="s">
+        <v>6862</v>
       </c>
       <c r="L1119" t="s">
-        <v>1900</v>
+        <v>6863</v>
+      </c>
+      <c r="M1119" t="s">
+        <v>6864</v>
+      </c>
+      <c r="N1119" t="s">
+        <v>6865</v>
+      </c>
+      <c r="O1119" t="s">
+        <v>6866</v>
       </c>
       <c r="Q1119" t="s">
-        <v>3470</v>
+        <v>6871</v>
       </c>
     </row>
     <row r="1120" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1120" s="1" t="s">
-        <v>6858</v>
+        <v>6872</v>
       </c>
       <c r="C1120" t="s">
-        <v>6859</v>
+        <v>6873</v>
       </c>
       <c r="D1120" s="1" t="s">
-        <v>6860</v>
+        <v>2</v>
       </c>
       <c r="E1120" t="s">
-        <v>6861</v>
-      </c>
-      <c r="F1120" t="s">
-        <v>6862</v>
+        <v>2426</v>
       </c>
       <c r="L1120" t="s">
-        <v>6863</v>
+        <v>5071</v>
       </c>
       <c r="M1120" t="s">
-        <v>6864</v>
-      </c>
-      <c r="N1120" t="s">
-        <v>6865</v>
-      </c>
-      <c r="O1120" t="s">
-        <v>6866</v>
+        <v>3974</v>
       </c>
       <c r="Q1120" t="s">
-        <v>6867</v>
+        <v>6874</v>
       </c>
     </row>
     <row r="1121" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1121" s="1" t="s">
-        <v>6868</v>
+        <v>3490</v>
       </c>
       <c r="C1121" t="s">
-        <v>6859</v>
+        <v>6873</v>
       </c>
       <c r="D1121" s="1" t="s">
-        <v>6860</v>
+        <v>2</v>
       </c>
       <c r="E1121" t="s">
-        <v>6861</v>
-      </c>
-      <c r="F1121" t="s">
-        <v>6862</v>
+        <v>2426</v>
       </c>
       <c r="L1121" t="s">
-        <v>6863</v>
+        <v>5071</v>
       </c>
       <c r="M1121" t="s">
-        <v>6864</v>
-      </c>
-      <c r="N1121" t="s">
-        <v>6865</v>
-      </c>
-      <c r="O1121" t="s">
-        <v>6866</v>
+        <v>3974</v>
       </c>
       <c r="Q1121" t="s">
-        <v>6869</v>
+        <v>6875</v>
       </c>
     </row>
     <row r="1122" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1122" s="1" t="s">
-        <v>6870</v>
+        <v>6876</v>
       </c>
       <c r="C1122" t="s">
-        <v>6859</v>
-      </c>
-      <c r="D1122" s="1" t="s">
-        <v>6860</v>
+        <v>6877</v>
+      </c>
+      <c r="D1122" s="1">
+        <v>68000</v>
       </c>
       <c r="E1122" t="s">
-        <v>6861</v>
-      </c>
-      <c r="F1122" t="s">
-        <v>6862</v>
+        <v>2426</v>
       </c>
       <c r="L1122" t="s">
-        <v>6863</v>
+        <v>5071</v>
       </c>
       <c r="M1122" t="s">
-        <v>6864</v>
-      </c>
-      <c r="N1122" t="s">
-        <v>6865</v>
-      </c>
-      <c r="O1122" t="s">
-        <v>6866</v>
+        <v>1687</v>
       </c>
       <c r="Q1122" t="s">
-        <v>6871</v>
+        <v>6878</v>
       </c>
     </row>
     <row r="1123" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1123" s="1" t="s">
-        <v>6872</v>
+        <v>6879</v>
       </c>
       <c r="C1123" t="s">
-        <v>6873</v>
-      </c>
-      <c r="D1123" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1123" t="s">
-        <v>2426</v>
+        <v>6877</v>
+      </c>
+      <c r="D1123" s="1">
+        <v>68000</v>
       </c>
       <c r="L1123" t="s">
-        <v>5071</v>
-      </c>
-      <c r="M1123" t="s">
-        <v>3974</v>
+        <v>1687</v>
       </c>
       <c r="Q1123" t="s">
-        <v>6874</v>
+        <v>6880</v>
       </c>
     </row>
     <row r="1124" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1124" s="1" t="s">
-        <v>3490</v>
+        <v>6881</v>
       </c>
       <c r="C1124" t="s">
-        <v>6873</v>
-      </c>
-      <c r="D1124" s="1" t="s">
-        <v>2</v>
+        <v>6882</v>
+      </c>
+      <c r="D1124" s="1">
+        <v>68000</v>
       </c>
       <c r="E1124" t="s">
         <v>2426</v>
       </c>
       <c r="L1124" t="s">
+        <v>5070</v>
+      </c>
+      <c r="M1124" t="s">
         <v>5071</v>
       </c>
-      <c r="M1124" t="s">
-        <v>3974</v>
+      <c r="N1124" t="s">
+        <v>1687</v>
       </c>
       <c r="Q1124" t="s">
-        <v>6875</v>
+        <v>6883</v>
       </c>
     </row>
     <row r="1125" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1125" s="1" t="s">
-        <v>6876</v>
+        <v>6884</v>
       </c>
       <c r="C1125" t="s">
-        <v>6877</v>
+        <v>6882</v>
       </c>
       <c r="D1125" s="1">
         <v>68000</v>
@@ -51019,90 +51025,90 @@
         <v>2426</v>
       </c>
       <c r="L1125" t="s">
+        <v>5070</v>
+      </c>
+      <c r="M1125" t="s">
         <v>5071</v>
       </c>
-      <c r="M1125" t="s">
+      <c r="N1125" t="s">
         <v>1687</v>
       </c>
       <c r="Q1125" t="s">
-        <v>6878</v>
+        <v>6885</v>
       </c>
     </row>
     <row r="1126" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1126" s="1" t="s">
-        <v>6879</v>
+        <v>6886</v>
       </c>
       <c r="C1126" t="s">
-        <v>6877</v>
+        <v>6882</v>
       </c>
       <c r="D1126" s="1">
         <v>68000</v>
       </c>
+      <c r="E1126" t="s">
+        <v>2426</v>
+      </c>
       <c r="L1126" t="s">
+        <v>5070</v>
+      </c>
+      <c r="M1126" t="s">
+        <v>5071</v>
+      </c>
+      <c r="N1126" t="s">
         <v>1687</v>
       </c>
       <c r="Q1126" t="s">
-        <v>6880</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="1127" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1127" s="1" t="s">
-        <v>6881</v>
+        <v>6888</v>
       </c>
       <c r="C1127" t="s">
-        <v>6882</v>
+        <v>6889</v>
       </c>
       <c r="D1127" s="1">
         <v>68000</v>
       </c>
-      <c r="E1127" t="s">
-        <v>2426</v>
-      </c>
       <c r="L1127" t="s">
-        <v>5070</v>
+        <v>5071</v>
       </c>
       <c r="M1127" t="s">
-        <v>5071</v>
-      </c>
-      <c r="N1127" t="s">
         <v>1687</v>
       </c>
       <c r="Q1127" t="s">
-        <v>6883</v>
+        <v>6890</v>
       </c>
     </row>
     <row r="1128" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1128" s="1" t="s">
-        <v>6884</v>
+        <v>6891</v>
       </c>
       <c r="C1128" t="s">
-        <v>6882</v>
+        <v>6889</v>
       </c>
       <c r="D1128" s="1">
         <v>68000</v>
       </c>
-      <c r="E1128" t="s">
-        <v>2426</v>
-      </c>
       <c r="L1128" t="s">
-        <v>5070</v>
+        <v>5071</v>
       </c>
       <c r="M1128" t="s">
-        <v>5071</v>
-      </c>
-      <c r="N1128" t="s">
         <v>1687</v>
       </c>
       <c r="Q1128" t="s">
-        <v>6885</v>
+        <v>6892</v>
       </c>
     </row>
     <row r="1129" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1129" s="1" t="s">
-        <v>6886</v>
+        <v>6893</v>
       </c>
       <c r="C1129" t="s">
-        <v>6882</v>
+        <v>6894</v>
       </c>
       <c r="D1129" s="1">
         <v>68000</v>
@@ -51111,47 +51117,50 @@
         <v>2426</v>
       </c>
       <c r="L1129" t="s">
-        <v>5070</v>
+        <v>5238</v>
       </c>
       <c r="M1129" t="s">
-        <v>5071</v>
-      </c>
-      <c r="N1129" t="s">
         <v>1687</v>
       </c>
       <c r="Q1129" t="s">
-        <v>6887</v>
+        <v>6895</v>
       </c>
     </row>
     <row r="1130" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1130" s="1" t="s">
-        <v>6888</v>
+        <v>6896</v>
       </c>
       <c r="C1130" t="s">
-        <v>6889</v>
+        <v>6894</v>
       </c>
       <c r="D1130" s="1">
         <v>68000</v>
       </c>
+      <c r="E1130" t="s">
+        <v>2426</v>
+      </c>
       <c r="L1130" t="s">
-        <v>5071</v>
+        <v>5238</v>
       </c>
       <c r="M1130" t="s">
         <v>1687</v>
       </c>
       <c r="Q1130" t="s">
-        <v>6890</v>
+        <v>6897</v>
       </c>
     </row>
     <row r="1131" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1131" s="1" t="s">
-        <v>6891</v>
+        <v>6898</v>
       </c>
       <c r="C1131" t="s">
-        <v>6889</v>
+        <v>6899</v>
       </c>
       <c r="D1131" s="1">
         <v>68000</v>
+      </c>
+      <c r="E1131" t="s">
+        <v>2426</v>
       </c>
       <c r="L1131" t="s">
         <v>5071</v>
@@ -51160,238 +51169,226 @@
         <v>1687</v>
       </c>
       <c r="Q1131" t="s">
-        <v>6892</v>
+        <v>6900</v>
       </c>
     </row>
     <row r="1132" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1132" s="1" t="s">
-        <v>6893</v>
+        <v>3419</v>
       </c>
       <c r="C1132" t="s">
-        <v>6894</v>
-      </c>
-      <c r="D1132" s="1">
-        <v>68000</v>
+        <v>3420</v>
+      </c>
+      <c r="D1132" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="E1132" t="s">
         <v>2426</v>
       </c>
       <c r="L1132" t="s">
-        <v>5238</v>
-      </c>
-      <c r="M1132" t="s">
-        <v>1687</v>
+        <v>1155</v>
       </c>
       <c r="Q1132" t="s">
-        <v>6895</v>
+        <v>3421</v>
       </c>
     </row>
     <row r="1133" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1133" s="1" t="s">
-        <v>6896</v>
+        <v>3422</v>
       </c>
       <c r="C1133" t="s">
-        <v>6894</v>
-      </c>
-      <c r="D1133" s="1">
-        <v>68000</v>
-      </c>
-      <c r="E1133" t="s">
-        <v>2426</v>
+        <v>3423</v>
+      </c>
+      <c r="D1133" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="L1133" t="s">
-        <v>5238</v>
-      </c>
-      <c r="M1133" t="s">
-        <v>1687</v>
+        <v>1155</v>
       </c>
       <c r="Q1133" t="s">
-        <v>6897</v>
+        <v>3424</v>
       </c>
     </row>
     <row r="1134" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1134" s="1" t="s">
-        <v>6898</v>
+        <v>3425</v>
       </c>
       <c r="C1134" t="s">
-        <v>6899</v>
-      </c>
-      <c r="D1134" s="1">
-        <v>68000</v>
-      </c>
-      <c r="E1134" t="s">
-        <v>2426</v>
+        <v>3423</v>
+      </c>
+      <c r="D1134" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="L1134" t="s">
-        <v>5071</v>
-      </c>
-      <c r="M1134" t="s">
-        <v>1687</v>
+        <v>1155</v>
       </c>
       <c r="Q1134" t="s">
-        <v>6900</v>
+        <v>3426</v>
       </c>
     </row>
     <row r="1135" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1135" s="1" t="s">
-        <v>3419</v>
+        <v>3444</v>
       </c>
       <c r="C1135" t="s">
-        <v>3420</v>
-      </c>
-      <c r="D1135" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1135" t="s">
-        <v>2426</v>
-      </c>
-      <c r="L1135" t="s">
-        <v>1155</v>
+        <v>3445</v>
+      </c>
+      <c r="D1135" s="1">
+        <v>8080</v>
       </c>
       <c r="Q1135" t="s">
-        <v>3421</v>
+        <v>3446</v>
       </c>
     </row>
     <row r="1136" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1136" s="1" t="s">
-        <v>3422</v>
+        <v>3447</v>
       </c>
       <c r="C1136" t="s">
-        <v>3423</v>
+        <v>3448</v>
       </c>
       <c r="D1136" s="1" t="s">
-        <v>2</v>
+        <v>3006</v>
+      </c>
+      <c r="E1136" t="s">
+        <v>3006</v>
+      </c>
+      <c r="F1136" t="s">
+        <v>3899</v>
+      </c>
+      <c r="G1136" t="s">
+        <v>3899</v>
       </c>
       <c r="L1136" t="s">
-        <v>1155</v>
+        <v>2605</v>
+      </c>
+      <c r="M1136" t="s">
+        <v>5238</v>
       </c>
       <c r="Q1136" t="s">
-        <v>3424</v>
+        <v>4581</v>
       </c>
     </row>
     <row r="1137" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1137" s="1" t="s">
-        <v>3425</v>
+        <v>3463</v>
       </c>
       <c r="C1137" t="s">
-        <v>3423</v>
-      </c>
-      <c r="D1137" s="1" t="s">
-        <v>2</v>
+        <v>3464</v>
+      </c>
+      <c r="D1137" s="1">
+        <v>8080</v>
       </c>
       <c r="L1137" t="s">
-        <v>1155</v>
+        <v>352</v>
       </c>
       <c r="Q1137" t="s">
-        <v>3426</v>
+        <v>3465</v>
       </c>
     </row>
     <row r="1138" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1138" s="1" t="s">
-        <v>3444</v>
+        <v>3466</v>
       </c>
       <c r="C1138" t="s">
-        <v>3445</v>
-      </c>
-      <c r="D1138" s="1">
-        <v>8080</v>
+        <v>3356</v>
+      </c>
+      <c r="D1138" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1138" t="s">
+        <v>2426</v>
+      </c>
+      <c r="L1138" t="s">
+        <v>5070</v>
       </c>
       <c r="Q1138" t="s">
-        <v>3446</v>
+        <v>3467</v>
       </c>
     </row>
     <row r="1139" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1139" s="1" t="s">
-        <v>3447</v>
+        <v>3471</v>
       </c>
       <c r="C1139" t="s">
-        <v>3448</v>
-      </c>
-      <c r="D1139" s="1" t="s">
-        <v>3006</v>
+        <v>3472</v>
+      </c>
+      <c r="D1139" s="1">
+        <v>68000</v>
       </c>
       <c r="E1139" t="s">
-        <v>3006</v>
-      </c>
-      <c r="F1139" t="s">
-        <v>3899</v>
-      </c>
-      <c r="G1139" t="s">
-        <v>3899</v>
+        <v>2426</v>
       </c>
       <c r="L1139" t="s">
-        <v>2605</v>
-      </c>
-      <c r="M1139" t="s">
-        <v>5238</v>
+        <v>3954</v>
       </c>
       <c r="Q1139" t="s">
-        <v>4581</v>
+        <v>3473</v>
       </c>
     </row>
     <row r="1140" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1140" s="1" t="s">
-        <v>3463</v>
+        <v>6914</v>
       </c>
       <c r="C1140" t="s">
-        <v>3464</v>
-      </c>
-      <c r="D1140" s="1">
-        <v>8080</v>
+        <v>6915</v>
+      </c>
+      <c r="D1140" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1140" t="s">
+        <v>2</v>
       </c>
       <c r="L1140" t="s">
-        <v>352</v>
+        <v>5238</v>
       </c>
       <c r="Q1140" t="s">
-        <v>3465</v>
+        <v>6916</v>
       </c>
     </row>
     <row r="1141" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1141" s="1" t="s">
-        <v>3466</v>
+        <v>6917</v>
       </c>
       <c r="C1141" t="s">
-        <v>3356</v>
+        <v>6915</v>
       </c>
       <c r="D1141" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1141" t="s">
-        <v>2426</v>
+        <v>2</v>
       </c>
       <c r="L1141" t="s">
-        <v>5070</v>
+        <v>5238</v>
       </c>
       <c r="Q1141" t="s">
-        <v>3467</v>
+        <v>6918</v>
       </c>
     </row>
     <row r="1142" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1142" s="1" t="s">
-        <v>3471</v>
+        <v>6919</v>
       </c>
       <c r="C1142" t="s">
-        <v>3472</v>
-      </c>
-      <c r="D1142" s="1">
-        <v>68000</v>
-      </c>
-      <c r="E1142" t="s">
-        <v>2426</v>
+        <v>6920</v>
+      </c>
+      <c r="D1142" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="L1142" t="s">
-        <v>3954</v>
+        <v>55</v>
       </c>
       <c r="Q1142" t="s">
-        <v>3473</v>
+        <v>6921</v>
       </c>
     </row>
     <row r="1143" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1143" s="1" t="s">
-        <v>6914</v>
+        <v>6922</v>
       </c>
       <c r="C1143" t="s">
-        <v>6915</v>
+        <v>6920</v>
       </c>
       <c r="D1143" s="1" t="s">
         <v>2</v>
@@ -51399,19 +51396,25 @@
       <c r="E1143" t="s">
         <v>2</v>
       </c>
+      <c r="F1143" t="s">
+        <v>2426</v>
+      </c>
       <c r="L1143" t="s">
-        <v>5238</v>
+        <v>542</v>
+      </c>
+      <c r="M1143" t="s">
+        <v>55</v>
       </c>
       <c r="Q1143" t="s">
-        <v>6916</v>
+        <v>6923</v>
       </c>
     </row>
     <row r="1144" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1144" s="1" t="s">
-        <v>6917</v>
+        <v>6924</v>
       </c>
       <c r="C1144" t="s">
-        <v>6915</v>
+        <v>6920</v>
       </c>
       <c r="D1144" s="1" t="s">
         <v>2</v>
@@ -51419,102 +51422,99 @@
       <c r="E1144" t="s">
         <v>2</v>
       </c>
+      <c r="F1144" t="s">
+        <v>2426</v>
+      </c>
       <c r="L1144" t="s">
-        <v>5238</v>
+        <v>542</v>
+      </c>
+      <c r="M1144" t="s">
+        <v>55</v>
       </c>
       <c r="Q1144" t="s">
-        <v>6918</v>
+        <v>6925</v>
       </c>
     </row>
     <row r="1145" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1145" s="1" t="s">
-        <v>6919</v>
+        <v>6926</v>
       </c>
       <c r="C1145" t="s">
-        <v>6920</v>
-      </c>
-      <c r="D1145" s="1" t="s">
-        <v>2</v>
+        <v>6927</v>
+      </c>
+      <c r="D1145" s="1">
+        <v>68000</v>
       </c>
       <c r="L1145" t="s">
-        <v>55</v>
+        <v>1687</v>
       </c>
       <c r="Q1145" t="s">
-        <v>6921</v>
+        <v>6928</v>
       </c>
     </row>
     <row r="1146" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1146" s="1" t="s">
-        <v>6922</v>
+        <v>3494</v>
       </c>
       <c r="C1146" t="s">
-        <v>6920</v>
-      </c>
-      <c r="D1146" s="1" t="s">
-        <v>2</v>
+        <v>3495</v>
+      </c>
+      <c r="D1146" s="1">
+        <v>68000</v>
       </c>
       <c r="E1146" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1146" t="s">
         <v>2426</v>
       </c>
       <c r="L1146" t="s">
-        <v>542</v>
-      </c>
-      <c r="M1146" t="s">
-        <v>55</v>
+        <v>5549</v>
       </c>
       <c r="Q1146" t="s">
-        <v>6923</v>
+        <v>3496</v>
       </c>
     </row>
     <row r="1147" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1147" s="1" t="s">
-        <v>6924</v>
+        <v>3497</v>
       </c>
       <c r="C1147" t="s">
-        <v>6920</v>
-      </c>
-      <c r="D1147" s="1" t="s">
-        <v>2</v>
+        <v>3495</v>
+      </c>
+      <c r="D1147" s="1">
+        <v>68000</v>
       </c>
       <c r="E1147" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1147" t="s">
         <v>2426</v>
       </c>
       <c r="L1147" t="s">
-        <v>542</v>
-      </c>
-      <c r="M1147" t="s">
-        <v>55</v>
+        <v>5549</v>
       </c>
       <c r="Q1147" t="s">
-        <v>6925</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="1148" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1148" s="1" t="s">
-        <v>6926</v>
+        <v>3498</v>
       </c>
       <c r="C1148" t="s">
-        <v>6927</v>
+        <v>3495</v>
       </c>
       <c r="D1148" s="1">
         <v>68000</v>
       </c>
+      <c r="E1148" t="s">
+        <v>2426</v>
+      </c>
       <c r="L1148" t="s">
-        <v>1687</v>
+        <v>5549</v>
       </c>
       <c r="Q1148" t="s">
-        <v>6928</v>
+        <v>3499</v>
       </c>
     </row>
     <row r="1149" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1149" s="1" t="s">
-        <v>3494</v>
+        <v>3500</v>
       </c>
       <c r="C1149" t="s">
         <v>3495</v>
@@ -51529,12 +51529,12 @@
         <v>5549</v>
       </c>
       <c r="Q1149" t="s">
-        <v>3496</v>
+        <v>3501</v>
       </c>
     </row>
     <row r="1150" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1150" s="1" t="s">
-        <v>3497</v>
+        <v>3502</v>
       </c>
       <c r="C1150" t="s">
         <v>3495</v>
@@ -51549,12 +51549,12 @@
         <v>5549</v>
       </c>
       <c r="Q1150" t="s">
-        <v>4587</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="1151" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1151" s="1" t="s">
-        <v>3498</v>
+        <v>3504</v>
       </c>
       <c r="C1151" t="s">
         <v>3495</v>
@@ -51569,12 +51569,12 @@
         <v>5549</v>
       </c>
       <c r="Q1151" t="s">
-        <v>3499</v>
+        <v>3505</v>
       </c>
     </row>
     <row r="1152" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1152" s="1" t="s">
-        <v>3500</v>
+        <v>3506</v>
       </c>
       <c r="C1152" t="s">
         <v>3495</v>
@@ -51589,12 +51589,12 @@
         <v>5549</v>
       </c>
       <c r="Q1152" t="s">
-        <v>3501</v>
+        <v>6929</v>
       </c>
     </row>
     <row r="1153" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1153" s="1" t="s">
-        <v>3502</v>
+        <v>6930</v>
       </c>
       <c r="C1153" t="s">
         <v>3495</v>
@@ -51609,12 +51609,12 @@
         <v>5549</v>
       </c>
       <c r="Q1153" t="s">
-        <v>3503</v>
+        <v>6931</v>
       </c>
     </row>
     <row r="1154" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1154" s="1" t="s">
-        <v>3504</v>
+        <v>3507</v>
       </c>
       <c r="C1154" t="s">
         <v>3495</v>
@@ -51629,12 +51629,12 @@
         <v>5549</v>
       </c>
       <c r="Q1154" t="s">
-        <v>3505</v>
+        <v>4952</v>
       </c>
     </row>
     <row r="1155" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1155" s="1" t="s">
-        <v>3506</v>
+        <v>3508</v>
       </c>
       <c r="C1155" t="s">
         <v>3495</v>
@@ -51649,12 +51649,12 @@
         <v>5549</v>
       </c>
       <c r="Q1155" t="s">
-        <v>6929</v>
+        <v>3509</v>
       </c>
     </row>
     <row r="1156" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1156" s="1" t="s">
-        <v>6930</v>
+        <v>3510</v>
       </c>
       <c r="C1156" t="s">
         <v>3495</v>
@@ -51669,12 +51669,12 @@
         <v>5549</v>
       </c>
       <c r="Q1156" t="s">
-        <v>6931</v>
+        <v>3511</v>
       </c>
     </row>
     <row r="1157" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1157" s="1" t="s">
-        <v>3507</v>
+        <v>3512</v>
       </c>
       <c r="C1157" t="s">
         <v>3495</v>
@@ -51689,12 +51689,12 @@
         <v>5549</v>
       </c>
       <c r="Q1157" t="s">
-        <v>4952</v>
+        <v>3513</v>
       </c>
     </row>
     <row r="1158" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1158" s="1" t="s">
-        <v>3508</v>
+        <v>3514</v>
       </c>
       <c r="C1158" t="s">
         <v>3495</v>
@@ -51709,12 +51709,12 @@
         <v>5549</v>
       </c>
       <c r="Q1158" t="s">
-        <v>3509</v>
+        <v>3515</v>
       </c>
     </row>
     <row r="1159" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1159" s="1" t="s">
-        <v>3510</v>
+        <v>3516</v>
       </c>
       <c r="C1159" t="s">
         <v>3495</v>
@@ -51729,12 +51729,12 @@
         <v>5549</v>
       </c>
       <c r="Q1159" t="s">
-        <v>3511</v>
+        <v>3517</v>
       </c>
     </row>
     <row r="1160" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1160" s="1" t="s">
-        <v>3512</v>
+        <v>3518</v>
       </c>
       <c r="C1160" t="s">
         <v>3495</v>
@@ -51749,12 +51749,12 @@
         <v>5549</v>
       </c>
       <c r="Q1160" t="s">
-        <v>3513</v>
+        <v>4953</v>
       </c>
     </row>
     <row r="1161" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1161" s="1" t="s">
-        <v>3514</v>
+        <v>3519</v>
       </c>
       <c r="C1161" t="s">
         <v>3495</v>
@@ -51769,12 +51769,12 @@
         <v>5549</v>
       </c>
       <c r="Q1161" t="s">
-        <v>3515</v>
+        <v>4954</v>
       </c>
     </row>
     <row r="1162" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1162" s="1" t="s">
-        <v>3516</v>
+        <v>3520</v>
       </c>
       <c r="C1162" t="s">
         <v>3495</v>
@@ -51789,12 +51789,12 @@
         <v>5549</v>
       </c>
       <c r="Q1162" t="s">
-        <v>3517</v>
+        <v>3521</v>
       </c>
     </row>
     <row r="1163" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1163" s="1" t="s">
-        <v>3518</v>
+        <v>3522</v>
       </c>
       <c r="C1163" t="s">
         <v>3495</v>
@@ -51809,12 +51809,12 @@
         <v>5549</v>
       </c>
       <c r="Q1163" t="s">
-        <v>4953</v>
+        <v>3523</v>
       </c>
     </row>
     <row r="1164" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1164" s="1" t="s">
-        <v>3519</v>
+        <v>3524</v>
       </c>
       <c r="C1164" t="s">
         <v>3495</v>
@@ -51829,12 +51829,12 @@
         <v>5549</v>
       </c>
       <c r="Q1164" t="s">
-        <v>4954</v>
+        <v>3525</v>
       </c>
     </row>
     <row r="1165" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1165" s="1" t="s">
-        <v>3520</v>
+        <v>3526</v>
       </c>
       <c r="C1165" t="s">
         <v>3495</v>
@@ -51849,12 +51849,12 @@
         <v>5549</v>
       </c>
       <c r="Q1165" t="s">
-        <v>3521</v>
+        <v>3527</v>
       </c>
     </row>
     <row r="1166" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1166" s="1" t="s">
-        <v>3522</v>
+        <v>3528</v>
       </c>
       <c r="C1166" t="s">
         <v>3495</v>
@@ -51869,12 +51869,12 @@
         <v>5549</v>
       </c>
       <c r="Q1166" t="s">
-        <v>3523</v>
+        <v>3529</v>
       </c>
     </row>
     <row r="1167" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1167" s="1" t="s">
-        <v>3524</v>
+        <v>3530</v>
       </c>
       <c r="C1167" t="s">
         <v>3495</v>
@@ -51889,12 +51889,12 @@
         <v>5549</v>
       </c>
       <c r="Q1167" t="s">
-        <v>3525</v>
+        <v>3531</v>
       </c>
     </row>
     <row r="1168" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1168" s="1" t="s">
-        <v>3526</v>
+        <v>3532</v>
       </c>
       <c r="C1168" t="s">
         <v>3495</v>
@@ -51909,12 +51909,12 @@
         <v>5549</v>
       </c>
       <c r="Q1168" t="s">
-        <v>3527</v>
+        <v>4955</v>
       </c>
     </row>
     <row r="1169" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1169" s="1" t="s">
-        <v>3528</v>
+        <v>3533</v>
       </c>
       <c r="C1169" t="s">
         <v>3495</v>
@@ -51929,12 +51929,12 @@
         <v>5549</v>
       </c>
       <c r="Q1169" t="s">
-        <v>3529</v>
+        <v>3534</v>
       </c>
     </row>
     <row r="1170" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1170" s="1" t="s">
-        <v>3530</v>
+        <v>3535</v>
       </c>
       <c r="C1170" t="s">
         <v>3495</v>
@@ -51949,12 +51949,12 @@
         <v>5549</v>
       </c>
       <c r="Q1170" t="s">
-        <v>3531</v>
+        <v>3536</v>
       </c>
     </row>
     <row r="1171" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1171" s="1" t="s">
-        <v>3532</v>
+        <v>3537</v>
       </c>
       <c r="C1171" t="s">
         <v>3495</v>
@@ -51969,12 +51969,12 @@
         <v>5549</v>
       </c>
       <c r="Q1171" t="s">
-        <v>4955</v>
+        <v>3538</v>
       </c>
     </row>
     <row r="1172" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1172" s="1" t="s">
-        <v>3533</v>
+        <v>3539</v>
       </c>
       <c r="C1172" t="s">
         <v>3495</v>
@@ -51989,12 +51989,12 @@
         <v>5549</v>
       </c>
       <c r="Q1172" t="s">
-        <v>3534</v>
+        <v>4956</v>
       </c>
     </row>
     <row r="1173" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1173" s="1" t="s">
-        <v>3535</v>
+        <v>3540</v>
       </c>
       <c r="C1173" t="s">
         <v>3495</v>
@@ -52009,12 +52009,12 @@
         <v>5549</v>
       </c>
       <c r="Q1173" t="s">
-        <v>3536</v>
+        <v>4588</v>
       </c>
     </row>
     <row r="1174" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1174" s="1" t="s">
-        <v>3537</v>
+        <v>3541</v>
       </c>
       <c r="C1174" t="s">
         <v>3495</v>
@@ -52029,12 +52029,12 @@
         <v>5549</v>
       </c>
       <c r="Q1174" t="s">
-        <v>3538</v>
+        <v>4589</v>
       </c>
     </row>
     <row r="1175" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1175" s="1" t="s">
-        <v>3539</v>
+        <v>3542</v>
       </c>
       <c r="C1175" t="s">
         <v>3495</v>
@@ -52049,12 +52049,12 @@
         <v>5549</v>
       </c>
       <c r="Q1175" t="s">
-        <v>4956</v>
+        <v>3543</v>
       </c>
     </row>
     <row r="1176" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1176" s="1" t="s">
-        <v>3540</v>
+        <v>3544</v>
       </c>
       <c r="C1176" t="s">
         <v>3495</v>
@@ -52069,12 +52069,12 @@
         <v>5549</v>
       </c>
       <c r="Q1176" t="s">
-        <v>4588</v>
+        <v>3545</v>
       </c>
     </row>
     <row r="1177" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1177" s="1" t="s">
-        <v>3541</v>
+        <v>3546</v>
       </c>
       <c r="C1177" t="s">
         <v>3495</v>
@@ -52089,12 +52089,12 @@
         <v>5549</v>
       </c>
       <c r="Q1177" t="s">
-        <v>4589</v>
+        <v>4957</v>
       </c>
     </row>
     <row r="1178" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1178" s="1" t="s">
-        <v>3542</v>
+        <v>3547</v>
       </c>
       <c r="C1178" t="s">
         <v>3495</v>
@@ -52109,12 +52109,12 @@
         <v>5549</v>
       </c>
       <c r="Q1178" t="s">
-        <v>3543</v>
+        <v>3548</v>
       </c>
     </row>
     <row r="1179" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1179" s="1" t="s">
-        <v>3544</v>
+        <v>3549</v>
       </c>
       <c r="C1179" t="s">
         <v>3495</v>
@@ -52129,12 +52129,12 @@
         <v>5549</v>
       </c>
       <c r="Q1179" t="s">
-        <v>3545</v>
+        <v>4590</v>
       </c>
     </row>
     <row r="1180" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1180" s="1" t="s">
-        <v>3546</v>
+        <v>3550</v>
       </c>
       <c r="C1180" t="s">
         <v>3495</v>
@@ -52149,12 +52149,12 @@
         <v>5549</v>
       </c>
       <c r="Q1180" t="s">
-        <v>4957</v>
+        <v>3551</v>
       </c>
     </row>
     <row r="1181" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1181" s="1" t="s">
-        <v>3547</v>
+        <v>3552</v>
       </c>
       <c r="C1181" t="s">
         <v>3495</v>
@@ -52169,12 +52169,12 @@
         <v>5549</v>
       </c>
       <c r="Q1181" t="s">
-        <v>3548</v>
+        <v>3553</v>
       </c>
     </row>
     <row r="1182" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1182" s="1" t="s">
-        <v>3549</v>
+        <v>3554</v>
       </c>
       <c r="C1182" t="s">
         <v>3495</v>
@@ -52189,12 +52189,12 @@
         <v>5549</v>
       </c>
       <c r="Q1182" t="s">
-        <v>4590</v>
+        <v>4958</v>
       </c>
     </row>
     <row r="1183" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1183" s="1" t="s">
-        <v>3550</v>
+        <v>3555</v>
       </c>
       <c r="C1183" t="s">
         <v>3495</v>
@@ -52209,12 +52209,12 @@
         <v>5549</v>
       </c>
       <c r="Q1183" t="s">
-        <v>3551</v>
+        <v>4591</v>
       </c>
     </row>
     <row r="1184" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1184" s="1" t="s">
-        <v>3552</v>
+        <v>3556</v>
       </c>
       <c r="C1184" t="s">
         <v>3495</v>
@@ -52229,12 +52229,12 @@
         <v>5549</v>
       </c>
       <c r="Q1184" t="s">
-        <v>3553</v>
+        <v>3557</v>
       </c>
     </row>
     <row r="1185" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1185" s="1" t="s">
-        <v>3554</v>
+        <v>3558</v>
       </c>
       <c r="C1185" t="s">
         <v>3495</v>
@@ -52249,12 +52249,12 @@
         <v>5549</v>
       </c>
       <c r="Q1185" t="s">
-        <v>4958</v>
+        <v>4959</v>
       </c>
     </row>
     <row r="1186" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1186" s="1" t="s">
-        <v>3555</v>
+        <v>3559</v>
       </c>
       <c r="C1186" t="s">
         <v>3495</v>
@@ -52269,12 +52269,12 @@
         <v>5549</v>
       </c>
       <c r="Q1186" t="s">
-        <v>4591</v>
+        <v>4592</v>
       </c>
     </row>
     <row r="1187" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1187" s="1" t="s">
-        <v>3556</v>
+        <v>3560</v>
       </c>
       <c r="C1187" t="s">
         <v>3495</v>
@@ -52289,12 +52289,12 @@
         <v>5549</v>
       </c>
       <c r="Q1187" t="s">
-        <v>3557</v>
+        <v>4593</v>
       </c>
     </row>
     <row r="1188" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1188" s="1" t="s">
-        <v>3558</v>
+        <v>3561</v>
       </c>
       <c r="C1188" t="s">
         <v>3495</v>
@@ -52309,12 +52309,12 @@
         <v>5549</v>
       </c>
       <c r="Q1188" t="s">
-        <v>4959</v>
+        <v>4960</v>
       </c>
     </row>
     <row r="1189" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1189" s="1" t="s">
-        <v>3559</v>
+        <v>3562</v>
       </c>
       <c r="C1189" t="s">
         <v>3495</v>
@@ -52329,12 +52329,12 @@
         <v>5549</v>
       </c>
       <c r="Q1189" t="s">
-        <v>4592</v>
+        <v>4594</v>
       </c>
     </row>
     <row r="1190" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1190" s="1" t="s">
-        <v>3560</v>
+        <v>3563</v>
       </c>
       <c r="C1190" t="s">
         <v>3495</v>
@@ -52349,12 +52349,12 @@
         <v>5549</v>
       </c>
       <c r="Q1190" t="s">
-        <v>4593</v>
+        <v>4961</v>
       </c>
     </row>
     <row r="1191" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1191" s="1" t="s">
-        <v>3561</v>
+        <v>3564</v>
       </c>
       <c r="C1191" t="s">
         <v>3495</v>
@@ -52369,12 +52369,12 @@
         <v>5549</v>
       </c>
       <c r="Q1191" t="s">
-        <v>4960</v>
+        <v>4962</v>
       </c>
     </row>
     <row r="1192" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1192" s="1" t="s">
-        <v>3562</v>
+        <v>3565</v>
       </c>
       <c r="C1192" t="s">
         <v>3495</v>
@@ -52389,12 +52389,12 @@
         <v>5549</v>
       </c>
       <c r="Q1192" t="s">
-        <v>4594</v>
+        <v>3566</v>
       </c>
     </row>
     <row r="1193" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1193" s="1" t="s">
-        <v>3563</v>
+        <v>3567</v>
       </c>
       <c r="C1193" t="s">
         <v>3495</v>
@@ -52409,12 +52409,12 @@
         <v>5549</v>
       </c>
       <c r="Q1193" t="s">
-        <v>4961</v>
+        <v>3568</v>
       </c>
     </row>
     <row r="1194" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1194" s="1" t="s">
-        <v>3564</v>
+        <v>3569</v>
       </c>
       <c r="C1194" t="s">
         <v>3495</v>
@@ -52429,12 +52429,12 @@
         <v>5549</v>
       </c>
       <c r="Q1194" t="s">
-        <v>4962</v>
+        <v>3570</v>
       </c>
     </row>
     <row r="1195" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1195" s="1" t="s">
-        <v>3565</v>
+        <v>3571</v>
       </c>
       <c r="C1195" t="s">
         <v>3495</v>
@@ -52449,12 +52449,12 @@
         <v>5549</v>
       </c>
       <c r="Q1195" t="s">
-        <v>3566</v>
+        <v>4595</v>
       </c>
     </row>
     <row r="1196" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1196" s="1" t="s">
-        <v>3567</v>
+        <v>3572</v>
       </c>
       <c r="C1196" t="s">
         <v>3495</v>
@@ -52469,12 +52469,12 @@
         <v>5549</v>
       </c>
       <c r="Q1196" t="s">
-        <v>3568</v>
+        <v>3573</v>
       </c>
     </row>
     <row r="1197" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1197" s="1" t="s">
-        <v>3569</v>
+        <v>3574</v>
       </c>
       <c r="C1197" t="s">
         <v>3495</v>
@@ -52489,12 +52489,12 @@
         <v>5549</v>
       </c>
       <c r="Q1197" t="s">
-        <v>3570</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="1198" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1198" s="1" t="s">
-        <v>3571</v>
+        <v>3576</v>
       </c>
       <c r="C1198" t="s">
         <v>3495</v>
@@ -52509,12 +52509,12 @@
         <v>5549</v>
       </c>
       <c r="Q1198" t="s">
-        <v>4595</v>
+        <v>4963</v>
       </c>
     </row>
     <row r="1199" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1199" s="1" t="s">
-        <v>3572</v>
+        <v>3577</v>
       </c>
       <c r="C1199" t="s">
         <v>3495</v>
@@ -52529,12 +52529,12 @@
         <v>5549</v>
       </c>
       <c r="Q1199" t="s">
-        <v>3573</v>
+        <v>3578</v>
       </c>
     </row>
     <row r="1200" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1200" s="1" t="s">
-        <v>3574</v>
+        <v>3579</v>
       </c>
       <c r="C1200" t="s">
         <v>3495</v>
@@ -52549,12 +52549,12 @@
         <v>5549</v>
       </c>
       <c r="Q1200" t="s">
-        <v>3575</v>
+        <v>4964</v>
       </c>
     </row>
     <row r="1201" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1201" s="1" t="s">
-        <v>3576</v>
+        <v>3580</v>
       </c>
       <c r="C1201" t="s">
         <v>3495</v>
@@ -52569,12 +52569,12 @@
         <v>5549</v>
       </c>
       <c r="Q1201" t="s">
-        <v>4963</v>
+        <v>4965</v>
       </c>
     </row>
     <row r="1202" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1202" s="1" t="s">
-        <v>3577</v>
+        <v>3581</v>
       </c>
       <c r="C1202" t="s">
         <v>3495</v>
@@ -52589,12 +52589,12 @@
         <v>5549</v>
       </c>
       <c r="Q1202" t="s">
-        <v>3578</v>
+        <v>4596</v>
       </c>
     </row>
     <row r="1203" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1203" s="1" t="s">
-        <v>3579</v>
+        <v>3582</v>
       </c>
       <c r="C1203" t="s">
         <v>3495</v>
@@ -52609,12 +52609,12 @@
         <v>5549</v>
       </c>
       <c r="Q1203" t="s">
-        <v>4964</v>
+        <v>4966</v>
       </c>
     </row>
     <row r="1204" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1204" s="1" t="s">
-        <v>3580</v>
+        <v>3583</v>
       </c>
       <c r="C1204" t="s">
         <v>3495</v>
@@ -52629,12 +52629,12 @@
         <v>5549</v>
       </c>
       <c r="Q1204" t="s">
-        <v>4965</v>
+        <v>4597</v>
       </c>
     </row>
     <row r="1205" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1205" s="1" t="s">
-        <v>3581</v>
+        <v>3584</v>
       </c>
       <c r="C1205" t="s">
         <v>3495</v>
@@ -52649,12 +52649,12 @@
         <v>5549</v>
       </c>
       <c r="Q1205" t="s">
-        <v>4596</v>
+        <v>4967</v>
       </c>
     </row>
     <row r="1206" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1206" s="1" t="s">
-        <v>3582</v>
+        <v>3585</v>
       </c>
       <c r="C1206" t="s">
         <v>3495</v>
@@ -52669,12 +52669,12 @@
         <v>5549</v>
       </c>
       <c r="Q1206" t="s">
-        <v>4966</v>
+        <v>3586</v>
       </c>
     </row>
     <row r="1207" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1207" s="1" t="s">
-        <v>3583</v>
+        <v>3587</v>
       </c>
       <c r="C1207" t="s">
         <v>3495</v>
@@ -52689,12 +52689,12 @@
         <v>5549</v>
       </c>
       <c r="Q1207" t="s">
-        <v>4597</v>
+        <v>4598</v>
       </c>
     </row>
     <row r="1208" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1208" s="1" t="s">
-        <v>3584</v>
+        <v>3588</v>
       </c>
       <c r="C1208" t="s">
         <v>3495</v>
@@ -52709,12 +52709,12 @@
         <v>5549</v>
       </c>
       <c r="Q1208" t="s">
-        <v>4967</v>
+        <v>4968</v>
       </c>
     </row>
     <row r="1209" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1209" s="1" t="s">
-        <v>3585</v>
+        <v>3589</v>
       </c>
       <c r="C1209" t="s">
         <v>3495</v>
@@ -52729,12 +52729,12 @@
         <v>5549</v>
       </c>
       <c r="Q1209" t="s">
-        <v>3586</v>
+        <v>3590</v>
       </c>
     </row>
     <row r="1210" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1210" s="1" t="s">
-        <v>3587</v>
+        <v>3591</v>
       </c>
       <c r="C1210" t="s">
         <v>3495</v>
@@ -52749,12 +52749,12 @@
         <v>5549</v>
       </c>
       <c r="Q1210" t="s">
-        <v>4598</v>
+        <v>3592</v>
       </c>
     </row>
     <row r="1211" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1211" s="1" t="s">
-        <v>3588</v>
+        <v>3593</v>
       </c>
       <c r="C1211" t="s">
         <v>3495</v>
@@ -52769,12 +52769,12 @@
         <v>5549</v>
       </c>
       <c r="Q1211" t="s">
-        <v>4968</v>
+        <v>4969</v>
       </c>
     </row>
     <row r="1212" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1212" s="1" t="s">
-        <v>3589</v>
+        <v>3594</v>
       </c>
       <c r="C1212" t="s">
         <v>3495</v>
@@ -52789,12 +52789,12 @@
         <v>5549</v>
       </c>
       <c r="Q1212" t="s">
-        <v>3590</v>
+        <v>3595</v>
       </c>
     </row>
     <row r="1213" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1213" s="1" t="s">
-        <v>3591</v>
+        <v>3596</v>
       </c>
       <c r="C1213" t="s">
         <v>3495</v>
@@ -52809,12 +52809,12 @@
         <v>5549</v>
       </c>
       <c r="Q1213" t="s">
-        <v>3592</v>
+        <v>4970</v>
       </c>
     </row>
     <row r="1214" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1214" s="1" t="s">
-        <v>3593</v>
+        <v>3597</v>
       </c>
       <c r="C1214" t="s">
         <v>3495</v>
@@ -52829,12 +52829,12 @@
         <v>5549</v>
       </c>
       <c r="Q1214" t="s">
-        <v>4969</v>
+        <v>4599</v>
       </c>
     </row>
     <row r="1215" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1215" s="1" t="s">
-        <v>3594</v>
+        <v>3598</v>
       </c>
       <c r="C1215" t="s">
         <v>3495</v>
@@ -52849,12 +52849,12 @@
         <v>5549</v>
       </c>
       <c r="Q1215" t="s">
-        <v>3595</v>
+        <v>4600</v>
       </c>
     </row>
     <row r="1216" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1216" s="1" t="s">
-        <v>3596</v>
+        <v>3599</v>
       </c>
       <c r="C1216" t="s">
         <v>3495</v>
@@ -52869,12 +52869,12 @@
         <v>5549</v>
       </c>
       <c r="Q1216" t="s">
-        <v>4970</v>
+        <v>4971</v>
       </c>
     </row>
     <row r="1217" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1217" s="1" t="s">
-        <v>3597</v>
+        <v>3600</v>
       </c>
       <c r="C1217" t="s">
         <v>3495</v>
@@ -52889,12 +52889,12 @@
         <v>5549</v>
       </c>
       <c r="Q1217" t="s">
-        <v>4599</v>
+        <v>4972</v>
       </c>
     </row>
     <row r="1218" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1218" s="1" t="s">
-        <v>3598</v>
+        <v>3601</v>
       </c>
       <c r="C1218" t="s">
         <v>3495</v>
@@ -52909,12 +52909,12 @@
         <v>5549</v>
       </c>
       <c r="Q1218" t="s">
-        <v>4600</v>
+        <v>3602</v>
       </c>
     </row>
     <row r="1219" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1219" s="1" t="s">
-        <v>3599</v>
+        <v>3603</v>
       </c>
       <c r="C1219" t="s">
         <v>3495</v>
@@ -52929,12 +52929,12 @@
         <v>5549</v>
       </c>
       <c r="Q1219" t="s">
-        <v>4971</v>
+        <v>4973</v>
       </c>
     </row>
     <row r="1220" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1220" s="1" t="s">
-        <v>3600</v>
+        <v>3604</v>
       </c>
       <c r="C1220" t="s">
         <v>3495</v>
@@ -52949,12 +52949,12 @@
         <v>5549</v>
       </c>
       <c r="Q1220" t="s">
-        <v>4972</v>
+        <v>3605</v>
       </c>
     </row>
     <row r="1221" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1221" s="1" t="s">
-        <v>3601</v>
+        <v>6932</v>
       </c>
       <c r="C1221" t="s">
         <v>3495</v>
@@ -52969,12 +52969,12 @@
         <v>5549</v>
       </c>
       <c r="Q1221" t="s">
-        <v>3602</v>
+        <v>4974</v>
       </c>
     </row>
     <row r="1222" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1222" s="1" t="s">
-        <v>3603</v>
+        <v>3607</v>
       </c>
       <c r="C1222" t="s">
         <v>3495</v>
@@ -52989,12 +52989,12 @@
         <v>5549</v>
       </c>
       <c r="Q1222" t="s">
-        <v>4973</v>
+        <v>3608</v>
       </c>
     </row>
     <row r="1223" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1223" s="1" t="s">
-        <v>3604</v>
+        <v>3609</v>
       </c>
       <c r="C1223" t="s">
         <v>3495</v>
@@ -53009,12 +53009,12 @@
         <v>5549</v>
       </c>
       <c r="Q1223" t="s">
-        <v>3605</v>
+        <v>3610</v>
       </c>
     </row>
     <row r="1224" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1224" s="1" t="s">
-        <v>6932</v>
+        <v>3611</v>
       </c>
       <c r="C1224" t="s">
         <v>3495</v>
@@ -53029,12 +53029,12 @@
         <v>5549</v>
       </c>
       <c r="Q1224" t="s">
-        <v>4974</v>
+        <v>4975</v>
       </c>
     </row>
     <row r="1225" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1225" s="1" t="s">
-        <v>3607</v>
+        <v>3612</v>
       </c>
       <c r="C1225" t="s">
         <v>3495</v>
@@ -53049,12 +53049,12 @@
         <v>5549</v>
       </c>
       <c r="Q1225" t="s">
-        <v>3608</v>
+        <v>4976</v>
       </c>
     </row>
     <row r="1226" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1226" s="1" t="s">
-        <v>3609</v>
+        <v>3613</v>
       </c>
       <c r="C1226" t="s">
         <v>3495</v>
@@ -53069,12 +53069,12 @@
         <v>5549</v>
       </c>
       <c r="Q1226" t="s">
-        <v>3610</v>
+        <v>3614</v>
       </c>
     </row>
     <row r="1227" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1227" s="1" t="s">
-        <v>3611</v>
+        <v>3615</v>
       </c>
       <c r="C1227" t="s">
         <v>3495</v>
@@ -53089,12 +53089,12 @@
         <v>5549</v>
       </c>
       <c r="Q1227" t="s">
-        <v>4975</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="1228" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1228" s="1" t="s">
-        <v>3612</v>
+        <v>3617</v>
       </c>
       <c r="C1228" t="s">
         <v>3495</v>
@@ -53109,12 +53109,12 @@
         <v>5549</v>
       </c>
       <c r="Q1228" t="s">
-        <v>4976</v>
+        <v>4977</v>
       </c>
     </row>
     <row r="1229" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1229" s="1" t="s">
-        <v>3613</v>
+        <v>3618</v>
       </c>
       <c r="C1229" t="s">
         <v>3495</v>
@@ -53129,12 +53129,12 @@
         <v>5549</v>
       </c>
       <c r="Q1229" t="s">
-        <v>3614</v>
+        <v>3619</v>
       </c>
     </row>
     <row r="1230" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1230" s="1" t="s">
-        <v>3615</v>
+        <v>3620</v>
       </c>
       <c r="C1230" t="s">
         <v>3495</v>
@@ -53149,12 +53149,12 @@
         <v>5549</v>
       </c>
       <c r="Q1230" t="s">
-        <v>3616</v>
+        <v>4978</v>
       </c>
     </row>
     <row r="1231" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1231" s="1" t="s">
-        <v>3617</v>
+        <v>3621</v>
       </c>
       <c r="C1231" t="s">
         <v>3495</v>
@@ -53169,12 +53169,12 @@
         <v>5549</v>
       </c>
       <c r="Q1231" t="s">
-        <v>4977</v>
+        <v>4979</v>
       </c>
     </row>
     <row r="1232" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1232" s="1" t="s">
-        <v>3618</v>
+        <v>3622</v>
       </c>
       <c r="C1232" t="s">
         <v>3495</v>
@@ -53189,12 +53189,12 @@
         <v>5549</v>
       </c>
       <c r="Q1232" t="s">
-        <v>3619</v>
+        <v>4980</v>
       </c>
     </row>
     <row r="1233" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1233" s="1" t="s">
-        <v>3620</v>
+        <v>3623</v>
       </c>
       <c r="C1233" t="s">
         <v>3495</v>
@@ -53209,12 +53209,12 @@
         <v>5549</v>
       </c>
       <c r="Q1233" t="s">
-        <v>4978</v>
+        <v>4601</v>
       </c>
     </row>
     <row r="1234" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1234" s="1" t="s">
-        <v>3621</v>
+        <v>3624</v>
       </c>
       <c r="C1234" t="s">
         <v>3495</v>
@@ -53229,12 +53229,12 @@
         <v>5549</v>
       </c>
       <c r="Q1234" t="s">
-        <v>4979</v>
+        <v>4981</v>
       </c>
     </row>
     <row r="1235" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1235" s="1" t="s">
-        <v>3622</v>
+        <v>3625</v>
       </c>
       <c r="C1235" t="s">
         <v>3495</v>
@@ -53249,12 +53249,12 @@
         <v>5549</v>
       </c>
       <c r="Q1235" t="s">
-        <v>4980</v>
+        <v>4602</v>
       </c>
     </row>
     <row r="1236" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1236" s="1" t="s">
-        <v>3623</v>
+        <v>3626</v>
       </c>
       <c r="C1236" t="s">
         <v>3495</v>
@@ -53269,12 +53269,12 @@
         <v>5549</v>
       </c>
       <c r="Q1236" t="s">
-        <v>4601</v>
+        <v>3627</v>
       </c>
     </row>
     <row r="1237" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1237" s="1" t="s">
-        <v>3624</v>
+        <v>3628</v>
       </c>
       <c r="C1237" t="s">
         <v>3495</v>
@@ -53289,12 +53289,12 @@
         <v>5549</v>
       </c>
       <c r="Q1237" t="s">
-        <v>4981</v>
+        <v>4982</v>
       </c>
     </row>
     <row r="1238" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1238" s="1" t="s">
-        <v>3625</v>
+        <v>3629</v>
       </c>
       <c r="C1238" t="s">
         <v>3495</v>
@@ -53309,12 +53309,12 @@
         <v>5549</v>
       </c>
       <c r="Q1238" t="s">
-        <v>4602</v>
+        <v>4603</v>
       </c>
     </row>
     <row r="1239" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1239" s="1" t="s">
-        <v>3626</v>
+        <v>3630</v>
       </c>
       <c r="C1239" t="s">
         <v>3495</v>
@@ -53329,12 +53329,12 @@
         <v>5549</v>
       </c>
       <c r="Q1239" t="s">
-        <v>3627</v>
+        <v>3631</v>
       </c>
     </row>
     <row r="1240" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1240" s="1" t="s">
-        <v>3628</v>
+        <v>3632</v>
       </c>
       <c r="C1240" t="s">
         <v>3495</v>
@@ -53349,12 +53349,12 @@
         <v>5549</v>
       </c>
       <c r="Q1240" t="s">
-        <v>4982</v>
+        <v>4983</v>
       </c>
     </row>
     <row r="1241" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1241" s="1" t="s">
-        <v>3629</v>
+        <v>3633</v>
       </c>
       <c r="C1241" t="s">
         <v>3495</v>
@@ -53369,12 +53369,12 @@
         <v>5549</v>
       </c>
       <c r="Q1241" t="s">
-        <v>4603</v>
+        <v>3634</v>
       </c>
     </row>
     <row r="1242" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1242" s="1" t="s">
-        <v>3630</v>
+        <v>3635</v>
       </c>
       <c r="C1242" t="s">
         <v>3495</v>
@@ -53389,12 +53389,12 @@
         <v>5549</v>
       </c>
       <c r="Q1242" t="s">
-        <v>3631</v>
+        <v>3636</v>
       </c>
     </row>
     <row r="1243" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1243" s="1" t="s">
-        <v>3632</v>
+        <v>3637</v>
       </c>
       <c r="C1243" t="s">
         <v>3495</v>
@@ -53409,12 +53409,12 @@
         <v>5549</v>
       </c>
       <c r="Q1243" t="s">
-        <v>4983</v>
+        <v>4604</v>
       </c>
     </row>
     <row r="1244" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1244" s="1" t="s">
-        <v>3633</v>
+        <v>3638</v>
       </c>
       <c r="C1244" t="s">
         <v>3495</v>
@@ -53429,12 +53429,12 @@
         <v>5549</v>
       </c>
       <c r="Q1244" t="s">
-        <v>3634</v>
+        <v>3639</v>
       </c>
     </row>
     <row r="1245" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1245" s="1" t="s">
-        <v>3635</v>
+        <v>3640</v>
       </c>
       <c r="C1245" t="s">
         <v>3495</v>
@@ -53449,12 +53449,12 @@
         <v>5549</v>
       </c>
       <c r="Q1245" t="s">
-        <v>3636</v>
+        <v>4984</v>
       </c>
     </row>
     <row r="1246" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1246" s="1" t="s">
-        <v>3637</v>
+        <v>3641</v>
       </c>
       <c r="C1246" t="s">
         <v>3495</v>
@@ -53469,12 +53469,12 @@
         <v>5549</v>
       </c>
       <c r="Q1246" t="s">
-        <v>4604</v>
+        <v>4985</v>
       </c>
     </row>
     <row r="1247" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1247" s="1" t="s">
-        <v>3638</v>
+        <v>3642</v>
       </c>
       <c r="C1247" t="s">
         <v>3495</v>
@@ -53489,12 +53489,12 @@
         <v>5549</v>
       </c>
       <c r="Q1247" t="s">
-        <v>3639</v>
+        <v>4605</v>
       </c>
     </row>
     <row r="1248" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1248" s="1" t="s">
-        <v>3640</v>
+        <v>3643</v>
       </c>
       <c r="C1248" t="s">
         <v>3495</v>
@@ -53509,12 +53509,12 @@
         <v>5549</v>
       </c>
       <c r="Q1248" t="s">
-        <v>4984</v>
+        <v>4986</v>
       </c>
     </row>
     <row r="1249" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1249" s="1" t="s">
-        <v>3641</v>
+        <v>3644</v>
       </c>
       <c r="C1249" t="s">
         <v>3495</v>
@@ -53529,12 +53529,12 @@
         <v>5549</v>
       </c>
       <c r="Q1249" t="s">
-        <v>4985</v>
+        <v>4987</v>
       </c>
     </row>
     <row r="1250" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1250" s="1" t="s">
-        <v>3642</v>
+        <v>3645</v>
       </c>
       <c r="C1250" t="s">
         <v>3495</v>
@@ -53549,12 +53549,12 @@
         <v>5549</v>
       </c>
       <c r="Q1250" t="s">
-        <v>4605</v>
+        <v>3646</v>
       </c>
     </row>
     <row r="1251" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1251" s="1" t="s">
-        <v>3643</v>
+        <v>3647</v>
       </c>
       <c r="C1251" t="s">
         <v>3495</v>
@@ -53569,12 +53569,12 @@
         <v>5549</v>
       </c>
       <c r="Q1251" t="s">
-        <v>4986</v>
+        <v>4988</v>
       </c>
     </row>
     <row r="1252" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1252" s="1" t="s">
-        <v>3644</v>
+        <v>3648</v>
       </c>
       <c r="C1252" t="s">
         <v>3495</v>
@@ -53589,12 +53589,12 @@
         <v>5549</v>
       </c>
       <c r="Q1252" t="s">
-        <v>4987</v>
+        <v>4989</v>
       </c>
     </row>
     <row r="1253" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1253" s="1" t="s">
-        <v>3645</v>
+        <v>3649</v>
       </c>
       <c r="C1253" t="s">
         <v>3495</v>
@@ -53609,12 +53609,12 @@
         <v>5549</v>
       </c>
       <c r="Q1253" t="s">
-        <v>3646</v>
+        <v>3650</v>
       </c>
     </row>
     <row r="1254" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1254" s="1" t="s">
-        <v>3647</v>
+        <v>3651</v>
       </c>
       <c r="C1254" t="s">
         <v>3495</v>
@@ -53629,12 +53629,12 @@
         <v>5549</v>
       </c>
       <c r="Q1254" t="s">
-        <v>4988</v>
+        <v>3652</v>
       </c>
     </row>
     <row r="1255" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1255" s="1" t="s">
-        <v>3648</v>
+        <v>3653</v>
       </c>
       <c r="C1255" t="s">
         <v>3495</v>
@@ -53649,12 +53649,12 @@
         <v>5549</v>
       </c>
       <c r="Q1255" t="s">
-        <v>4989</v>
+        <v>3654</v>
       </c>
     </row>
     <row r="1256" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1256" s="1" t="s">
-        <v>3649</v>
+        <v>3655</v>
       </c>
       <c r="C1256" t="s">
         <v>3495</v>
@@ -53669,12 +53669,12 @@
         <v>5549</v>
       </c>
       <c r="Q1256" t="s">
-        <v>3650</v>
+        <v>3656</v>
       </c>
     </row>
     <row r="1257" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1257" s="1" t="s">
-        <v>3651</v>
+        <v>3657</v>
       </c>
       <c r="C1257" t="s">
         <v>3495</v>
@@ -53689,12 +53689,12 @@
         <v>5549</v>
       </c>
       <c r="Q1257" t="s">
-        <v>3652</v>
+        <v>4990</v>
       </c>
     </row>
     <row r="1258" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1258" s="1" t="s">
-        <v>3653</v>
+        <v>3658</v>
       </c>
       <c r="C1258" t="s">
         <v>3495</v>
@@ -53709,12 +53709,12 @@
         <v>5549</v>
       </c>
       <c r="Q1258" t="s">
-        <v>3654</v>
+        <v>3659</v>
       </c>
     </row>
     <row r="1259" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1259" s="1" t="s">
-        <v>3655</v>
+        <v>3660</v>
       </c>
       <c r="C1259" t="s">
         <v>3495</v>
@@ -53729,12 +53729,12 @@
         <v>5549</v>
       </c>
       <c r="Q1259" t="s">
-        <v>3656</v>
+        <v>3661</v>
       </c>
     </row>
     <row r="1260" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1260" s="1" t="s">
-        <v>3657</v>
+        <v>3662</v>
       </c>
       <c r="C1260" t="s">
         <v>3495</v>
@@ -53749,12 +53749,12 @@
         <v>5549</v>
       </c>
       <c r="Q1260" t="s">
-        <v>4990</v>
+        <v>4991</v>
       </c>
     </row>
     <row r="1261" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1261" s="1" t="s">
-        <v>3658</v>
+        <v>3663</v>
       </c>
       <c r="C1261" t="s">
         <v>3495</v>
@@ -53769,12 +53769,12 @@
         <v>5549</v>
       </c>
       <c r="Q1261" t="s">
-        <v>3659</v>
+        <v>3664</v>
       </c>
     </row>
     <row r="1262" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1262" s="1" t="s">
-        <v>3660</v>
+        <v>3665</v>
       </c>
       <c r="C1262" t="s">
         <v>3495</v>
@@ -53789,12 +53789,12 @@
         <v>5549</v>
       </c>
       <c r="Q1262" t="s">
-        <v>3661</v>
+        <v>4992</v>
       </c>
     </row>
     <row r="1263" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1263" s="1" t="s">
-        <v>3662</v>
+        <v>3666</v>
       </c>
       <c r="C1263" t="s">
         <v>3495</v>
@@ -53809,12 +53809,12 @@
         <v>5549</v>
       </c>
       <c r="Q1263" t="s">
-        <v>4991</v>
+        <v>3667</v>
       </c>
     </row>
     <row r="1264" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1264" s="1" t="s">
-        <v>3663</v>
+        <v>3668</v>
       </c>
       <c r="C1264" t="s">
         <v>3495</v>
@@ -53829,12 +53829,12 @@
         <v>5549</v>
       </c>
       <c r="Q1264" t="s">
-        <v>3664</v>
+        <v>3669</v>
       </c>
     </row>
     <row r="1265" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1265" s="1" t="s">
-        <v>3665</v>
+        <v>3670</v>
       </c>
       <c r="C1265" t="s">
         <v>3495</v>
@@ -53849,12 +53849,12 @@
         <v>5549</v>
       </c>
       <c r="Q1265" t="s">
-        <v>4992</v>
+        <v>3671</v>
       </c>
     </row>
     <row r="1266" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1266" s="1" t="s">
-        <v>3666</v>
+        <v>3672</v>
       </c>
       <c r="C1266" t="s">
         <v>3495</v>
@@ -53869,12 +53869,12 @@
         <v>5549</v>
       </c>
       <c r="Q1266" t="s">
-        <v>3667</v>
+        <v>3673</v>
       </c>
     </row>
     <row r="1267" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1267" s="1" t="s">
-        <v>3668</v>
+        <v>3674</v>
       </c>
       <c r="C1267" t="s">
         <v>3495</v>
@@ -53889,12 +53889,12 @@
         <v>5549</v>
       </c>
       <c r="Q1267" t="s">
-        <v>3669</v>
+        <v>4993</v>
       </c>
     </row>
     <row r="1268" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1268" s="1" t="s">
-        <v>3670</v>
+        <v>3675</v>
       </c>
       <c r="C1268" t="s">
         <v>3495</v>
@@ -53909,12 +53909,12 @@
         <v>5549</v>
       </c>
       <c r="Q1268" t="s">
-        <v>3671</v>
+        <v>4994</v>
       </c>
     </row>
     <row r="1269" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1269" s="1" t="s">
-        <v>3672</v>
+        <v>3676</v>
       </c>
       <c r="C1269" t="s">
         <v>3495</v>
@@ -53929,12 +53929,12 @@
         <v>5549</v>
       </c>
       <c r="Q1269" t="s">
-        <v>3673</v>
+        <v>4995</v>
       </c>
     </row>
     <row r="1270" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1270" s="1" t="s">
-        <v>3674</v>
+        <v>3677</v>
       </c>
       <c r="C1270" t="s">
         <v>3495</v>
@@ -53949,12 +53949,12 @@
         <v>5549</v>
       </c>
       <c r="Q1270" t="s">
-        <v>4993</v>
+        <v>4996</v>
       </c>
     </row>
     <row r="1271" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1271" s="1" t="s">
-        <v>3675</v>
+        <v>3678</v>
       </c>
       <c r="C1271" t="s">
         <v>3495</v>
@@ -53969,12 +53969,12 @@
         <v>5549</v>
       </c>
       <c r="Q1271" t="s">
-        <v>4994</v>
+        <v>4997</v>
       </c>
     </row>
     <row r="1272" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1272" s="1" t="s">
-        <v>3676</v>
+        <v>3679</v>
       </c>
       <c r="C1272" t="s">
         <v>3495</v>
@@ -53989,12 +53989,12 @@
         <v>5549</v>
       </c>
       <c r="Q1272" t="s">
-        <v>4995</v>
+        <v>3680</v>
       </c>
     </row>
     <row r="1273" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1273" s="1" t="s">
-        <v>3677</v>
+        <v>3681</v>
       </c>
       <c r="C1273" t="s">
         <v>3495</v>
@@ -54009,12 +54009,12 @@
         <v>5549</v>
       </c>
       <c r="Q1273" t="s">
-        <v>4996</v>
+        <v>4606</v>
       </c>
     </row>
     <row r="1274" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1274" s="1" t="s">
-        <v>3678</v>
+        <v>3682</v>
       </c>
       <c r="C1274" t="s">
         <v>3495</v>
@@ -54029,12 +54029,12 @@
         <v>5549</v>
       </c>
       <c r="Q1274" t="s">
-        <v>4997</v>
+        <v>3683</v>
       </c>
     </row>
     <row r="1275" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1275" s="1" t="s">
-        <v>3679</v>
+        <v>6933</v>
       </c>
       <c r="C1275" t="s">
         <v>3495</v>
@@ -54049,12 +54049,12 @@
         <v>5549</v>
       </c>
       <c r="Q1275" t="s">
-        <v>3680</v>
+        <v>6934</v>
       </c>
     </row>
     <row r="1276" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1276" s="1" t="s">
-        <v>3681</v>
+        <v>6935</v>
       </c>
       <c r="C1276" t="s">
         <v>3495</v>
@@ -54069,12 +54069,12 @@
         <v>5549</v>
       </c>
       <c r="Q1276" t="s">
-        <v>4606</v>
+        <v>6936</v>
       </c>
     </row>
     <row r="1277" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1277" s="1" t="s">
-        <v>3682</v>
+        <v>6937</v>
       </c>
       <c r="C1277" t="s">
         <v>3495</v>
@@ -54089,12 +54089,12 @@
         <v>5549</v>
       </c>
       <c r="Q1277" t="s">
-        <v>3683</v>
+        <v>6938</v>
       </c>
     </row>
     <row r="1278" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1278" s="1" t="s">
-        <v>6933</v>
+        <v>6939</v>
       </c>
       <c r="C1278" t="s">
         <v>3495</v>
@@ -54109,12 +54109,12 @@
         <v>5549</v>
       </c>
       <c r="Q1278" t="s">
-        <v>6934</v>
+        <v>6940</v>
       </c>
     </row>
     <row r="1279" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1279" s="1" t="s">
-        <v>6935</v>
+        <v>6941</v>
       </c>
       <c r="C1279" t="s">
         <v>3495</v>
@@ -54129,12 +54129,12 @@
         <v>5549</v>
       </c>
       <c r="Q1279" t="s">
-        <v>6936</v>
+        <v>6942</v>
       </c>
     </row>
     <row r="1280" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1280" s="1" t="s">
-        <v>6937</v>
+        <v>6943</v>
       </c>
       <c r="C1280" t="s">
         <v>3495</v>
@@ -54149,12 +54149,12 @@
         <v>5549</v>
       </c>
       <c r="Q1280" t="s">
-        <v>6938</v>
+        <v>6944</v>
       </c>
     </row>
     <row r="1281" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1281" s="1" t="s">
-        <v>6939</v>
+        <v>6945</v>
       </c>
       <c r="C1281" t="s">
         <v>3495</v>
@@ -54169,12 +54169,12 @@
         <v>5549</v>
       </c>
       <c r="Q1281" t="s">
-        <v>6940</v>
+        <v>6946</v>
       </c>
     </row>
     <row r="1282" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1282" s="1" t="s">
-        <v>6941</v>
+        <v>6947</v>
       </c>
       <c r="C1282" t="s">
         <v>3495</v>
@@ -54189,12 +54189,12 @@
         <v>5549</v>
       </c>
       <c r="Q1282" t="s">
-        <v>6942</v>
+        <v>6948</v>
       </c>
     </row>
     <row r="1283" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1283" s="1" t="s">
-        <v>6943</v>
+        <v>6949</v>
       </c>
       <c r="C1283" t="s">
         <v>3495</v>
@@ -54209,12 +54209,12 @@
         <v>5549</v>
       </c>
       <c r="Q1283" t="s">
-        <v>6944</v>
+        <v>6950</v>
       </c>
     </row>
     <row r="1284" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1284" s="1" t="s">
-        <v>6945</v>
+        <v>6951</v>
       </c>
       <c r="C1284" t="s">
         <v>3495</v>
@@ -54229,12 +54229,12 @@
         <v>5549</v>
       </c>
       <c r="Q1284" t="s">
-        <v>6946</v>
+        <v>6952</v>
       </c>
     </row>
     <row r="1285" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1285" s="1" t="s">
-        <v>6947</v>
+        <v>6953</v>
       </c>
       <c r="C1285" t="s">
         <v>3495</v>
@@ -54249,89 +54249,107 @@
         <v>5549</v>
       </c>
       <c r="Q1285" t="s">
-        <v>6948</v>
+        <v>6954</v>
       </c>
     </row>
     <row r="1286" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1286" s="1" t="s">
-        <v>6949</v>
+        <v>2668</v>
       </c>
       <c r="C1286" t="s">
-        <v>3495</v>
+        <v>2669</v>
       </c>
       <c r="D1286" s="1">
         <v>68000</v>
       </c>
-      <c r="E1286" t="s">
-        <v>2426</v>
-      </c>
       <c r="L1286" t="s">
-        <v>5549</v>
+        <v>2670</v>
       </c>
       <c r="Q1286" t="s">
-        <v>6950</v>
+        <v>2671</v>
       </c>
     </row>
     <row r="1287" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1287" s="1" t="s">
-        <v>6951</v>
+        <v>2691</v>
       </c>
       <c r="C1287" t="s">
-        <v>3495</v>
+        <v>2689</v>
       </c>
       <c r="D1287" s="1">
-        <v>68000</v>
+        <v>68010</v>
       </c>
       <c r="E1287" t="s">
-        <v>2426</v>
+        <v>351</v>
       </c>
       <c r="L1287" t="s">
-        <v>5549</v>
+        <v>5238</v>
+      </c>
+      <c r="M1287" t="s">
+        <v>2534</v>
+      </c>
+      <c r="N1287" t="s">
+        <v>3889</v>
       </c>
       <c r="Q1287" t="s">
-        <v>6952</v>
+        <v>4870</v>
       </c>
     </row>
     <row r="1288" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1288" s="1" t="s">
-        <v>6953</v>
+        <v>2688</v>
       </c>
       <c r="C1288" t="s">
-        <v>3495</v>
+        <v>2689</v>
       </c>
       <c r="D1288" s="1">
-        <v>68000</v>
+        <v>68010</v>
       </c>
       <c r="E1288" t="s">
-        <v>2426</v>
+        <v>351</v>
       </c>
       <c r="L1288" t="s">
-        <v>5549</v>
+        <v>5238</v>
+      </c>
+      <c r="M1288" t="s">
+        <v>2534</v>
+      </c>
+      <c r="N1288" t="s">
+        <v>3889</v>
       </c>
       <c r="Q1288" t="s">
-        <v>6954</v>
+        <v>4867</v>
       </c>
     </row>
     <row r="1289" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1289" s="1" t="s">
-        <v>2668</v>
+        <v>2690</v>
       </c>
       <c r="C1289" t="s">
-        <v>2669</v>
+        <v>2689</v>
       </c>
       <c r="D1289" s="1">
-        <v>68000</v>
+        <v>68010</v>
+      </c>
+      <c r="E1289" t="s">
+        <v>351</v>
       </c>
       <c r="L1289" t="s">
-        <v>2670</v>
+        <v>5238</v>
+      </c>
+      <c r="M1289" t="s">
+        <v>2534</v>
+      </c>
+      <c r="N1289" t="s">
+        <v>3889</v>
       </c>
       <c r="Q1289" t="s">
-        <v>2671</v>
+        <v>4868</v>
       </c>
     </row>
     <row r="1290" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1290" s="1" t="s">
-        <v>2691</v>
+        <v>6487</v>
       </c>
       <c r="C1290" t="s">
         <v>2689</v>
@@ -54352,12 +54370,12 @@
         <v>3889</v>
       </c>
       <c r="Q1290" t="s">
-        <v>4870</v>
+        <v>4869</v>
       </c>
     </row>
     <row r="1291" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1291" s="1" t="s">
-        <v>2688</v>
+        <v>6488</v>
       </c>
       <c r="C1291" t="s">
         <v>2689</v>
@@ -54378,12 +54396,12 @@
         <v>3889</v>
       </c>
       <c r="Q1291" t="s">
-        <v>4867</v>
+        <v>6489</v>
       </c>
     </row>
     <row r="1292" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1292" s="1" t="s">
-        <v>2690</v>
+        <v>2692</v>
       </c>
       <c r="C1292" t="s">
         <v>2689</v>
@@ -54404,12 +54422,12 @@
         <v>3889</v>
       </c>
       <c r="Q1292" t="s">
-        <v>4868</v>
+        <v>4871</v>
       </c>
     </row>
     <row r="1293" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1293" s="1" t="s">
-        <v>6487</v>
+        <v>2693</v>
       </c>
       <c r="C1293" t="s">
         <v>2689</v>
@@ -54430,12 +54448,12 @@
         <v>3889</v>
       </c>
       <c r="Q1293" t="s">
-        <v>4869</v>
+        <v>4872</v>
       </c>
     </row>
     <row r="1294" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1294" s="1" t="s">
-        <v>6488</v>
+        <v>2694</v>
       </c>
       <c r="C1294" t="s">
         <v>2689</v>
@@ -54456,12 +54474,12 @@
         <v>3889</v>
       </c>
       <c r="Q1294" t="s">
-        <v>6489</v>
+        <v>4873</v>
       </c>
     </row>
     <row r="1295" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1295" s="1" t="s">
-        <v>2692</v>
+        <v>2695</v>
       </c>
       <c r="C1295" t="s">
         <v>2689</v>
@@ -54482,12 +54500,12 @@
         <v>3889</v>
       </c>
       <c r="Q1295" t="s">
-        <v>4871</v>
+        <v>4874</v>
       </c>
     </row>
     <row r="1296" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1296" s="1" t="s">
-        <v>2693</v>
+        <v>6490</v>
       </c>
       <c r="C1296" t="s">
         <v>2689</v>
@@ -54508,12 +54526,12 @@
         <v>3889</v>
       </c>
       <c r="Q1296" t="s">
-        <v>4872</v>
+        <v>6491</v>
       </c>
     </row>
     <row r="1297" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1297" s="1" t="s">
-        <v>2694</v>
+        <v>2696</v>
       </c>
       <c r="C1297" t="s">
         <v>2689</v>
@@ -54534,12 +54552,12 @@
         <v>3889</v>
       </c>
       <c r="Q1297" t="s">
-        <v>4873</v>
+        <v>4875</v>
       </c>
     </row>
     <row r="1298" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1298" s="1" t="s">
-        <v>2695</v>
+        <v>2697</v>
       </c>
       <c r="C1298" t="s">
         <v>2689</v>
@@ -54560,18 +54578,18 @@
         <v>3889</v>
       </c>
       <c r="Q1298" t="s">
-        <v>4874</v>
+        <v>4876</v>
       </c>
     </row>
     <row r="1299" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1299" s="1" t="s">
-        <v>6490</v>
+        <v>2698</v>
       </c>
       <c r="C1299" t="s">
-        <v>2689</v>
-      </c>
-      <c r="D1299" s="1">
-        <v>68010</v>
+        <v>2699</v>
+      </c>
+      <c r="D1299" s="1" t="s">
+        <v>2700</v>
       </c>
       <c r="E1299" t="s">
         <v>351</v>
@@ -54580,24 +54598,24 @@
         <v>5238</v>
       </c>
       <c r="M1299" t="s">
-        <v>2534</v>
+        <v>2538</v>
       </c>
       <c r="N1299" t="s">
         <v>3889</v>
       </c>
       <c r="Q1299" t="s">
-        <v>6491</v>
+        <v>4877</v>
       </c>
     </row>
     <row r="1300" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1300" s="1" t="s">
-        <v>2696</v>
+        <v>2701</v>
       </c>
       <c r="C1300" t="s">
-        <v>2689</v>
-      </c>
-      <c r="D1300" s="1">
-        <v>68010</v>
+        <v>2699</v>
+      </c>
+      <c r="D1300" s="1" t="s">
+        <v>2700</v>
       </c>
       <c r="E1300" t="s">
         <v>351</v>
@@ -54606,24 +54624,21 @@
         <v>5238</v>
       </c>
       <c r="M1300" t="s">
-        <v>2534</v>
-      </c>
-      <c r="N1300" t="s">
-        <v>3889</v>
+        <v>2538</v>
       </c>
       <c r="Q1300" t="s">
-        <v>4875</v>
+        <v>4416</v>
       </c>
     </row>
     <row r="1301" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1301" s="1" t="s">
-        <v>2697</v>
+        <v>2702</v>
       </c>
       <c r="C1301" t="s">
-        <v>2689</v>
-      </c>
-      <c r="D1301" s="1">
-        <v>68010</v>
+        <v>2699</v>
+      </c>
+      <c r="D1301" s="1" t="s">
+        <v>2700</v>
       </c>
       <c r="E1301" t="s">
         <v>351</v>
@@ -54632,18 +54647,15 @@
         <v>5238</v>
       </c>
       <c r="M1301" t="s">
-        <v>2534</v>
-      </c>
-      <c r="N1301" t="s">
-        <v>3889</v>
+        <v>2538</v>
       </c>
       <c r="Q1301" t="s">
-        <v>4876</v>
+        <v>4417</v>
       </c>
     </row>
     <row r="1302" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1302" s="1" t="s">
-        <v>2698</v>
+        <v>6492</v>
       </c>
       <c r="C1302" t="s">
         <v>2699</v>
@@ -54664,12 +54676,12 @@
         <v>3889</v>
       </c>
       <c r="Q1302" t="s">
-        <v>4877</v>
+        <v>4878</v>
       </c>
     </row>
     <row r="1303" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1303" s="1" t="s">
-        <v>2701</v>
+        <v>2703</v>
       </c>
       <c r="C1303" t="s">
         <v>2699</v>
@@ -54686,13 +54698,16 @@
       <c r="M1303" t="s">
         <v>2538</v>
       </c>
+      <c r="N1303" t="s">
+        <v>3889</v>
+      </c>
       <c r="Q1303" t="s">
-        <v>4416</v>
+        <v>4879</v>
       </c>
     </row>
     <row r="1304" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1304" s="1" t="s">
-        <v>2702</v>
+        <v>2704</v>
       </c>
       <c r="C1304" t="s">
         <v>2699</v>
@@ -54709,13 +54724,16 @@
       <c r="M1304" t="s">
         <v>2538</v>
       </c>
+      <c r="N1304" t="s">
+        <v>3889</v>
+      </c>
       <c r="Q1304" t="s">
-        <v>4417</v>
+        <v>4880</v>
       </c>
     </row>
     <row r="1305" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1305" s="1" t="s">
-        <v>6492</v>
+        <v>2705</v>
       </c>
       <c r="C1305" t="s">
         <v>2699</v>
@@ -54736,89 +54754,11 @@
         <v>3889</v>
       </c>
       <c r="Q1305" t="s">
-        <v>4878</v>
-      </c>
-    </row>
-    <row r="1306" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B1306" s="1" t="s">
-        <v>2703</v>
-      </c>
-      <c r="C1306" t="s">
-        <v>2699</v>
-      </c>
-      <c r="D1306" s="1" t="s">
-        <v>2700</v>
-      </c>
-      <c r="E1306" t="s">
-        <v>351</v>
-      </c>
-      <c r="L1306" t="s">
-        <v>5238</v>
-      </c>
-      <c r="M1306" t="s">
-        <v>2538</v>
-      </c>
-      <c r="N1306" t="s">
-        <v>3889</v>
-      </c>
-      <c r="Q1306" t="s">
-        <v>4879</v>
-      </c>
-    </row>
-    <row r="1307" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B1307" s="1" t="s">
-        <v>2704</v>
-      </c>
-      <c r="C1307" t="s">
-        <v>2699</v>
-      </c>
-      <c r="D1307" s="1" t="s">
-        <v>2700</v>
-      </c>
-      <c r="E1307" t="s">
-        <v>351</v>
-      </c>
-      <c r="L1307" t="s">
-        <v>5238</v>
-      </c>
-      <c r="M1307" t="s">
-        <v>2538</v>
-      </c>
-      <c r="N1307" t="s">
-        <v>3889</v>
-      </c>
-      <c r="Q1307" t="s">
-        <v>4880</v>
-      </c>
-    </row>
-    <row r="1308" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B1308" s="1" t="s">
-        <v>2705</v>
-      </c>
-      <c r="C1308" t="s">
-        <v>2699</v>
-      </c>
-      <c r="D1308" s="1" t="s">
-        <v>2700</v>
-      </c>
-      <c r="E1308" t="s">
-        <v>351</v>
-      </c>
-      <c r="L1308" t="s">
-        <v>5238</v>
-      </c>
-      <c r="M1308" t="s">
-        <v>2538</v>
-      </c>
-      <c r="N1308" t="s">
-        <v>3889</v>
-      </c>
-      <c r="Q1308" t="s">
         <v>4881</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:R1288"/>
+  <autoFilter ref="B1:R1285"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -64490,10 +64430,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R1187"/>
+  <dimension ref="B1:R1190"/>
   <sheetViews>
     <sheetView topLeftCell="A1171" workbookViewId="0">
-      <selection activeCell="A1186" sqref="A1186:XFD1187"/>
+      <selection activeCell="A1188" sqref="A1188:XFD1190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -89788,6 +89728,66 @@
         <v>3443</v>
       </c>
     </row>
+    <row r="1188" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B1188" s="1" t="s">
+        <v>6853</v>
+      </c>
+      <c r="C1188" t="s">
+        <v>6854</v>
+      </c>
+      <c r="D1188" s="1" t="s">
+        <v>3469</v>
+      </c>
+      <c r="E1188" t="s">
+        <v>3794</v>
+      </c>
+      <c r="L1188" t="s">
+        <v>1900</v>
+      </c>
+      <c r="Q1188" t="s">
+        <v>6855</v>
+      </c>
+    </row>
+    <row r="1189" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B1189" s="1" t="s">
+        <v>6856</v>
+      </c>
+      <c r="C1189" t="s">
+        <v>6854</v>
+      </c>
+      <c r="D1189" s="1" t="s">
+        <v>3469</v>
+      </c>
+      <c r="E1189" t="s">
+        <v>3794</v>
+      </c>
+      <c r="L1189" t="s">
+        <v>1900</v>
+      </c>
+      <c r="Q1189" t="s">
+        <v>6857</v>
+      </c>
+    </row>
+    <row r="1190" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B1190" s="1" t="s">
+        <v>3468</v>
+      </c>
+      <c r="C1190" t="s">
+        <v>6854</v>
+      </c>
+      <c r="D1190" s="1" t="s">
+        <v>3469</v>
+      </c>
+      <c r="E1190" t="s">
+        <v>3794</v>
+      </c>
+      <c r="L1190" t="s">
+        <v>1900</v>
+      </c>
+      <c r="Q1190" t="s">
+        <v>3470</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>